<commit_message>
First commit for 264 -331 and refactor UI test
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,19 +5,23 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\cbtautomation-auvenir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Data for Learning\Automation Testing\Selenium\AdvancedJavaSelenium\IdeaProjects\Auvenir-Test-Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11805" windowHeight="8730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11805" windowHeight="8730" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
+    <sheet name="owners" sheetId="2" r:id="rId2"/>
+    <sheet name="consumers" sheetId="3" r:id="rId3"/>
+    <sheet name="institutions" sheetId="4" r:id="rId4"/>
+    <sheet name="consumerAccounts" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="107">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -171,6 +175,183 @@
   </si>
   <si>
     <t>98108</t>
+  </si>
+  <si>
+    <t>ownerUID</t>
+  </si>
+  <si>
+    <t>uid</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>dateCreated</t>
+  </si>
+  <si>
+    <t>Owner1</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>1492599536</t>
+  </si>
+  <si>
+    <t>institutionID</t>
+  </si>
+  <si>
+    <t>consumerUID</t>
+  </si>
+  <si>
+    <t>ownerID</t>
+  </si>
+  <si>
+    <t>userID</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e51</t>
+  </si>
+  <si>
+    <t>callbackURL</t>
+  </si>
+  <si>
+    <t>https://finicity-qa.com/v2</t>
+  </si>
+  <si>
+    <t>integration</t>
+  </si>
+  <si>
+    <t>finicity</t>
+  </si>
+  <si>
+    <t>finLoginID</t>
+  </si>
+  <si>
+    <t>888888</t>
+  </si>
+  <si>
+    <t>Consumer1</t>
+  </si>
+  <si>
+    <t>78958649580</t>
+  </si>
+  <si>
+    <t>454684125154</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>Institution1</t>
+  </si>
+  <si>
+    <t>finID</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>typeDescription</t>
+  </si>
+  <si>
+    <t>urlHomeApp</t>
+  </si>
+  <si>
+    <t>urlLogonApp</t>
+  </si>
+  <si>
+    <t>urlProductApp</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>specialText</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>raw</t>
+  </si>
+  <si>
+    <t>FinBank-local</t>
+  </si>
+  <si>
+    <t>8283407</t>
+  </si>
+  <si>
+    <t>bank free for testing</t>
+  </si>
+  <si>
+    <t>064-984963856</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>consumerID</t>
+  </si>
+  <si>
+    <t>58fe0947e785201de07d335b</t>
+  </si>
+  <si>
+    <t>selected</t>
+  </si>
+  <si>
+    <t>dateSelected</t>
+  </si>
+  <si>
+    <t>finAccountID</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>loaded</t>
+  </si>
+  <si>
+    <t>dateLoaded</t>
+  </si>
+  <si>
+    <t>loadFailCode</t>
+  </si>
+  <si>
+    <t>txnFromDate</t>
+  </si>
+  <si>
+    <t>txnToDate</t>
+  </si>
+  <si>
+    <t>ConsumerAccount1</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>58f8105668c7b0b557c4465f</t>
   </si>
 </sst>
 </file>
@@ -223,7 +404,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -246,12 +427,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -299,6 +493,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -610,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,4 +1105,431 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="L2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
+      <c r="B1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="P1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add more data for Excel test file: Account
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Data for Learning\Automation Testing\Selenium\AdvancedJavaSelenium\IdeaProjects\Auvenir-Test-Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT LOCAL\automation\automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,6 +17,7 @@
     <sheet name="consumers" sheetId="3" r:id="rId3"/>
     <sheet name="institutions" sheetId="4" r:id="rId4"/>
     <sheet name="consumerAccounts" sheetId="5" r:id="rId5"/>
+    <sheet name="accounts" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="118">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -351,7 +352,40 @@
     <t>true</t>
   </si>
   <si>
-    <t>58f8105668c7b0b557c4465f</t>
+    <t>finCustomerID</t>
+  </si>
+  <si>
+    <t>finInstitutionID</t>
+  </si>
+  <si>
+    <t>balance</t>
+  </si>
+  <si>
+    <t>balanceDate</t>
+  </si>
+  <si>
+    <t>finDateCreated</t>
+  </si>
+  <si>
+    <t>lastTransactionDate</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Test account</t>
+  </si>
+  <si>
+    <t>Account1</t>
+  </si>
+  <si>
+    <t>1568274958</t>
+  </si>
+  <si>
+    <t>11111</t>
+  </si>
+  <si>
+    <t>548693585</t>
   </si>
 </sst>
 </file>
@@ -445,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -501,6 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1194,7 +1229,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,7 +1325,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,7 +1451,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,8 +1537,8 @@
       <c r="G2" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>106</v>
+      <c r="H2" t="s">
+        <v>90</v>
       </c>
       <c r="I2" t="s">
         <v>90</v>
@@ -1526,6 +1561,153 @@
       </c>
       <c r="P2" s="14" t="s">
         <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for test script- 331
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11805" windowHeight="8730" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11805" windowHeight="8730" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="121">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -232,9 +232,6 @@
     <t>finLoginID</t>
   </si>
   <si>
-    <t>888888</t>
-  </si>
-  <si>
     <t>Consumer1</t>
   </si>
   <si>
@@ -386,6 +383,18 @@
   </si>
   <si>
     <t>548693585</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>7777</t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1156,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,7 +1174,7 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>48</v>
@@ -1180,7 +1189,7 @@
         <v>51</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H1" s="26" t="s">
         <v>56</v>
@@ -1194,13 +1203,13 @@
         <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>69</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>53</v>
@@ -1209,10 +1218,10 @@
         <v>55</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I2" s="14" t="s">
         <v>53</v>
@@ -1229,7 +1238,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,7 +1258,7 @@
         <v>54</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>58</v>
@@ -1281,19 +1290,19 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>60</v>
@@ -1325,7 +1334,7 @@
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,7 +1354,7 @@
         <v>54</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>63</v>
@@ -1354,48 +1363,48 @@
         <v>51</v>
       </c>
       <c r="E1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>82</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
@@ -1403,41 +1412,41 @@
       <c r="D2" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
         <v>85</v>
       </c>
-      <c r="F2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="H2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J2" t="s">
-        <v>88</v>
-      </c>
-      <c r="K2" s="25" t="s">
+      <c r="L2" t="s">
         <v>87</v>
       </c>
-      <c r="L2" t="s">
-        <v>88</v>
-      </c>
       <c r="M2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1450,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,10 +1479,10 @@
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>50</v>
@@ -1482,48 +1491,48 @@
         <v>51</v>
       </c>
       <c r="F1" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="K1" s="14" t="s">
+      <c r="L1" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="P1" t="s">
         <v>99</v>
-      </c>
-      <c r="P1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>53</v>
@@ -1532,35 +1541,35 @@
         <v>55</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K2" s="14"/>
       <c r="L2" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M2" s="17" t="s">
         <v>55</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1571,10 +1580,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,10 +1599,10 @@
     <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
       <c r="B1" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>58</v>
@@ -1608,60 +1617,66 @@
         <v>51</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>106</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>107</v>
       </c>
       <c r="J1" s="19" t="s">
         <v>65</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M1" s="19" t="s">
         <v>50</v>
       </c>
       <c r="N1" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O1" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="R1" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="S1" s="19" t="s">
-        <v>111</v>
-      </c>
       <c r="T1" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="U1" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" s="14" t="s">
         <v>64</v>
@@ -1670,44 +1685,50 @@
         <v>55</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="J2" s="14"/>
+        <v>84</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17" t="s">
+        <v>119</v>
+      </c>
       <c r="K2" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M2" s="14" t="s">
         <v>53</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O2" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q2" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S2" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepare data for Test 334
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11805" windowHeight="8730" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11805" windowHeight="8730" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="institutions" sheetId="4" r:id="rId4"/>
     <sheet name="consumerAccounts" sheetId="5" r:id="rId5"/>
     <sheet name="accounts" sheetId="6" r:id="rId6"/>
+    <sheet name="authSessions" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="141">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -395,6 +396,315 @@
   </si>
   <si>
     <t>[]</t>
+  </si>
+  <si>
+    <t>AuthSession1</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>{
+    "$schema": "http://json-schema.org/draft-04/schema#",
+    "definitions": {},
+    "id": "http://example.com/example.json",
+    "properties": {
+        "_id": {
+            "id": "/properties/_id",
+            "type": "string"
+        },
+        "accounts": {
+            "id": "/properties/accounts",
+            "items": {
+                "id": "/properties/accounts/items",
+                "properties": {
+                    "0": {
+                        "id": "/properties/accounts/items/properties/0",
+                        "type": "string"
+                    },
+                    "1": {
+                        "id": "/properties/accounts/items/properties/1",
+                        "type": "string"
+                    },
+                    "2": {
+                        "id": "/properties/accounts/items/properties/2",
+                        "type": "string"
+                    },
+                    "3": {
+                        "id": "/properties/accounts/items/properties/3",
+                        "type": "string"
+                    },
+                    "4": {
+                        "id": "/properties/accounts/items/properties/4",
+                        "type": "string"
+                    },
+                    "5": {
+                        "id": "/properties/accounts/items/properties/5",
+                        "type": "string"
+                    },
+                    "6": {
+                        "id": "/properties/accounts/items/properties/6",
+                        "type": "string"
+                    },
+                    "7": {
+                        "id": "/properties/accounts/items/properties/7",
+                        "type": "string"
+                    },
+                    "8": {
+                        "id": "/properties/accounts/items/properties/8",
+                        "type": "string"
+                    },
+                    "9": {
+                        "id": "/properties/accounts/items/properties/9",
+                        "type": "string"
+                    },
+                    "10": {
+                        "id": "/properties/accounts/items/properties/10",
+                        "type": "string"
+                    },
+                    "11": {
+                        "id": "/properties/accounts/items/properties/11",
+                        "type": "string"
+                    },
+                    "12": {
+                        "id": "/properties/accounts/items/properties/12",
+                        "type": "string"
+                    },
+                    "dateCreated": {
+                        "id": "/properties/accounts/items/properties/dateCreated",
+                        "type": "null"
+                    },
+                    "dateSelected": {
+                        "id": "/properties/accounts/items/properties/dateSelected",
+                        "type": "null"
+                    },
+                    "finID": {
+                        "id": "/properties/accounts/items/properties/finID",
+                        "type": "null"
+                    },
+                    "name": {
+                        "id": "/properties/accounts/items/properties/name",
+                        "type": "null"
+                    },
+                    "number": {
+                        "id": "/properties/accounts/items/properties/number",
+                        "type": "null"
+                    },
+                    "selected": {
+                        "id": "/properties/accounts/items/properties/selected",
+                        "type": "boolean"
+                    },
+                    "status": {
+                        "id": "/properties/accounts/items/properties/status",
+                        "type": "null"
+                    },
+                    "transactions": {
+                        "id": "/properties/accounts/items/properties/transactions",
+                        "properties": {
+                            "dateLoaded": {
+                                "id": "/properties/accounts/items/properties/transactions/properties/dateLoaded",
+                                "type": "null"
+                            },
+                            "loadFailCode": {
+                                "id": "/properties/accounts/items/properties/transactions/properties/loadFailCode",
+                                "type": "null"
+                            },
+                            "loaded": {
+                                "id": "/properties/accounts/items/properties/transactions/properties/loaded",
+                                "type": "boolean"
+                            }
+                        },
+                        "type": "object"
+                    },
+                    "type": {
+                        "id": "/properties/accounts/items/properties/type",
+                        "type": "null"
+                    }
+                },
+                "type": "object"
+            },
+            "type": "array"
+        },
+        "callbackURL": {
+            "id": "/properties/callbackURL",
+            "type": "string"
+        },
+        "consumerID": {
+            "id": "/properties/consumerID",
+            "type": "string"
+        },
+        "consumerUID": {
+            "id": "/properties/consumerUID",
+            "type": "string"
+        },
+        "dateCreated": {
+            "id": "/properties/dateCreated",
+            "type": "integer"
+        },
+        "expires": {
+            "id": "/properties/expires",
+            "type": "integer"
+        },
+        "finCustomerID": {
+            "id": "/properties/finCustomerID",
+            "type": "string"
+        },
+        "finLoginID": {
+            "id": "/properties/finLoginID",
+            "type": "null"
+        },
+        "institution": {
+            "id": "/properties/institution",
+            "items": {
+                "id": "/properties/institution/items",
+                "properties": {
+                    "authorized": {
+                        "id": "/properties/institution/items/properties/authorized",
+                        "type": "string"
+                    },
+                    "dateCreated": {
+                        "id": "/properties/institution/items/properties/dateCreated",
+                        "type": "string"
+                    },
+                    "finID": {
+                        "id": "/properties/institution/items/properties/finID",
+                        "type": "string"
+                    },
+                    "name": {
+                        "id": "/properties/institution/items/properties/name",
+                        "type": "string"
+                    },
+                    "rawSource": {
+                        "id": "/properties/institution/items/properties/rawSource",
+                        "type": "string"
+                    }
+                },
+                "type": "object"
+            },
+            "type": "array"
+        },
+        "loginForm": {
+            "id": "/properties/loginForm",
+            "items": {
+                "id": "/properties/loginForm/items",
+                "properties": {
+                    "dateCreated": {
+                        "id": "/properties/loginForm/items/properties/dateCreated",
+                        "type": "string"
+                    },
+                    "formDetails": {
+                        "id": "/properties/loginForm/items/properties/formDetails",
+                        "type": "string"
+                    }
+                },
+                "type": "object"
+            },
+            "type": "array"
+        },
+        "mfa": {
+            "id": "/properties/mfa",
+            "items": {
+                "id": "/properties/mfa/items",
+                "properties": {
+                    "dateCreated": {
+                        "id": "/properties/mfa/items/properties/dateCreated",
+                        "type": "string"
+                    },
+                    "details": {
+                        "id": "/properties/mfa/items/properties/details",
+                        "type": "string"
+                    }
+                },
+                "type": "object"
+            },
+            "type": "array"
+        },
+        "ownerID": {
+            "id": "/properties/ownerID",
+            "type": "string"
+        },
+        "ownerUID": {
+            "id": "/properties/ownerUID",
+            "type": "string"
+        },
+        "previousState": {
+            "id": "/properties/previousState",
+            "type": "string"
+        },
+        "provider": {
+            "id": "/properties/provider",
+            "type": "string"
+        },
+        "socketID": {
+            "id": "/properties/socketID",
+            "type": "string"
+        },
+        "state": {
+            "id": "/properties/state",
+            "type": "string"
+        },
+        "uid": {
+            "id": "/properties/uid",
+            "type": "string"
+        },
+        "userID": {
+            "id": "/properties/userID",
+            "type": "string"
+        }
+    },
+    "type": "object"
+}</t>
+  </si>
+  <si>
+    <t>accounts</t>
+  </si>
+  <si>
+    <t>58f896b67d63f54b5a0200fd</t>
+  </si>
+  <si>
+    <t>expires</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>previousState</t>
+  </si>
+  <si>
+    <t>socketID</t>
+  </si>
+  <si>
+    <t>provider</t>
+  </si>
+  <si>
+    <t>formDetails</t>
+  </si>
+  <si>
+    <t>loginForm</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>mfa</t>
+  </si>
+  <si>
+    <t>institution</t>
+  </si>
+  <si>
+    <t>authorized</t>
+  </si>
+  <si>
+    <t>rawSource</t>
+  </si>
+  <si>
+    <t>accountSchema</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>INIT</t>
   </si>
 </sst>
 </file>
@@ -447,7 +757,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -483,12 +793,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -545,6 +886,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1582,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,4 +2099,239 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="14"/>
+      <c r="B1" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" s="31"/>
+      <c r="T1" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="U1" s="28"/>
+      <c r="V1" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB1" s="30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="V2" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z2" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
+    </row>
+    <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB3" s="16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="M1:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Repart data for Json Schema Verification
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT LOCAL\automation\automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT LOCAL\automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11805" windowHeight="8730" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11805" windowHeight="8730" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="146">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -705,6 +705,211 @@
   </si>
   <si>
     <t>INIT</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "$schema": "http://json-schema.org/draft-04/schema#",
+    "definitions": {},
+    "id": "http://example.com/example.json",
+    "properties": {
+        "consumers": {
+            "id": "/properties/consumers",
+            "items": {
+                "id": "/properties/consumers/items",
+                "properties": {
+                    "consumerID": {
+                        "id": "/properties/consumers/items/properties/consumerID",
+                        "type": "string"
+                    },
+                    "institutionID": {
+                        "id": "/properties/consumers/items/properties/institutionID",
+                        "type": "string"
+                    },
+                    "status": {
+                        "id": "/properties/consumers/items/properties/status",
+                        "type": "string"
+                    }
+                },
+                "type": "object"
+            },
+            "type": "array"
+        },
+        "dateCreated": {
+            "id": "/properties/dateCreated",
+            "type": "integer"
+        },
+        "ownerID": {
+            "id": "/properties/ownerID",
+            "type": "string"
+        },
+        "status": {
+            "id": "/properties/status",
+            "type": "string"
+        },
+        "uid": {
+            "id": "/properties/uid",
+            "type": "string"
+        }
+    },
+    "type": "object"
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "$schema": "http://json-schema.org/draft-04/schema#",
+    "definitions": {},
+    "id": "http://example.com/example.json",
+    "properties": {
+        "callbackURL": {
+            "id": "/properties/callbackURL",
+            "type": "string"
+        },
+        "consumerID": {
+            "id": "/properties/consumerID",
+            "type": "string"
+        },
+        "dateCreated": {
+            "id": "/properties/dateCreated",
+            "type": "integer"
+        },
+        "institutionID": {
+            "id": "/properties/institutionID",
+            "type": "string"
+        },
+        "status": {
+            "id": "/properties/status",
+            "type": "string"
+        },
+        "userID": {
+            "id": "/properties/userID",
+            "type": "string"
+        }
+    },
+    "type": "object"
+}
+</t>
+  </si>
+  <si>
+    <t>{
+  "identifier": "58fe0947e785201de07d335b",
+  "name": "FinBank-local",
+  "typeDescription": "bank free for testing",
+  "urlHomeApp": "none",
+  "urlLogonApp": "none",
+  "urlProductApp": "none",
+  "phone": "064-984963856",
+  "currency": "none",
+  "email": "none",
+  "specialText": "none",
+  "address": "none"
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+    "$schema": "http://json-schema.org/draft-04/schema#",
+    "definitions": {},
+    "id": "http://example.com/example.json",
+    "properties": {
+        "result": {
+            "id": "/properties/result",
+            "items": {
+                "id": "/properties/result/items",
+                "properties": {
+                    "_id": {
+                        "id": "/properties/result/items/properties/_id",
+                        "type": "string"
+                    },
+                    "balanceDate": {
+                        "id": "/properties/result/items/properties/balanceDate",
+                        "type": "integer"
+                    },
+                    "currency": {
+                        "id": "/properties/result/items/properties/currency",
+                        "type": "string"
+                    },
+                    "dateCreated": {
+                        "id": "/properties/result/items/properties/dateCreated",
+                        "type": "integer"
+                    },
+                    "finCustomerID": {
+                        "id": "/properties/result/items/properties/finCustomerID",
+                        "type": "string"
+                    },
+                    "finDateCreated": {
+                        "id": "/properties/result/items/properties/finDateCreated",
+                        "type": "integer"
+                    },
+                    "finID": {
+                        "id": "/properties/result/items/properties/finID",
+                        "type": "string"
+                    },
+                    "finInstitutionID": {
+                        "id": "/properties/result/items/properties/finInstitutionID",
+                        "type": "string"
+                    },
+                    "finLoginID": {
+                        "id": "/properties/result/items/properties/finLoginID",
+                        "type": "integer"
+                    },
+                    "institutionID": {
+                        "id": "/properties/result/items/properties/institutionID",
+                        "type": "string"
+                    },
+                    "integration": {
+                        "id": "/properties/result/items/properties/integration",
+                        "type": "string"
+                    },
+                    "lastTransactionDate": {
+                        "id": "/properties/result/items/properties/lastTransactionDate",
+                        "type": "integer"
+                    },
+                    "name": {
+                        "id": "/properties/result/items/properties/name",
+                        "type": "string"
+                    },
+                    "number": {
+                        "id": "/properties/result/items/properties/number",
+                        "type": "string"
+                    },
+                    "order": {
+                        "id": "/properties/result/items/properties/order",
+                        "items": {},
+                        "type": "array"
+                    },
+                    "ownerID": {
+                        "id": "/properties/result/items/properties/ownerID",
+                        "type": "string"
+                    },
+                    "position": {
+                        "id": "/properties/result/items/properties/position",
+                        "items": {},
+                        "type": "array"
+                    },
+                    "raw": {
+                        "id": "/properties/result/items/properties/raw",
+                        "type": "string"
+                    },
+                    "status": {
+                        "id": "/properties/result/items/properties/status",
+                        "type": "string"
+                    },
+                    "type": {
+                        "id": "/properties/result/items/properties/type",
+                        "type": "string"
+                    }
+                },
+                "type": "object"
+            },
+            "type": "array"
+        }
+    },
+    "type": "object"
+}
+</t>
   </si>
 </sst>
 </file>
@@ -757,7 +962,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -824,12 +1029,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -886,29 +1102,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1517,10 +1737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,7 +1753,7 @@
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>54</v>
       </c>
@@ -1561,8 +1781,11 @@
       <c r="I1" s="26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>52</v>
       </c>
@@ -1589,6 +1812,9 @@
       </c>
       <c r="I2" s="14" t="s">
         <v>53</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1599,10 +1825,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1843,7 @@
     <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>54</v>
       </c>
@@ -1651,8 +1877,11 @@
       <c r="K1" s="22" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>66</v>
       </c>
@@ -1685,6 +1914,9 @@
       </c>
       <c r="K2" s="14" t="s">
         <v>60</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1695,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,7 +1945,7 @@
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>54</v>
       </c>
@@ -1762,8 +1994,11 @@
       <c r="P1" s="21" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>70</v>
       </c>
@@ -1811,6 +2046,9 @@
       </c>
       <c r="P2" t="s">
         <v>87</v>
+      </c>
+      <c r="Q2" s="38" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1944,10 +2182,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,7 +2201,7 @@
     <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19"/>
       <c r="B1" s="19" t="s">
         <v>69</v>
@@ -2028,8 +2266,11 @@
       <c r="V1" s="19" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W1" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>113</v>
       </c>
@@ -2093,6 +2334,9 @@
       </c>
       <c r="V2" s="14" t="s">
         <v>120</v>
+      </c>
+      <c r="W2" s="38" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2105,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,94 +2381,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="S1" s="31"/>
-      <c r="T1" s="35" t="s">
+      <c r="S1" s="35"/>
+      <c r="T1" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="U1" s="28"/>
-      <c r="V1" s="31" t="s">
+      <c r="U1" s="32"/>
+      <c r="V1" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="28" t="s">
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="AB1" s="30" t="s">
+      <c r="AB1" s="36" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
       <c r="R2" s="19" t="s">
         <v>51</v>
       </c>
@@ -2252,45 +2496,45 @@
       <c r="Z2" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="AA2" s="29"/>
-      <c r="AB2" s="29"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
       <c r="T3" s="14"/>
       <c r="U3" s="14"/>
       <c r="V3" s="17" t="s">
@@ -2309,6 +2553,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="T1:U1"/>
@@ -2319,11 +2568,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="P1:P2"/>

</xml_diff>

<commit_message>
finish template code for MongoDB task
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT LOCAL\automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepo\Auvenir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11805" windowHeight="8730" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11805" windowHeight="8730" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="consumerAccounts" sheetId="5" r:id="rId5"/>
     <sheet name="accounts" sheetId="6" r:id="rId6"/>
     <sheet name="authSessions" sheetId="7" r:id="rId7"/>
+    <sheet name="usersRegression" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="179">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -910,6 +911,105 @@
     "type": "object"
 }
 </t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>AUDITOR</t>
+  </si>
+  <si>
+    <t>cuongnguyen@gmail.com</t>
+  </si>
+  <si>
+    <t>doaitran@gmail.com</t>
+  </si>
+  <si>
+    <t>trungngo@gmail.com</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>huy</t>
+  </si>
+  <si>
+    <t>cuong</t>
+  </si>
+  <si>
+    <t>doai</t>
+  </si>
+  <si>
+    <t>trung</t>
+  </si>
+  <si>
+    <t>thuan</t>
+  </si>
+  <si>
+    <t>huynh</t>
+  </si>
+  <si>
+    <t>nguyen</t>
+  </si>
+  <si>
+    <t>tran</t>
+  </si>
+  <si>
+    <t>ngo</t>
+  </si>
+  <si>
+    <t>thuanduong@gmail.com</t>
+  </si>
+  <si>
+    <t>duong</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>591eaabe21dd435e4179739b</t>
+  </si>
+  <si>
+    <t>591eac807d63f54b5a017606</t>
+  </si>
+  <si>
+    <t>591eacec7d63f54b5a017608</t>
+  </si>
+  <si>
+    <t>591eacfc21dd435e417973ab</t>
+  </si>
+  <si>
+    <t>591eba647d63f54b5a01760a</t>
+  </si>
+  <si>
+    <t>JSON String</t>
+  </si>
+  <si>
+    <t>huy.huynh@gmail.com</t>
+  </si>
+  <si>
+    <t>{"_id" : ObjectId("5922b8ae7d63f54b5a01760d"),"status" : "ACTIVE","email" : "cuongnguyen@gmail.com","type" : "ADMIN","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"auth" : {"id" : "DwaPhuT7HzBo-dc4D8v7QjP3G","access" : {"expires" : ISODate("2017-05-22T10:14:11.447Z"),"token" : "$2a$10$wTPiDb0tV9o29dGGN/Phb.sEun3E58vX8wkLvoV0no1CrCtJZWJaK"}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"lastLogin" : ISODate("2017-05-22T08:39:36.797Z"),"dateCreated" : ISODate("2017-05-19T08:20:14.720Z"),"phone" : "","jobTitle" : "","lastName" : "nguyen","firstName" : "cuong","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"_id" : ObjectId("58f9f7e8e5f8e0067a9daf51"),"status" : "ACTIVE","email" : "doai.tran@titancorpvn.com","type" : "ADMIN","auth" : {"id" : "iz09gsKbxF4C-LKqop6KUC2h8","access" : {"expires" : ISODate("2017-05-12T08:51:07.264Z")},"agreements" : [],"devices" : [ {"type" : "DESKTOP","userAgent" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","uniqueID" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","browser" : "Chrome 57.0.2987","model" : "Desktop","access" : {"lastLogin" : ISODate("2017-04-21T12:18:43.706Z")},"os" : "Windows 10 0.0.0","name" : "Tran's Desktop"}, {"type" : "DESKTOP","userAgent" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/58.0.3029.96 Safari/537.36","uniqueID" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/58.0.3029.96 Safari/537.36","browser" : "Chrome 58.0.3029","model" : "Desktop","access" : {"lastLogin" : ISODate("2017-05-04T03:16:45.404Z")},"os" : "Windows 10 0.0.0","name" : "Tran's Desktop"}, {"type" : "DESKTOP","userAgent" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/58.0.3029.81 Safari/537.36","uniqueID" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/58.0.3029.81 Safari/537.36","browser" : "Chrome 58.0.3029","model" : "Desktop","access" : {"lastLogin" : ISODate("2017-05-10T11:24:02.959Z")},"os" : "Windows 10 0.0.0","name" : "Admin's Desktop"}]},"notifications" : {"newRequest" : {"email" : false},"newComment" : {"email" : false},"documentUploaded" : {"email" : false},"messageSent" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"managedBusinesses" : [],"verified" : true,"lastLogin" : ISODate("2017-05-12T08:51:35.282Z"),"dateCreated" : ISODate("2017-04-21T12:15:36.821Z"),"profilePicture" : "58f9f7e8e5f8e0067a9daf51/5915779dde532ae3713e9f8b","howdid" : "","jobTitle" : "","phone" : "0906973162","lastName" : "test","firstName" : "Admin","__v" : 4}</t>
+  </si>
+  <si>
+    <t>{"_id" : ObjectId("58f9fbbce5f8e0067a9daf5d"),"status" : "ACTIVE","email" : "trungngo@gmail.com","type" : "CLIENT","auth" : {"id" : "rWxoGeJfrUf6-J7A6eUOMl0tj","agreements" : [],"devices" : [ {"type" : "DESKTOP","userAgent" : "Mozilla/5.0 (Windows NT 10.0; WOW64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","uniqueID" : "Mozilla/5.0 (Windows NT 10.0; WOW64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","browser" : "Chrome 57.0.2987","model" : "Desktop","access" : {"lastLogin" : ISODate("2017-04-21T12:42:00.512Z")},"os" : "Windows 10 0.0.0","name" : "trung's Desktop"}, {"type" : "DESKTOP","userAgent" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","uniqueID" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","browser" : "Chrome 57.0.2987","model" : "Desktop","access" : {"lastLogin" : ISODate("2017-04-27T01:50:13.190Z")},"os" : "Windows 10 0.0.0","name" : "client's Desktop"}],"access" : {"expires" : ISODate("2017-05-22T09:13:03.530Z")}},"notifications" : {"newRequest" : {"email" : false},"newComment" : {"email" : false},"documentUploaded" : {"email" : false},"messageSent" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"managedBusinesses" : [],"verified" : true,"lastLogin" : ISODate("2017-05-22T09:13:41.937Z"),"dateCreated" : ISODate("2017-04-21T12:31:56.354Z"),"profilePicture" : "58f9fbbce5f8e0067a9daf5d/58f9ff23e5f8e0067a9daf6a","howdid" : "","jobTitle" : "","phone" : "2222222222","lastName" : "so","firstName" : "client","__v" : 4,"agreements" : [],"integrations" : []}</t>
+  </si>
+  <si>
+    <t>{"_id" : ObjectId("58f9fffc433e22f17b1c00a7"),"status" : "ACTIVE","email" : "client06@gmail.com","type" : "CLIENT","auth" : {"id" : "9hfsmY4aBczt-vDQz31UVMNWj","agreements" : [],"devices" : [],"access" : {"expires" : ISODate("2017-05-22T09:14:49.274Z")}},"notifications" : {"newRequest" : {"email" : false},"newComment" : {"email" : false},"documentUploaded" : {"email" : false},"messageSent" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"managedBusinesses" : [],"verified" : false,"lastLogin" : ISODate("2017-05-22T09:15:29.281Z"),"dateCreated" : ISODate("2017-04-21T12:50:04.740Z"),"profilePicture" : "","howdid" : "","jobTitle" : "","phone" : "1234567897","lastName" : "","firstName" : "dfdasfs","__v" : 2,"agreements" : [],"integrations" : []}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "huy.huynh@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "huynh","firstName" : "huy","__v" : 0}</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1107,6 +1207,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1124,10 +1229,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1740,7 +1841,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,7 +1882,7 @@
       <c r="I1" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="31" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1813,7 +1914,7 @@
       <c r="I2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="32" t="s">
         <v>142</v>
       </c>
     </row>
@@ -1915,7 +2016,7 @@
       <c r="K2" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="32" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2047,7 +2148,7 @@
       <c r="P2" t="s">
         <v>87</v>
       </c>
-      <c r="Q2" s="38" t="s">
+      <c r="Q2" s="32" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2184,7 +2285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
@@ -2335,7 +2436,7 @@
       <c r="V2" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="W2" s="38" t="s">
+      <c r="W2" s="32" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2381,94 +2482,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="K1" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="M1" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="N1" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="O1" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="Q1" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="35" t="s">
+      <c r="R1" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="S1" s="35"/>
-      <c r="T1" s="34" t="s">
+      <c r="S1" s="38"/>
+      <c r="T1" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="U1" s="32"/>
-      <c r="V1" s="35" t="s">
+      <c r="U1" s="35"/>
+      <c r="V1" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="32" t="s">
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="AB1" s="36" t="s">
+      <c r="AB1" s="39" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
       <c r="R2" s="19" t="s">
         <v>51</v>
       </c>
@@ -2496,8 +2597,8 @@
       <c r="Z2" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -2553,11 +2654,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="AA1:AA2"/>
     <mergeCell ref="T1:U1"/>
@@ -2574,8 +2670,163 @@
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finish init(drop and create) users on DB with multiple roles for Regression Testing
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="362">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -976,40 +976,589 @@
     <t>ID</t>
   </si>
   <si>
-    <t>591eaabe21dd435e4179739b</t>
-  </si>
-  <si>
-    <t>591eac807d63f54b5a017606</t>
-  </si>
-  <si>
-    <t>591eacec7d63f54b5a017608</t>
-  </si>
-  <si>
-    <t>591eacfc21dd435e417973ab</t>
-  </si>
-  <si>
-    <t>591eba647d63f54b5a01760a</t>
-  </si>
-  <si>
-    <t>JSON String</t>
-  </si>
-  <si>
-    <t>huy.huynh@gmail.com</t>
-  </si>
-  <si>
-    <t>{"_id" : ObjectId("5922b8ae7d63f54b5a01760d"),"status" : "ACTIVE","email" : "cuongnguyen@gmail.com","type" : "ADMIN","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"auth" : {"id" : "DwaPhuT7HzBo-dc4D8v7QjP3G","access" : {"expires" : ISODate("2017-05-22T10:14:11.447Z"),"token" : "$2a$10$wTPiDb0tV9o29dGGN/Phb.sEun3E58vX8wkLvoV0no1CrCtJZWJaK"}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"lastLogin" : ISODate("2017-05-22T08:39:36.797Z"),"dateCreated" : ISODate("2017-05-19T08:20:14.720Z"),"phone" : "","jobTitle" : "","lastName" : "nguyen","firstName" : "cuong","__v" : 0}</t>
-  </si>
-  <si>
-    <t>{"_id" : ObjectId("58f9f7e8e5f8e0067a9daf51"),"status" : "ACTIVE","email" : "doai.tran@titancorpvn.com","type" : "ADMIN","auth" : {"id" : "iz09gsKbxF4C-LKqop6KUC2h8","access" : {"expires" : ISODate("2017-05-12T08:51:07.264Z")},"agreements" : [],"devices" : [ {"type" : "DESKTOP","userAgent" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","uniqueID" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","browser" : "Chrome 57.0.2987","model" : "Desktop","access" : {"lastLogin" : ISODate("2017-04-21T12:18:43.706Z")},"os" : "Windows 10 0.0.0","name" : "Tran's Desktop"}, {"type" : "DESKTOP","userAgent" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/58.0.3029.96 Safari/537.36","uniqueID" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/58.0.3029.96 Safari/537.36","browser" : "Chrome 58.0.3029","model" : "Desktop","access" : {"lastLogin" : ISODate("2017-05-04T03:16:45.404Z")},"os" : "Windows 10 0.0.0","name" : "Tran's Desktop"}, {"type" : "DESKTOP","userAgent" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/58.0.3029.81 Safari/537.36","uniqueID" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/58.0.3029.81 Safari/537.36","browser" : "Chrome 58.0.3029","model" : "Desktop","access" : {"lastLogin" : ISODate("2017-05-10T11:24:02.959Z")},"os" : "Windows 10 0.0.0","name" : "Admin's Desktop"}]},"notifications" : {"newRequest" : {"email" : false},"newComment" : {"email" : false},"documentUploaded" : {"email" : false},"messageSent" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"managedBusinesses" : [],"verified" : true,"lastLogin" : ISODate("2017-05-12T08:51:35.282Z"),"dateCreated" : ISODate("2017-04-21T12:15:36.821Z"),"profilePicture" : "58f9f7e8e5f8e0067a9daf51/5915779dde532ae3713e9f8b","howdid" : "","jobTitle" : "","phone" : "0906973162","lastName" : "test","firstName" : "Admin","__v" : 4}</t>
-  </si>
-  <si>
-    <t>{"_id" : ObjectId("58f9fbbce5f8e0067a9daf5d"),"status" : "ACTIVE","email" : "trungngo@gmail.com","type" : "CLIENT","auth" : {"id" : "rWxoGeJfrUf6-J7A6eUOMl0tj","agreements" : [],"devices" : [ {"type" : "DESKTOP","userAgent" : "Mozilla/5.0 (Windows NT 10.0; WOW64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","uniqueID" : "Mozilla/5.0 (Windows NT 10.0; WOW64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","browser" : "Chrome 57.0.2987","model" : "Desktop","access" : {"lastLogin" : ISODate("2017-04-21T12:42:00.512Z")},"os" : "Windows 10 0.0.0","name" : "trung's Desktop"}, {"type" : "DESKTOP","userAgent" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","uniqueID" : "Mozilla/5.0 (Windows NT 10.0; Win64; x64) AppleWebKit/537.36 (KHTML, like Gecko) Chrome/57.0.2987.133 Safari/537.36","browser" : "Chrome 57.0.2987","model" : "Desktop","access" : {"lastLogin" : ISODate("2017-04-27T01:50:13.190Z")},"os" : "Windows 10 0.0.0","name" : "client's Desktop"}],"access" : {"expires" : ISODate("2017-05-22T09:13:03.530Z")}},"notifications" : {"newRequest" : {"email" : false},"newComment" : {"email" : false},"documentUploaded" : {"email" : false},"messageSent" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"managedBusinesses" : [],"verified" : true,"lastLogin" : ISODate("2017-05-22T09:13:41.937Z"),"dateCreated" : ISODate("2017-04-21T12:31:56.354Z"),"profilePicture" : "58f9fbbce5f8e0067a9daf5d/58f9ff23e5f8e0067a9daf6a","howdid" : "","jobTitle" : "","phone" : "2222222222","lastName" : "so","firstName" : "client","__v" : 4,"agreements" : [],"integrations" : []}</t>
-  </si>
-  <si>
-    <t>{"_id" : ObjectId("58f9fffc433e22f17b1c00a7"),"status" : "ACTIVE","email" : "client06@gmail.com","type" : "CLIENT","auth" : {"id" : "9hfsmY4aBczt-vDQz31UVMNWj","agreements" : [],"devices" : [],"access" : {"expires" : ISODate("2017-05-22T09:14:49.274Z")}},"notifications" : {"newRequest" : {"email" : false},"newComment" : {"email" : false},"documentUploaded" : {"email" : false},"messageSent" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"managedBusinesses" : [],"verified" : false,"lastLogin" : ISODate("2017-05-22T09:15:29.281Z"),"dateCreated" : ISODate("2017-04-21T12:50:04.740Z"),"profilePicture" : "","howdid" : "","jobTitle" : "","phone" : "1234567897","lastName" : "","firstName" : "dfdasfs","__v" : 2,"agreements" : [],"integrations" : []}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "huy.huynh@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "huynh","firstName" : "huy","__v" : 0}</t>
+    <t>{"status" : "ACTIVE","email" : "huyhuynh@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "huynh","firstName" : "huy","__v" : 0}</t>
+  </si>
+  <si>
+    <t>LastLogin</t>
+  </si>
+  <si>
+    <t>DateCreated</t>
+  </si>
+  <si>
+    <t>Expires</t>
+  </si>
+  <si>
+    <t>2017-05-22T08:39:36.797Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T08:20:14.720Z</t>
+  </si>
+  <si>
+    <t>2017-05-22T10:14:11.447Z</t>
+  </si>
+  <si>
+    <t>AuthId</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc4D8v7QjP3G</t>
+  </si>
+  <si>
+    <t>User Json</t>
+  </si>
+  <si>
+    <t>Firm Json</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "cuongnguyen@gmail.com","type" : "ADMIN","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "","lastName" : "nguyen","firstName" : "cuong","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "trungngo@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "ngo","firstName" : "trung","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "thuanduong@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "duong","firstName" : "thuan","__v" : 0}</t>
+  </si>
+  <si>
+    <t>tannguyen@gmail.com</t>
+  </si>
+  <si>
+    <t>duongnguyen@gmail.com</t>
+  </si>
+  <si>
+    <t>vienpham@gmail.com</t>
+  </si>
+  <si>
+    <t>minhnguyen@gmail.com</t>
+  </si>
+  <si>
+    <t>toantrieu@gmail.com</t>
+  </si>
+  <si>
+    <t>tan</t>
+  </si>
+  <si>
+    <t>minh</t>
+  </si>
+  <si>
+    <t>vien</t>
+  </si>
+  <si>
+    <t>toan</t>
+  </si>
+  <si>
+    <t>pham</t>
+  </si>
+  <si>
+    <t>trieu</t>
+  </si>
+  <si>
+    <t>2017-05-23T07:37:56.456Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T07:38:17.986Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T04:45:49.514Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T04:46:05.250Z</t>
+  </si>
+  <si>
+    <t>2017-05-22T08:38:36.797Z</t>
+  </si>
+  <si>
+    <t>2017-05-22T08:31:36.797Z</t>
+  </si>
+  <si>
+    <t>2017-05-22T08:32:36.797Z</t>
+  </si>
+  <si>
+    <t>2017-05-22T08:33:36.797Z</t>
+  </si>
+  <si>
+    <t>2017-05-22T08:34:36.797Z</t>
+  </si>
+  <si>
+    <t>2017-05-22T08:35:36.797Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T08:21:14.720Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T08:22:14.720Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T08:23:14.720Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T08:24:14.720Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T08:25:14.720Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T08:26:14.720Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T08:27:14.720Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T08:28:14.720Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T08:29:14.720Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T07:38:56.456Z</t>
+  </si>
+  <si>
+    <t>2017-05-22T10:15:11.447Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T04:46:49.514Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T07:37:51.456Z</t>
+  </si>
+  <si>
+    <t>2017-05-22T10:14:12.447Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T04:45:43.514Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T07:37:54.456Z</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc4D1v7QjP3G</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc4D2v7QjP3G</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc4D3v7QjP3G</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc4D4v7QjP3G</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc4D5v7QjP3G</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc4D6v7QjP3G</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc4D7v7QjP3G</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc4D9v7QjP3G</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc4D0v7QjP3G</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "doaitran@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "tran","firstName" : "doai","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "tannguyen@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "nguyen","firstName" : "tan","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "duongnguyen@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "nguyen","firstName" : "duong","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "minhnguyen@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "nguyen","firstName" : "minh","__v" : 0}</t>
+  </si>
+  <si>
+    <t>2017-05-22T08:37:36.797Z</t>
+  </si>
+  <si>
+    <t>2017-05-19T09:29:14.720Z</t>
+  </si>
+  <si>
+    <t>DwaPhuT7HzBo-dc5D0v7QjP3G</t>
+  </si>
+  <si>
+    <t>2017-05-23T07:31:54.456Z</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "toantrieu@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "trieu","firstName" : "toan","__v" : 0}</t>
+  </si>
+  <si>
+    <t>auditor</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "huyauditor@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "auditor","firstName" : "huy","__v" : 0}</t>
+  </si>
+  <si>
+    <t>huyauditor@gmail.com</t>
+  </si>
+  <si>
+    <t>huyhuynh@gmail.com</t>
+  </si>
+  <si>
+    <t>{"name" : "cuong","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "huy","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "doai","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "trung","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "thuan","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "tan","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "duong","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "vien","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "minh","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "toan","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "auditor","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
+  </si>
+  <si>
+    <t>haho@gmail.com</t>
+  </si>
+  <si>
+    <t>ha</t>
+  </si>
+  <si>
+    <t>ho</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:13.453Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:21.126Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:03:43.194Z</t>
+  </si>
+  <si>
+    <t>AUwNlTknX9uX-eocvmew1EszS</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "haho@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "ho","firstName" : "ha","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "hacompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
+  </si>
+  <si>
+    <t>uyen</t>
+  </si>
+  <si>
+    <t>linh</t>
+  </si>
+  <si>
+    <t>le</t>
+  </si>
+  <si>
+    <t>quyen</t>
+  </si>
+  <si>
+    <t>thuy</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>dong</t>
+  </si>
+  <si>
+    <t>nhi</t>
+  </si>
+  <si>
+    <t>toc</t>
+  </si>
+  <si>
+    <t>tien</t>
+  </si>
+  <si>
+    <t>huong</t>
+  </si>
+  <si>
+    <t>tram</t>
+  </si>
+  <si>
+    <t>phuong</t>
+  </si>
+  <si>
+    <t>bich</t>
+  </si>
+  <si>
+    <t>khoi</t>
+  </si>
+  <si>
+    <t>uyenlinh@gmail.com</t>
+  </si>
+  <si>
+    <t>lequyen@gmail.com</t>
+  </si>
+  <si>
+    <t>thuychi@gmail.com</t>
+  </si>
+  <si>
+    <t>bichphuong@gmail.com</t>
+  </si>
+  <si>
+    <t>khoimy@gmail.com</t>
+  </si>
+  <si>
+    <t>dongnhi@gmail.com</t>
+  </si>
+  <si>
+    <t>toctien@gmail.com</t>
+  </si>
+  <si>
+    <t>huongtram@gmail.com</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:22.126Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:23.126Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:24.126Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:25.126Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:26.126Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:27.126Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:28.126Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:29.126Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:41:20.126Z</t>
+  </si>
+  <si>
+    <t>miu</t>
+  </si>
+  <si>
+    <t>miule@gmail.com</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:00:40.194Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:03:41.194Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:03:42.194Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:03:44.194Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:03:45.194Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:03:46.194Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:03:47.194Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:03:48.194Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:03:49.194Z</t>
+  </si>
+  <si>
+    <t>AUwNlTknX9uX-eocvmew2EszS</t>
+  </si>
+  <si>
+    <t>AUwNlTknX9uX-eocvmew3EszS</t>
+  </si>
+  <si>
+    <t>AUwNlTknX9uX-eocvmew4EszS</t>
+  </si>
+  <si>
+    <t>AUwNlTknX9uX-eocvmew5EszS</t>
+  </si>
+  <si>
+    <t>AUwNlTknX9uX-eocvmew6EszS</t>
+  </si>
+  <si>
+    <t>AUwNlTknX9uX-eocvmew7EszS</t>
+  </si>
+  <si>
+    <t>AUwNlTknX9uX-eocvmew8EszS</t>
+  </si>
+  <si>
+    <t>AUwNlTknX9uX-eocvmew9EszS</t>
+  </si>
+  <si>
+    <t>AUwNlTknX9uX-eocvmew0EszS</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:42:13.453Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:43:13.453Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:44:13.453Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:45:13.453Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:46:13.453Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:47:13.453Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:48:13.453Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:49:13.453Z</t>
+  </si>
+  <si>
+    <t>2017-05-23T09:40:13.453Z</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "uyenlinh@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "uyen","firstName" : "linh","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "lequyen@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "le","firstName" : "quyen","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "thuychi@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "thuy","firstName" : "chi","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "miule@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "miu","firstName" : "le","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "bichphuong@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "bich","firstName" : "phuong","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "dongnhi@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "dong","firstName" : "nhi","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "khoimy@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "khoi","firstName" : "my","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "toctien@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "toc","firstName" : "tien","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "huongtram@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "huong","firstName" : "tram","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"name" : "linhcompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
+  </si>
+  <si>
+    <t>{"name" : "quyencompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
+  </si>
+  <si>
+    <t>{"name" : "chicompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
+  </si>
+  <si>
+    <t>{"name" : "lecompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
+  </si>
+  <si>
+    <t>{"name" : "phuongcompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
+  </si>
+  <si>
+    <t>{"name" : "mycompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
+  </si>
+  <si>
+    <t>{"name" : "nhicompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
+  </si>
+  <si>
+    <t>{"name" : "tiencompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
+  </si>
+  <si>
+    <t>{"name" : "tramcompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
+  </si>
+  <si>
+    <t>5922b8ae7d63f54b5a017600</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e41</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e42</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e43</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e44</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e45</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e46</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e47</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e48</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e49</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e50</t>
+  </si>
+  <si>
+    <t>5923faefa4f66bc75c90c251</t>
+  </si>
+  <si>
+    <t>5923faefa4f66bc75c90c252</t>
+  </si>
+  <si>
+    <t>5923faefa4f66bc75c90c253</t>
+  </si>
+  <si>
+    <t>5923faefa4f66bc75c90c254</t>
+  </si>
+  <si>
+    <t>5923faefa4f66bc75c90c255</t>
+  </si>
+  <si>
+    <t>5923faefa4f66bc75c90c256</t>
+  </si>
+  <si>
+    <t>5923faefa4f66bc75c90c257</t>
+  </si>
+  <si>
+    <t>5923faefa4f66bc75c90c258</t>
+  </si>
+  <si>
+    <t>5923faefa4f66bc75c90c259</t>
+  </si>
+  <si>
+    <t>5923faefa4f66bc75c90c260</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "vienpham@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "pham","firstName" : "vien","__v" : 0}</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1597,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1058,6 +1607,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1145,7 +1700,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1212,6 +1767,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2482,94 +3038,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="38" t="s">
+      <c r="R1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="S1" s="38"/>
-      <c r="T1" s="37" t="s">
+      <c r="S1" s="39"/>
+      <c r="T1" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="U1" s="35"/>
-      <c r="V1" s="38" t="s">
+      <c r="U1" s="36"/>
+      <c r="V1" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="35" t="s">
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="AB1" s="39" t="s">
+      <c r="AB1" s="40" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
       <c r="R2" s="19" t="s">
         <v>51</v>
       </c>
@@ -2597,8 +3153,8 @@
       <c r="Z2" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
+      <c r="AA2" s="37"/>
+      <c r="AB2" s="37"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
@@ -2683,150 +3239,820 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="B1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="F1" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I2" t="s">
+        <v>192</v>
+      </c>
+      <c r="J2" t="s">
+        <v>178</v>
+      </c>
+      <c r="K2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" t="s">
+        <v>341</v>
+      </c>
+      <c r="F3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" t="s">
+        <v>202</v>
+      </c>
+      <c r="H3" t="s">
+        <v>218</v>
+      </c>
+      <c r="I3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J3" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="33" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="K3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" t="s">
         <v>150</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E4" t="s">
+        <v>342</v>
+      </c>
+      <c r="F4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H4" t="s">
+        <v>219</v>
+      </c>
+      <c r="I4" t="s">
+        <v>194</v>
+      </c>
+      <c r="J4" t="s">
+        <v>227</v>
+      </c>
+      <c r="K4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" t="s">
+        <v>343</v>
+      </c>
+      <c r="F5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G5" t="s">
+        <v>204</v>
+      </c>
+      <c r="H5" t="s">
+        <v>220</v>
+      </c>
+      <c r="I5" t="s">
+        <v>211</v>
+      </c>
+      <c r="J5" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" t="s">
+        <v>344</v>
+      </c>
+      <c r="F6" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H6" t="s">
+        <v>221</v>
+      </c>
+      <c r="I6" t="s">
+        <v>212</v>
+      </c>
+      <c r="J6" t="s">
+        <v>180</v>
+      </c>
+      <c r="K6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" t="s">
+        <v>345</v>
+      </c>
+      <c r="F7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" t="s">
+        <v>222</v>
+      </c>
+      <c r="I7" t="s">
+        <v>213</v>
+      </c>
+      <c r="J7" t="s">
+        <v>228</v>
+      </c>
+      <c r="K7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" t="s">
+        <v>346</v>
+      </c>
+      <c r="F8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G8" t="s">
+        <v>207</v>
+      </c>
+      <c r="H8" t="s">
+        <v>223</v>
+      </c>
+      <c r="I8" t="s">
+        <v>214</v>
+      </c>
+      <c r="J8" t="s">
+        <v>229</v>
+      </c>
+      <c r="K8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E9" t="s">
+        <v>347</v>
+      </c>
+      <c r="F9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" t="s">
+        <v>208</v>
+      </c>
+      <c r="H9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I9" t="s">
+        <v>215</v>
+      </c>
+      <c r="J9" t="s">
+        <v>361</v>
+      </c>
+      <c r="K9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" t="s">
+        <v>348</v>
+      </c>
+      <c r="F10" t="s">
+        <v>200</v>
+      </c>
+      <c r="G10" t="s">
+        <v>209</v>
+      </c>
+      <c r="H10" t="s">
+        <v>225</v>
+      </c>
+      <c r="I10" t="s">
+        <v>216</v>
+      </c>
+      <c r="J10" t="s">
+        <v>230</v>
+      </c>
+      <c r="K10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>185</v>
+      </c>
+      <c r="B11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E11" t="s">
+        <v>349</v>
+      </c>
+      <c r="F11" t="s">
+        <v>201</v>
+      </c>
+      <c r="G11" t="s">
+        <v>210</v>
+      </c>
+      <c r="H11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I11" t="s">
+        <v>217</v>
+      </c>
+      <c r="J11" t="s">
+        <v>235</v>
+      </c>
+      <c r="K11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="B12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" t="s">
         <v>155</v>
       </c>
-      <c r="E2" t="s">
-        <v>160</v>
-      </c>
-      <c r="F2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>169</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D12" t="s">
+        <v>236</v>
+      </c>
+      <c r="E12" t="s">
+        <v>350</v>
+      </c>
+      <c r="F12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G12" t="s">
+        <v>232</v>
+      </c>
+      <c r="H12" t="s">
+        <v>233</v>
+      </c>
+      <c r="I12" t="s">
+        <v>234</v>
+      </c>
+      <c r="J12" t="s">
+        <v>237</v>
+      </c>
+      <c r="K12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="D5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E5" t="s">
-        <v>163</v>
-      </c>
-      <c r="F5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D13" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13" t="s">
+        <v>351</v>
+      </c>
+      <c r="F13" t="s">
+        <v>255</v>
+      </c>
+      <c r="G13" t="s">
+        <v>295</v>
+      </c>
+      <c r="H13" t="s">
+        <v>257</v>
+      </c>
+      <c r="I13" t="s">
+        <v>254</v>
+      </c>
+      <c r="J13" t="s">
+        <v>258</v>
+      </c>
+      <c r="K13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>276</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E6" t="s">
-        <v>165</v>
-      </c>
-      <c r="F6" t="s">
-        <v>177</v>
+      <c r="C14" t="s">
+        <v>260</v>
+      </c>
+      <c r="D14" t="s">
+        <v>261</v>
+      </c>
+      <c r="E14" t="s">
+        <v>352</v>
+      </c>
+      <c r="F14" t="s">
+        <v>284</v>
+      </c>
+      <c r="G14" t="s">
+        <v>296</v>
+      </c>
+      <c r="H14" t="s">
+        <v>304</v>
+      </c>
+      <c r="I14" t="s">
+        <v>313</v>
+      </c>
+      <c r="J14" t="s">
+        <v>322</v>
+      </c>
+      <c r="K14" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>262</v>
+      </c>
+      <c r="D15" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15" t="s">
+        <v>353</v>
+      </c>
+      <c r="F15" t="s">
+        <v>285</v>
+      </c>
+      <c r="G15" t="s">
+        <v>297</v>
+      </c>
+      <c r="H15" t="s">
+        <v>305</v>
+      </c>
+      <c r="I15" t="s">
+        <v>314</v>
+      </c>
+      <c r="J15" t="s">
+        <v>323</v>
+      </c>
+      <c r="K15" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D16" t="s">
+        <v>265</v>
+      </c>
+      <c r="E16" t="s">
+        <v>354</v>
+      </c>
+      <c r="F16" t="s">
+        <v>286</v>
+      </c>
+      <c r="G16" t="s">
+        <v>256</v>
+      </c>
+      <c r="H16" t="s">
+        <v>306</v>
+      </c>
+      <c r="I16" t="s">
+        <v>315</v>
+      </c>
+      <c r="J16" t="s">
+        <v>324</v>
+      </c>
+      <c r="K16" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>294</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>293</v>
+      </c>
+      <c r="D17" t="s">
+        <v>262</v>
+      </c>
+      <c r="E17" t="s">
+        <v>355</v>
+      </c>
+      <c r="F17" t="s">
+        <v>287</v>
+      </c>
+      <c r="G17" t="s">
+        <v>298</v>
+      </c>
+      <c r="H17" t="s">
+        <v>307</v>
+      </c>
+      <c r="I17" t="s">
+        <v>316</v>
+      </c>
+      <c r="J17" t="s">
+        <v>325</v>
+      </c>
+      <c r="K17" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>274</v>
+      </c>
+      <c r="D18" t="s">
+        <v>273</v>
+      </c>
+      <c r="E18" t="s">
+        <v>356</v>
+      </c>
+      <c r="F18" t="s">
+        <v>288</v>
+      </c>
+      <c r="G18" t="s">
+        <v>299</v>
+      </c>
+      <c r="H18" t="s">
+        <v>308</v>
+      </c>
+      <c r="I18" t="s">
+        <v>317</v>
+      </c>
+      <c r="J18" t="s">
+        <v>326</v>
+      </c>
+      <c r="K18" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
+        <v>280</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>275</v>
+      </c>
+      <c r="D19" t="s">
+        <v>266</v>
+      </c>
+      <c r="E19" t="s">
+        <v>357</v>
+      </c>
+      <c r="F19" t="s">
+        <v>289</v>
+      </c>
+      <c r="G19" t="s">
+        <v>300</v>
+      </c>
+      <c r="H19" t="s">
+        <v>309</v>
+      </c>
+      <c r="I19" t="s">
+        <v>318</v>
+      </c>
+      <c r="J19" t="s">
+        <v>328</v>
+      </c>
+      <c r="K19" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>267</v>
+      </c>
+      <c r="D20" t="s">
+        <v>268</v>
+      </c>
+      <c r="E20" t="s">
+        <v>358</v>
+      </c>
+      <c r="F20" t="s">
+        <v>290</v>
+      </c>
+      <c r="G20" t="s">
+        <v>301</v>
+      </c>
+      <c r="H20" t="s">
+        <v>310</v>
+      </c>
+      <c r="I20" t="s">
+        <v>319</v>
+      </c>
+      <c r="J20" t="s">
+        <v>327</v>
+      </c>
+      <c r="K20" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" t="s">
+        <v>269</v>
+      </c>
+      <c r="D21" t="s">
+        <v>270</v>
+      </c>
+      <c r="E21" t="s">
+        <v>359</v>
+      </c>
+      <c r="F21" t="s">
+        <v>291</v>
+      </c>
+      <c r="G21" t="s">
+        <v>302</v>
+      </c>
+      <c r="H21" t="s">
+        <v>311</v>
+      </c>
+      <c r="I21" t="s">
+        <v>320</v>
+      </c>
+      <c r="J21" t="s">
+        <v>329</v>
+      </c>
+      <c r="K21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>271</v>
+      </c>
+      <c r="D22" t="s">
+        <v>272</v>
+      </c>
+      <c r="E22" t="s">
+        <v>360</v>
+      </c>
+      <c r="F22" t="s">
+        <v>292</v>
+      </c>
+      <c r="G22" t="s">
+        <v>303</v>
+      </c>
+      <c r="H22" t="s">
+        <v>312</v>
+      </c>
+      <c r="I22" t="s">
+        <v>321</v>
+      </c>
+      <c r="J22" t="s">
+        <v>330</v>
+      </c>
+      <c r="K22" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
+    <hyperlink ref="A11" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A15" r:id="rId14"/>
+    <hyperlink ref="A16" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A18" r:id="rId17"/>
+    <hyperlink ref="A19" r:id="rId18"/>
+    <hyperlink ref="A20" r:id="rId19"/>
+    <hyperlink ref="A21" r:id="rId20"/>
+    <hyperlink ref="A22" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor AuditorFirmInvalidTest: Combine 29 testcases into one testcase, Rename file FirmPO to AuditorSignUpFirmPage.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="440">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1976,15 +1976,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2043,26 +2034,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2404,136 +2404,136 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" style="25" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="25" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="25" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="25" customWidth="1"/>
-    <col min="7" max="7" width="23" style="25" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="25" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="25" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" style="25" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20" style="25" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" width="28" style="22" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="22" customWidth="1"/>
+    <col min="7" max="7" width="23" style="22" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="22" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" style="22" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" style="22" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="30" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="36" t="s">
+      <c r="I2" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="L2" s="36" t="s">
+      <c r="L2" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
     </row>
     <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="K3" s="33" t="s">
+      <c r="K3" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
     </row>
     <row r="4" spans="1:14" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -2548,7 +2548,7 @@
       <c r="D4" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="32" t="s">
         <v>103</v>
       </c>
       <c r="F4" s="13" t="s">
@@ -2569,120 +2569,120 @@
       <c r="K4" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="L4" s="34"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="29"/>
-      <c r="D10" s="29"/>
+      <c r="B10" s="26"/>
+      <c r="D10" s="26"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C14" s="27"/>
-      <c r="D14" s="26"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="23"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="27"/>
-      <c r="D18" s="26"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2717,11 +2717,11 @@
       <c r="B1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
       <c r="F1" s="10" t="s">
         <v>49</v>
       </c>
@@ -2798,42 +2798,42 @@
       <c r="A1" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="41" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="F1" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="39" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>138</v>
       </c>
       <c r="B2" t="s">
@@ -2866,7 +2866,7 @@
       <c r="K2" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="37" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2897,60 +2897,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="40" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="40" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="M1" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="N1" s="43" t="s">
+      <c r="N1" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="O1" s="43" t="s">
+      <c r="O1" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="P1" s="43" t="s">
+      <c r="P1" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="40" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>156</v>
       </c>
       <c r="B2" t="s">
@@ -2959,7 +2959,7 @@
       <c r="C2" t="s">
         <v>133</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="43" t="s">
         <v>132</v>
       </c>
       <c r="E2" s="13" t="s">
@@ -2980,7 +2980,7 @@
       <c r="J2" t="s">
         <v>152</v>
       </c>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="43" t="s">
         <v>153</v>
       </c>
       <c r="L2" t="s">
@@ -2998,7 +2998,7 @@
       <c r="P2" t="s">
         <v>152</v>
       </c>
-      <c r="Q2" s="40" t="s">
+      <c r="Q2" s="37" t="s">
         <v>151</v>
       </c>
     </row>
@@ -3031,25 +3031,25 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="38" t="s">
         <v>182</v>
       </c>
       <c r="I1" s="7" t="s">
@@ -3078,7 +3078,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="38" t="s">
         <v>174</v>
       </c>
       <c r="B2" t="s">
@@ -3093,7 +3093,7 @@
       <c r="E2" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="28" t="s">
         <v>173</v>
       </c>
       <c r="G2" s="13" t="s">
@@ -3109,7 +3109,7 @@
         <v>172</v>
       </c>
       <c r="K2" s="7"/>
-      <c r="L2" s="31" t="s">
+      <c r="L2" s="28" t="s">
         <v>171</v>
       </c>
       <c r="M2" s="13" t="s">
@@ -3152,72 +3152,72 @@
     <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38"/>
+      <c r="B1" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="O1" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="Q1" s="41" t="s">
+      <c r="Q1" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="R1" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="S1" s="41" t="s">
+      <c r="S1" s="38" t="s">
         <v>197</v>
       </c>
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="U1" s="41" t="s">
+      <c r="U1" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="V1" s="41" t="s">
+      <c r="V1" s="38" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="43" t="s">
+      <c r="W1" s="40" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3262,7 +3262,7 @@
       <c r="N2" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="O2" s="47" t="s">
+      <c r="O2" s="44" t="s">
         <v>152</v>
       </c>
       <c r="P2" s="13" t="s">
@@ -3286,7 +3286,7 @@
       <c r="V2" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="W2" s="40" t="s">
+      <c r="W2" s="37" t="s">
         <v>186</v>
       </c>
     </row>
@@ -3332,160 +3332,160 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="50" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="50" t="s">
         <v>223</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="O1" s="52" t="s">
+      <c r="O1" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="50" t="s">
         <v>217</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="R1" s="51" t="s">
         <v>216</v>
       </c>
-      <c r="S1" s="55"/>
-      <c r="T1" s="56" t="s">
+      <c r="S1" s="51"/>
+      <c r="T1" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="U1" s="54"/>
-      <c r="V1" s="55" t="s">
+      <c r="U1" s="52"/>
+      <c r="V1" s="51" t="s">
         <v>214</v>
       </c>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="54" t="s">
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="AB1" s="53" t="s">
+      <c r="AB1" s="55" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="41" t="s">
+    <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="S2" s="41" t="s">
+      <c r="S2" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="T2" s="43" t="s">
+      <c r="T2" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="U2" s="43" t="s">
+      <c r="U2" s="40" t="s">
         <v>211</v>
       </c>
-      <c r="V2" s="41" t="s">
+      <c r="V2" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="W2" s="41" t="s">
+      <c r="W2" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="X2" s="41" t="s">
+      <c r="X2" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="Y2" s="41" t="s">
+      <c r="Y2" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="Z2" s="41" t="s">
+      <c r="Z2" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="40" t="s">
         <v>208</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="47" t="s">
         <v>207</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="G3" s="48" t="s">
+      <c r="G3" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="45" t="s">
         <v>205</v>
       </c>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="48"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
       <c r="V3" s="13" t="s">
@@ -3498,12 +3498,23 @@
       <c r="AA3" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="AB3" s="35" t="s">
+      <c r="AB3" s="32" t="s">
         <v>203</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -3513,18 +3524,7 @@
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3565,19 +3565,19 @@
       <c r="D1" t="s">
         <v>436</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="49" t="s">
         <v>435</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="49" t="s">
         <v>434</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="49" t="s">
         <v>433</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="49" t="s">
         <v>432</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="49" t="s">
         <v>431</v>
       </c>
       <c r="J1" t="s">
@@ -3588,7 +3588,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="48" t="s">
         <v>428</v>
       </c>
       <c r="B2" t="s">
@@ -3623,7 +3623,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="48" t="s">
         <v>418</v>
       </c>
       <c r="B3" t="s">
@@ -3658,7 +3658,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="48" t="s">
         <v>410</v>
       </c>
       <c r="B4" t="s">
@@ -3693,7 +3693,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="48" t="s">
         <v>400</v>
       </c>
       <c r="B5" t="s">
@@ -3728,7 +3728,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="48" t="s">
         <v>390</v>
       </c>
       <c r="B6" t="s">
@@ -3763,7 +3763,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="48" t="s">
         <v>381</v>
       </c>
       <c r="B7" t="s">
@@ -3798,7 +3798,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="48" t="s">
         <v>372</v>
       </c>
       <c r="B8" t="s">
@@ -3833,7 +3833,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="48" t="s">
         <v>363</v>
       </c>
       <c r="B9" t="s">
@@ -3868,7 +3868,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="48" t="s">
         <v>353</v>
       </c>
       <c r="B10" t="s">
@@ -3903,7 +3903,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="48" t="s">
         <v>343</v>
       </c>
       <c r="B11" t="s">
@@ -3938,7 +3938,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="48" t="s">
         <v>333</v>
       </c>
       <c r="B12" t="s">
@@ -3973,7 +3973,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="48" t="s">
         <v>322</v>
       </c>
       <c r="B13" t="s">
@@ -4008,7 +4008,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="48" t="s">
         <v>312</v>
       </c>
       <c r="B14" t="s">
@@ -4043,7 +4043,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="48" t="s">
         <v>302</v>
       </c>
       <c r="B15" t="s">
@@ -4078,7 +4078,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="48" t="s">
         <v>293</v>
       </c>
       <c r="B16" t="s">
@@ -4113,7 +4113,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="48" t="s">
         <v>283</v>
       </c>
       <c r="B17" t="s">
@@ -4148,7 +4148,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="48" t="s">
         <v>273</v>
       </c>
       <c r="B18" t="s">
@@ -4183,7 +4183,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="48" t="s">
         <v>263</v>
       </c>
       <c r="B19" t="s">
@@ -4218,7 +4218,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="48" t="s">
         <v>253</v>
       </c>
       <c r="B20" t="s">
@@ -4253,7 +4253,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="48" t="s">
         <v>243</v>
       </c>
       <c r="B21" t="s">
@@ -4288,7 +4288,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="57" t="s">
+      <c r="A22" s="48" t="s">
         <v>233</v>
       </c>
       <c r="B22" t="s">
@@ -4355,8 +4355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4839,9 +4839,7 @@
       <c r="B17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>78</v>
-      </c>
+      <c r="C17" s="13"/>
       <c r="D17" s="13" t="s">
         <v>63</v>
       </c>
@@ -4971,12 +4969,12 @@
     <hyperlink ref="F3" r:id="rId4"/>
     <hyperlink ref="E7" r:id="rId5"/>
     <hyperlink ref="E8" r:id="rId6"/>
-    <hyperlink ref="F9" r:id="rId7"/>
-    <hyperlink ref="F10" r:id="rId8"/>
-    <hyperlink ref="G12" r:id="rId9"/>
-    <hyperlink ref="E15" r:id="rId10"/>
-    <hyperlink ref="E18" r:id="rId11"/>
-    <hyperlink ref="E9" r:id="rId12" display="ww@.test.com"/>
+    <hyperlink ref="F10" r:id="rId7"/>
+    <hyperlink ref="G12" r:id="rId8"/>
+    <hyperlink ref="E15" r:id="rId9"/>
+    <hyperlink ref="E18" r:id="rId10"/>
+    <hyperlink ref="E9" r:id="rId11" display="ww@.test.com"/>
+    <hyperlink ref="F9" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId13"/>
@@ -4987,7 +4985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -5008,11 +5006,11 @@
       <c r="B1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
       <c r="F1" s="10" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
update new testdata Excel
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -15,8 +15,9 @@
     <sheet name="authSessions" sheetId="9" r:id="rId6"/>
     <sheet name="usersRegression" sheetId="10" r:id="rId7"/>
     <sheet name="OnBoarding" sheetId="1" r:id="rId8"/>
-    <sheet name="ForgotPassword" sheetId="2" r:id="rId9"/>
-    <sheet name="Login" sheetId="3" r:id="rId10"/>
+    <sheet name="LoginData" sheetId="11" r:id="rId9"/>
+    <sheet name="ForgotPassword" sheetId="2" r:id="rId10"/>
+    <sheet name="Login" sheetId="3" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="448">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1741,12 +1742,36 @@
   <si>
     <t>Email</t>
   </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Auditor</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Valid User</t>
+  </si>
+  <si>
+    <t>InValid User</t>
+  </si>
+  <si>
+    <t>auditor01@gmail.com</t>
+  </si>
+  <si>
+    <t>client01@gmail.com</t>
+  </si>
+  <si>
+    <t>admin01@gmail.com</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1787,6 +1812,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1927,7 +1959,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2039,9 +2071,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2049,6 +2078,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2062,6 +2094,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2399,7 +2441,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2694,6 +2736,102 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="46.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4" display="auvenir.automation.s3@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId5"/>
+    <hyperlink ref="E2" r:id="rId6"/>
+    <hyperlink ref="F2" r:id="rId7"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -3380,22 +3518,22 @@
       <c r="Q1" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="51" t="s">
+      <c r="R1" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="S1" s="51"/>
-      <c r="T1" s="54" t="s">
+      <c r="S1" s="54"/>
+      <c r="T1" s="53" t="s">
         <v>215</v>
       </c>
-      <c r="U1" s="52"/>
-      <c r="V1" s="51" t="s">
+      <c r="U1" s="51"/>
+      <c r="V1" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="52" t="s">
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="51" t="s">
         <v>213</v>
       </c>
       <c r="AB1" s="55" t="s">
@@ -3447,8 +3585,8 @@
       <c r="Z2" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
+      <c r="AA2" s="52"/>
+      <c r="AB2" s="52"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -3504,17 +3642,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -3525,6 +3652,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4355,7 +4493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
@@ -4983,96 +5121,64 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="46.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="57"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="60" t="s">
+        <v>440</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
+        <v>443</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>445</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="s">
+        <v>444</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:E1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4" display="auvenir.automation.s3@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId5"/>
-    <hyperlink ref="E2" r:id="rId6"/>
-    <hyperlink ref="F2" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minhnh updated simpleLogin -> ValidateForgotPasswordTest
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="452">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1758,6 +1758,24 @@
   </si>
   <si>
     <t>9QB5Mpc4</t>
+  </si>
+  <si>
+    <t>t7NelfQF</t>
+  </si>
+  <si>
+    <t>kb3zrNMl</t>
+  </si>
+  <si>
+    <t>gMx9h2jR</t>
+  </si>
+  <si>
+    <t>l6N7UZIH</t>
+  </si>
+  <si>
+    <t>iQ5011Ye</t>
+  </si>
+  <si>
+    <t>J08lZSL0</t>
   </si>
 </sst>
 </file>
@@ -5074,7 +5092,7 @@
         <v>47</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>

</xml_diff>

<commit_message>
vien.Pham edited emailTemplate at 3:19pm June6th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -19,15 +19,15 @@
     <sheet name="Login" sheetId="3" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1"><![CDATA[REPT(LOCAL_YEAR_FORMAT,4)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_MONTH_FORMAT,2)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_DAY_FORMAT,2)&" "&REPT(LOCAL_HOUR_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_MINUTE_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_SECOND_FORMAT,2)]]></definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1"><![CDATA[REPT(LOCAL_YEAR_FORMAT,4)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_MONTH_FORMAT,2)&LOCAL_DATE_SEPARATOR&REPT(LOCAL_DAY_FORMAT,2)&" "&REPT(LOCAL_HOUR_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_MINUTE_FORMAT,2)&LOCAL_TIME_SEPARATOR&REPT(LOCAL_SECOND_FORMAT,2)]]></definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="443">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -125,6 +125,9 @@
     <t>165782</t>
   </si>
   <si>
+    <t>auvenir.automation.s3@gmail.com</t>
+  </si>
+  <si>
     <t>12345678x@X</t>
   </si>
   <si>
@@ -176,9 +179,6 @@
     <t>NOT EXIST</t>
   </si>
   <si>
-    <t>toan.nguyenp@s3corp.com.vn</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>Online</t>
+  </si>
+  <si>
+    <t>n2fPiNNJ</t>
   </si>
   <si>
     <t>Jack Kennady</t>
@@ -1736,35 +1739,22 @@
     <t>Email</t>
   </si>
   <si>
-    <t>C4BGNpYn</t>
-  </si>
-  <si>
-    <t>hoangminh1240</t>
-  </si>
-  <si>
-    <t>minh.nguyentest1212@gmail.com</t>
-  </si>
-  <si>
-    <t>E3y7DMIl</t>
-  </si>
-  <si>
-    <t>9FV19jXW</t>
-  </si>
-  <si>
-    <t>XdW57kfN</t>
-  </si>
-  <si>
-    <t>R4GGftRo</t>
-  </si>
-  <si>
-    <t>9QB5Mpc4</t>
+    <t>admin@auvenir.com</t>
+  </si>
+  <si>
+    <t>Changeit@123</t>
+  </si>
+  <si>
+    <t>ADMIN_ID</t>
+  </si>
+  <si>
+    <t>ADMIN_PWD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2061,6 +2051,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2068,9 +2061,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2426,48 +2416,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="22" width="28.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="22" width="26.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="22" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="22" width="19.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="22" width="20.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="22" width="22.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="22" width="23.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="22" width="22.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="22" width="25.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="22" width="26.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="22" width="15.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="22" width="20.0" collapsed="true"/>
-    <col min="13" max="16384" style="22" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="28" style="22" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="22" customWidth="1"/>
+    <col min="7" max="7" width="23" style="22" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" style="22" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="22" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" style="22" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20" style="22" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="E1" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="F1" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>124</v>
-      </c>
       <c r="G1" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="I1" s="30" t="s">
         <v>108</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>107</v>
       </c>
       <c r="J1" s="30" t="s">
         <v>15</v>
@@ -2476,82 +2466,82 @@
         <v>17</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="34" t="s">
         <v>122</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>121</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>74</v>
       </c>
       <c r="D2" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="F2" s="33" t="s">
         <v>119</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>118</v>
       </c>
       <c r="G2" s="33" t="s">
         <v>71</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I2" s="33" t="s">
         <v>71</v>
       </c>
       <c r="J2" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="K2" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="L2" s="33" t="s">
         <v>115</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>114</v>
       </c>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
     </row>
     <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B3" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="D3" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="E3" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="F3" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="G3" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="H3" s="30" t="s">
         <v>108</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>107</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="K3" s="30" t="s">
         <v>106</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>105</v>
       </c>
       <c r="L3" s="33"/>
       <c r="M3" s="29"/>
@@ -2559,37 +2549,37 @@
     </row>
     <row r="4" spans="1:14" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="F4" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="G4" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="13" t="s">
         <v>96</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>95</v>
       </c>
       <c r="L4" s="31"/>
       <c r="M4" s="29"/>
@@ -2597,19 +2587,19 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="C5" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="D5" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="E5" s="30" t="s">
         <v>91</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>90</v>
       </c>
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
@@ -2623,19 +2613,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="C6" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="D6" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="E6" s="28" t="s">
         <v>86</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>85</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
@@ -2717,69 +2707,85 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="33.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="44.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" s="58"/>
       <c r="E1" s="59"/>
       <c r="F1" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>49</v>
+        <v>38</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>439</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>440</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B5" s="50" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -2790,9 +2796,11 @@
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2806,90 +2814,90 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="37.140625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="D1" s="41" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="E1" s="41" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="F1" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="G1" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="J1" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="K1" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="L1" s="39" t="s">
         <v>138</v>
-      </c>
-      <c r="L1" s="39" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
         <v>136</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="H2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="L2" s="37" t="s">
         <v>129</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="L2" s="37" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2908,120 +2916,120 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="37.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="8" max="9" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>147</v>
-      </c>
       <c r="C1" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="40" t="s">
-        <v>139</v>
-      </c>
       <c r="E1" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="G1" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="40" t="s">
         <v>165</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="J1" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="K1" s="40" t="s">
         <v>162</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="L1" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="M1" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="N1" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="O1" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="P1" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="Q1" s="40" t="s">
         <v>156</v>
-      </c>
-      <c r="Q1" s="40" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" t="s">
         <v>154</v>
       </c>
-      <c r="B2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>153</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" t="s">
+        <v>151</v>
+      </c>
+      <c r="K2" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M2" t="s">
+        <v>151</v>
+      </c>
+      <c r="N2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" t="s">
+        <v>151</v>
+      </c>
+      <c r="P2" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q2" s="37" t="s">
         <v>150</v>
-      </c>
-      <c r="I2" t="s">
-        <v>150</v>
-      </c>
-      <c r="J2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K2" s="43" t="s">
-        <v>151</v>
-      </c>
-      <c r="L2" t="s">
-        <v>150</v>
-      </c>
-      <c r="M2" t="s">
-        <v>150</v>
-      </c>
-      <c r="N2" t="s">
-        <v>150</v>
-      </c>
-      <c r="O2" t="s">
-        <v>150</v>
-      </c>
-      <c r="P2" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q2" s="37" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3040,111 +3048,111 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="14" max="15" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="38" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C1" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="38" t="s">
+      <c r="G1" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="H1" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="I1" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" t="s">
         <v>174</v>
-      </c>
-      <c r="P1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="B2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" s="28" t="s">
+      <c r="G2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="H2" t="s">
-        <v>135</v>
-      </c>
-      <c r="I2" t="s">
-        <v>135</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>170</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>168</v>
-      </c>
       <c r="O2" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3163,153 +3171,153 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38"/>
       <c r="B1" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="D1" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="38" t="s">
-        <v>145</v>
-      </c>
       <c r="E1" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="G1" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="J1" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="K1" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="L1" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="I1" s="38" t="s">
+      <c r="M1" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="N1" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="O1" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="P1" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q1" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="R1" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="S1" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="T1" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="U1" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="V1" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="W1" s="40" t="s">
         <v>138</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="L1" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="M1" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="N1" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="O1" s="38" t="s">
-        <v>198</v>
-      </c>
-      <c r="P1" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q1" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="R1" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="S1" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="T1" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="U1" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="V1" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="W1" s="40" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="H2" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>134</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="L2" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="P2" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="O2" s="44" t="s">
-        <v>150</v>
-      </c>
-      <c r="P2" s="13" t="s">
+      <c r="Q2" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="S2" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="U2" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="V2" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="T2" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="U2" s="7" t="s">
+      <c r="W2" s="37" t="s">
         <v>185</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="W2" s="37" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3328,100 +3336,100 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="23" max="24" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="51" t="s">
-        <v>146</v>
-      </c>
       <c r="D1" s="51" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E1" s="51" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="51" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="51" t="s">
+        <v>221</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>218</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="L1" s="51" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="G1" s="51" t="s">
-        <v>220</v>
-      </c>
-      <c r="H1" s="51" t="s">
-        <v>219</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>218</v>
-      </c>
-      <c r="J1" s="51" t="s">
+      <c r="M1" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="K1" s="51" t="s">
-        <v>200</v>
-      </c>
-      <c r="L1" s="51" t="s">
+      <c r="N1" s="51" t="s">
+        <v>144</v>
+      </c>
+      <c r="O1" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="P1" s="51" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q1" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="R1" s="52" t="s">
+        <v>215</v>
+      </c>
+      <c r="S1" s="52"/>
+      <c r="T1" s="55" t="s">
+        <v>214</v>
+      </c>
+      <c r="U1" s="53"/>
+      <c r="V1" s="52" t="s">
+        <v>213</v>
+      </c>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="53" t="s">
+        <v>212</v>
+      </c>
+      <c r="AB1" s="56" t="s">
         <v>138</v>
-      </c>
-      <c r="M1" s="51" t="s">
-        <v>216</v>
-      </c>
-      <c r="N1" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="O1" s="51" t="s">
-        <v>142</v>
-      </c>
-      <c r="P1" s="51" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q1" s="51" t="s">
-        <v>144</v>
-      </c>
-      <c r="R1" s="55" t="s">
-        <v>214</v>
-      </c>
-      <c r="S1" s="55"/>
-      <c r="T1" s="54" t="s">
-        <v>213</v>
-      </c>
-      <c r="U1" s="52"/>
-      <c r="V1" s="55" t="s">
-        <v>212</v>
-      </c>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="52" t="s">
-        <v>211</v>
-      </c>
-      <c r="AB1" s="56" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
@@ -3443,59 +3451,59 @@
       <c r="P2" s="51"/>
       <c r="Q2" s="51"/>
       <c r="R2" s="38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S2" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="U2" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="T2" s="40" t="s">
-        <v>139</v>
-      </c>
-      <c r="U2" s="40" t="s">
+      <c r="V2" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="X2" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y2" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="V2" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="W2" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="X2" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="Y2" s="38" t="s">
+      <c r="Z2" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="Z2" s="38" t="s">
-        <v>207</v>
-      </c>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="47" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="C3" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="46" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="46" t="s">
+      <c r="G3" s="45" t="s">
         <v>204</v>
       </c>
-      <c r="G3" s="45" t="s">
-        <v>203</v>
-      </c>
       <c r="H3" s="45" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I3" s="45"/>
       <c r="J3" s="45"/>
@@ -3511,21 +3519,32 @@
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
       <c r="V3" s="13" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB3" s="32" t="s">
         <v>202</v>
-      </c>
-      <c r="AB3" s="32" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -3536,17 +3555,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3563,785 +3571,785 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="9.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="29.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B1" t="s">
         <v>437</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>436</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>435</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="49" t="s">
         <v>434</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="F1" s="49" t="s">
         <v>433</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="G1" s="49" t="s">
         <v>432</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="H1" s="49" t="s">
         <v>431</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="I1" s="49" t="s">
         <v>430</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="J1" t="s">
         <v>429</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>428</v>
-      </c>
-      <c r="K1" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
+        <v>427</v>
+      </c>
+      <c r="B2" t="s">
         <v>426</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>425</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>350</v>
+      </c>
+      <c r="E2" t="s">
         <v>424</v>
       </c>
-      <c r="D2" t="s">
-        <v>349</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>423</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>422</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>421</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>420</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>419</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>418</v>
-      </c>
-      <c r="K2" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
+        <v>417</v>
+      </c>
+      <c r="B3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D3" t="s">
         <v>416</v>
       </c>
-      <c r="B3" t="s">
-        <v>330</v>
-      </c>
-      <c r="C3" t="s">
-        <v>329</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>415</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>386</v>
+      </c>
+      <c r="G3" t="s">
         <v>414</v>
       </c>
-      <c r="F3" t="s">
-        <v>385</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>413</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>412</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>411</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>410</v>
-      </c>
-      <c r="K3" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
+        <v>409</v>
+      </c>
+      <c r="B4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C4" t="s">
         <v>408</v>
       </c>
-      <c r="B4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>407</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>406</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>405</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>404</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>403</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>402</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>401</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>400</v>
-      </c>
-      <c r="K4" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
+        <v>399</v>
+      </c>
+      <c r="B5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C5" t="s">
         <v>398</v>
       </c>
-      <c r="B5" t="s">
-        <v>330</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>397</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>396</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>395</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>394</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>393</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>392</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>391</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>390</v>
-      </c>
-      <c r="K5" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
+        <v>389</v>
+      </c>
+      <c r="B6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C6" t="s">
         <v>388</v>
       </c>
-      <c r="B6" t="s">
-        <v>330</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>370</v>
+      </c>
+      <c r="E6" t="s">
         <v>387</v>
       </c>
-      <c r="D6" t="s">
-        <v>369</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>386</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>385</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>384</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>383</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>382</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>381</v>
-      </c>
-      <c r="K6" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
+        <v>380</v>
+      </c>
+      <c r="B7" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" t="s">
         <v>379</v>
       </c>
-      <c r="B7" t="s">
-        <v>330</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>350</v>
+      </c>
+      <c r="E7" t="s">
         <v>378</v>
       </c>
-      <c r="D7" t="s">
-        <v>349</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>377</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>376</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>375</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>374</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>373</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>372</v>
-      </c>
-      <c r="K7" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
+        <v>371</v>
+      </c>
+      <c r="B8" t="s">
+        <v>331</v>
+      </c>
+      <c r="C8" t="s">
         <v>370</v>
       </c>
-      <c r="B8" t="s">
-        <v>330</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E8" t="s">
         <v>369</v>
       </c>
-      <c r="D8" t="s">
-        <v>349</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>368</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>367</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>366</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>365</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>364</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>363</v>
-      </c>
-      <c r="K8" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9" t="s">
+        <v>331</v>
+      </c>
+      <c r="C9" t="s">
         <v>361</v>
       </c>
-      <c r="B9" t="s">
-        <v>330</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>360</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>359</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>358</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>357</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>356</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>355</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>354</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>353</v>
-      </c>
-      <c r="K9" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
+        <v>352</v>
+      </c>
+      <c r="B10" t="s">
+        <v>331</v>
+      </c>
+      <c r="C10" t="s">
         <v>351</v>
       </c>
-      <c r="B10" t="s">
-        <v>330</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>350</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>349</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>348</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>347</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>346</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>345</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>344</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>343</v>
-      </c>
-      <c r="K10" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
+        <v>342</v>
+      </c>
+      <c r="B11" t="s">
+        <v>331</v>
+      </c>
+      <c r="C11" t="s">
         <v>341</v>
       </c>
-      <c r="B11" t="s">
-        <v>330</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>340</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>339</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>338</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>337</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>336</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>335</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>334</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>333</v>
-      </c>
-      <c r="K11" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
+        <v>332</v>
+      </c>
+      <c r="B12" t="s">
         <v>331</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>330</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>329</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>328</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>327</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>326</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>325</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>324</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>323</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>322</v>
-      </c>
-      <c r="K12" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
+        <v>321</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s">
         <v>320</v>
       </c>
-      <c r="B13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>319</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>318</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>317</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>316</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>315</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>314</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>313</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>312</v>
-      </c>
-      <c r="K13" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
+        <v>311</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
         <v>310</v>
       </c>
-      <c r="B14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>309</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>308</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>307</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>306</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>305</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>304</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>303</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>302</v>
-      </c>
-      <c r="K14" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
+        <v>301</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>280</v>
+      </c>
+      <c r="D15" t="s">
         <v>300</v>
       </c>
-      <c r="B15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" t="s">
-        <v>279</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>299</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>298</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>297</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>296</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>295</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>294</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>293</v>
-      </c>
-      <c r="K15" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
         <v>291</v>
       </c>
-      <c r="B16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>290</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>289</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>288</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>287</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>286</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>285</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>284</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>283</v>
-      </c>
-      <c r="K16" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
         <v>281</v>
       </c>
-      <c r="B17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>280</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>279</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>278</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>277</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>276</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>275</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>274</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>273</v>
-      </c>
-      <c r="K17" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
+        <v>272</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
         <v>271</v>
       </c>
-      <c r="B18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>270</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>269</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>268</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>267</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>266</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>265</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>264</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>263</v>
-      </c>
-      <c r="K18" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
         <v>261</v>
       </c>
-      <c r="B19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>260</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>259</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>258</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>257</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>256</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>255</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>254</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>253</v>
-      </c>
-      <c r="K19" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
+        <v>252</v>
+      </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
         <v>251</v>
       </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>250</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>249</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>248</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>247</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>246</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>245</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>244</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>243</v>
-      </c>
-      <c r="K20" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
         <v>241</v>
       </c>
-      <c r="B21" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>240</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>239</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>238</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>237</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>236</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>235</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>234</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>233</v>
-      </c>
-      <c r="K21" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
         <v>231</v>
       </c>
-      <c r="B22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>230</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>229</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>228</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>227</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>226</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>225</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>224</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>223</v>
-      </c>
-      <c r="K22" t="s">
-        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -4383,22 +4391,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -5007,62 +5015,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="41.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="34.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="46.85546875" collapsed="true"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="46.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" s="58"/>
       <c r="E1" s="59"/>
       <c r="F1" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>440</v>
+        <v>40</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>439</v>
+        <v>41</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -5071,10 +5079,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>445</v>
+        <v>85</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -5087,7 +5095,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2" display="2017@TiTan"/>
+    <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="C2" r:id="rId4" display="auvenir.automation.s3@gmail.com"/>
     <hyperlink ref="D2" r:id="rId5"/>

</xml_diff>

<commit_message>
refactor and review smoke test
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
     <sheet name="consumers" sheetId="5" r:id="rId2"/>
     <sheet name="institutions" sheetId="6" r:id="rId3"/>
     <sheet name="consumerAccounts" sheetId="7" r:id="rId4"/>
-    <sheet name="accounts" sheetId="8" r:id="rId5"/>
-    <sheet name="authSessions" sheetId="9" r:id="rId6"/>
-    <sheet name="usersRegression" sheetId="10" r:id="rId7"/>
-    <sheet name="OnBoarding" sheetId="1" r:id="rId8"/>
-    <sheet name="ForgotPassword" sheetId="2" r:id="rId9"/>
-    <sheet name="Login" sheetId="3" r:id="rId10"/>
+    <sheet name="LoginData" sheetId="11" r:id="rId5"/>
+    <sheet name="accounts" sheetId="8" r:id="rId6"/>
+    <sheet name="authSessions" sheetId="9" r:id="rId7"/>
+    <sheet name="usersRegression" sheetId="10" r:id="rId8"/>
+    <sheet name="OnBoarding" sheetId="1" r:id="rId9"/>
+    <sheet name="ForgotPassword" sheetId="2" r:id="rId10"/>
+    <sheet name="Login" sheetId="3" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="455">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1750,6 +1751,42 @@
   <si>
     <t>ADMIN_PWD</t>
   </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Auditor</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>admin.user01@gmail.com</t>
+  </si>
+  <si>
+    <t>auditor.user01@gmail.com</t>
+  </si>
+  <si>
+    <t>client.user01@gmail.com</t>
+  </si>
+  <si>
+    <t>Valid User</t>
+  </si>
+  <si>
+    <t>Valid User2</t>
+  </si>
+  <si>
+    <t>Auditor Lead</t>
+  </si>
+  <si>
+    <t>admin.user02@gmail.com</t>
+  </si>
+  <si>
+    <t>auditor.user02gmail.com</t>
+  </si>
+  <si>
+    <t>client.user02@gmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -1936,7 +1973,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2075,6 +2112,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2707,9 +2745,105 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="46.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="57" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4" display="auvenir.automation.s3@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId5"/>
+    <hyperlink ref="E2" r:id="rId6"/>
+    <hyperlink ref="F2" r:id="rId7"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId8"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3163,6 +3297,84 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="60" t="s">
+        <v>443</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>445</v>
+      </c>
+      <c r="E1" s="60" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>449</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>452</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>453</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="48"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId5" display="auditor.user01@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -3326,7 +3538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB3"/>
   <sheetViews>
@@ -3561,7 +3773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
@@ -4381,7 +4593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
@@ -5009,100 +5221,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId13"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="46.85546875" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:E1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4" display="auvenir.automation.s3@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId5"/>
-    <hyperlink ref="E2" r:id="rId6"/>
-    <hyperlink ref="F2" r:id="rId7"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId8"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor AuditorFirmInvalidTest class and AuditorOnBoardingTest class into one class Autditor
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="456">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1786,6 +1786,9 @@
   </si>
   <si>
     <t>client.user02@gmail.com</t>
+  </si>
+  <si>
+    <t>test.loginauvenir@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2085,11 +2088,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2098,6 +2099,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2112,7 +2116,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2768,11 +2771,11 @@
       <c r="B1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="10" t="s">
         <v>49</v>
       </c>
@@ -2843,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2863,11 +2866,11 @@
       <c r="B1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="60"/>
       <c r="F1" s="10" t="s">
         <v>49</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>439</v>
+        <v>455</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>35</v>
@@ -3299,7 +3302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3314,21 +3317,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="51" t="s">
         <v>443</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="51" t="s">
         <v>445</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="51" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="51" t="s">
         <v>449</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -3343,7 +3346,7 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="51" t="s">
         <v>450</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -3574,94 +3577,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="52" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="52" t="s">
         <v>222</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="52" t="s">
         <v>221</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="52" t="s">
         <v>220</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="52" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="52" t="s">
         <v>218</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="52" t="s">
         <v>139</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="52" t="s">
         <v>217</v>
       </c>
-      <c r="N1" s="51" t="s">
+      <c r="N1" s="52" t="s">
         <v>144</v>
       </c>
-      <c r="O1" s="51" t="s">
+      <c r="O1" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="P1" s="51" t="s">
+      <c r="P1" s="52" t="s">
         <v>216</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="Q1" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="S1" s="52"/>
+      <c r="S1" s="56"/>
       <c r="T1" s="55" t="s">
         <v>214</v>
       </c>
       <c r="U1" s="53"/>
-      <c r="V1" s="52" t="s">
+      <c r="V1" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
       <c r="AA1" s="53" t="s">
         <v>212</v>
       </c>
-      <c r="AB1" s="56" t="s">
+      <c r="AB1" s="57" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
       <c r="R2" s="38" t="s">
         <v>140</v>
       </c>
@@ -3746,17 +3749,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -3767,6 +3759,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix get [user]_ID from excel
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="453">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1740,18 +1740,9 @@
     <t>Email</t>
   </si>
   <si>
-    <t>admin@auvenir.com</t>
-  </si>
-  <si>
     <t>Changeit@123</t>
   </si>
   <si>
-    <t>ADMIN_ID</t>
-  </si>
-  <si>
-    <t>ADMIN_PWD</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -1761,12 +1752,6 @@
     <t>Client</t>
   </si>
   <si>
-    <t>admin.user01@gmail.com</t>
-  </si>
-  <si>
-    <t>auditor.user01@gmail.com</t>
-  </si>
-  <si>
     <t>client.user01@gmail.com</t>
   </si>
   <si>
@@ -1789,6 +1774,12 @@
   </si>
   <si>
     <t>test.loginauvenir@gmail.com</t>
+  </si>
+  <si>
+    <t>ADMIN_USER_ID</t>
+  </si>
+  <si>
+    <t>ADMIN_USER_PWD</t>
   </si>
 </sst>
 </file>
@@ -2092,6 +2083,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2099,9 +2093,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2846,8 +2837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2880,7 +2871,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>35</v>
@@ -2900,7 +2891,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -2910,19 +2901,19 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>441</v>
+      <c r="A4" s="9" t="s">
+        <v>451</v>
       </c>
       <c r="B4" s="50" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>439</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>442</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -3302,8 +3293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3318,45 +3309,45 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C1" s="51" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>446</v>
+        <v>417</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>447</v>
+        <v>417</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -3625,22 +3616,22 @@
       <c r="Q1" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="53" t="s">
         <v>215</v>
       </c>
-      <c r="S1" s="56"/>
-      <c r="T1" s="55" t="s">
+      <c r="S1" s="53"/>
+      <c r="T1" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="56" t="s">
+      <c r="U1" s="54"/>
+      <c r="V1" s="53" t="s">
         <v>213</v>
       </c>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="53" t="s">
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="54" t="s">
         <v>212</v>
       </c>
       <c r="AB1" s="57" t="s">
@@ -3692,8 +3683,8 @@
       <c r="Z2" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -3749,6 +3740,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -3759,17 +3761,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vien.Pham edited emailTemplate at 5:52pm June12th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="459">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1781,6 +1781,24 @@
   <si>
     <t>ADMIN_USER_PWD</t>
   </si>
+  <si>
+    <t>Valid User3</t>
+  </si>
+  <si>
+    <t>auvenirtest@gmail.com</t>
+  </si>
+  <si>
+    <t>auvenirclient@gmail.com</t>
+  </si>
+  <si>
+    <t>admin@auvenir.com</t>
+  </si>
+  <si>
+    <t>COMMON_PWD</t>
+  </si>
+  <si>
+    <t>Change@123</t>
+  </si>
 </sst>
 </file>
 
@@ -1858,7 +1876,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1962,12 +1980,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2083,9 +2112,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2093,6 +2119,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2106,6 +2135,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2742,7 +2774,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2835,10 +2867,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2916,6 +2948,14 @@
         <v>439</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="61" t="s">
+        <v>457</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>458</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:E1"/>
@@ -2926,9 +2966,10 @@
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="B4" r:id="rId4"/>
     <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -3294,7 +3335,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3351,6 +3392,20 @@
       </c>
       <c r="E3" s="7"/>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>453</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>456</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>454</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>455</v>
+      </c>
+    </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="48"/>
     </row>
@@ -3362,6 +3417,9 @@
     <hyperlink ref="B3" r:id="rId4"/>
     <hyperlink ref="C3" r:id="rId5" display="auditor.user01@gmail.com"/>
     <hyperlink ref="D3" r:id="rId6"/>
+    <hyperlink ref="C4" r:id="rId7"/>
+    <hyperlink ref="D4" r:id="rId8"/>
+    <hyperlink ref="B4" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3616,22 +3674,22 @@
       <c r="Q1" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="R1" s="53" t="s">
+      <c r="R1" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="S1" s="53"/>
-      <c r="T1" s="56" t="s">
+      <c r="S1" s="56"/>
+      <c r="T1" s="55" t="s">
         <v>214</v>
       </c>
-      <c r="U1" s="54"/>
-      <c r="V1" s="53" t="s">
+      <c r="U1" s="53"/>
+      <c r="V1" s="56" t="s">
         <v>213</v>
       </c>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="54" t="s">
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="53" t="s">
         <v>212</v>
       </c>
       <c r="AB1" s="57" t="s">
@@ -3683,8 +3741,8 @@
       <c r="Z2" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -3740,17 +3798,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -3761,6 +3808,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor smoke test follow new bussiness
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1752,9 +1752,6 @@
     <t>Client</t>
   </si>
   <si>
-    <t>client.user01@gmail.com</t>
-  </si>
-  <si>
     <t>Valid User</t>
   </si>
   <si>
@@ -1780,6 +1777,9 @@
   </si>
   <si>
     <t>ADMIN_USER_PWD</t>
+  </si>
+  <si>
+    <t>auvenirtest01@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2871,7 +2871,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>35</v>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B4" s="50" t="s">
         <v>417</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B5" s="50" t="s">
         <v>439</v>
@@ -3294,7 +3294,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3318,36 +3318,36 @@
         <v>442</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>417</v>
+        <v>362</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>447</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>448</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>449</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -3357,11 +3357,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="C3" r:id="rId5" display="auditor.user01@gmail.com"/>
-    <hyperlink ref="D3" r:id="rId6"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4" display="auditor.user01@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId5"/>
+    <hyperlink ref="C2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
minhnh updated email in Forgotemail in excel file
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>165782</t>
-  </si>
-  <si>
-    <t>auvenir.automation.s3@gmail.com</t>
   </si>
   <si>
     <t>12345678x@X</t>
@@ -1798,6 +1795,9 @@
   </si>
   <si>
     <t>Change@123</t>
+  </si>
+  <si>
+    <t>minhtest@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2109,8 +2109,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2119,9 +2125,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2135,9 +2138,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2497,31 +2497,31 @@
   <sheetData>
     <row r="1" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J1" s="30" t="s">
         <v>15</v>
@@ -2530,82 +2530,82 @@
         <v>17</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
     </row>
     <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K3" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L3" s="33"/>
       <c r="M3" s="29"/>
@@ -2613,37 +2613,37 @@
     </row>
     <row r="4" spans="1:14" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L4" s="31"/>
       <c r="M4" s="29"/>
@@ -2651,19 +2651,19 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
@@ -2677,19 +2677,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
@@ -2773,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,46 +2789,46 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
       <c r="F1" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>458</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -2837,10 +2837,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -2884,76 +2884,76 @@
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
       <c r="F1" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="E2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>42</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="52" t="s">
+        <v>456</v>
+      </c>
+      <c r="B6" s="48" t="s">
         <v>457</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -2995,78 +2995,78 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J1" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K1" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L1" s="39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>131</v>
-      </c>
       <c r="K2" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L2" s="37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3097,108 +3097,108 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J1" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K1" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L1" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N1" s="40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O1" s="40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P1" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q1" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" t="s">
+        <v>150</v>
+      </c>
+      <c r="J2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K2" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="I2" t="s">
-        <v>151</v>
-      </c>
-      <c r="J2" t="s">
-        <v>151</v>
-      </c>
-      <c r="K2" s="43" t="s">
-        <v>152</v>
-      </c>
       <c r="L2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q2" s="37" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3231,97 +3231,97 @@
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3334,7 +3334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -3350,60 +3350,60 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
+        <v>439</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>440</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="51" t="s">
         <v>441</v>
       </c>
-      <c r="D1" s="51" t="s">
-        <v>442</v>
-      </c>
       <c r="E1" s="51" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>446</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>447</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>448</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>449</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
+        <v>452</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>455</v>
+      </c>
+      <c r="C4" s="48" t="s">
         <v>453</v>
       </c>
-      <c r="B4" s="48" t="s">
-        <v>456</v>
-      </c>
-      <c r="C4" s="48" t="s">
+      <c r="D4" s="48" t="s">
         <v>454</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3429,7 +3429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -3449,139 +3449,139 @@
     <row r="1" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38"/>
       <c r="B1" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E1" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="M1" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="J1" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="L1" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="M1" s="38" t="s">
-        <v>142</v>
-      </c>
       <c r="N1" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O1" s="38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P1" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q1" s="38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R1" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S1" s="38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T1" s="38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="U1" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V1" s="38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="W1" s="40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O2" s="44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R2" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S2" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="W2" s="37" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3626,148 +3626,148 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="52" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" s="52" t="s">
+      <c r="B1" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="52" t="s">
-        <v>184</v>
-      </c>
-      <c r="E1" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>222</v>
-      </c>
-      <c r="G1" s="52" t="s">
+      <c r="C1" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="53" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="G1" s="53" t="s">
         <v>220</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="H1" s="53" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="I1" s="53" t="s">
         <v>218</v>
       </c>
-      <c r="K1" s="52" t="s">
-        <v>201</v>
-      </c>
-      <c r="L1" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="M1" s="52" t="s">
+      <c r="J1" s="53" t="s">
         <v>217</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="K1" s="53" t="s">
+        <v>200</v>
+      </c>
+      <c r="L1" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="N1" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="O1" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="P1" s="53" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q1" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="O1" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="P1" s="52" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q1" s="52" t="s">
-        <v>145</v>
-      </c>
-      <c r="R1" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="S1" s="56"/>
-      <c r="T1" s="55" t="s">
+      <c r="R1" s="54" t="s">
         <v>214</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="56" t="s">
+      <c r="S1" s="54"/>
+      <c r="T1" s="57" t="s">
         <v>213</v>
       </c>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="53" t="s">
+      <c r="U1" s="55"/>
+      <c r="V1" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="AB1" s="57" t="s">
-        <v>138</v>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="AB1" s="58" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S2" s="38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="T2" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="U2" s="40" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V2" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="W2" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="X2" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y2" s="38" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Z2" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
+        <v>207</v>
+      </c>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H3" s="45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I3" s="45"/>
       <c r="J3" s="45"/>
@@ -3783,21 +3783,32 @@
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
       <c r="V3" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AB3" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -3808,17 +3819,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3848,772 +3848,772 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E1" s="49" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F1" s="49" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H1" s="49" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I1" s="49" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="K1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="J6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B10" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C11" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="J11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H21" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -4675,13 +4675,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>52</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -4706,22 +4706,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -4738,19 +4738,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>60</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -4795,19 +4795,19 @@
         <v>30</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="18" t="s">
         <v>78</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>79</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -4825,7 +4825,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -4851,13 +4851,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="20"/>
@@ -4880,13 +4880,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="20"/>
@@ -4906,19 +4906,19 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>83</v>
-      </c>
       <c r="F9" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -4939,16 +4939,16 @@
         <v>12</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="F10" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="7"/>
@@ -4967,13 +4967,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" s="16"/>
       <c r="G11" s="20"/>
@@ -4993,22 +4993,22 @@
         <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="G12" s="21" t="s">
         <v>69</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>70</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -5029,13 +5029,13 @@
         <v>16</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="20"/>
@@ -5055,7 +5055,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
@@ -5081,16 +5081,16 @@
         <v>31</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -5108,7 +5108,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -5131,20 +5131,20 @@
         <v>20</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="15" t="s">
-        <v>63</v>
-      </c>
       <c r="F17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="13" t="s">
         <v>78</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>79</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -5165,13 +5165,13 @@
         <v>22</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>

</xml_diff>

<commit_message>
Update TestData.xlsx by Thuan
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="accounts" sheetId="8" r:id="rId6"/>
     <sheet name="authSessions" sheetId="9" r:id="rId7"/>
     <sheet name="usersRegression" sheetId="10" r:id="rId8"/>
-    <sheet name="OnBoarding" sheetId="1" r:id="rId9"/>
+    <sheet name="AuditorSignUpTest" sheetId="1" r:id="rId9"/>
     <sheet name="ForgotPassword" sheetId="2" r:id="rId10"/>
     <sheet name="Login" sheetId="3" r:id="rId11"/>
     <sheet name="ClientTestData" sheetId="12" r:id="rId12"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="484">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1838,6 +1838,66 @@
   <si>
     <t>PasswordAdmin</t>
   </si>
+  <si>
+    <t>Valid User4</t>
+  </si>
+  <si>
+    <t>USER_PWD</t>
+  </si>
+  <si>
+    <t>INVALID VALUE1</t>
+  </si>
+  <si>
+    <t>INVALID VALUE2</t>
+  </si>
+  <si>
+    <t>INVALID VALUE3</t>
+  </si>
+  <si>
+    <t>blankPassword</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>invalidLengthPassword</t>
+  </si>
+  <si>
+    <t>aA12345</t>
+  </si>
+  <si>
+    <t>noUpperCasePassword</t>
+  </si>
+  <si>
+    <t>abc1234d</t>
+  </si>
+  <si>
+    <t>noLowerCasePassword</t>
+  </si>
+  <si>
+    <t>1234ABCD</t>
+  </si>
+  <si>
+    <t>noDigitsPassword</t>
+  </si>
+  <si>
+    <t>abcdABCD</t>
+  </si>
+  <si>
+    <t>noCharPassword</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>successPassword</t>
+  </si>
+  <si>
+    <t>12345678X</t>
+  </si>
+  <si>
+    <t>confirmPassword</t>
+  </si>
 </sst>
 </file>
 
@@ -2049,7 +2109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2165,8 +2225,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2175,9 +2245,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2192,13 +2259,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2854,11 +2915,11 @@
       <c r="B1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="61"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="64"/>
       <c r="F1" s="10" t="s">
         <v>48</v>
       </c>
@@ -2949,11 +3010,11 @@
       <c r="B1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="61"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="64"/>
       <c r="F1" s="10" t="s">
         <v>48</v>
       </c>
@@ -3066,10 +3127,10 @@
       <c r="E1" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="53" t="s">
         <v>459</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="53" t="s">
         <v>461</v>
       </c>
     </row>
@@ -3089,10 +3150,10 @@
       <c r="E2" s="48" t="s">
         <v>438</v>
       </c>
-      <c r="F2" s="63" t="s">
+      <c r="F2" s="54" t="s">
         <v>460</v>
       </c>
-      <c r="G2" s="63" t="s">
+      <c r="G2" s="54" t="s">
         <v>462</v>
       </c>
     </row>
@@ -3112,8 +3173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3141,10 +3202,10 @@
       <c r="E1" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="53" t="s">
         <v>463</v>
       </c>
-      <c r="G1" s="62"/>
+      <c r="G1" s="53"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
@@ -3162,10 +3223,10 @@
       <c r="E2" s="48" t="s">
         <v>457</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="55" t="s">
         <v>438</v>
       </c>
-      <c r="G2" s="63"/>
+      <c r="G2" s="54"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3538,17 +3599,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="A1:E4"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.140625" customWidth="1"/>
@@ -3613,8 +3674,60 @@
         <v>454</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="53" t="s">
+        <v>464</v>
+      </c>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48" t="s">
+        <v>449</v>
+      </c>
+      <c r="D5" s="48"/>
+    </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="48"/>
+      <c r="A6" s="53" t="s">
+        <v>465</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>438</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>438</v>
+      </c>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="53" t="s">
+        <v>466</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="53" t="s">
+        <v>467</v>
+      </c>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="53" t="s">
+        <v>468</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3627,6 +3740,12 @@
     <hyperlink ref="C4" r:id="rId7"/>
     <hyperlink ref="D4" r:id="rId8"/>
     <hyperlink ref="B4" r:id="rId9"/>
+    <hyperlink ref="C7" r:id="rId10"/>
+    <hyperlink ref="C8" r:id="rId11"/>
+    <hyperlink ref="C10" r:id="rId12"/>
+    <hyperlink ref="B6" r:id="rId13"/>
+    <hyperlink ref="C6" r:id="rId14"/>
+    <hyperlink ref="C5" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3833,62 +3952,62 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="56" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="56" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="56" t="s">
         <v>221</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="56" t="s">
         <v>220</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="56" t="s">
         <v>219</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="56" t="s">
         <v>218</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="56" t="s">
         <v>217</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="L1" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="56" t="s">
         <v>216</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="N1" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="O1" s="53" t="s">
+      <c r="O1" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="P1" s="53" t="s">
+      <c r="P1" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="Q1" s="53" t="s">
+      <c r="Q1" s="56" t="s">
         <v>144</v>
       </c>
       <c r="R1" s="57" t="s">
         <v>214</v>
       </c>
       <c r="S1" s="57"/>
-      <c r="T1" s="56" t="s">
+      <c r="T1" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="54"/>
+      <c r="U1" s="58"/>
       <c r="V1" s="57" t="s">
         <v>212</v>
       </c>
@@ -3896,31 +4015,31 @@
       <c r="X1" s="57"/>
       <c r="Y1" s="57"/>
       <c r="Z1" s="57"/>
-      <c r="AA1" s="54" t="s">
+      <c r="AA1" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="AB1" s="58" t="s">
+      <c r="AB1" s="61" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
+      <c r="P2" s="56"/>
+      <c r="Q2" s="56"/>
       <c r="R2" s="38" t="s">
         <v>139</v>
       </c>
@@ -3948,8 +4067,8 @@
       <c r="Z2" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
+      <c r="AA2" s="59"/>
+      <c r="AB2" s="59"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4005,6 +4124,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4015,17 +4145,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4854,10 +4973,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5462,6 +5581,86 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="50" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="65" t="s">
+        <v>469</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="65" t="s">
+        <v>471</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="65" t="s">
+        <v>473</v>
+      </c>
+      <c r="C26" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="65" t="s">
+        <v>475</v>
+      </c>
+      <c r="C27" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="65" t="s">
+        <v>477</v>
+      </c>
+      <c r="C28" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="65" t="s">
+        <v>479</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="65" t="s">
+        <v>481</v>
+      </c>
+      <c r="C30" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="65" t="s">
+        <v>483</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
@@ -5476,8 +5675,10 @@
     <hyperlink ref="E18" r:id="rId10"/>
     <hyperlink ref="E9" r:id="rId11" display="ww@.test.com"/>
     <hyperlink ref="F9" r:id="rId12"/>
+    <hyperlink ref="B22" r:id="rId13"/>
+    <hyperlink ref="B23" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId13"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First three cases for SmokeTest_R2
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="OnBoarding" sheetId="1" r:id="rId9"/>
     <sheet name="ForgotPassword" sheetId="2" r:id="rId10"/>
     <sheet name="Login" sheetId="3" r:id="rId11"/>
+    <sheet name="SmokeTest" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="461">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1798,6 +1799,12 @@
   </si>
   <si>
     <t>Change@123</t>
+  </si>
+  <si>
+    <t>auveniradm01@gmail.com</t>
+  </si>
+  <si>
+    <t>auvenirclient01@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2109,6 +2116,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2135,9 +2145,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2794,11 +2801,11 @@
       <c r="B1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
       <c r="F1" s="10" t="s">
         <v>49</v>
       </c>
@@ -2870,7 +2877,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2889,11 +2896,11 @@
       <c r="B1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
       <c r="F1" s="10" t="s">
         <v>49</v>
       </c>
@@ -2949,7 +2956,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="52" t="s">
         <v>457</v>
       </c>
       <c r="B6" s="48" t="s">
@@ -2970,6 +2977,101 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="51" t="s">
+        <v>440</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>442</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>444</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>417</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>445</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>447</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>449</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="51" t="s">
+        <v>453</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>456</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>454</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="48"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3" display="auditor.user01@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="D4" r:id="rId6"/>
+    <hyperlink ref="B4" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="D2" r:id="rId9"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3334,8 +3436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3367,7 +3469,7 @@
         <v>444</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>417</v>
@@ -3422,6 +3524,7 @@
     <hyperlink ref="B4" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -3626,94 +3729,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="53" t="s">
         <v>220</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="53" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="53" t="s">
         <v>218</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="53" t="s">
         <v>217</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="O1" s="52" t="s">
+      <c r="O1" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="53" t="s">
         <v>216</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="57" t="s">
         <v>215</v>
       </c>
-      <c r="S1" s="56"/>
-      <c r="T1" s="55" t="s">
+      <c r="S1" s="57"/>
+      <c r="T1" s="56" t="s">
         <v>214</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="56" t="s">
+      <c r="U1" s="54"/>
+      <c r="V1" s="57" t="s">
         <v>213</v>
       </c>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="53" t="s">
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="54" t="s">
         <v>212</v>
       </c>
-      <c r="AB1" s="57" t="s">
+      <c r="AB1" s="58" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="38" t="s">
         <v>140</v>
       </c>
@@ -3741,8 +3844,8 @@
       <c r="Z2" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4649,7 +4752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
vien.Pham edited emailTemplate at 9:15am June14th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -16,8 +16,9 @@
     <sheet name="authSessions" sheetId="9" r:id="rId7"/>
     <sheet name="usersRegression" sheetId="10" r:id="rId8"/>
     <sheet name="OnBoarding" sheetId="1" r:id="rId9"/>
-    <sheet name="ForgotPassword" sheetId="2" r:id="rId10"/>
-    <sheet name="Login" sheetId="3" r:id="rId11"/>
+    <sheet name="TodoTest" sheetId="12" r:id="rId10"/>
+    <sheet name="ForgotPassword" sheetId="2" r:id="rId11"/>
+    <sheet name="Login" sheetId="3" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="461">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1798,6 +1799,12 @@
   </si>
   <si>
     <t>Change@123</t>
+  </si>
+  <si>
+    <t>Engagement Name</t>
+  </si>
+  <si>
+    <t>Engagement 01</t>
   </si>
 </sst>
 </file>
@@ -2109,8 +2116,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2119,9 +2132,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2135,9 +2145,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2771,6 +2778,41 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2794,11 +2836,11 @@
       <c r="B1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
       <c r="F1" s="10" t="s">
         <v>49</v>
       </c>
@@ -2865,7 +2907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
@@ -2889,11 +2931,11 @@
       <c r="B1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="61"/>
       <c r="F1" s="10" t="s">
         <v>49</v>
       </c>
@@ -2949,7 +2991,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="52" t="s">
         <v>457</v>
       </c>
       <c r="B6" s="48" t="s">
@@ -3334,8 +3376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3626,94 +3668,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="53" t="s">
         <v>222</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="53" t="s">
         <v>220</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="53" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="J1" s="53" t="s">
         <v>218</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="K1" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="53" t="s">
         <v>217</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="N1" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="O1" s="52" t="s">
+      <c r="O1" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="53" t="s">
         <v>216</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="54" t="s">
         <v>215</v>
       </c>
-      <c r="S1" s="56"/>
-      <c r="T1" s="55" t="s">
+      <c r="S1" s="54"/>
+      <c r="T1" s="57" t="s">
         <v>214</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="56" t="s">
+      <c r="U1" s="55"/>
+      <c r="V1" s="54" t="s">
         <v>213</v>
       </c>
-      <c r="W1" s="56"/>
-      <c r="X1" s="56"/>
-      <c r="Y1" s="56"/>
-      <c r="Z1" s="56"/>
-      <c r="AA1" s="53" t="s">
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="55" t="s">
         <v>212</v>
       </c>
-      <c r="AB1" s="57" t="s">
+      <c r="AB1" s="58" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="R2" s="38" t="s">
         <v>140</v>
       </c>
@@ -3741,8 +3783,8 @@
       <c r="Z2" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -3798,6 +3840,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -3808,17 +3861,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
minhnh updated -	AccountSettingsTest, -	AuditorEngagementReviewTest
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="484">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>165782</t>
-  </si>
-  <si>
-    <t>12345678x@X</t>
   </si>
   <si>
     <t>auvenir.automation.s3</t>
@@ -1897,6 +1894,9 @@
   </si>
   <si>
     <t>confirmPassword</t>
+  </si>
+  <si>
+    <t>hoangminh1240</t>
   </si>
 </sst>
 </file>
@@ -2232,11 +2232,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2245,6 +2243,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2259,7 +2260,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2618,31 +2618,31 @@
   <sheetData>
     <row r="1" spans="1:14" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J1" s="30" t="s">
         <v>15</v>
@@ -2651,82 +2651,82 @@
         <v>17</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J2" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K2" s="33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L2" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
     </row>
     <row r="3" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>15</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K3" s="30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L3" s="33"/>
       <c r="M3" s="29"/>
@@ -2734,37 +2734,37 @@
     </row>
     <row r="4" spans="1:14" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L4" s="31"/>
       <c r="M4" s="29"/>
@@ -2772,19 +2772,19 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" s="29"/>
       <c r="G5" s="29"/>
@@ -2798,19 +2798,19 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="27"/>
@@ -2910,46 +2910,46 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
       <c r="F1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>32</v>
+        <v>483</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -2958,10 +2958,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -2974,7 +2974,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId2" display="12345678x@X"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="C2" r:id="rId4" display="auvenir.automation.s3@gmail.com"/>
     <hyperlink ref="D2" r:id="rId5"/>
@@ -3005,76 +3005,76 @@
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="62" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
       <c r="F1" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="E2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
+        <v>455</v>
+      </c>
+      <c r="B6" s="48" t="s">
         <v>456</v>
-      </c>
-      <c r="B6" s="48" t="s">
-        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -3116,45 +3116,45 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>439</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="51" t="s">
         <v>440</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>441</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C2" s="48" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" s="48" t="s">
         <v>453</v>
       </c>
-      <c r="D2" s="48" t="s">
-        <v>454</v>
-      </c>
       <c r="E2" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F2" s="54" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G2" s="54" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -3191,40 +3191,40 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>439</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="51" t="s">
         <v>440</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>441</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G1" s="53"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C2" s="48" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" s="48" t="s">
         <v>453</v>
       </c>
-      <c r="D2" s="48" t="s">
-        <v>454</v>
-      </c>
       <c r="E2" s="48" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F2" s="55" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G2" s="54"/>
     </row>
@@ -3262,78 +3262,78 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J1" s="40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K1" s="39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L1" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>130</v>
-      </c>
       <c r="K2" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L2" s="37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3364,108 +3364,108 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E1" s="40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F1" s="40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J1" s="40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K1" s="40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L1" s="40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M1" s="40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N1" s="40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="O1" s="40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P1" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q1" s="40" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H2" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K2" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="I2" t="s">
-        <v>150</v>
-      </c>
-      <c r="J2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K2" s="43" t="s">
-        <v>151</v>
-      </c>
       <c r="L2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q2" s="37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3498,97 +3498,97 @@
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H1" s="38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3599,10 +3599,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3618,115 +3618,129 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
+        <v>438</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>439</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="D1" s="51" t="s">
         <v>440</v>
       </c>
-      <c r="D1" s="51" t="s">
-        <v>441</v>
-      </c>
       <c r="E1" s="51" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B3" s="16" t="s">
+        <v>445</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>447</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>448</v>
       </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>454</v>
+      </c>
+      <c r="C4" s="48" t="s">
         <v>452</v>
       </c>
-      <c r="B4" s="48" t="s">
-        <v>455</v>
-      </c>
-      <c r="C4" s="48" t="s">
+      <c r="D4" s="48" t="s">
         <v>453</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D5" s="48"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="53" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D6" s="48"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B8" s="48"/>
       <c r="C8" s="48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="51" t="s">
+        <v>463</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -3746,6 +3760,9 @@
     <hyperlink ref="B6" r:id="rId13"/>
     <hyperlink ref="C6" r:id="rId14"/>
     <hyperlink ref="C5" r:id="rId15"/>
+    <hyperlink ref="B11" r:id="rId16"/>
+    <hyperlink ref="C11" r:id="rId17"/>
+    <hyperlink ref="D11" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3775,139 +3792,139 @@
     <row r="1" spans="1:23" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38"/>
       <c r="B1" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E1" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="M1" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="F1" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>199</v>
-      </c>
-      <c r="J1" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="L1" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="M1" s="38" t="s">
-        <v>141</v>
-      </c>
       <c r="N1" s="38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O1" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P1" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q1" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R1" s="38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="S1" s="38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="T1" s="38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U1" s="38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="V1" s="38" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="W1" s="40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O2" s="44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P2" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R2" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="S2" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="W2" s="37" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -3952,148 +3969,148 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="56" t="s">
-        <v>147</v>
-      </c>
-      <c r="C1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="56" t="s">
-        <v>183</v>
-      </c>
-      <c r="E1" s="56" t="s">
-        <v>139</v>
-      </c>
-      <c r="F1" s="56" t="s">
-        <v>221</v>
-      </c>
-      <c r="G1" s="56" t="s">
+      <c r="C1" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="57" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="57" t="s">
         <v>220</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="G1" s="57" t="s">
         <v>219</v>
       </c>
-      <c r="I1" s="56" t="s">
+      <c r="H1" s="57" t="s">
         <v>218</v>
       </c>
-      <c r="J1" s="56" t="s">
+      <c r="I1" s="57" t="s">
         <v>217</v>
       </c>
-      <c r="K1" s="56" t="s">
-        <v>200</v>
-      </c>
-      <c r="L1" s="56" t="s">
-        <v>138</v>
-      </c>
-      <c r="M1" s="56" t="s">
+      <c r="J1" s="57" t="s">
         <v>216</v>
       </c>
-      <c r="N1" s="56" t="s">
+      <c r="K1" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="L1" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" s="57" t="s">
+        <v>215</v>
+      </c>
+      <c r="N1" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="O1" s="57" t="s">
+        <v>141</v>
+      </c>
+      <c r="P1" s="57" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q1" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="O1" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="P1" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q1" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="R1" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="S1" s="57"/>
+      <c r="R1" s="61" t="s">
+        <v>213</v>
+      </c>
+      <c r="S1" s="61"/>
       <c r="T1" s="60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U1" s="58"/>
-      <c r="V1" s="57" t="s">
-        <v>212</v>
-      </c>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="57"/>
+      <c r="V1" s="61" t="s">
+        <v>211</v>
+      </c>
+      <c r="W1" s="61"/>
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
       <c r="AA1" s="58" t="s">
-        <v>211</v>
-      </c>
-      <c r="AB1" s="61" t="s">
-        <v>137</v>
+        <v>210</v>
+      </c>
+      <c r="AB1" s="62" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
       <c r="R2" s="38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="S2" s="38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="T2" s="40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="U2" s="40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="V2" s="38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="W2" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X2" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y2" s="38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z2" s="38" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AA2" s="59"/>
       <c r="AB2" s="59"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" s="46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F3" s="46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H3" s="45" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I3" s="45"/>
       <c r="J3" s="45"/>
@@ -4109,32 +4126,21 @@
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
       <c r="V3" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="W3" s="7"/>
       <c r="X3" s="7"/>
       <c r="Y3" s="7"/>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AB3" s="32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4145,6 +4151,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4174,772 +4191,772 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E1" s="49" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F1" s="49" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G1" s="49" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H1" s="49" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I1" s="49" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="48" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="J9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="48" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B11" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D11" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H11" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="J11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="48" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C12" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H12" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="48" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D13" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F13" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="48" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="48" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="48" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="48" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="48" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G21" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -4975,7 +4992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -5001,13 +5018,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -5032,22 +5049,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -5064,19 +5081,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -5121,19 +5138,19 @@
         <v>30</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>78</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -5151,7 +5168,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -5177,13 +5194,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="20"/>
@@ -5206,13 +5223,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="20"/>
@@ -5232,19 +5249,19 @@
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>82</v>
-      </c>
       <c r="F9" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -5265,16 +5282,16 @@
         <v>12</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>56</v>
-      </c>
       <c r="F10" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="7"/>
@@ -5293,13 +5310,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E11" s="16"/>
       <c r="G11" s="20"/>
@@ -5319,22 +5336,22 @@
         <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="G12" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>69</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -5355,13 +5372,13 @@
         <v>16</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="20"/>
@@ -5381,7 +5398,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
@@ -5407,16 +5424,16 @@
         <v>31</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -5434,7 +5451,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -5457,20 +5474,20 @@
         <v>20</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="15" t="s">
-        <v>62</v>
-      </c>
       <c r="F17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="13" t="s">
         <v>77</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>78</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -5491,13 +5508,13 @@
         <v>22</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -5583,82 +5600,82 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="50" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="56" t="s">
+        <v>468</v>
+      </c>
+      <c r="C24" s="43" t="s">
         <v>469</v>
       </c>
-      <c r="C24" s="43" t="s">
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="65" t="s">
+      <c r="C25" s="43" t="s">
         <v>471</v>
       </c>
-      <c r="C25" s="43" t="s">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="56" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" s="65" t="s">
+      <c r="C26" t="s">
         <v>473</v>
       </c>
-      <c r="C26" t="s">
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="65" t="s">
+      <c r="C27" t="s">
         <v>475</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="56" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" s="65" t="s">
+      <c r="C28" t="s">
         <v>477</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="56" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="65" t="s">
+      <c r="C29" s="43" t="s">
         <v>479</v>
       </c>
-      <c r="C29" s="43" t="s">
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="56" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="65" t="s">
+      <c r="C30" t="s">
         <v>481</v>
       </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="56" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="65" t="s">
-        <v>483</v>
-      </c>
       <c r="C31" s="43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added brandnew  tc #10: verifyClientLogsInAndActive
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="488">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1907,7 +1907,10 @@
     <t>auvenirclient01@gmail.com</t>
   </si>
   <si>
-    <t>auvenirauditor01@gmail.com</t>
+    <t>Client Email Password</t>
+  </si>
+  <si>
+    <t>TESTPASSWORD</t>
   </si>
 </sst>
 </file>
@@ -2244,8 +2247,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2254,9 +2266,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2271,12 +2280,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2932,11 +2935,11 @@
       <c r="B1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="10" t="s">
         <v>48</v>
       </c>
@@ -3027,11 +3030,11 @@
       <c r="B1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="10" t="s">
         <v>48</v>
       </c>
@@ -3259,108 +3262,114 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" style="66" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="66" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" style="66" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="66" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="66" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="66"/>
+    <col min="1" max="1" width="15.5703125" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="57" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" style="57" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="57" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="67"/>
-      <c r="B1" s="70" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="58"/>
+      <c r="B1" s="61" t="s">
         <v>439</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="61" t="s">
         <v>440</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="61" t="s">
         <v>441</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="61" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="F1" s="61" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="61" t="s">
         <v>443</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="59" t="s">
         <v>484</v>
       </c>
-      <c r="C2" s="68" t="s">
-        <v>486</v>
-      </c>
-      <c r="D2" s="68" t="s">
+      <c r="C2" s="59" t="s">
+        <v>379</v>
+      </c>
+      <c r="D2" s="59" t="s">
         <v>485</v>
       </c>
-      <c r="E2" s="67"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="E2" s="58"/>
+      <c r="F2" s="57" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="s">
         <v>444</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="59" t="s">
         <v>446</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="59" t="s">
         <v>447</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="59" t="s">
         <v>448</v>
       </c>
-      <c r="E3" s="67"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="E3" s="58"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="61" t="s">
         <v>452</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="60" t="s">
         <v>455</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="60" t="s">
         <v>453</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="60" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="71"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
-      <c r="C7" s="69"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="69"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="62"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="62"/>
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="62"/>
+      <c r="C7" s="60"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="62"/>
+      <c r="B8" s="60"/>
+      <c r="C8" s="60"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="62"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="60"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4084,94 +4093,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="63" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="63" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="63" t="s">
         <v>221</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="63" t="s">
         <v>220</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="63" t="s">
         <v>219</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="63" t="s">
         <v>218</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="63" t="s">
         <v>217</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="63" t="s">
         <v>200</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="L1" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="63" t="s">
         <v>216</v>
       </c>
-      <c r="N1" s="57" t="s">
+      <c r="N1" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="O1" s="57" t="s">
+      <c r="O1" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="P1" s="57" t="s">
+      <c r="P1" s="63" t="s">
         <v>215</v>
       </c>
-      <c r="Q1" s="57" t="s">
+      <c r="Q1" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="R1" s="61" t="s">
+      <c r="R1" s="64" t="s">
         <v>214</v>
       </c>
-      <c r="S1" s="61"/>
-      <c r="T1" s="60" t="s">
+      <c r="S1" s="64"/>
+      <c r="T1" s="67" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="58"/>
-      <c r="V1" s="61" t="s">
+      <c r="U1" s="65"/>
+      <c r="V1" s="64" t="s">
         <v>212</v>
       </c>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="58" t="s">
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
+      <c r="AA1" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="AB1" s="62" t="s">
+      <c r="AB1" s="68" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
       <c r="R2" s="38" t="s">
         <v>139</v>
       </c>
@@ -4199,8 +4208,8 @@
       <c r="Z2" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="59"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4256,6 +4265,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4266,17 +4286,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vien.Pham implement smoketest at 6:13pm June15th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="493">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1917,6 +1917,15 @@
   </si>
   <si>
     <t>TESTPASSWORD</t>
+  </si>
+  <si>
+    <t>EngagementName</t>
+  </si>
+  <si>
+    <t>Engagement 01</t>
+  </si>
+  <si>
+    <t>Valid value4</t>
   </si>
 </sst>
 </file>
@@ -2256,6 +2265,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2263,9 +2275,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2616,7 +2625,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3262,23 +3271,24 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3295,8 +3305,11 @@
       <c r="F1" s="51" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
@@ -3314,7 +3327,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3329,7 +3342,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3343,31 +3356,36 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="51" t="s">
+        <v>492</v>
+      </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
       <c r="C7" s="48"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="48"/>
     </row>
   </sheetData>
@@ -4156,22 +4174,22 @@
       <c r="Q1" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="61" t="s">
+      <c r="R1" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="61"/>
-      <c r="T1" s="60" t="s">
+      <c r="S1" s="58"/>
+      <c r="T1" s="61" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="58"/>
-      <c r="V1" s="61" t="s">
+      <c r="U1" s="59"/>
+      <c r="V1" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="58" t="s">
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="59" t="s">
         <v>210</v>
       </c>
       <c r="AB1" s="62" t="s">
@@ -4223,8 +4241,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="59"/>
+      <c r="AA2" s="60"/>
+      <c r="AB2" s="60"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4280,6 +4298,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4290,17 +4319,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vien.Pham implement smoketest at 6:46pm June15th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="496">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1926,6 +1926,15 @@
   </si>
   <si>
     <t>Testpassword1!</t>
+  </si>
+  <si>
+    <t>Valid value4</t>
+  </si>
+  <si>
+    <t>EngagementName</t>
+  </si>
+  <si>
+    <t>Engagement 01</t>
   </si>
 </sst>
 </file>
@@ -2262,8 +2271,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2272,9 +2286,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2289,8 +2300,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2946,11 +2955,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3041,11 +3050,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3273,10 +3282,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,9 +3296,10 @@
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3306,8 +3316,11 @@
       <c r="F1" s="51" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="53" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
@@ -3325,7 +3338,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3340,7 +3353,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3354,31 +3367,36 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>493</v>
+      </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
       <c r="C7" s="48"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="48"/>
     </row>
   </sheetData>
@@ -3751,7 +3769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -3780,10 +3798,10 @@
       <c r="E1" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="58" t="s">
         <v>491</v>
       </c>
     </row>
@@ -3801,10 +3819,10 @@
         <v>441</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="F2" s="66" t="s">
+      <c r="F2" s="57" t="s">
         <v>489</v>
       </c>
-      <c r="G2" s="66" t="s">
+      <c r="G2" s="57" t="s">
         <v>492</v>
       </c>
     </row>
@@ -4133,94 +4151,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="59" t="s">
         <v>216</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="59" t="s">
         <v>199</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="L1" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="N1" s="57" t="s">
+      <c r="N1" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="57" t="s">
+      <c r="O1" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="57" t="s">
+      <c r="P1" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="Q1" s="57" t="s">
+      <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="61" t="s">
+      <c r="R1" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="61"/>
-      <c r="T1" s="60" t="s">
+      <c r="S1" s="60"/>
+      <c r="T1" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="58"/>
-      <c r="V1" s="61" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="58" t="s">
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>210</v>
       </c>
-      <c r="AB1" s="62" t="s">
+      <c r="AB1" s="64" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -4248,8 +4266,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="59"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4305,6 +4323,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4315,17 +4344,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vien.Pham implement smoketest at 7:00pm June15th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="494">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1904,12 +1904,6 @@
     <t>Valid Userminh</t>
   </si>
   <si>
-    <t>auveniradm01@gmail.com</t>
-  </si>
-  <si>
-    <t>auvenirauditor01@gmail.com</t>
-  </si>
-  <si>
     <t>auvenirclient01@gmail.com</t>
   </si>
   <si>
@@ -1926,6 +1920,15 @@
   </si>
   <si>
     <t>Testpassword1!</t>
+  </si>
+  <si>
+    <t>Valid value</t>
+  </si>
+  <si>
+    <t>EngagementName</t>
+  </si>
+  <si>
+    <t>Engagement 01</t>
   </si>
 </sst>
 </file>
@@ -2262,8 +2265,13 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2272,9 +2280,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2289,8 +2294,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2946,11 +2949,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3041,11 +3044,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="65"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="67"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3273,10 +3276,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3287,9 +3290,10 @@
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3304,28 +3308,31 @@
         <v>444</v>
       </c>
       <c r="F1" s="51" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+      <c r="G1" s="53" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>425</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>485</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>486</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>487</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3340,7 +3347,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3354,39 +3361,45 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>491</v>
+      </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
       <c r="C7" s="48"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="48"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3751,8 +3764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3780,11 +3793,11 @@
       <c r="E1" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="F1" s="67" t="s">
-        <v>488</v>
-      </c>
-      <c r="G1" s="67" t="s">
-        <v>491</v>
+      <c r="F1" s="58" t="s">
+        <v>486</v>
+      </c>
+      <c r="G1" s="58" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3801,11 +3814,11 @@
         <v>441</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="F2" s="66" t="s">
-        <v>489</v>
-      </c>
-      <c r="G2" s="66" t="s">
-        <v>492</v>
+      <c r="F2" s="57" t="s">
+        <v>487</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3816,7 +3829,7 @@
         <v>445</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>447</v>
@@ -4133,94 +4146,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="59" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="59" t="s">
         <v>220</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="59" t="s">
         <v>219</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="59" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="59" t="s">
         <v>216</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="59" t="s">
         <v>199</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="L1" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="59" t="s">
         <v>215</v>
       </c>
-      <c r="N1" s="57" t="s">
+      <c r="N1" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="57" t="s">
+      <c r="O1" s="59" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="57" t="s">
+      <c r="P1" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="Q1" s="57" t="s">
+      <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="61" t="s">
+      <c r="R1" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="61"/>
-      <c r="T1" s="60" t="s">
+      <c r="S1" s="60"/>
+      <c r="T1" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="58"/>
-      <c r="V1" s="61" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="58" t="s">
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>210</v>
       </c>
-      <c r="AB1" s="62" t="s">
+      <c r="AB1" s="64" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -4248,8 +4261,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="59"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4305,6 +4318,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4315,17 +4339,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vien.Pham implement smoketest at 9:11am June16th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1904,9 +1904,6 @@
     <t>Valid Userminh</t>
   </si>
   <si>
-    <t>auvenirclient01@gmail.com</t>
-  </si>
-  <si>
     <t>Client Email Password</t>
   </si>
   <si>
@@ -1929,6 +1926,9 @@
   </si>
   <si>
     <t>Engagement 01</t>
+  </si>
+  <si>
+    <t>auvenirad@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2270,9 +2270,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2280,6 +2277,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3279,7 +3279,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3308,10 +3308,10 @@
         <v>444</v>
       </c>
       <c r="F1" s="51" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3319,17 +3319,20 @@
         <v>442</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>425</v>
+        <v>493</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>360</v>
+        <v>487</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>485</v>
+        <v>453</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" t="s">
-        <v>487</v>
+        <v>486</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3363,14 +3366,11 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
-      <c r="G5" t="s">
-        <v>493</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
@@ -3397,9 +3397,12 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -3794,10 +3797,10 @@
         <v>444</v>
       </c>
       <c r="F1" s="58" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G1" s="58" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3815,10 +3818,10 @@
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="57" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G2" s="57" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3829,7 +3832,7 @@
         <v>445</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>447</v>
@@ -4194,22 +4197,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="63" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="60"/>
-      <c r="T1" s="63" t="s">
+      <c r="S1" s="63"/>
+      <c r="T1" s="62" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="61"/>
-      <c r="V1" s="60" t="s">
+      <c r="U1" s="60"/>
+      <c r="V1" s="63" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="61" t="s">
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="63"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="60" t="s">
         <v>210</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -4261,8 +4264,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4318,17 +4321,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4339,6 +4331,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Excel file, Move Test case following the priority
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="494">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2141,7 +2141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2270,6 +2270,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2277,9 +2280,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2294,6 +2294,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3276,10 +3277,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3290,10 +3291,11 @@
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3313,8 +3315,11 @@
       <c r="G1" s="53" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
@@ -3334,8 +3339,11 @@
       <c r="G2" s="57" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="68" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3350,7 +3358,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3364,7 +3372,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>490</v>
       </c>
@@ -3372,25 +3380,25 @@
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
       <c r="C7" s="48"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="48"/>
     </row>
   </sheetData>
@@ -3400,9 +3408,10 @@
     <hyperlink ref="B3" r:id="rId3"/>
     <hyperlink ref="D4" r:id="rId4"/>
     <hyperlink ref="D2" r:id="rId5"/>
+    <hyperlink ref="H2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -4197,22 +4206,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="60"/>
+      <c r="T1" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="63" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="60" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="60" t="s">
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>210</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -4264,8 +4273,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4321,6 +4330,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4331,17 +4351,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5173,7 +5182,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change data and read
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="497">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1930,6 +1930,15 @@
   <si>
     <t>auvenirad@gmail.com</t>
   </si>
+  <si>
+    <t>Engagement Name Generated</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>Users Auvenir Password</t>
+  </si>
 </sst>
 </file>
 
@@ -2141,7 +2150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2267,6 +2276,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2294,7 +2305,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2950,11 +2960,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3045,11 +3055,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3277,10 +3287,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3289,13 +3299,15 @@
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3316,10 +3328,16 @@
         <v>491</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>496</v>
+      </c>
+      <c r="I1" s="60" t="s">
+        <v>488</v>
+      </c>
+      <c r="J1" s="60" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
@@ -3339,11 +3357,17 @@
       <c r="G2" s="57" t="s">
         <v>492</v>
       </c>
-      <c r="H2" s="68" t="s">
+      <c r="H2" s="59" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>489</v>
+      </c>
+      <c r="J2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3358,7 +3382,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3372,7 +3396,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>490</v>
       </c>
@@ -3380,25 +3404,25 @@
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
       <c r="C7" s="48"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="48"/>
     </row>
   </sheetData>
@@ -3774,10 +3798,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3787,11 +3811,9 @@
     <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3805,14 +3827,8 @@
       <c r="E1" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="F1" s="58" t="s">
-        <v>485</v>
-      </c>
-      <c r="G1" s="58" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
@@ -3826,14 +3842,8 @@
         <v>441</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="F2" s="57" t="s">
-        <v>486</v>
-      </c>
-      <c r="G2" s="57" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3848,7 +3858,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3862,7 +3872,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>463</v>
       </c>
@@ -3872,7 +3882,7 @@
       </c>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="53" t="s">
         <v>464</v>
       </c>
@@ -3884,7 +3894,7 @@
       </c>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
         <v>465</v>
       </c>
@@ -3892,7 +3902,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
         <v>466</v>
       </c>
@@ -3901,7 +3911,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="53" t="s">
         <v>467</v>
       </c>
@@ -3909,7 +3919,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -3917,7 +3927,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="51" t="s">
         <v>484</v>
       </c>
@@ -4158,94 +4168,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="61" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="61" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="61" t="s">
         <v>220</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="61" t="s">
         <v>219</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="61" t="s">
         <v>218</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="61" t="s">
         <v>217</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="61" t="s">
         <v>216</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="61" t="s">
         <v>199</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="61" t="s">
         <v>215</v>
       </c>
-      <c r="N1" s="59" t="s">
+      <c r="N1" s="61" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="59" t="s">
+      <c r="O1" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="59" t="s">
+      <c r="P1" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="60"/>
-      <c r="T1" s="63" t="s">
+      <c r="S1" s="62"/>
+      <c r="T1" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="61"/>
-      <c r="V1" s="60" t="s">
+      <c r="U1" s="63"/>
+      <c r="V1" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="61" t="s">
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="63" t="s">
         <v>210</v>
       </c>
-      <c r="AB1" s="64" t="s">
+      <c r="AB1" s="66" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -4273,8 +4283,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">

</xml_diff>

<commit_message>
vien.Pham added new uploadREquest at 6:23pm June16th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="502">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1942,6 +1942,18 @@
   <si>
     <t>auvenirad@gmail.com</t>
   </si>
+  <si>
+    <t>Path of Location</t>
+  </si>
+  <si>
+    <t>\src\test\resources\upload\</t>
+  </si>
+  <si>
+    <t>File Upload Name</t>
+  </si>
+  <si>
+    <t>TXT_helloAuvenir.txt</t>
+  </si>
 </sst>
 </file>
 
@@ -2153,7 +2165,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2283,9 +2295,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2293,6 +2302,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2307,6 +2319,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3289,10 +3302,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3307,9 +3320,11 @@
     <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3338,8 +3353,14 @@
       <c r="J1" s="53" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="53" t="s">
+        <v>498</v>
+      </c>
+      <c r="L1" s="53" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
@@ -3368,8 +3389,14 @@
       <c r="J2" s="57" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="59" t="s">
+        <v>499</v>
+      </c>
+      <c r="L2" s="69" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3384,7 +3411,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3398,7 +3425,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>491</v>
       </c>
@@ -3406,33 +3433,34 @@
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
       <c r="C7" s="48"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="48"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId2" display="\\src\\test\\resources\\upload\\"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -4227,22 +4255,22 @@
       <c r="Q1" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="61" t="s">
+      <c r="R1" s="64" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="61"/>
-      <c r="T1" s="64" t="s">
+      <c r="S1" s="64"/>
+      <c r="T1" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="61" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="61"/>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="61"/>
-      <c r="AA1" s="62" t="s">
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
+      <c r="AA1" s="61" t="s">
         <v>210</v>
       </c>
       <c r="AB1" s="65" t="s">
@@ -4294,8 +4322,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4351,17 +4379,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4372,6 +4389,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix Code for Signout in Gmail, Edit test data TestData.xlsx, fix xpath for click Comment Icon
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="507">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1928,9 +1928,6 @@
     <t>Engagement 01</t>
   </si>
   <si>
-    <t>Users Auvenir Password</t>
-  </si>
-  <si>
     <t>Engagement Name Generated</t>
   </si>
   <si>
@@ -1965,6 +1962,12 @@
   </si>
   <si>
     <t>TXT_helloAuvenir.txt</t>
+  </si>
+  <si>
+    <t>Auditor Auvenir Password</t>
+  </si>
+  <si>
+    <t>Admin Auvenir Password</t>
   </si>
 </sst>
 </file>
@@ -2308,6 +2311,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2315,9 +2321,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3314,10 +3317,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3329,18 +3332,19 @@
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.85546875" customWidth="1"/>
-    <col min="12" max="12" width="24" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.7109375" style="57" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="57" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.85546875" customWidth="1"/>
+    <col min="13" max="13" width="24" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3361,39 +3365,42 @@
         <v>491</v>
       </c>
       <c r="H1" s="53" t="s">
+        <v>505</v>
+      </c>
+      <c r="I1" s="53" t="s">
+        <v>506</v>
+      </c>
+      <c r="J1" s="53" t="s">
+        <v>489</v>
+      </c>
+      <c r="K1" s="53" t="s">
         <v>493</v>
       </c>
-      <c r="I1" s="53" t="s">
-        <v>489</v>
-      </c>
-      <c r="J1" s="53" t="s">
-        <v>494</v>
-      </c>
-      <c r="K1" s="53" t="s">
+      <c r="L1" s="53" t="s">
+        <v>497</v>
+      </c>
+      <c r="M1" s="53" t="s">
         <v>498</v>
       </c>
-      <c r="L1" s="53" t="s">
+      <c r="N1" s="53" t="s">
         <v>499</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="O1" s="53" t="s">
         <v>500</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="P1" s="53" t="s">
         <v>501</v>
       </c>
-      <c r="O1" s="53" t="s">
+      <c r="Q1" s="53" t="s">
         <v>502</v>
       </c>
-      <c r="P1" s="53" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>488</v>
@@ -3411,32 +3418,35 @@
       <c r="H2" s="59" t="s">
         <v>437</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="59" t="s">
+        <v>437</v>
+      </c>
+      <c r="J2" s="57" t="s">
         <v>490</v>
       </c>
-      <c r="J2" s="57" t="s">
-        <v>495</v>
-      </c>
-      <c r="K2" s="59" t="s">
+      <c r="K2" s="57" t="s">
+        <v>494</v>
+      </c>
+      <c r="L2" s="59" t="s">
+        <v>496</v>
+      </c>
+      <c r="M2" s="60" t="s">
         <v>497</v>
-      </c>
-      <c r="L2" s="60" t="s">
-        <v>498</v>
-      </c>
-      <c r="M2" s="59" t="s">
-        <v>437</v>
       </c>
       <c r="N2" s="59" t="s">
         <v>437</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="59" t="s">
+        <v>437</v>
+      </c>
+      <c r="P2" t="s">
+        <v>503</v>
+      </c>
+      <c r="Q2" t="s">
         <v>504</v>
       </c>
-      <c r="P2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3451,7 +3461,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3465,44 +3475,45 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
       <c r="C7" s="48"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C10" s="48"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="B2" r:id="rId3"/>
-    <hyperlink ref="K2" r:id="rId4"/>
-    <hyperlink ref="M2" r:id="rId5"/>
-    <hyperlink ref="N2" r:id="rId6"/>
+    <hyperlink ref="L2" r:id="rId4"/>
+    <hyperlink ref="N2" r:id="rId5"/>
+    <hyperlink ref="O2" r:id="rId6"/>
+    <hyperlink ref="H2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -4297,22 +4308,22 @@
       <c r="Q1" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="R1" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="65"/>
-      <c r="T1" s="64" t="s">
+      <c r="S1" s="62"/>
+      <c r="T1" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="65" t="s">
+      <c r="U1" s="63"/>
+      <c r="V1" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="62" t="s">
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="63" t="s">
         <v>210</v>
       </c>
       <c r="AB1" s="66" t="s">
@@ -4364,8 +4375,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4421,6 +4432,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4431,17 +4453,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vien.Pham updated smoketest at 11:21am June20th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="508">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1955,9 +1955,6 @@
     <t>Auditor Invited Password</t>
   </si>
   <si>
-    <t>Path of Location</t>
-  </si>
-  <si>
     <t>File Upload Name</t>
   </si>
   <si>
@@ -1965,6 +1962,15 @@
   </si>
   <si>
     <t>TXT_helloAuvenir.txt</t>
+  </si>
+  <si>
+    <t>Path of Upload Location</t>
+  </si>
+  <si>
+    <t>Path of Download Location</t>
+  </si>
+  <si>
+    <t>\Downloads\</t>
   </si>
 </sst>
 </file>
@@ -3314,10 +3320,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3337,10 +3343,11 @@
     <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.7109375" style="57" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" style="57" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3382,13 +3389,16 @@
         <v>501</v>
       </c>
       <c r="O1" s="53" t="s">
+        <v>505</v>
+      </c>
+      <c r="P1" s="53" t="s">
+        <v>506</v>
+      </c>
+      <c r="Q1" s="53" t="s">
         <v>502</v>
       </c>
-      <c r="P1" s="53" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
@@ -3430,13 +3440,16 @@
         <v>437</v>
       </c>
       <c r="O2" t="s">
+        <v>503</v>
+      </c>
+      <c r="P2" s="57" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q2" t="s">
         <v>504</v>
       </c>
-      <c r="P2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3451,7 +3464,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3465,31 +3478,31 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
       <c r="C7" s="48"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C10" s="48"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vien.Pham updated Testdata at 10:23am June16th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="512">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1977,6 +1977,12 @@
   </si>
   <si>
     <t>Invited Auditor Password</t>
+  </si>
+  <si>
+    <t>Path of Download Location</t>
+  </si>
+  <si>
+    <t>\Downloads\</t>
   </si>
 </sst>
 </file>
@@ -2320,9 +2326,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2330,6 +2333,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3326,10 +3332,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3351,9 +3357,10 @@
     <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3406,8 +3413,11 @@
       <c r="R1" s="53" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" s="53" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
@@ -3460,8 +3470,11 @@
       <c r="R2" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3476,7 +3489,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3490,31 +3503,31 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
       <c r="C7" s="48"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C10" s="48"/>
     </row>
   </sheetData>
@@ -4323,22 +4336,22 @@
       <c r="Q1" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="62" t="s">
+      <c r="R1" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="65" t="s">
+      <c r="S1" s="65"/>
+      <c r="T1" s="64" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="63"/>
-      <c r="V1" s="62" t="s">
+      <c r="U1" s="62"/>
+      <c r="V1" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="63" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="62" t="s">
         <v>210</v>
       </c>
       <c r="AB1" s="66" t="s">
@@ -4390,8 +4403,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4447,17 +4460,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4468,6 +4470,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
vien.Pham updated Testdata at 11:59am June20th 2017
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1940,9 +1940,6 @@
     <t>Auditor Invited</t>
   </si>
   <si>
-    <t>Path of Location</t>
-  </si>
-  <si>
     <t>File Upload Name</t>
   </si>
   <si>
@@ -1983,6 +1980,9 @@
   </si>
   <si>
     <t>\Downloads\</t>
+  </si>
+  <si>
+    <t>Path of Upload Location</t>
   </si>
 </sst>
 </file>
@@ -2326,6 +2326,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2333,9 +2336,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3335,7 +3335,7 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3375,31 +3375,31 @@
         <v>444</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I1" s="53" t="s">
         <v>489</v>
       </c>
       <c r="J1" s="58" t="s">
+        <v>504</v>
+      </c>
+      <c r="K1" s="58" t="s">
         <v>505</v>
-      </c>
-      <c r="K1" s="58" t="s">
-        <v>506</v>
       </c>
       <c r="L1" s="58" t="s">
         <v>486</v>
       </c>
       <c r="M1" s="53" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="N1" s="53" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="O1" s="53" t="s">
         <v>493</v>
@@ -3408,13 +3408,13 @@
         <v>491</v>
       </c>
       <c r="Q1" s="53" t="s">
+        <v>511</v>
+      </c>
+      <c r="R1" s="53" t="s">
         <v>497</v>
       </c>
-      <c r="R1" s="53" t="s">
-        <v>498</v>
-      </c>
       <c r="S1" s="53" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3422,10 +3422,10 @@
         <v>442</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>502</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>503</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>504</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>485</v>
@@ -3465,13 +3465,13 @@
         <v>492</v>
       </c>
       <c r="Q2" t="s">
+        <v>498</v>
+      </c>
+      <c r="R2" t="s">
         <v>499</v>
       </c>
-      <c r="R2" t="s">
-        <v>500</v>
-      </c>
       <c r="S2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -4336,22 +4336,22 @@
       <c r="Q1" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="R1" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="65"/>
-      <c r="T1" s="64" t="s">
+      <c r="S1" s="62"/>
+      <c r="T1" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="65" t="s">
+      <c r="U1" s="63"/>
+      <c r="V1" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="62" t="s">
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="63" t="s">
         <v>210</v>
       </c>
       <c r="AB1" s="66" t="s">
@@ -4403,8 +4403,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4460,6 +4460,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4470,17 +4481,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Merge excel with Vien
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1979,27 +1979,9 @@
     <t>Path of Download Location</t>
   </si>
   <si>
-    <t>\Downloads\</t>
-  </si>
-  <si>
     <t>Path of Upload Location</t>
   </si>
   <si>
-    <t>ToDoName</t>
-  </si>
-  <si>
-    <t>AuditorComment</t>
-  </si>
-  <si>
-    <t>ClientComment</t>
-  </si>
-  <si>
-    <t>AuditorAssignee</t>
-  </si>
-  <si>
-    <t>ClientAssignee</t>
-  </si>
-  <si>
     <t>Todo-01</t>
   </si>
   <si>
@@ -2010,6 +1992,24 @@
   </si>
   <si>
     <t>minh nguyen</t>
+  </si>
+  <si>
+    <t>ToDo Name</t>
+  </si>
+  <si>
+    <t>Auditor Comment</t>
+  </si>
+  <si>
+    <t>Client Comment</t>
+  </si>
+  <si>
+    <t>Auditor Assignee</t>
+  </si>
+  <si>
+    <t>Client Assignee</t>
+  </si>
+  <si>
+    <t>\src\test\resources\download\</t>
   </si>
 </sst>
 </file>
@@ -2353,6 +2353,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2360,9 +2363,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3361,8 +3361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3440,7 +3440,7 @@
         <v>491</v>
       </c>
       <c r="Q1" s="53" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="R1" s="53" t="s">
         <v>497</v>
@@ -3449,19 +3449,19 @@
         <v>509</v>
       </c>
       <c r="T1" s="53" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="U1" s="53" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="V1" s="53" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="W1" s="53" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="X1" s="53" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -3518,22 +3518,22 @@
         <v>499</v>
       </c>
       <c r="S2" t="s">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="T2" s="57" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="U2" s="57" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="V2" s="57" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="W2" s="57" t="s">
         <v>1</v>
       </c>
       <c r="X2" s="57" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4411,22 +4411,22 @@
       <c r="Q1" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="R1" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="65"/>
-      <c r="T1" s="64" t="s">
+      <c r="S1" s="62"/>
+      <c r="T1" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="62"/>
-      <c r="V1" s="65" t="s">
+      <c r="U1" s="63"/>
+      <c r="V1" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="62" t="s">
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="63" t="s">
         <v>210</v>
       </c>
       <c r="AB1" s="66" t="s">
@@ -4478,8 +4478,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4535,6 +4535,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4545,17 +4556,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Apply using specific name for engagement, delete engagement via DB, change st in excel
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1922,12 +1922,6 @@
     <t>Testpassword1!</t>
   </si>
   <si>
-    <t>EngagementName</t>
-  </si>
-  <si>
-    <t>Engagement 01</t>
-  </si>
-  <si>
     <t>Engagement Name Generated</t>
   </si>
   <si>
@@ -1937,9 +1931,6 @@
     <t>auditor.user04@gmail.com</t>
   </si>
   <si>
-    <t>Auditor Invited</t>
-  </si>
-  <si>
     <t>File Upload Name</t>
   </si>
   <si>
@@ -1982,9 +1973,6 @@
     <t>Path of Upload Location</t>
   </si>
   <si>
-    <t>Todo-01</t>
-  </si>
-  <si>
     <t>Hello client</t>
   </si>
   <si>
@@ -2010,6 +1998,18 @@
   </si>
   <si>
     <t>\src\test\resources\download\</t>
+  </si>
+  <si>
+    <t>Smoke Engagement Name</t>
+  </si>
+  <si>
+    <t>Smoke ToDo name</t>
+  </si>
+  <si>
+    <t>Smoke Invited Auditor Full Name</t>
+  </si>
+  <si>
+    <t>Engagement Name</t>
   </si>
 </sst>
 </file>
@@ -3361,8 +3361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3379,13 +3379,13 @@
     <col min="10" max="11" width="20.7109375" style="57" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.7109375" style="57" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24" customWidth="1"/>
+    <col min="14" max="14" width="31" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -3407,61 +3407,61 @@
         <v>444</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="I1" s="53" t="s">
         <v>489</v>
       </c>
       <c r="J1" s="58" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="K1" s="58" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="L1" s="58" t="s">
         <v>486</v>
       </c>
       <c r="M1" s="53" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="N1" s="53" t="s">
+        <v>504</v>
+      </c>
+      <c r="O1" s="53" t="s">
+        <v>491</v>
+      </c>
+      <c r="P1" s="53" t="s">
+        <v>520</v>
+      </c>
+      <c r="Q1" s="53" t="s">
         <v>507</v>
       </c>
-      <c r="O1" s="53" t="s">
-        <v>493</v>
-      </c>
-      <c r="P1" s="53" t="s">
-        <v>491</v>
-      </c>
-      <c r="Q1" s="53" t="s">
-        <v>510</v>
-      </c>
       <c r="R1" s="53" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="S1" s="53" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="T1" s="53" t="s">
+        <v>511</v>
+      </c>
+      <c r="U1" s="53" t="s">
+        <v>512</v>
+      </c>
+      <c r="V1" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="W1" s="53" t="s">
+        <v>514</v>
+      </c>
+      <c r="X1" s="53" t="s">
         <v>515</v>
-      </c>
-      <c r="U1" s="53" t="s">
-        <v>516</v>
-      </c>
-      <c r="V1" s="53" t="s">
-        <v>517</v>
-      </c>
-      <c r="W1" s="53" t="s">
-        <v>518</v>
-      </c>
-      <c r="X1" s="53" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -3469,17 +3469,17 @@
         <v>442</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>485</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="59" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="G2" s="59" t="s">
         <v>437</v>
@@ -3503,37 +3503,37 @@
         <v>437</v>
       </c>
       <c r="N2" s="60" t="s">
+        <v>519</v>
+      </c>
+      <c r="O2" s="57" t="s">
+        <v>492</v>
+      </c>
+      <c r="P2" s="57" t="s">
+        <v>517</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>495</v>
+      </c>
+      <c r="R2" t="s">
         <v>496</v>
       </c>
-      <c r="O2" s="57" t="s">
-        <v>494</v>
-      </c>
-      <c r="P2" s="57" t="s">
-        <v>492</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>498</v>
-      </c>
-      <c r="R2" t="s">
-        <v>499</v>
-      </c>
       <c r="S2" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="T2" s="57" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="U2" s="57" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="V2" s="57" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="W2" s="57" t="s">
         <v>1</v>
       </c>
       <c r="X2" s="57" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create new test case verifyAssignToDoBulkAction(). Add new function deleteMemberInEngagementByName()
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="513">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1922,9 +1922,6 @@
     <t>Testpassword1!</t>
   </si>
   <si>
-    <t>EngagementName</t>
-  </si>
-  <si>
     <t>Engagement 01</t>
   </si>
   <si>
@@ -1977,6 +1974,18 @@
   </si>
   <si>
     <t>Invited Auditor Password</t>
+  </si>
+  <si>
+    <t>ToDoName</t>
+  </si>
+  <si>
+    <t>Todo-01</t>
+  </si>
+  <si>
+    <t>Auditor Lead Name</t>
+  </si>
+  <si>
+    <t>Engagement Name</t>
   </si>
 </sst>
 </file>
@@ -2320,9 +2329,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2330,6 +2336,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3326,10 +3335,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,7 +3347,7 @@
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.140625" style="57" customWidth="1"/>
@@ -3351,9 +3360,10 @@
     <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="51" t="s">
         <v>438</v>
@@ -3365,64 +3375,69 @@
         <v>440</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>444</v>
+        <v>511</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I1" s="53" t="s">
         <v>489</v>
       </c>
       <c r="J1" s="58" t="s">
+        <v>504</v>
+      </c>
+      <c r="K1" s="58" t="s">
         <v>505</v>
-      </c>
-      <c r="K1" s="58" t="s">
-        <v>506</v>
       </c>
       <c r="L1" s="58" t="s">
         <v>486</v>
       </c>
       <c r="M1" s="53" t="s">
+        <v>508</v>
+      </c>
+      <c r="N1" s="53" t="s">
+        <v>507</v>
+      </c>
+      <c r="O1" s="53" t="s">
+        <v>492</v>
+      </c>
+      <c r="P1" s="53" t="s">
+        <v>512</v>
+      </c>
+      <c r="Q1" s="53" t="s">
+        <v>496</v>
+      </c>
+      <c r="R1" s="53" t="s">
+        <v>497</v>
+      </c>
+      <c r="S1" s="53" t="s">
         <v>509</v>
       </c>
-      <c r="N1" s="53" t="s">
-        <v>508</v>
-      </c>
-      <c r="O1" s="53" t="s">
-        <v>493</v>
-      </c>
-      <c r="P1" s="53" t="s">
-        <v>491</v>
-      </c>
-      <c r="Q1" s="53" t="s">
-        <v>497</v>
-      </c>
-      <c r="R1" s="53" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>442</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>502</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>503</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>504</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>485</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="F2" s="59" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G2" s="59" t="s">
         <v>437</v>
@@ -3446,22 +3461,25 @@
         <v>437</v>
       </c>
       <c r="N2" s="60" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O2" s="57" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="P2" s="57" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q2" t="s">
+        <v>498</v>
+      </c>
+      <c r="R2" t="s">
         <v>499</v>
       </c>
-      <c r="R2" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="57" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>443</v>
       </c>
@@ -3476,7 +3494,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="51" t="s">
         <v>451</v>
       </c>
@@ -3490,31 +3508,31 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="58"/>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
       <c r="B6" s="48"/>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="53"/>
       <c r="C7" s="48"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="53"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="53"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C10" s="48"/>
     </row>
   </sheetData>
@@ -4323,22 +4341,22 @@
       <c r="Q1" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="62" t="s">
+      <c r="R1" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="65" t="s">
+      <c r="S1" s="65"/>
+      <c r="T1" s="64" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="63"/>
-      <c r="V1" s="62" t="s">
+      <c r="U1" s="62"/>
+      <c r="V1" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="63" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="62" t="s">
         <v>210</v>
       </c>
       <c r="AB1" s="66" t="s">
@@ -4390,8 +4408,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4447,17 +4465,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4468,6 +4475,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5299,7 +5317,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minhnh add new verifyClientUploadDownloadOnRequest
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -28,12 +28,11 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="0" calcOnSave="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="496">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1830,6 +1829,12 @@
   </si>
   <si>
     <t>minh nguyen</t>
+  </si>
+  <si>
+    <t>TXT_helloAuvenir_client.txt</t>
+  </si>
+  <si>
+    <t>\src\test\resources\download\</t>
   </si>
 </sst>
 </file>
@@ -2169,6 +2174,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2176,9 +2184,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3116,10 +3121,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3148,7 +3153,7 @@
     <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="50" t="s">
         <v>422</v>
@@ -3217,7 +3222,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>425</v>
       </c>
@@ -3286,8 +3291,8 @@
         <v>493</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+    <row r="3" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
         <v>426</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -3300,8 +3305,35 @@
         <v>430</v>
       </c>
       <c r="E3" s="7"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P3" s="55" t="s">
+        <v>467</v>
+      </c>
+      <c r="Q3" s="55" t="s">
+        <v>474</v>
+      </c>
+      <c r="R3" s="55" t="s">
+        <v>494</v>
+      </c>
+      <c r="S3" s="55" t="s">
+        <v>495</v>
+      </c>
+      <c r="T3" s="55" t="s">
+        <v>490</v>
+      </c>
+      <c r="U3" s="55" t="s">
+        <v>491</v>
+      </c>
+      <c r="V3" s="55" t="s">
+        <v>492</v>
+      </c>
+      <c r="W3" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="X3" s="55" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
         <v>434</v>
       </c>
@@ -3315,31 +3347,31 @@
         <v>436</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="56"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="47"/>
       <c r="C6" s="47"/>
       <c r="D6" s="47"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="C7" s="47"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="47"/>
       <c r="C8" s="47"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C10" s="47"/>
     </row>
   </sheetData>
@@ -3822,22 +3854,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="60"/>
+      <c r="T1" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="63" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="60" t="s">
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -3889,8 +3921,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -3946,6 +3978,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -3956,17 +3999,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update TestData: Add white space in Engagement Name
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="521">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="522">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1922,9 +1922,6 @@
     <t>Testpassword1!</t>
   </si>
   <si>
-    <t>EngagementName</t>
-  </si>
-  <si>
     <t>Engagement 01</t>
   </si>
   <si>
@@ -1958,58 +1955,64 @@
     <t>auveniradm@gmail.com</t>
   </si>
   <si>
+    <t>Admin Email Password</t>
+  </si>
+  <si>
+    <t>Auditor Email Password</t>
+  </si>
+  <si>
+    <t>Invited Auditor</t>
+  </si>
+  <si>
+    <t>Invited Auditor Full Name</t>
+  </si>
+  <si>
+    <t>Invited Auditor Password</t>
+  </si>
+  <si>
+    <t>Path of Download Location</t>
+  </si>
+  <si>
+    <t>Path of Upload Location</t>
+  </si>
+  <si>
+    <t>Todo-01</t>
+  </si>
+  <si>
+    <t>Hello client</t>
+  </si>
+  <si>
+    <t>Hello auditor</t>
+  </si>
+  <si>
+    <t>minh nguyen</t>
+  </si>
+  <si>
+    <t>ToDo Name</t>
+  </si>
+  <si>
+    <t>Auditor Comment</t>
+  </si>
+  <si>
+    <t>Client Comment</t>
+  </si>
+  <si>
+    <t>Auditor Assignee</t>
+  </si>
+  <si>
+    <t>Client Assignee</t>
+  </si>
+  <si>
+    <t>\src\test\resources\download\</t>
+  </si>
+  <si>
+    <t>Auditor Lead Name</t>
+  </si>
+  <si>
+    <t>Engagement Name</t>
+  </si>
+  <si>
     <t>auvenirauditor@gmail.com</t>
-  </si>
-  <si>
-    <t>Admin Email Password</t>
-  </si>
-  <si>
-    <t>Auditor Email Password</t>
-  </si>
-  <si>
-    <t>Invited Auditor</t>
-  </si>
-  <si>
-    <t>Invited Auditor Full Name</t>
-  </si>
-  <si>
-    <t>Invited Auditor Password</t>
-  </si>
-  <si>
-    <t>Path of Download Location</t>
-  </si>
-  <si>
-    <t>Path of Upload Location</t>
-  </si>
-  <si>
-    <t>Todo-01</t>
-  </si>
-  <si>
-    <t>Hello client</t>
-  </si>
-  <si>
-    <t>Hello auditor</t>
-  </si>
-  <si>
-    <t>minh nguyen</t>
-  </si>
-  <si>
-    <t>ToDo Name</t>
-  </si>
-  <si>
-    <t>Auditor Comment</t>
-  </si>
-  <si>
-    <t>Client Comment</t>
-  </si>
-  <si>
-    <t>Auditor Assignee</t>
-  </si>
-  <si>
-    <t>Client Assignee</t>
-  </si>
-  <si>
-    <t>\src\test\resources\download\</t>
   </si>
 </sst>
 </file>
@@ -2353,9 +2356,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2363,6 +2363,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3361,8 +3364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3404,64 +3407,64 @@
         <v>440</v>
       </c>
       <c r="E1" s="51" t="s">
-        <v>444</v>
+        <v>519</v>
       </c>
       <c r="F1" s="53" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H1" s="53" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I1" s="53" t="s">
         <v>489</v>
       </c>
       <c r="J1" s="58" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="K1" s="58" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="L1" s="58" t="s">
         <v>486</v>
       </c>
       <c r="M1" s="53" t="s">
+        <v>506</v>
+      </c>
+      <c r="N1" s="53" t="s">
+        <v>505</v>
+      </c>
+      <c r="O1" s="53" t="s">
+        <v>492</v>
+      </c>
+      <c r="P1" s="53" t="s">
+        <v>520</v>
+      </c>
+      <c r="Q1" s="53" t="s">
         <v>508</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="R1" s="53" t="s">
+        <v>496</v>
+      </c>
+      <c r="S1" s="53" t="s">
         <v>507</v>
       </c>
-      <c r="O1" s="53" t="s">
-        <v>493</v>
-      </c>
-      <c r="P1" s="53" t="s">
-        <v>491</v>
-      </c>
-      <c r="Q1" s="53" t="s">
-        <v>510</v>
-      </c>
-      <c r="R1" s="53" t="s">
-        <v>497</v>
-      </c>
-      <c r="S1" s="53" t="s">
-        <v>509</v>
-      </c>
       <c r="T1" s="53" t="s">
+        <v>513</v>
+      </c>
+      <c r="U1" s="53" t="s">
+        <v>514</v>
+      </c>
+      <c r="V1" s="53" t="s">
         <v>515</v>
       </c>
-      <c r="U1" s="53" t="s">
+      <c r="W1" s="53" t="s">
         <v>516</v>
       </c>
-      <c r="V1" s="53" t="s">
+      <c r="X1" s="53" t="s">
         <v>517</v>
-      </c>
-      <c r="W1" s="53" t="s">
-        <v>518</v>
-      </c>
-      <c r="X1" s="53" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -3469,17 +3472,19 @@
         <v>442</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>503</v>
+        <v>521</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>485</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="F2" s="59" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G2" s="59" t="s">
         <v>437</v>
@@ -3503,37 +3508,37 @@
         <v>437</v>
       </c>
       <c r="N2" s="60" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O2" s="57" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="P2" s="57" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q2" t="s">
+        <v>497</v>
+      </c>
+      <c r="R2" t="s">
         <v>498</v>
       </c>
-      <c r="R2" t="s">
-        <v>499</v>
-      </c>
       <c r="S2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="T2" s="57" t="s">
+        <v>509</v>
+      </c>
+      <c r="U2" s="57" t="s">
+        <v>510</v>
+      </c>
+      <c r="V2" s="57" t="s">
         <v>511</v>
-      </c>
-      <c r="U2" s="57" t="s">
-        <v>512</v>
-      </c>
-      <c r="V2" s="57" t="s">
-        <v>513</v>
       </c>
       <c r="W2" s="57" t="s">
         <v>1</v>
       </c>
       <c r="X2" s="57" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4411,22 +4416,22 @@
       <c r="Q1" s="61" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="62" t="s">
+      <c r="R1" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="65" t="s">
+      <c r="S1" s="65"/>
+      <c r="T1" s="64" t="s">
         <v>212</v>
       </c>
-      <c r="U1" s="63"/>
-      <c r="V1" s="62" t="s">
+      <c r="U1" s="62"/>
+      <c r="V1" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="63" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="62" t="s">
         <v>210</v>
       </c>
       <c r="AB1" s="66" t="s">
@@ -4478,8 +4483,8 @@
       <c r="Z2" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="64"/>
+      <c r="AA2" s="63"/>
+      <c r="AB2" s="63"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4535,17 +4540,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4556,6 +4550,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update test data for Client Assignee testcase
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="496">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1799,9 +1799,6 @@
   </si>
   <si>
     <t>Client Comment</t>
-  </si>
-  <si>
-    <t>Auditor Assignee</t>
   </si>
   <si>
     <t>Client Assignee</t>
@@ -2177,6 +2174,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2184,9 +2184,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3124,10 +3121,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3153,11 +3150,10 @@
     <col min="20" max="20" width="17.42578125" customWidth="1"/>
     <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="50" t="s">
         <v>422</v>
@@ -3169,7 +3165,7 @@
         <v>424</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F1" s="52" t="s">
         <v>478</v>
@@ -3202,13 +3198,13 @@
         <v>466</v>
       </c>
       <c r="P1" s="52" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="Q1" s="52" t="s">
+        <v>493</v>
+      </c>
+      <c r="R1" s="52" t="s">
         <v>494</v>
-      </c>
-      <c r="R1" s="52" t="s">
-        <v>495</v>
       </c>
       <c r="S1" s="52" t="s">
         <v>470</v>
@@ -3225,11 +3221,8 @@
       <c r="W1" t="s">
         <v>484</v>
       </c>
-      <c r="X1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>425</v>
       </c>
@@ -3237,7 +3230,7 @@
         <v>475</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>460</v>
@@ -3282,28 +3275,25 @@
         <v>471</v>
       </c>
       <c r="R2" s="55" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="S2" t="s">
         <v>472</v>
       </c>
       <c r="T2" t="s">
+        <v>485</v>
+      </c>
+      <c r="U2" t="s">
         <v>486</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>487</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>488</v>
       </c>
-      <c r="W2" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>426</v>
       </c>
@@ -3324,28 +3314,25 @@
         <v>471</v>
       </c>
       <c r="R3" s="55" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="S3" s="55" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="T3" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="U3" s="55" t="s">
         <v>486</v>
       </c>
-      <c r="U3" s="55" t="s">
+      <c r="V3" s="55" t="s">
         <v>487</v>
       </c>
-      <c r="V3" s="55" t="s">
+      <c r="W3" s="55" t="s">
         <v>488</v>
       </c>
-      <c r="W3" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="X3" s="55" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
         <v>433</v>
       </c>
@@ -3359,31 +3346,31 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="56"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="47"/>
       <c r="C6" s="47"/>
       <c r="D6" s="47"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="C7" s="47"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="47"/>
       <c r="C8" s="47"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C10" s="47"/>
     </row>
   </sheetData>
@@ -3866,22 +3853,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="60"/>
+      <c r="T1" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="63" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="60" t="s">
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -3933,8 +3920,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -3990,6 +3977,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4000,17 +3998,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update test case verifyAssignToDoBulkAction, Add test cases verifyClientViewAuditorComment, verifyAuditorViewClientComment
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="494">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1741,9 +1741,6 @@
     <t>Client Auvenir Password</t>
   </si>
   <si>
-    <t>Testpassword1!</t>
-  </si>
-  <si>
     <t>Engagement 01</t>
   </si>
   <si>
@@ -1753,9 +1750,6 @@
     <t>aa</t>
   </si>
   <si>
-    <t>auditor.user04@gmail.com</t>
-  </si>
-  <si>
     <t>Auditor Invited</t>
   </si>
   <si>
@@ -1834,7 +1828,7 @@
     <t>Path of Download Location</t>
   </si>
   <si>
-    <t>auvenirauditor@gmail.com</t>
+    <t>auditor.user02@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2174,9 +2168,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2184,6 +2175,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3123,15 +3117,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
@@ -3165,61 +3159,61 @@
         <v>424</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I1" s="52" t="s">
         <v>463</v>
       </c>
       <c r="J1" s="56" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="K1" s="56" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="L1" s="56" t="s">
         <v>461</v>
       </c>
       <c r="M1" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="N1" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>465</v>
+      </c>
+      <c r="P1" s="52" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q1" s="52" t="s">
+        <v>491</v>
+      </c>
+      <c r="R1" s="52" t="s">
+        <v>492</v>
+      </c>
+      <c r="S1" s="52" t="s">
+        <v>468</v>
+      </c>
+      <c r="T1" t="s">
+        <v>479</v>
+      </c>
+      <c r="U1" t="s">
         <v>480</v>
       </c>
-      <c r="N1" s="52" t="s">
-        <v>479</v>
-      </c>
-      <c r="O1" s="52" t="s">
-        <v>466</v>
-      </c>
-      <c r="P1" s="52" t="s">
-        <v>490</v>
-      </c>
-      <c r="Q1" s="52" t="s">
-        <v>493</v>
-      </c>
-      <c r="R1" s="52" t="s">
-        <v>494</v>
-      </c>
-      <c r="S1" s="52" t="s">
-        <v>470</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>481</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>482</v>
-      </c>
-      <c r="V1" t="s">
-        <v>483</v>
-      </c>
-      <c r="W1" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -3227,10 +3221,10 @@
         <v>425</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>495</v>
+        <v>430</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>460</v>
@@ -3239,7 +3233,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="57" t="s">
-        <v>468</v>
+        <v>493</v>
       </c>
       <c r="G2" s="57" t="s">
         <v>421</v>
@@ -3247,8 +3241,8 @@
       <c r="H2" s="57" t="s">
         <v>421</v>
       </c>
-      <c r="I2" s="55" t="s">
-        <v>464</v>
+      <c r="I2" s="47" t="s">
+        <v>421</v>
       </c>
       <c r="J2" s="57" t="s">
         <v>421</v>
@@ -3263,34 +3257,34 @@
         <v>421</v>
       </c>
       <c r="N2" s="58" t="s">
+        <v>467</v>
+      </c>
+      <c r="O2" s="55" t="s">
+        <v>466</v>
+      </c>
+      <c r="P2" s="55" t="s">
+        <v>464</v>
+      </c>
+      <c r="Q2" t="s">
         <v>469</v>
       </c>
-      <c r="O2" s="55" t="s">
-        <v>467</v>
-      </c>
-      <c r="P2" s="55" t="s">
-        <v>465</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>471</v>
-      </c>
       <c r="R2" s="55" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="S2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="T2" t="s">
+        <v>483</v>
+      </c>
+      <c r="U2" t="s">
+        <v>484</v>
+      </c>
+      <c r="V2" t="s">
         <v>485</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>486</v>
-      </c>
-      <c r="V2" t="s">
-        <v>487</v>
-      </c>
-      <c r="W2" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -3308,28 +3302,28 @@
       </c>
       <c r="E3" s="7"/>
       <c r="P3" s="55" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Q3" s="55" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="R3" s="55" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="S3" s="55" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="T3" s="55" t="s">
+        <v>483</v>
+      </c>
+      <c r="U3" s="55" t="s">
+        <v>484</v>
+      </c>
+      <c r="V3" s="55" t="s">
         <v>485</v>
       </c>
-      <c r="U3" s="55" t="s">
+      <c r="W3" s="55" t="s">
         <v>486</v>
-      </c>
-      <c r="V3" s="55" t="s">
-        <v>487</v>
-      </c>
-      <c r="W3" s="55" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -3382,6 +3376,8 @@
     <hyperlink ref="C2" r:id="rId5"/>
     <hyperlink ref="B2" r:id="rId6"/>
     <hyperlink ref="J2" r:id="rId7"/>
+    <hyperlink ref="D2" r:id="rId8"/>
+    <hyperlink ref="I2" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3853,22 +3849,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="63" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="60"/>
-      <c r="T1" s="63" t="s">
+      <c r="S1" s="63"/>
+      <c r="T1" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="61"/>
-      <c r="V1" s="60" t="s">
+      <c r="U1" s="60"/>
+      <c r="V1" s="63" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="61" t="s">
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="63"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="60" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -3920,8 +3916,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -3977,17 +3973,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -3998,6 +3983,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update testData, delete column Auditor Assignee
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="495">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1741,9 +1741,6 @@
     <t>Client Auvenir Password</t>
   </si>
   <si>
-    <t>Testpassword1!</t>
-  </si>
-  <si>
     <t>Engagement 01</t>
   </si>
   <si>
@@ -1802,9 +1799,6 @@
   </si>
   <si>
     <t>Client Comment</t>
-  </si>
-  <si>
-    <t>Auditor Assignee</t>
   </si>
   <si>
     <t>Client Assignee</t>
@@ -2177,6 +2171,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2184,9 +2181,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3124,10 +3118,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3153,11 +3147,10 @@
     <col min="20" max="20" width="17.42578125" customWidth="1"/>
     <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="50" t="s">
         <v>422</v>
@@ -3169,75 +3162,72 @@
         <v>424</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I1" s="52" t="s">
         <v>463</v>
       </c>
       <c r="J1" s="56" t="s">
+        <v>476</v>
+      </c>
+      <c r="K1" s="56" t="s">
         <v>477</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>478</v>
       </c>
       <c r="L1" s="56" t="s">
         <v>461</v>
       </c>
       <c r="M1" s="52" t="s">
+        <v>480</v>
+      </c>
+      <c r="N1" s="52" t="s">
+        <v>479</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>465</v>
+      </c>
+      <c r="P1" s="52" t="s">
+        <v>490</v>
+      </c>
+      <c r="Q1" s="52" t="s">
+        <v>493</v>
+      </c>
+      <c r="R1" s="52" t="s">
+        <v>494</v>
+      </c>
+      <c r="S1" s="52" t="s">
+        <v>469</v>
+      </c>
+      <c r="T1" t="s">
         <v>481</v>
       </c>
-      <c r="N1" s="52" t="s">
-        <v>480</v>
-      </c>
-      <c r="O1" s="52" t="s">
-        <v>466</v>
-      </c>
-      <c r="P1" s="52" t="s">
-        <v>492</v>
-      </c>
-      <c r="Q1" s="52" t="s">
-        <v>495</v>
-      </c>
-      <c r="R1" s="52" t="s">
-        <v>496</v>
-      </c>
-      <c r="S1" s="52" t="s">
-        <v>470</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>482</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>483</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>484</v>
       </c>
-      <c r="W1" t="s">
-        <v>485</v>
-      </c>
-      <c r="X1" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
         <v>425</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>475</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>476</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>460</v>
@@ -3246,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="57" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G2" s="57" t="s">
         <v>421</v>
@@ -3254,8 +3244,8 @@
       <c r="H2" s="57" t="s">
         <v>421</v>
       </c>
-      <c r="I2" s="55" t="s">
-        <v>464</v>
+      <c r="I2" s="47" t="s">
+        <v>421</v>
       </c>
       <c r="J2" s="57" t="s">
         <v>421</v>
@@ -3270,40 +3260,37 @@
         <v>421</v>
       </c>
       <c r="N2" s="58" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="O2" s="55" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P2" s="55" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Q2" t="s">
+        <v>470</v>
+      </c>
+      <c r="R2" s="55" t="s">
+        <v>492</v>
+      </c>
+      <c r="S2" t="s">
         <v>471</v>
       </c>
-      <c r="R2" s="55" t="s">
-        <v>494</v>
-      </c>
-      <c r="S2" t="s">
-        <v>472</v>
-      </c>
       <c r="T2" t="s">
+        <v>485</v>
+      </c>
+      <c r="U2" t="s">
+        <v>486</v>
+      </c>
+      <c r="V2" t="s">
         <v>487</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>488</v>
       </c>
-      <c r="V2" t="s">
-        <v>489</v>
-      </c>
-      <c r="W2" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:23" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>426</v>
       </c>
@@ -3318,34 +3305,31 @@
       </c>
       <c r="E3" s="7"/>
       <c r="P3" s="55" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="Q3" s="55" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="R3" s="55" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="S3" s="55" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="T3" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="U3" s="55" t="s">
+        <v>486</v>
+      </c>
+      <c r="V3" s="55" t="s">
         <v>487</v>
       </c>
-      <c r="U3" s="55" t="s">
+      <c r="W3" s="55" t="s">
         <v>488</v>
       </c>
-      <c r="V3" s="55" t="s">
-        <v>489</v>
-      </c>
-      <c r="W3" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="X3" s="55" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
         <v>433</v>
       </c>
@@ -3359,31 +3343,31 @@
         <v>435</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="56"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="52"/>
       <c r="B6" s="47"/>
       <c r="C6" s="47"/>
       <c r="D6" s="47"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="C7" s="47"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="47"/>
       <c r="C8" s="47"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C10" s="47"/>
     </row>
   </sheetData>
@@ -3395,6 +3379,7 @@
     <hyperlink ref="C2" r:id="rId5"/>
     <hyperlink ref="B2" r:id="rId6"/>
     <hyperlink ref="J2" r:id="rId7"/>
+    <hyperlink ref="I2" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3866,22 +3851,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="60"/>
+      <c r="T1" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="63" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="60" t="s">
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -3933,8 +3918,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -3990,6 +3975,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4000,17 +3996,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update testData, add data for loginData sheet
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="9810" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="508">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1838,6 +1838,39 @@
   </si>
   <si>
     <t>TXT_ATTACHMENT.docx</t>
+  </si>
+  <si>
+    <t>Auditor Lead</t>
+  </si>
+  <si>
+    <t>client.user01@gmail.com</t>
+  </si>
+  <si>
+    <t>TESTPASSWORD</t>
+  </si>
+  <si>
+    <t>Testpassword1!</t>
+  </si>
+  <si>
+    <t>auditor.user02@gmail.com</t>
+  </si>
+  <si>
+    <t>Valid User4</t>
+  </si>
+  <si>
+    <t>USER_PWD</t>
+  </si>
+  <si>
+    <t>INVALID VALUE1</t>
+  </si>
+  <si>
+    <t>INVALID VALUE2</t>
+  </si>
+  <si>
+    <t>INVALID VALUE3</t>
+  </si>
+  <si>
+    <t>Valid Userminh</t>
   </si>
 </sst>
 </file>
@@ -2177,6 +2210,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2184,9 +2220,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3126,7 +3159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
@@ -3761,12 +3794,217 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="56" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>423</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>424</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>497</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>460</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="56" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="55" t="s">
+        <v>499</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>426</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>501</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>429</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>433</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>436</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>434</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>502</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>503</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="D6" s="47"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>504</v>
+      </c>
+      <c r="B7" s="55"/>
+      <c r="C7" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>505</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>506</v>
+      </c>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="55"/>
+      <c r="C10" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="s">
+        <v>507</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>439</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>439</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>439</v>
+      </c>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="D3" r:id="rId5"/>
+    <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="D4" r:id="rId7"/>
+    <hyperlink ref="B4" r:id="rId8"/>
+    <hyperlink ref="C7" r:id="rId9"/>
+    <hyperlink ref="C8" r:id="rId10"/>
+    <hyperlink ref="C10" r:id="rId11"/>
+    <hyperlink ref="B6" r:id="rId12"/>
+    <hyperlink ref="C6" r:id="rId13"/>
+    <hyperlink ref="C5" r:id="rId14"/>
+    <hyperlink ref="B11" r:id="rId15"/>
+    <hyperlink ref="C11" r:id="rId16"/>
+    <hyperlink ref="D11" r:id="rId17"/>
+    <hyperlink ref="C2" r:id="rId18"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3867,22 +4105,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="60"/>
+      <c r="T1" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="63" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="60" t="s">
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -3934,8 +4172,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -3991,6 +4229,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4001,17 +4250,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix test case verifyAdminChangeStatusUserToOnBoarding(). The xpath is changed.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="9810" firstSheet="11" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="9810" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="507">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1611,9 +1611,6 @@
     <t>admin.user02@gmail.com</t>
   </si>
   <si>
-    <t>auditor.user02gmail.com</t>
-  </si>
-  <si>
     <t>client.user02@gmail.com</t>
   </si>
   <si>
@@ -1816,28 +1813,61 @@
     <t>Path of Download Location</t>
   </si>
   <si>
+    <t>client03.auvenir@gmail.com</t>
+  </si>
+  <si>
+    <t>Titan client</t>
+  </si>
+  <si>
+    <t>Auditor Invited</t>
+  </si>
+  <si>
+    <t>TXT_helloAuvenir.docx</t>
+  </si>
+  <si>
+    <t>TXT_helloAuvenir_client.docx</t>
+  </si>
+  <si>
+    <t>File Attach Name</t>
+  </si>
+  <si>
+    <t>TXT_ATTACHMENT.docx</t>
+  </si>
+  <si>
+    <t>Auditor Lead</t>
+  </si>
+  <si>
+    <t>client.user01@gmail.com</t>
+  </si>
+  <si>
+    <t>TESTPASSWORD</t>
+  </si>
+  <si>
+    <t>Testpassword1!</t>
+  </si>
+  <si>
+    <t>auditor.user02@gmail.com</t>
+  </si>
+  <si>
+    <t>Valid User4</t>
+  </si>
+  <si>
+    <t>USER_PWD</t>
+  </si>
+  <si>
+    <t>INVALID VALUE1</t>
+  </si>
+  <si>
+    <t>INVALID VALUE2</t>
+  </si>
+  <si>
+    <t>INVALID VALUE3</t>
+  </si>
+  <si>
+    <t>Valid Userminh</t>
+  </si>
+  <si>
     <t>auditor01.auvenir@gmail.com</t>
-  </si>
-  <si>
-    <t>client03.auvenir@gmail.com</t>
-  </si>
-  <si>
-    <t>Titan client</t>
-  </si>
-  <si>
-    <t>Auditor Invited</t>
-  </si>
-  <si>
-    <t>TXT_helloAuvenir.docx</t>
-  </si>
-  <si>
-    <t>TXT_helloAuvenir_client.docx</t>
-  </si>
-  <si>
-    <t>File Attach Name</t>
-  </si>
-  <si>
-    <t>TXT_ATTACHMENT.docx</t>
   </si>
 </sst>
 </file>
@@ -2870,7 +2900,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>32</v>
@@ -2890,7 +2920,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -2965,7 +2995,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>33</v>
@@ -2996,7 +3026,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B4" s="49" t="s">
         <v>399</v>
@@ -3004,7 +3034,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B5" s="49" t="s">
         <v>421</v>
@@ -3012,10 +3042,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
+        <v>436</v>
+      </c>
+      <c r="B6" s="47" t="s">
         <v>437</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -3069,10 +3099,10 @@
         <v>25</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3080,22 +3110,22 @@
         <v>425</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C2" s="47" t="s">
+        <v>433</v>
+      </c>
+      <c r="D2" s="47" t="s">
         <v>434</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>435</v>
       </c>
       <c r="E2" s="47" t="s">
         <v>421</v>
       </c>
       <c r="F2" s="53" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G2" s="53" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -3126,8 +3156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,64 +3199,64 @@
         <v>424</v>
       </c>
       <c r="E1" s="50" t="s">
+        <v>483</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>472</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>468</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>467</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>460</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>470</v>
+      </c>
+      <c r="K1" s="56" t="s">
+        <v>471</v>
+      </c>
+      <c r="L1" s="56" t="s">
+        <v>459</v>
+      </c>
+      <c r="M1" s="52" t="s">
+        <v>474</v>
+      </c>
+      <c r="N1" s="52" t="s">
+        <v>473</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>462</v>
+      </c>
+      <c r="P1" s="52" t="s">
         <v>484</v>
       </c>
-      <c r="F1" s="52" t="s">
-        <v>473</v>
-      </c>
-      <c r="G1" s="52" t="s">
-        <v>469</v>
-      </c>
-      <c r="H1" s="52" t="s">
-        <v>468</v>
-      </c>
-      <c r="I1" s="52" t="s">
-        <v>461</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>471</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>472</v>
-      </c>
-      <c r="L1" s="56" t="s">
-        <v>460</v>
-      </c>
-      <c r="M1" s="52" t="s">
+      <c r="Q1" s="52" t="s">
+        <v>486</v>
+      </c>
+      <c r="R1" s="52" t="s">
+        <v>487</v>
+      </c>
+      <c r="S1" s="52" t="s">
+        <v>465</v>
+      </c>
+      <c r="T1" s="52" t="s">
         <v>475</v>
       </c>
-      <c r="N1" s="52" t="s">
-        <v>474</v>
-      </c>
-      <c r="O1" s="52" t="s">
-        <v>463</v>
-      </c>
-      <c r="P1" s="52" t="s">
-        <v>485</v>
-      </c>
-      <c r="Q1" s="52" t="s">
-        <v>487</v>
-      </c>
-      <c r="R1" s="52" t="s">
-        <v>488</v>
-      </c>
-      <c r="S1" s="52" t="s">
-        <v>466</v>
-      </c>
-      <c r="T1" s="52" t="s">
+      <c r="U1" s="52" t="s">
         <v>476</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="V1" s="52" t="s">
         <v>477</v>
       </c>
-      <c r="V1" s="52" t="s">
+      <c r="W1" s="52" t="s">
         <v>478</v>
       </c>
-      <c r="W1" s="52" t="s">
-        <v>479</v>
-      </c>
       <c r="X1" s="52" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -3234,19 +3264,19 @@
         <v>425</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>489</v>
+        <v>506</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="57" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G2" s="57" t="s">
         <v>421</v>
@@ -3270,37 +3300,37 @@
         <v>421</v>
       </c>
       <c r="N2" s="58" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="O2" s="55" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="P2" s="55" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R2" s="55" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="S2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="T2" t="s">
+        <v>479</v>
+      </c>
+      <c r="U2" t="s">
         <v>480</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>481</v>
       </c>
-      <c r="V2" t="s">
-        <v>482</v>
-      </c>
       <c r="W2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="X2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -3311,49 +3341,49 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>428</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>429</v>
       </c>
       <c r="E3" s="7"/>
       <c r="P3" s="55" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q3" s="55" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R3" s="55" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="S3" s="55" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="T3" s="55" t="s">
+        <v>479</v>
+      </c>
+      <c r="U3" s="55" t="s">
         <v>480</v>
       </c>
-      <c r="U3" s="55" t="s">
+      <c r="V3" s="55" t="s">
         <v>481</v>
       </c>
-      <c r="V3" s="55" t="s">
+      <c r="W3" s="55" t="s">
         <v>482</v>
-      </c>
-      <c r="W3" s="55" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
+        <v>432</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="C4" s="47" t="s">
         <v>433</v>
       </c>
-      <c r="B4" s="47" t="s">
-        <v>436</v>
-      </c>
-      <c r="C4" s="47" t="s">
+      <c r="D4" s="47" t="s">
         <v>434</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -3392,10 +3422,10 @@
     <hyperlink ref="B2" r:id="rId5"/>
     <hyperlink ref="J2" r:id="rId6"/>
     <hyperlink ref="I2" r:id="rId7"/>
-    <hyperlink ref="C2" r:id="rId8"/>
-    <hyperlink ref="D2" r:id="rId9"/>
-    <hyperlink ref="K2" r:id="rId10"/>
-    <hyperlink ref="L2" r:id="rId11"/>
+    <hyperlink ref="D2" r:id="rId8"/>
+    <hyperlink ref="K2" r:id="rId9"/>
+    <hyperlink ref="L2" r:id="rId10"/>
+    <hyperlink ref="C3" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3761,12 +3791,217 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="56" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>423</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>424</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>495</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>459</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="56" t="s">
+        <v>425</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>399</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>496</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="55" t="s">
+        <v>497</v>
+      </c>
+      <c r="G2" s="55" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>426</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>428</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>432</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>433</v>
+      </c>
+      <c r="D4" s="47" t="s">
+        <v>434</v>
+      </c>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>500</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47" t="s">
+        <v>429</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>501</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="D6" s="47"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="52" t="s">
+        <v>502</v>
+      </c>
+      <c r="B7" s="55"/>
+      <c r="C7" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>503</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="52" t="s">
+        <v>504</v>
+      </c>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="55"/>
+      <c r="C10" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="s">
+        <v>505</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="D3" r:id="rId5"/>
+    <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="D4" r:id="rId7"/>
+    <hyperlink ref="B4" r:id="rId8"/>
+    <hyperlink ref="C7" r:id="rId9"/>
+    <hyperlink ref="C8" r:id="rId10"/>
+    <hyperlink ref="C10" r:id="rId11"/>
+    <hyperlink ref="B6" r:id="rId12"/>
+    <hyperlink ref="C6" r:id="rId13"/>
+    <hyperlink ref="C5" r:id="rId14"/>
+    <hyperlink ref="B11" r:id="rId15"/>
+    <hyperlink ref="C11" r:id="rId16"/>
+    <hyperlink ref="D11" r:id="rId17"/>
+    <hyperlink ref="C2" r:id="rId18"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5453,7 +5688,7 @@
         <v>36</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -5466,63 +5701,63 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="54" t="s">
+        <v>443</v>
+      </c>
+      <c r="C24" s="43" t="s">
         <v>444</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="54" t="s">
+        <v>445</v>
+      </c>
+      <c r="C25" s="43" t="s">
         <v>446</v>
-      </c>
-      <c r="C25" s="43" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="C26" t="s">
         <v>448</v>
-      </c>
-      <c r="C26" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="54" t="s">
+        <v>449</v>
+      </c>
+      <c r="C27" t="s">
         <v>450</v>
-      </c>
-      <c r="C27" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="54" t="s">
+        <v>451</v>
+      </c>
+      <c r="C28" t="s">
         <v>452</v>
-      </c>
-      <c r="C28" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
+        <v>453</v>
+      </c>
+      <c r="C29" s="43" t="s">
         <v>454</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="54" t="s">
+        <v>455</v>
+      </c>
+      <c r="C30" t="s">
         <v>456</v>
-      </c>
-      <c r="C30" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C31" s="43" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Update testData, Update LoginData Sheet, copy user from R2_SmokeTest
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="506">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1611,9 +1611,6 @@
     <t>admin.user02@gmail.com</t>
   </si>
   <si>
-    <t>auditor.user02gmail.com</t>
-  </si>
-  <si>
     <t>client.user02@gmail.com</t>
   </si>
   <si>
@@ -1841,9 +1838,6 @@
   </si>
   <si>
     <t>Auditor Lead</t>
-  </si>
-  <si>
-    <t>client.user01@gmail.com</t>
   </si>
   <si>
     <t>TESTPASSWORD</t>
@@ -2210,9 +2204,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2220,6 +2211,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2903,7 +2897,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>32</v>
@@ -2923,7 +2917,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -2998,7 +2992,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>33</v>
@@ -3029,7 +3023,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B4" s="49" t="s">
         <v>399</v>
@@ -3037,7 +3031,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B5" s="49" t="s">
         <v>421</v>
@@ -3045,10 +3039,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
+        <v>436</v>
+      </c>
+      <c r="B6" s="47" t="s">
         <v>437</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -3102,10 +3096,10 @@
         <v>25</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3113,22 +3107,22 @@
         <v>425</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C2" s="47" t="s">
+        <v>433</v>
+      </c>
+      <c r="D2" s="47" t="s">
         <v>434</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>435</v>
       </c>
       <c r="E2" s="47" t="s">
         <v>421</v>
       </c>
       <c r="F2" s="53" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G2" s="53" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>
@@ -3159,8 +3153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3202,64 +3196,64 @@
         <v>424</v>
       </c>
       <c r="E1" s="50" t="s">
+        <v>483</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>472</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>468</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>467</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>460</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>470</v>
+      </c>
+      <c r="K1" s="56" t="s">
+        <v>471</v>
+      </c>
+      <c r="L1" s="56" t="s">
+        <v>459</v>
+      </c>
+      <c r="M1" s="52" t="s">
+        <v>474</v>
+      </c>
+      <c r="N1" s="52" t="s">
+        <v>473</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>462</v>
+      </c>
+      <c r="P1" s="52" t="s">
         <v>484</v>
       </c>
-      <c r="F1" s="52" t="s">
-        <v>473</v>
-      </c>
-      <c r="G1" s="52" t="s">
-        <v>469</v>
-      </c>
-      <c r="H1" s="52" t="s">
-        <v>468</v>
-      </c>
-      <c r="I1" s="52" t="s">
-        <v>461</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>471</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>472</v>
-      </c>
-      <c r="L1" s="56" t="s">
-        <v>460</v>
-      </c>
-      <c r="M1" s="52" t="s">
+      <c r="Q1" s="52" t="s">
+        <v>486</v>
+      </c>
+      <c r="R1" s="52" t="s">
+        <v>487</v>
+      </c>
+      <c r="S1" s="52" t="s">
+        <v>465</v>
+      </c>
+      <c r="T1" s="52" t="s">
         <v>475</v>
       </c>
-      <c r="N1" s="52" t="s">
-        <v>474</v>
-      </c>
-      <c r="O1" s="52" t="s">
-        <v>463</v>
-      </c>
-      <c r="P1" s="52" t="s">
-        <v>485</v>
-      </c>
-      <c r="Q1" s="52" t="s">
-        <v>487</v>
-      </c>
-      <c r="R1" s="52" t="s">
-        <v>488</v>
-      </c>
-      <c r="S1" s="52" t="s">
-        <v>466</v>
-      </c>
-      <c r="T1" s="52" t="s">
+      <c r="U1" s="52" t="s">
         <v>476</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="V1" s="52" t="s">
         <v>477</v>
       </c>
-      <c r="V1" s="52" t="s">
+      <c r="W1" s="52" t="s">
         <v>478</v>
       </c>
-      <c r="W1" s="52" t="s">
-        <v>479</v>
-      </c>
       <c r="X1" s="52" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -3267,19 +3261,19 @@
         <v>425</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>488</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>489</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>490</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="57" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G2" s="57" t="s">
         <v>421</v>
@@ -3303,37 +3297,37 @@
         <v>421</v>
       </c>
       <c r="N2" s="58" t="s">
+        <v>491</v>
+      </c>
+      <c r="O2" s="55" t="s">
+        <v>463</v>
+      </c>
+      <c r="P2" s="55" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>466</v>
+      </c>
+      <c r="R2" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="S2" t="s">
         <v>492</v>
       </c>
-      <c r="O2" s="55" t="s">
-        <v>464</v>
-      </c>
-      <c r="P2" s="55" t="s">
-        <v>462</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>467</v>
-      </c>
-      <c r="R2" s="55" t="s">
-        <v>486</v>
-      </c>
-      <c r="S2" t="s">
-        <v>493</v>
-      </c>
       <c r="T2" t="s">
+        <v>479</v>
+      </c>
+      <c r="U2" t="s">
         <v>480</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>481</v>
       </c>
-      <c r="V2" t="s">
-        <v>482</v>
-      </c>
       <c r="W2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="X2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -3344,49 +3338,49 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>499</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>428</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>429</v>
       </c>
       <c r="E3" s="7"/>
       <c r="P3" s="55" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="Q3" s="55" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R3" s="55" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="S3" s="55" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="T3" s="55" t="s">
+        <v>479</v>
+      </c>
+      <c r="U3" s="55" t="s">
         <v>480</v>
       </c>
-      <c r="U3" s="55" t="s">
+      <c r="V3" s="55" t="s">
         <v>481</v>
       </c>
-      <c r="V3" s="55" t="s">
+      <c r="W3" s="55" t="s">
         <v>482</v>
-      </c>
-      <c r="W3" s="55" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
+        <v>432</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="C4" s="47" t="s">
         <v>433</v>
       </c>
-      <c r="B4" s="47" t="s">
-        <v>436</v>
-      </c>
-      <c r="C4" s="47" t="s">
+      <c r="D4" s="47" t="s">
         <v>434</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -3429,9 +3423,10 @@
     <hyperlink ref="D2" r:id="rId9"/>
     <hyperlink ref="K2" r:id="rId10"/>
     <hyperlink ref="L2" r:id="rId11"/>
+    <hyperlink ref="C3" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -3797,7 +3792,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3805,7 +3800,7 @@
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
@@ -3823,13 +3818,13 @@
         <v>424</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" s="56" t="s">
+        <v>459</v>
+      </c>
+      <c r="G1" s="56" t="s">
         <v>460</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3837,20 +3832,20 @@
         <v>425</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>399</v>
+        <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>399</v>
+        <v>488</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="55" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3861,10 +3856,10 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="55"/>
@@ -3872,16 +3867,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
+        <v>432</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>435</v>
+      </c>
+      <c r="C4" s="47" t="s">
         <v>433</v>
       </c>
-      <c r="B4" s="47" t="s">
-        <v>436</v>
-      </c>
-      <c r="C4" s="47" t="s">
+      <c r="D4" s="47" t="s">
         <v>434</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>435</v>
       </c>
       <c r="E4" s="55"/>
       <c r="F4" s="55"/>
@@ -3889,11 +3884,11 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="47" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D5" s="47"/>
       <c r="E5" s="55"/>
@@ -3902,7 +3897,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B6" s="47" t="s">
         <v>421</v>
@@ -3917,7 +3912,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="47" t="s">
@@ -3930,7 +3925,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="47" t="s">
@@ -3943,7 +3938,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B9" s="55"/>
       <c r="C9" s="55" t="s">
@@ -3969,16 +3964,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
@@ -3986,24 +3981,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="D3" r:id="rId5"/>
-    <hyperlink ref="C4" r:id="rId6"/>
-    <hyperlink ref="D4" r:id="rId7"/>
-    <hyperlink ref="B4" r:id="rId8"/>
-    <hyperlink ref="C7" r:id="rId9"/>
-    <hyperlink ref="C8" r:id="rId10"/>
-    <hyperlink ref="C10" r:id="rId11"/>
-    <hyperlink ref="B6" r:id="rId12"/>
-    <hyperlink ref="C6" r:id="rId13"/>
-    <hyperlink ref="C5" r:id="rId14"/>
-    <hyperlink ref="B11" r:id="rId15"/>
-    <hyperlink ref="C11" r:id="rId16"/>
-    <hyperlink ref="D11" r:id="rId17"/>
-    <hyperlink ref="C2" r:id="rId18"/>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="C10" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="C11" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="B2" r:id="rId10"/>
+    <hyperlink ref="C2" r:id="rId11"/>
+    <hyperlink ref="C3" r:id="rId12"/>
+    <hyperlink ref="D2" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4105,22 +4095,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="63" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="60"/>
-      <c r="T1" s="63" t="s">
+      <c r="S1" s="63"/>
+      <c r="T1" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="61"/>
-      <c r="V1" s="60" t="s">
+      <c r="U1" s="60"/>
+      <c r="V1" s="63" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="61" t="s">
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="63"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="60" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -4172,8 +4162,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4229,17 +4219,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4250,6 +4229,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5081,7 +5071,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5691,7 +5681,7 @@
         <v>36</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>430</v>
+        <v>499</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -5704,63 +5694,63 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="54" t="s">
+        <v>443</v>
+      </c>
+      <c r="C24" s="43" t="s">
         <v>444</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="54" t="s">
+        <v>445</v>
+      </c>
+      <c r="C25" s="43" t="s">
         <v>446</v>
-      </c>
-      <c r="C25" s="43" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="54" t="s">
+        <v>447</v>
+      </c>
+      <c r="C26" t="s">
         <v>448</v>
-      </c>
-      <c r="C26" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="54" t="s">
+        <v>449</v>
+      </c>
+      <c r="C27" t="s">
         <v>450</v>
-      </c>
-      <c r="C27" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="54" t="s">
+        <v>451</v>
+      </c>
+      <c r="C28" t="s">
         <v>452</v>
-      </c>
-      <c r="C28" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
+        <v>453</v>
+      </c>
+      <c r="C29" s="43" t="s">
         <v>454</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="54" t="s">
+        <v>455</v>
+      </c>
+      <c r="C30" t="s">
         <v>456</v>
-      </c>
-      <c r="C30" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C31" s="43" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Vienpham re-factor PLAT 2301
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="ClientTestData" sheetId="12" r:id="rId12"/>
     <sheet name="EmailTemplateData" sheetId="13" r:id="rId13"/>
     <sheet name="SmokeTest" sheetId="14" r:id="rId14"/>
+    <sheet name="TodoTestPage" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="515">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1865,6 +1866,33 @@
   </si>
   <si>
     <t>Valid Userminh</t>
+  </si>
+  <si>
+    <t>Vien_Engagement</t>
+  </si>
+  <si>
+    <t>Todo Name  01</t>
+  </si>
+  <si>
+    <t>Number Value</t>
+  </si>
+  <si>
+    <t>Todo 01</t>
+  </si>
+  <si>
+    <t>1212122121</t>
+  </si>
+  <si>
+    <t>Special Chars</t>
+  </si>
+  <si>
+    <t>#$%^&amp;*</t>
+  </si>
+  <si>
+    <t>Category Name</t>
+  </si>
+  <si>
+    <t>Cate_Vien_01</t>
   </si>
 </sst>
 </file>
@@ -3153,8 +3181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D2:D4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3264,7 +3292,7 @@
         <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>488</v>
+        <v>429</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>489</v>
@@ -3303,7 +3331,7 @@
         <v>463</v>
       </c>
       <c r="P2" s="55" t="s">
-        <v>461</v>
+        <v>506</v>
       </c>
       <c r="Q2" t="s">
         <v>466</v>
@@ -3419,14 +3447,76 @@
     <hyperlink ref="B2" r:id="rId5"/>
     <hyperlink ref="J2" r:id="rId6"/>
     <hyperlink ref="I2" r:id="rId7"/>
-    <hyperlink ref="C2" r:id="rId8"/>
-    <hyperlink ref="D2" r:id="rId9"/>
-    <hyperlink ref="K2" r:id="rId10"/>
-    <hyperlink ref="L2" r:id="rId11"/>
-    <hyperlink ref="C3" r:id="rId12"/>
+    <hyperlink ref="D2" r:id="rId8"/>
+    <hyperlink ref="K2" r:id="rId9"/>
+    <hyperlink ref="L2" r:id="rId10"/>
+    <hyperlink ref="C3" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="55" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>484</v>
+      </c>
+      <c r="D1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="55" t="s">
+        <v>508</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3791,8 +3881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3991,9 +4081,9 @@
     <hyperlink ref="C11" r:id="rId8"/>
     <hyperlink ref="D11" r:id="rId9"/>
     <hyperlink ref="B2" r:id="rId10"/>
-    <hyperlink ref="C2" r:id="rId11"/>
-    <hyperlink ref="C3" r:id="rId12"/>
-    <hyperlink ref="D2" r:id="rId13"/>
+    <hyperlink ref="C3" r:id="rId11"/>
+    <hyperlink ref="D2" r:id="rId12"/>
+    <hyperlink ref="C2" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change excel for ClientTest #1
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="508">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1843,9 +1843,6 @@
     <t>TESTPASSWORD</t>
   </si>
   <si>
-    <t>Testpassword1!</t>
-  </si>
-  <si>
     <t>auditor.user02@gmail.com</t>
   </si>
   <si>
@@ -1865,6 +1862,15 @@
   </si>
   <si>
     <t>Valid Userminh</t>
+  </si>
+  <si>
+    <t>Engagement Huy</t>
+  </si>
+  <si>
+    <t>Invalid User</t>
+  </si>
+  <si>
+    <t>abc.xyz</t>
   </si>
 </sst>
 </file>
@@ -2077,7 +2083,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2204,6 +2210,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2211,9 +2220,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2228,6 +2234,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3338,7 +3346,7 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>428</v>
@@ -3789,10 +3797,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3804,9 +3812,26 @@
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="56" t="s">
         <v>422</v>
@@ -3820,14 +3845,65 @@
       <c r="E1" s="56" t="s">
         <v>496</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="52" t="s">
+        <v>472</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>468</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>467</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>460</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>470</v>
+      </c>
+      <c r="K1" s="56" t="s">
+        <v>471</v>
+      </c>
+      <c r="L1" s="56" t="s">
         <v>459</v>
       </c>
-      <c r="G1" s="56" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M1" s="52" t="s">
+        <v>474</v>
+      </c>
+      <c r="N1" s="52" t="s">
+        <v>473</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>462</v>
+      </c>
+      <c r="P1" s="52" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q1" s="52" t="s">
+        <v>486</v>
+      </c>
+      <c r="R1" s="52" t="s">
+        <v>487</v>
+      </c>
+      <c r="S1" s="52" t="s">
+        <v>465</v>
+      </c>
+      <c r="T1" s="52" t="s">
+        <v>475</v>
+      </c>
+      <c r="U1" s="52" t="s">
+        <v>476</v>
+      </c>
+      <c r="V1" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="W1" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="X1" s="52" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>425</v>
       </c>
@@ -3841,14 +3917,65 @@
         <v>489</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="F2" s="55" t="s">
+      <c r="F2" s="57" t="s">
+        <v>464</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="K2" s="57" t="s">
         <v>497</v>
       </c>
-      <c r="G2" s="55" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L2" s="57" t="s">
+        <v>497</v>
+      </c>
+      <c r="M2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="N2" s="58" t="s">
+        <v>491</v>
+      </c>
+      <c r="O2" s="55" t="s">
+        <v>463</v>
+      </c>
+      <c r="P2" s="55" t="s">
+        <v>505</v>
+      </c>
+      <c r="Q2" s="55" t="s">
+        <v>466</v>
+      </c>
+      <c r="R2" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="S2" s="55" t="s">
+        <v>492</v>
+      </c>
+      <c r="T2" s="55" t="s">
+        <v>479</v>
+      </c>
+      <c r="U2" s="55" t="s">
+        <v>480</v>
+      </c>
+      <c r="V2" s="55" t="s">
+        <v>481</v>
+      </c>
+      <c r="W2" s="55" t="s">
+        <v>490</v>
+      </c>
+      <c r="X2" s="55" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>426</v>
       </c>
@@ -3856,7 +3983,7 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>428</v>
@@ -3865,7 +3992,7 @@
       <c r="F3" s="55"/>
       <c r="G3" s="55"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>432</v>
       </c>
@@ -3882,9 +4009,9 @@
       <c r="F4" s="55"/>
       <c r="G4" s="55"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="47" t="s">
@@ -3895,9 +4022,9 @@
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B6" s="47" t="s">
         <v>421</v>
@@ -3910,9 +4037,9 @@
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="47" t="s">
@@ -3923,9 +4050,9 @@
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="47" t="s">
@@ -3936,9 +4063,9 @@
       <c r="F8" s="55"/>
       <c r="G8" s="55"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B9" s="55"/>
       <c r="C9" s="55" t="s">
@@ -3949,7 +4076,7 @@
       <c r="F9" s="55"/>
       <c r="G9" s="55"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>47</v>
       </c>
@@ -3962,9 +4089,9 @@
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B11" s="47" t="s">
         <v>438</v>
@@ -3978,6 +4105,16 @@
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
       <c r="G11" s="55"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="69" t="s">
+        <v>506</v>
+      </c>
+      <c r="B12" s="68"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68" t="s">
+        <v>507</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3994,6 +4131,14 @@
     <hyperlink ref="C2" r:id="rId11"/>
     <hyperlink ref="C3" r:id="rId12"/>
     <hyperlink ref="D2" r:id="rId13"/>
+    <hyperlink ref="G2" r:id="rId14"/>
+    <hyperlink ref="F2" r:id="rId15"/>
+    <hyperlink ref="M2" r:id="rId16"/>
+    <hyperlink ref="H2" r:id="rId17"/>
+    <hyperlink ref="J2" r:id="rId18"/>
+    <hyperlink ref="I2" r:id="rId19"/>
+    <hyperlink ref="K2" r:id="rId20" display="Changeit@123"/>
+    <hyperlink ref="L2" r:id="rId21" display="Changeit@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4095,22 +4240,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="60"/>
+      <c r="T1" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="63" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="60" t="s">
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -4162,8 +4307,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4219,6 +4364,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4229,17 +4385,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5681,7 +5826,7 @@
         <v>36</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Test Data for Login Data Sheet
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="9810" firstSheet="9" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="9810" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="509">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1837,9 +1837,6 @@
     <t>Auditor Lead</t>
   </si>
   <si>
-    <t>client.user01@gmail.com</t>
-  </si>
-  <si>
     <t>TESTPASSWORD</t>
   </si>
   <si>
@@ -1868,6 +1865,15 @@
   </si>
   <si>
     <t>auditor01.auvenir@gmail.com</t>
+  </si>
+  <si>
+    <t>auvenir.automation.ti@gmail@</t>
+  </si>
+  <si>
+    <t>auvenir.automation.ti@gmail</t>
+  </si>
+  <si>
+    <t>auvenir_devabc@titan.com.vn</t>
   </si>
 </sst>
 </file>
@@ -2207,6 +2213,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2214,9 +2223,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3156,8 +3162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3267,7 +3273,7 @@
         <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>488</v>
@@ -3341,7 +3347,7 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>428</v>
@@ -3793,8 +3799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3834,20 +3840,20 @@
         <v>425</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>399</v>
+        <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>399</v>
+        <v>505</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="55" t="s">
+        <v>496</v>
+      </c>
+      <c r="G2" s="55" t="s">
         <v>497</v>
-      </c>
-      <c r="G2" s="55" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3858,7 +3864,7 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>428</v>
@@ -3886,7 +3892,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="47" t="s">
@@ -3899,7 +3905,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B6" s="47" t="s">
         <v>421</v>
@@ -3914,11 +3920,11 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="47" t="s">
-        <v>33</v>
+        <v>507</v>
       </c>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
@@ -3927,11 +3933,11 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="47" t="s">
-        <v>34</v>
+        <v>506</v>
       </c>
       <c r="D8" s="55"/>
       <c r="E8" s="55"/>
@@ -3940,7 +3946,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B9" s="55"/>
       <c r="C9" s="55" t="s">
@@ -3957,7 +3963,7 @@
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="47" t="s">
-        <v>41</v>
+        <v>508</v>
       </c>
       <c r="D10" s="55"/>
       <c r="E10" s="55"/>
@@ -3966,7 +3972,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B11" s="47" t="s">
         <v>438</v>
@@ -3983,24 +3989,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId4"/>
-    <hyperlink ref="D3" r:id="rId5"/>
-    <hyperlink ref="C4" r:id="rId6"/>
-    <hyperlink ref="D4" r:id="rId7"/>
-    <hyperlink ref="B4" r:id="rId8"/>
-    <hyperlink ref="C7" r:id="rId9"/>
-    <hyperlink ref="C8" r:id="rId10"/>
-    <hyperlink ref="C10" r:id="rId11"/>
-    <hyperlink ref="B6" r:id="rId12"/>
-    <hyperlink ref="C6" r:id="rId13"/>
-    <hyperlink ref="C5" r:id="rId14"/>
-    <hyperlink ref="B11" r:id="rId15"/>
-    <hyperlink ref="C11" r:id="rId16"/>
-    <hyperlink ref="D11" r:id="rId17"/>
-    <hyperlink ref="C2" r:id="rId18"/>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="C10" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C5" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="C11" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="B2" r:id="rId10"/>
+    <hyperlink ref="D2" r:id="rId11"/>
+    <hyperlink ref="C3" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4102,22 +4102,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="60" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="62" t="s">
+      <c r="S1" s="60"/>
+      <c r="T1" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="63" t="s">
+      <c r="U1" s="61"/>
+      <c r="V1" s="60" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="60" t="s">
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="60"/>
+      <c r="AA1" s="61" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -4169,8 +4169,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4226,6 +4226,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4236,17 +4247,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5077,7 +5077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update TestData.xls, create new sheet AuditorToDoListTest.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14535" windowHeight="9810" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -21,8 +21,10 @@
     <sheet name="ClientTestData" sheetId="12" r:id="rId12"/>
     <sheet name="EmailTemplateData" sheetId="13" r:id="rId13"/>
     <sheet name="SmokeTest" sheetId="14" r:id="rId14"/>
+    <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="518">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1874,6 +1876,33 @@
   </si>
   <si>
     <t>auvenir_devabc@titan.com.vn</t>
+  </si>
+  <si>
+    <t>Category1</t>
+  </si>
+  <si>
+    <t>Category Name</t>
+  </si>
+  <si>
+    <t>ToDo 01</t>
+  </si>
+  <si>
+    <t>To Do Name</t>
+  </si>
+  <si>
+    <t>Company Auvenir</t>
+  </si>
+  <si>
+    <t>Company Name</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Engagement Type</t>
+  </si>
+  <si>
+    <t>Valid Data</t>
   </si>
 </sst>
 </file>
@@ -3438,6 +3467,73 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="55"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="56" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="56" t="s">
+        <v>484</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>516</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>514</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>512</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>510</v>
+      </c>
+      <c r="B6" s="58" t="s">
+        <v>509</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
@@ -3799,8 +3895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3808,7 +3904,7 @@
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Vienpham re-factor smoketestt as aTan's suggestions.
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -21,10 +21,9 @@
     <sheet name="ClientTestData" sheetId="12" r:id="rId12"/>
     <sheet name="EmailTemplateData" sheetId="13" r:id="rId13"/>
     <sheet name="SmokeTest" sheetId="14" r:id="rId14"/>
-    <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId15"/>
+    <sheet name="TodoTestPage" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="523">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1815,6 +1814,9 @@
     <t>Path of Download Location</t>
   </si>
   <si>
+    <t>auditor01.auvenir@gmail.com</t>
+  </si>
+  <si>
     <t>client03.auvenir@gmail.com</t>
   </si>
   <si>
@@ -1866,43 +1868,55 @@
     <t>Valid Userminh</t>
   </si>
   <si>
-    <t>auditor01.auvenir@gmail.com</t>
-  </si>
-  <si>
-    <t>auvenir.automation.ti@gmail@</t>
-  </si>
-  <si>
-    <t>auvenir.automation.ti@gmail</t>
-  </si>
-  <si>
-    <t>auvenir_devabc@titan.com.vn</t>
-  </si>
-  <si>
-    <t>Category1</t>
-  </si>
-  <si>
-    <t>Category Name</t>
-  </si>
-  <si>
-    <t>ToDo 01</t>
-  </si>
-  <si>
-    <t>To Do Name</t>
-  </si>
-  <si>
-    <t>Company Auvenir</t>
-  </si>
-  <si>
-    <t>Company Name</t>
-  </si>
-  <si>
-    <t>Review</t>
-  </si>
-  <si>
-    <t>Engagement Type</t>
-  </si>
-  <si>
-    <t>Valid Data</t>
+    <t>Vien_Engagement</t>
+  </si>
+  <si>
+    <t>Todo Name  01</t>
+  </si>
+  <si>
+    <t>Number Value</t>
+  </si>
+  <si>
+    <t>Todo 01</t>
+  </si>
+  <si>
+    <t>1212122121</t>
+  </si>
+  <si>
+    <t>Special Chars</t>
+  </si>
+  <si>
+    <t>#$%^&amp;*</t>
+  </si>
+  <si>
+    <t>Cate_Vien_01</t>
+  </si>
+  <si>
+    <t>Category Name 01</t>
+  </si>
+  <si>
+    <t>Category Name 02</t>
+  </si>
+  <si>
+    <t>Cate_Vien_02</t>
+  </si>
+  <si>
+    <t>DeadLine Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>07/30/2017</t>
+  </si>
+  <si>
+    <t>07/29/2017</t>
+  </si>
+  <si>
+    <t>06/29/2017</t>
   </si>
 </sst>
 </file>
@@ -1995,7 +2009,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -2110,12 +2124,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2242,9 +2265,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2252,6 +2272,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2266,6 +2289,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3192,7 +3217,7 @@
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3291,7 +3316,7 @@
         <v>478</v>
       </c>
       <c r="X1" s="52" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -3302,10 +3327,10 @@
         <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>505</v>
+        <v>429</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>1</v>
@@ -3335,13 +3360,13 @@
         <v>421</v>
       </c>
       <c r="N2" s="58" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="O2" s="55" t="s">
         <v>463</v>
       </c>
       <c r="P2" s="55" t="s">
-        <v>461</v>
+        <v>506</v>
       </c>
       <c r="Q2" t="s">
         <v>466</v>
@@ -3350,7 +3375,7 @@
         <v>485</v>
       </c>
       <c r="S2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="T2" t="s">
         <v>479</v>
@@ -3362,10 +3387,10 @@
         <v>481</v>
       </c>
       <c r="W2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="X2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
@@ -3376,7 +3401,7 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>428</v>
@@ -3392,7 +3417,7 @@
         <v>485</v>
       </c>
       <c r="S3" s="55" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="T3" s="55" t="s">
         <v>479</v>
@@ -3461,72 +3486,98 @@
     <hyperlink ref="K2" r:id="rId9"/>
     <hyperlink ref="L2" r:id="rId10"/>
     <hyperlink ref="C3" r:id="rId11"/>
+    <hyperlink ref="C2" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" style="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="55"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="56" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>484</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>514</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>515</v>
+      </c>
+      <c r="F1" s="68" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G1" s="68" t="s">
+        <v>518</v>
+      </c>
+      <c r="H1" s="68" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
-        <v>484</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E2" t="s">
+        <v>516</v>
+      </c>
+      <c r="F2" s="69" t="s">
+        <v>520</v>
+      </c>
+      <c r="G2" s="43" t="s">
+        <v>521</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>516</v>
-      </c>
-      <c r="B3" s="55" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>514</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
+        <v>511</v>
+      </c>
+      <c r="B4" t="s">
         <v>512</v>
       </c>
-      <c r="B5" s="58" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
-        <v>510</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>509</v>
-      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="55"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3896,7 +3947,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3922,7 +3973,7 @@
         <v>424</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="F1" s="56" t="s">
         <v>459</v>
@@ -3939,17 +3990,17 @@
         <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>505</v>
+        <v>488</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E2" s="7"/>
       <c r="F2" s="55" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="G2" s="55" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3960,7 +4011,7 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>428</v>
@@ -3988,7 +4039,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="47" t="s">
@@ -4001,7 +4052,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B6" s="47" t="s">
         <v>421</v>
@@ -4016,11 +4067,11 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="47" t="s">
-        <v>507</v>
+        <v>33</v>
       </c>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
@@ -4029,11 +4080,11 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="47" t="s">
-        <v>506</v>
+        <v>34</v>
       </c>
       <c r="D8" s="55"/>
       <c r="E8" s="55"/>
@@ -4042,7 +4093,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B9" s="55"/>
       <c r="C9" s="55" t="s">
@@ -4059,7 +4110,7 @@
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="47" t="s">
-        <v>508</v>
+        <v>41</v>
       </c>
       <c r="D10" s="55"/>
       <c r="E10" s="55"/>
@@ -4068,7 +4119,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B11" s="47" t="s">
         <v>438</v>
@@ -4095,8 +4146,9 @@
     <hyperlink ref="C11" r:id="rId8"/>
     <hyperlink ref="D11" r:id="rId9"/>
     <hyperlink ref="B2" r:id="rId10"/>
-    <hyperlink ref="D2" r:id="rId11"/>
-    <hyperlink ref="C3" r:id="rId12"/>
+    <hyperlink ref="C3" r:id="rId11"/>
+    <hyperlink ref="D2" r:id="rId12"/>
+    <hyperlink ref="C2" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4198,22 +4250,22 @@
       <c r="Q1" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="63" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="60"/>
-      <c r="T1" s="63" t="s">
+      <c r="S1" s="63"/>
+      <c r="T1" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="61"/>
-      <c r="V1" s="60" t="s">
+      <c r="U1" s="60"/>
+      <c r="V1" s="63" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="61" t="s">
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="63"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="60" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="64" t="s">
@@ -4265,8 +4317,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4322,17 +4374,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4343,6 +4384,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5173,8 +5225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5784,7 +5836,7 @@
         <v>36</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>429</v>
+        <v>499</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Vienpham add TestData: TodoPageTEst
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="EmailTemplateData" sheetId="13" r:id="rId13"/>
     <sheet name="SmokeTest" sheetId="14" r:id="rId14"/>
     <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId15"/>
+    <sheet name="TodoTestPage" sheetId="16" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="531">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1904,6 +1905,45 @@
   <si>
     <t>Valid Data</t>
   </si>
+  <si>
+    <t>Todo Name  01</t>
+  </si>
+  <si>
+    <t>Category Name 01</t>
+  </si>
+  <si>
+    <t>Category Name 02</t>
+  </si>
+  <si>
+    <t>DeadLine Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Todo 01</t>
+  </si>
+  <si>
+    <t>Vien_Engagement</t>
+  </si>
+  <si>
+    <t>Cate_Vien_01</t>
+  </si>
+  <si>
+    <t>Cate_Vien_02</t>
+  </si>
+  <si>
+    <t>Number Value</t>
+  </si>
+  <si>
+    <t>Special Chars</t>
+  </si>
+  <si>
+    <t>#$%^&amp;*</t>
+  </si>
 </sst>
 </file>
 
@@ -2115,7 +2155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2266,6 +2306,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3191,8 +3232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3471,8 +3512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3531,6 +3572,94 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="56" t="s">
+        <v>518</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>484</v>
+      </c>
+      <c r="D1" s="56" t="s">
+        <v>519</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>520</v>
+      </c>
+      <c r="F1" s="56" t="s">
+        <v>521</v>
+      </c>
+      <c r="G1" s="56" t="s">
+        <v>522</v>
+      </c>
+      <c r="H1" s="56" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>524</v>
+      </c>
+      <c r="C2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D2" t="s">
+        <v>526</v>
+      </c>
+      <c r="E2" t="s">
+        <v>527</v>
+      </c>
+      <c r="F2" s="68">
+        <v>42946</v>
+      </c>
+      <c r="G2" s="68">
+        <v>42945</v>
+      </c>
+      <c r="H2" s="68">
+        <v>42915</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>528</v>
+      </c>
+      <c r="B3">
+        <v>1212122121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>529</v>
+      </c>
+      <c r="B4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
R2.1 New #5 done
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="12" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -30,12 +30,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="0" calcOnSave="0"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="534">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1837,15 +1837,9 @@
     <t>TXT_ATTACHMENT.docx</t>
   </si>
   <si>
-    <t>Auditor Lead</t>
-  </si>
-  <si>
     <t>TESTPASSWORD</t>
   </si>
   <si>
-    <t>Testpassword1!</t>
-  </si>
-  <si>
     <t>auditor.user02@gmail.com</t>
   </si>
   <si>
@@ -1943,6 +1937,21 @@
   </si>
   <si>
     <t>#$%^&amp;*</t>
+  </si>
+  <si>
+    <t>auvenirauditor@gmail.com</t>
+  </si>
+  <si>
+    <t>auvenirclient01@gmail.com</t>
+  </si>
+  <si>
+    <t>Engagement Huy</t>
+  </si>
+  <si>
+    <t>Invalid User</t>
+  </si>
+  <si>
+    <t>abc.xyz</t>
   </si>
 </sst>
 </file>
@@ -2155,7 +2164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2279,6 +2288,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2306,7 +2318,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2962,11 +2973,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="70"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3057,11 +3068,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="70"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3232,8 +3243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3343,7 +3354,7 @@
         <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>488</v>
@@ -3417,7 +3428,7 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>428</v>
@@ -3526,7 +3537,7 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="56" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3539,34 +3550,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -3595,25 +3606,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="56" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C1" s="56" t="s">
         <v>484</v>
       </c>
       <c r="D1" s="56" t="s">
+        <v>517</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>518</v>
+      </c>
+      <c r="F1" s="56" t="s">
         <v>519</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="G1" s="56" t="s">
         <v>520</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="H1" s="56" t="s">
         <v>521</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>522</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3621,30 +3632,30 @@
         <v>49</v>
       </c>
       <c r="B2" t="s">
+        <v>522</v>
+      </c>
+      <c r="C2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D2" t="s">
         <v>524</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>525</v>
       </c>
-      <c r="D2" t="s">
-        <v>526</v>
-      </c>
-      <c r="E2" t="s">
-        <v>527</v>
-      </c>
-      <c r="F2" s="68">
+      <c r="F2" s="59">
         <v>42946</v>
       </c>
-      <c r="G2" s="68">
+      <c r="G2" s="59">
         <v>42945</v>
       </c>
-      <c r="H2" s="68">
+      <c r="H2" s="59">
         <v>42915</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B3">
         <v>1212122121</v>
@@ -3652,10 +3663,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -4022,24 +4033,39 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="A8:P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24" customWidth="1"/>
+    <col min="15" max="15" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.42578125" customWidth="1"/>
+    <col min="19" max="19" width="28" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" customWidth="1"/>
+    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="56" t="s">
         <v>422</v>
@@ -4051,16 +4077,67 @@
         <v>424</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>495</v>
-      </c>
-      <c r="F1" s="56" t="s">
+        <v>483</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>472</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>468</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>467</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>460</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>470</v>
+      </c>
+      <c r="K1" s="56" t="s">
+        <v>471</v>
+      </c>
+      <c r="L1" s="56" t="s">
         <v>459</v>
       </c>
-      <c r="G1" s="56" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M1" s="52" t="s">
+        <v>474</v>
+      </c>
+      <c r="N1" s="52" t="s">
+        <v>473</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>462</v>
+      </c>
+      <c r="P1" s="52" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q1" s="52" t="s">
+        <v>486</v>
+      </c>
+      <c r="R1" s="52" t="s">
+        <v>487</v>
+      </c>
+      <c r="S1" s="52" t="s">
+        <v>465</v>
+      </c>
+      <c r="T1" s="52" t="s">
+        <v>475</v>
+      </c>
+      <c r="U1" s="52" t="s">
+        <v>476</v>
+      </c>
+      <c r="V1" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="W1" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="X1" s="52" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>425</v>
       </c>
@@ -4068,20 +4145,73 @@
         <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>505</v>
+        <v>529</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>488</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="55" t="s">
-        <v>496</v>
-      </c>
-      <c r="G2" s="55" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>464</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="K2" s="57" t="s">
+        <v>495</v>
+      </c>
+      <c r="L2" s="57" t="s">
+        <v>495</v>
+      </c>
+      <c r="M2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="N2" s="58" t="s">
+        <v>490</v>
+      </c>
+      <c r="O2" s="55" t="s">
+        <v>463</v>
+      </c>
+      <c r="P2" s="55" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q2" s="55" t="s">
+        <v>466</v>
+      </c>
+      <c r="R2" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="S2" s="55" t="s">
+        <v>491</v>
+      </c>
+      <c r="T2" s="55" t="s">
+        <v>479</v>
+      </c>
+      <c r="U2" s="55" t="s">
+        <v>480</v>
+      </c>
+      <c r="V2" s="55" t="s">
+        <v>481</v>
+      </c>
+      <c r="W2" s="55" t="s">
+        <v>489</v>
+      </c>
+      <c r="X2" s="55" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>426</v>
       </c>
@@ -4089,7 +4219,7 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>428</v>
@@ -4098,7 +4228,7 @@
       <c r="F3" s="55"/>
       <c r="G3" s="55"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>432</v>
       </c>
@@ -4115,9 +4245,9 @@
       <c r="F4" s="55"/>
       <c r="G4" s="55"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="47" t="s">
@@ -4128,9 +4258,9 @@
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B6" s="47" t="s">
         <v>421</v>
@@ -4143,35 +4273,35 @@
       <c r="F6" s="55"/>
       <c r="G6" s="55"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="47" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
       <c r="F7" s="55"/>
       <c r="G7" s="55"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="47" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D8" s="55"/>
       <c r="E8" s="55"/>
       <c r="F8" s="55"/>
       <c r="G8" s="55"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B9" s="55"/>
       <c r="C9" s="55" t="s">
@@ -4182,22 +4312,22 @@
       <c r="F9" s="55"/>
       <c r="G9" s="55"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="47" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D10" s="55"/>
       <c r="E10" s="55"/>
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B11" s="47" t="s">
         <v>438</v>
@@ -4211,6 +4341,16 @@
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
       <c r="G11" s="55"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="61" t="s">
+        <v>532</v>
+      </c>
+      <c r="B12" s="60"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="60" t="s">
+        <v>533</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4223,11 +4363,21 @@
     <hyperlink ref="B11" r:id="rId7"/>
     <hyperlink ref="C11" r:id="rId8"/>
     <hyperlink ref="D11" r:id="rId9"/>
-    <hyperlink ref="B2" r:id="rId10"/>
-    <hyperlink ref="D2" r:id="rId11"/>
-    <hyperlink ref="C3" r:id="rId12"/>
+    <hyperlink ref="C3" r:id="rId10"/>
+    <hyperlink ref="G2" r:id="rId11"/>
+    <hyperlink ref="F2" r:id="rId12"/>
+    <hyperlink ref="M2" r:id="rId13"/>
+    <hyperlink ref="H2" r:id="rId14"/>
+    <hyperlink ref="J2" r:id="rId15"/>
+    <hyperlink ref="I2" r:id="rId16"/>
+    <hyperlink ref="C2" r:id="rId17"/>
+    <hyperlink ref="D2" r:id="rId18"/>
+    <hyperlink ref="K2" r:id="rId19" display="Changeit@123"/>
+    <hyperlink ref="L2" r:id="rId20" display="Changeit@123"/>
+    <hyperlink ref="B2" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -4279,94 +4429,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="62" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="62" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="59" t="s">
+      <c r="N1" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="59" t="s">
+      <c r="O1" s="62" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="59" t="s">
+      <c r="P1" s="62" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="63" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="60"/>
-      <c r="T1" s="63" t="s">
+      <c r="S1" s="63"/>
+      <c r="T1" s="66" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="61"/>
-      <c r="V1" s="60" t="s">
+      <c r="U1" s="64"/>
+      <c r="V1" s="63" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="61" t="s">
+      <c r="W1" s="63"/>
+      <c r="X1" s="63"/>
+      <c r="Y1" s="63"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="64" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="64" t="s">
+      <c r="AB1" s="67" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -4394,8 +4544,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
+      <c r="AA2" s="65"/>
+      <c r="AB2" s="65"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">

</xml_diff>

<commit_message>
Minhnh updated AuditorEngagementReviewTest, AuditorSettingsTest, AuditorTest
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="534">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2164,7 +2164,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2294,9 +2294,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2304,6 +2301,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2317,6 +2317,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2952,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2973,11 +2976,15 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="70"/>
+      <c r="D1" s="71" t="s">
+        <v>499</v>
+      </c>
+      <c r="E1" s="71" t="s">
+        <v>500</v>
+      </c>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3027,9 +3034,6 @@
       <c r="F4" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:E1"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2" display="12345678x@X"/>
@@ -3040,7 +3044,7 @@
     <hyperlink ref="F2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -4035,7 +4039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P9" sqref="A8:P9"/>
     </sheetView>
   </sheetViews>
@@ -4477,22 +4481,22 @@
       <c r="Q1" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="63"/>
-      <c r="T1" s="66" t="s">
+      <c r="S1" s="66"/>
+      <c r="T1" s="65" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="64"/>
-      <c r="V1" s="63" t="s">
+      <c r="U1" s="63"/>
+      <c r="V1" s="66" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="64" t="s">
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="63" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="67" t="s">
@@ -4544,8 +4548,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
+      <c r="AA2" s="64"/>
+      <c r="AB2" s="64"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4601,17 +4605,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4622,6 +4615,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Vienpham add @Test: VerifyCountry_State,memberID
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="12" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -30,12 +30,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="0" calcOnSave="0"/>
+  <calcPr calcId="152511" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="538">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1837,15 +1837,9 @@
     <t>TXT_ATTACHMENT.docx</t>
   </si>
   <si>
-    <t>Auditor Lead</t>
-  </si>
-  <si>
     <t>TESTPASSWORD</t>
   </si>
   <si>
-    <t>Testpassword1!</t>
-  </si>
-  <si>
     <t>auditor.user02@gmail.com</t>
   </si>
   <si>
@@ -1943,6 +1937,33 @@
   </si>
   <si>
     <t>#$%^&amp;*</t>
+  </si>
+  <si>
+    <t>auvenirauditor@gmail.com</t>
+  </si>
+  <si>
+    <t>auvenirclient01@gmail.com</t>
+  </si>
+  <si>
+    <t>Engagement Huy</t>
+  </si>
+  <si>
+    <t>Invalid User</t>
+  </si>
+  <si>
+    <t>abc.xyz</t>
+  </si>
+  <si>
+    <t>1212122121</t>
+  </si>
+  <si>
+    <t>07/30/2017</t>
+  </si>
+  <si>
+    <t>07/29/2017</t>
+  </si>
+  <si>
+    <t>06/29/2017</t>
   </si>
 </sst>
 </file>
@@ -2155,7 +2176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2279,6 +2300,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2306,7 +2333,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2942,7 +2968,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2962,11 +2988,15 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
+      <c r="D1" s="61" t="s">
+        <v>499</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>500</v>
+      </c>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3016,9 +3046,6 @@
       <c r="F4" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:E1"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2" display="12345678x@X"/>
@@ -3029,7 +3056,7 @@
     <hyperlink ref="F2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -3057,11 +3084,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="67"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3232,8 +3259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3343,7 +3370,7 @@
         <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>488</v>
@@ -3417,7 +3444,7 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>428</v>
@@ -3526,7 +3553,7 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="56" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3539,34 +3566,34 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -3579,8 +3606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3590,30 +3617,30 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="56" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C1" s="56" t="s">
         <v>484</v>
       </c>
       <c r="D1" s="56" t="s">
+        <v>517</v>
+      </c>
+      <c r="E1" s="56" t="s">
+        <v>518</v>
+      </c>
+      <c r="F1" s="56" t="s">
         <v>519</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="G1" s="56" t="s">
         <v>520</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="H1" s="56" t="s">
         <v>521</v>
-      </c>
-      <c r="G1" s="56" t="s">
-        <v>522</v>
-      </c>
-      <c r="H1" s="56" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3621,41 +3648,41 @@
         <v>49</v>
       </c>
       <c r="B2" t="s">
+        <v>522</v>
+      </c>
+      <c r="C2" t="s">
+        <v>523</v>
+      </c>
+      <c r="D2" t="s">
         <v>524</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>525</v>
       </c>
-      <c r="D2" t="s">
-        <v>526</v>
-      </c>
-      <c r="E2" t="s">
-        <v>527</v>
-      </c>
-      <c r="F2" s="68">
-        <v>42946</v>
-      </c>
-      <c r="G2" s="68">
-        <v>42945</v>
-      </c>
-      <c r="H2" s="68">
-        <v>42915</v>
+      <c r="F2" s="62" t="s">
+        <v>535</v>
+      </c>
+      <c r="G2" s="62" t="s">
+        <v>536</v>
+      </c>
+      <c r="H2" s="62" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>528</v>
-      </c>
-      <c r="B3">
-        <v>1212122121</v>
+        <v>526</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>
@@ -4022,24 +4049,39 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24" customWidth="1"/>
+    <col min="15" max="15" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.42578125" customWidth="1"/>
+    <col min="19" max="19" width="28" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" customWidth="1"/>
+    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="56" t="s">
         <v>422</v>
@@ -4051,16 +4093,67 @@
         <v>424</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>495</v>
-      </c>
-      <c r="F1" s="56" t="s">
+        <v>483</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>472</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>468</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>467</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>460</v>
+      </c>
+      <c r="J1" s="56" t="s">
+        <v>470</v>
+      </c>
+      <c r="K1" s="56" t="s">
+        <v>471</v>
+      </c>
+      <c r="L1" s="56" t="s">
         <v>459</v>
       </c>
-      <c r="G1" s="56" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="M1" s="52" t="s">
+        <v>474</v>
+      </c>
+      <c r="N1" s="52" t="s">
+        <v>473</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>462</v>
+      </c>
+      <c r="P1" s="52" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q1" s="52" t="s">
+        <v>486</v>
+      </c>
+      <c r="R1" s="52" t="s">
+        <v>487</v>
+      </c>
+      <c r="S1" s="52" t="s">
+        <v>465</v>
+      </c>
+      <c r="T1" s="52" t="s">
+        <v>475</v>
+      </c>
+      <c r="U1" s="52" t="s">
+        <v>476</v>
+      </c>
+      <c r="V1" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="W1" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="X1" s="52" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>425</v>
       </c>
@@ -4068,20 +4161,73 @@
         <v>469</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>505</v>
+        <v>529</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>488</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="55" t="s">
-        <v>496</v>
-      </c>
-      <c r="G2" s="55" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>530</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>464</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>495</v>
+      </c>
+      <c r="K2" s="57" t="s">
+        <v>495</v>
+      </c>
+      <c r="L2" s="57" t="s">
+        <v>495</v>
+      </c>
+      <c r="M2" s="57" t="s">
+        <v>421</v>
+      </c>
+      <c r="N2" s="58" t="s">
+        <v>490</v>
+      </c>
+      <c r="O2" s="55" t="s">
+        <v>463</v>
+      </c>
+      <c r="P2" s="55" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q2" s="55" t="s">
+        <v>466</v>
+      </c>
+      <c r="R2" s="55" t="s">
+        <v>485</v>
+      </c>
+      <c r="S2" s="55" t="s">
+        <v>491</v>
+      </c>
+      <c r="T2" s="55" t="s">
+        <v>479</v>
+      </c>
+      <c r="U2" s="55" t="s">
+        <v>480</v>
+      </c>
+      <c r="V2" s="55" t="s">
+        <v>481</v>
+      </c>
+      <c r="W2" s="55" t="s">
+        <v>489</v>
+      </c>
+      <c r="X2" s="55" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>426</v>
       </c>
@@ -4089,7 +4235,7 @@
         <v>427</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>428</v>
@@ -4098,7 +4244,7 @@
       <c r="F3" s="55"/>
       <c r="G3" s="55"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>432</v>
       </c>
@@ -4115,9 +4261,9 @@
       <c r="F4" s="55"/>
       <c r="G4" s="55"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="47" t="s">
@@ -4128,9 +4274,9 @@
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B6" s="47" t="s">
         <v>421</v>
@@ -4140,64 +4286,56 @@
       </c>
       <c r="D6" s="47"/>
       <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" s="52" t="s">
+        <v>500</v>
+      </c>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47" t="s">
+        <v>504</v>
+      </c>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="47" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
+      <c r="F7" s="52" t="s">
+        <v>501</v>
+      </c>
       <c r="G7" s="55"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
-        <v>502</v>
-      </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47" t="s">
-        <v>506</v>
-      </c>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
-        <v>503</v>
-      </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55" t="s">
+      <c r="H7" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="55"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="55" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="55"/>
       <c r="C10" s="47" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D10" s="55"/>
       <c r="E10" s="55"/>
       <c r="F10" s="55"/>
       <c r="G10" s="55"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="56" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="B11" s="47" t="s">
         <v>438</v>
@@ -4212,10 +4350,20 @@
       <c r="F11" s="55"/>
       <c r="G11" s="55"/>
     </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="60" t="s">
+        <v>532</v>
+      </c>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59" t="s">
+        <v>533</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
-    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="H6" r:id="rId2"/>
     <hyperlink ref="C10" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
@@ -4223,11 +4371,21 @@
     <hyperlink ref="B11" r:id="rId7"/>
     <hyperlink ref="C11" r:id="rId8"/>
     <hyperlink ref="D11" r:id="rId9"/>
-    <hyperlink ref="B2" r:id="rId10"/>
-    <hyperlink ref="D2" r:id="rId11"/>
-    <hyperlink ref="C3" r:id="rId12"/>
+    <hyperlink ref="C3" r:id="rId10"/>
+    <hyperlink ref="G2" r:id="rId11"/>
+    <hyperlink ref="F2" r:id="rId12"/>
+    <hyperlink ref="M2" r:id="rId13"/>
+    <hyperlink ref="H2" r:id="rId14"/>
+    <hyperlink ref="I2" r:id="rId15"/>
+    <hyperlink ref="C2" r:id="rId16"/>
+    <hyperlink ref="D2" r:id="rId17"/>
+    <hyperlink ref="K2" r:id="rId18" display="Changeit@123"/>
+    <hyperlink ref="L2" r:id="rId19" display="Changeit@123"/>
+    <hyperlink ref="B2" r:id="rId20"/>
+    <hyperlink ref="J2" r:id="rId21" display="Changeit@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -4279,94 +4437,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="63" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="C1" s="63" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="59" t="s">
+      <c r="E1" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="59" t="s">
+      <c r="F1" s="63" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="63" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="63" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="63" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="59" t="s">
+      <c r="L1" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="59" t="s">
+      <c r="M1" s="63" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="59" t="s">
+      <c r="N1" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="59" t="s">
+      <c r="O1" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="59" t="s">
+      <c r="P1" s="63" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="59" t="s">
+      <c r="Q1" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="60" t="s">
+      <c r="R1" s="64" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="60"/>
-      <c r="T1" s="63" t="s">
+      <c r="S1" s="64"/>
+      <c r="T1" s="67" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="61"/>
-      <c r="V1" s="60" t="s">
+      <c r="U1" s="65"/>
+      <c r="V1" s="64" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="60"/>
-      <c r="AA1" s="61" t="s">
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
+      <c r="AA1" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="64" t="s">
+      <c r="AB1" s="68" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -4394,8 +4552,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -5302,8 +5460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Vienpham 1. update Testdata: added Country row into AuditorSignupPage 2. add new strCountry into auditorsigupTEst
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="540">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1952,6 +1952,24 @@
   </si>
   <si>
     <t>abc.xyz</t>
+  </si>
+  <si>
+    <t>07/30/2017</t>
+  </si>
+  <si>
+    <t>07/29/2017</t>
+  </si>
+  <si>
+    <t>06/29/2017</t>
+  </si>
+  <si>
+    <t>1212122121</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Canada</t>
   </si>
 </sst>
 </file>
@@ -2288,12 +2306,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2976,13 +2994,13 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="61" t="s">
         <v>499</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="61" t="s">
         <v>500</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -3595,7 +3613,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3605,7 +3623,8 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3647,22 +3666,22 @@
       <c r="E2" t="s">
         <v>525</v>
       </c>
-      <c r="F2" s="59">
-        <v>42946</v>
-      </c>
-      <c r="G2" s="59">
-        <v>42945</v>
-      </c>
-      <c r="H2" s="59">
-        <v>42915</v>
+      <c r="F2" s="62" t="s">
+        <v>534</v>
+      </c>
+      <c r="G2" s="62" t="s">
+        <v>535</v>
+      </c>
+      <c r="H2" s="62" t="s">
+        <v>536</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>526</v>
       </c>
-      <c r="B3">
-        <v>1212122121</v>
+      <c r="B3" s="43" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4039,7 +4058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -4339,12 +4358,12 @@
       <c r="G11" s="55"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="60" t="s">
         <v>532</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60" t="s">
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59" t="s">
         <v>533</v>
       </c>
     </row>
@@ -5446,10 +5465,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5849,17 +5868,17 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
+        <v>538</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="20"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -5874,23 +5893,16 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>56</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -5904,16 +5916,23 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>56</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -5927,24 +5946,16 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>77</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -5958,22 +5969,24 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>59</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="13"/>
       <c r="D18" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+        <v>60</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>77</v>
+      </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -5985,16 +5998,22 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
     </row>
-    <row r="19" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>62</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
@@ -6008,12 +6027,12 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -6033,10 +6052,10 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -6056,81 +6075,104 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="49" t="s">
-        <v>429</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B24" s="49" t="s">
         <v>421</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="54" t="s">
-        <v>443</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="54" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C25" s="43" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="54" t="s">
-        <v>447</v>
-      </c>
-      <c r="C26" t="s">
-        <v>448</v>
+        <v>445</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="54" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C27" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="54" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C28" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
-        <v>453</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>454</v>
+        <v>451</v>
+      </c>
+      <c r="C29" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="54" t="s">
-        <v>455</v>
-      </c>
-      <c r="C30" t="s">
-        <v>456</v>
+        <v>453</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
+        <v>455</v>
+      </c>
+      <c r="C31" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="54" t="s">
         <v>457</v>
       </c>
-      <c r="C31" s="43" t="s">
+      <c r="C32" s="43" t="s">
         <v>69</v>
       </c>
     </row>
@@ -6138,18 +6180,18 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B9" r:id="rId2"/>
-    <hyperlink ref="B20" r:id="rId3"/>
+    <hyperlink ref="B21" r:id="rId3"/>
     <hyperlink ref="F3" r:id="rId4"/>
     <hyperlink ref="E7" r:id="rId5"/>
     <hyperlink ref="E8" r:id="rId6"/>
     <hyperlink ref="F10" r:id="rId7"/>
     <hyperlink ref="G12" r:id="rId8"/>
-    <hyperlink ref="E15" r:id="rId9"/>
-    <hyperlink ref="E18" r:id="rId10"/>
+    <hyperlink ref="E16" r:id="rId9"/>
+    <hyperlink ref="E19" r:id="rId10"/>
     <hyperlink ref="E9" r:id="rId11" display="ww@.test.com"/>
     <hyperlink ref="F9" r:id="rId12"/>
-    <hyperlink ref="B22" r:id="rId13"/>
-    <hyperlink ref="B23" r:id="rId14"/>
+    <hyperlink ref="B23" r:id="rId13"/>
+    <hyperlink ref="B24" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>

</xml_diff>

<commit_message>
Write new test script for Super Admin. Create new test verifyGUINormalAdminHomePage
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="12" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -23,10 +23,12 @@
     <sheet name="SmokeTest" sheetId="14" r:id="rId14"/>
     <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId15"/>
     <sheet name="TodoTestPage" sheetId="16" r:id="rId16"/>
+    <sheet name="SuperAdminTest" sheetId="17" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="561">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -1983,6 +1985,57 @@
   <si>
     <t>07/6/2017</t>
   </si>
+  <si>
+    <t>Todo Name  02</t>
+  </si>
+  <si>
+    <t>Todo 02</t>
+  </si>
+  <si>
+    <t>Category Name 03</t>
+  </si>
+  <si>
+    <t>Cate_03</t>
+  </si>
+  <si>
+    <t>Super Admin Email</t>
+  </si>
+  <si>
+    <t>Super Admin Password</t>
+  </si>
+  <si>
+    <t>Super Admin Name</t>
+  </si>
+  <si>
+    <t>Super Admin</t>
+  </si>
+  <si>
+    <t>Super Admin Phone</t>
+  </si>
+  <si>
+    <t>416-787-7865</t>
+  </si>
+  <si>
+    <t>Normal Admin Email</t>
+  </si>
+  <si>
+    <t>Normal Admin Password</t>
+  </si>
+  <si>
+    <t>Normal Admin Name</t>
+  </si>
+  <si>
+    <t>Normal Admin</t>
+  </si>
+  <si>
+    <t>Normal Admin Phone</t>
+  </si>
+  <si>
+    <t>Client Email</t>
+  </si>
+  <si>
+    <t>Auditor Email</t>
+  </si>
 </sst>
 </file>
 
@@ -2194,7 +2247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2324,8 +2377,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2334,9 +2391,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3102,11 +3156,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="72"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3622,10 +3676,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3640,15 +3694,17 @@
     <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="59" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" style="59" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="56" t="s">
         <v>423</v>
       </c>
@@ -3670,39 +3726,45 @@
       <c r="H1" s="56" t="s">
         <v>460</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="60" t="s">
         <v>478</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="60" t="s">
         <v>516</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="60" t="s">
+        <v>544</v>
+      </c>
+      <c r="L1" s="60" t="s">
         <v>537</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="60" t="s">
         <v>484</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="60" t="s">
         <v>517</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="60" t="s">
         <v>518</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="60" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q1" s="60" t="s">
         <v>519</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" s="60" t="s">
         <v>520</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" s="60" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="47" t="s">
         <v>527</v>
       </c>
       <c r="C2" t="s">
@@ -3729,29 +3791,35 @@
       <c r="J2" t="s">
         <v>522</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="63" t="s">
+        <v>545</v>
+      </c>
+      <c r="L2" t="s">
         <v>540</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>523</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>541</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>542</v>
       </c>
-      <c r="O2" s="62" t="s">
+      <c r="P2" s="59" t="s">
+        <v>547</v>
+      </c>
+      <c r="Q2" s="62" t="s">
         <v>532</v>
       </c>
-      <c r="P2" s="62" t="s">
+      <c r="R2" s="62" t="s">
         <v>533</v>
       </c>
-      <c r="Q2" s="62" t="s">
+      <c r="S2" s="62" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>524</v>
       </c>
@@ -3759,22 +3827,140 @@
       <c r="J3" s="43" t="s">
         <v>534</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="43"/>
+      <c r="L3" s="43" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>525</v>
       </c>
       <c r="J4" t="s">
         <v>526</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>526</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>548</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>549</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>550</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>552</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>554</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>555</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>556</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>558</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>559</v>
+      </c>
+      <c r="B10" s="57" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>560</v>
+      </c>
+      <c r="B11" s="57" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4526,94 +4712,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="64" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="64" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="64" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="H1" s="64" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="63" t="s">
+      <c r="I1" s="64" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="63" t="s">
+      <c r="J1" s="64" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="K1" s="64" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="63" t="s">
+      <c r="L1" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="63" t="s">
+      <c r="M1" s="64" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="63" t="s">
+      <c r="N1" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="63" t="s">
+      <c r="O1" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="63" t="s">
+      <c r="P1" s="64" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="63" t="s">
+      <c r="Q1" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="67" t="s">
+      <c r="R1" s="65" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="67"/>
-      <c r="T1" s="66" t="s">
+      <c r="S1" s="65"/>
+      <c r="T1" s="68" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="64"/>
-      <c r="V1" s="67" t="s">
+      <c r="U1" s="66"/>
+      <c r="V1" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="64" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="66" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="68" t="s">
+      <c r="AB1" s="69" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -4641,8 +4827,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="65"/>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="67"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4698,6 +4884,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4708,17 +4905,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5550,7 +5736,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Vienpham refactor SignUp auditor
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="9" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="570">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2035,6 +2035,33 @@
   </si>
   <si>
     <t>Auditor Email</t>
+  </si>
+  <si>
+    <t>Member I.D Alphabet</t>
+  </si>
+  <si>
+    <t>Member I.D Numberic</t>
+  </si>
+  <si>
+    <t>Member I.D SpecialChar</t>
+  </si>
+  <si>
+    <t>Member I.D More words</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>ABCDEF GHJKLO</t>
+  </si>
+  <si>
+    <t>Member I.D AlphaNumberic</t>
+  </si>
+  <si>
+    <t>A1B2C3D4E5F6</t>
   </si>
 </sst>
 </file>
@@ -2381,9 +2408,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2391,6 +2415,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3332,7 +3359,7 @@
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3441,7 +3468,7 @@
       <c r="B2" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="49" t="s">
         <v>503</v>
       </c>
       <c r="D2" s="16" t="s">
@@ -3580,7 +3607,7 @@
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
+      <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
@@ -3601,6 +3628,7 @@
     <hyperlink ref="K2" r:id="rId9"/>
     <hyperlink ref="L2" r:id="rId10"/>
     <hyperlink ref="C3" r:id="rId11"/>
+    <hyperlink ref="C2" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3678,8 +3706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3853,9 +3881,9 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -3890,7 +3918,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>550</v>
       </c>
@@ -3898,7 +3926,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>552</v>
       </c>
@@ -3946,7 +3974,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
         <v>560</v>
       </c>
@@ -3954,8 +3982,6 @@
         <v>528</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
@@ -4760,22 +4786,22 @@
       <c r="Q1" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="R1" s="68" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="65"/>
-      <c r="T1" s="68" t="s">
+      <c r="S1" s="68"/>
+      <c r="T1" s="67" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="66"/>
-      <c r="V1" s="65" t="s">
+      <c r="U1" s="65"/>
+      <c r="V1" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="66" t="s">
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="65" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="69" t="s">
@@ -4827,8 +4853,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="67"/>
-      <c r="AB2" s="67"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4884,17 +4910,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4905,6 +4920,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5733,10 +5759,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6444,6 +6470,51 @@
         <v>69</v>
       </c>
     </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="47" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B34" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B35" s="43" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="B36" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B37" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="B38" t="s">
+        <v>569</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>

</xml_diff>

<commit_message>
Create new test verifyGUISuperAdminHomePage(), verifyAssignSuperAdminRole(), finish test case verifyGUINormalAdminHomePage()
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="571">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2035,6 +2035,36 @@
   </si>
   <si>
     <t>Auditor Email</t>
+  </si>
+  <si>
+    <t>Member I.D Alphabet</t>
+  </si>
+  <si>
+    <t>Member I.D Numberic</t>
+  </si>
+  <si>
+    <t>Member I.D SpecialChar</t>
+  </si>
+  <si>
+    <t>Member I.D More words</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>ABCDEF GHJKLO</t>
+  </si>
+  <si>
+    <t>Member I.D AlphaNumberic</t>
+  </si>
+  <si>
+    <t>A1B2C3D4E5F6</t>
+  </si>
+  <si>
+    <t>auvenirad@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -3332,7 +3362,7 @@
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3441,7 +3471,7 @@
       <c r="B2" s="16" t="s">
         <v>469</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="49" t="s">
         <v>503</v>
       </c>
       <c r="D2" s="16" t="s">
@@ -3580,7 +3610,7 @@
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
+      <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
@@ -3601,6 +3631,7 @@
     <hyperlink ref="K2" r:id="rId9"/>
     <hyperlink ref="L2" r:id="rId10"/>
     <hyperlink ref="C3" r:id="rId11"/>
+    <hyperlink ref="C2" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3678,8 +3709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3853,10 +3884,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3879,7 +3910,7 @@
         <v>548</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>527</v>
+        <v>570</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3890,7 +3921,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>550</v>
       </c>
@@ -3898,7 +3929,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>552</v>
       </c>
@@ -3942,25 +3973,19 @@
       <c r="A10" s="60" t="s">
         <v>559</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="59" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
         <v>560</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="59" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:2" s="59" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5733,10 +5758,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6444,6 +6469,51 @@
         <v>69</v>
       </c>
     </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="47" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B34" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B35" s="43" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="B36" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B37" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="B38" t="s">
+        <v>569</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>

</xml_diff>

<commit_message>
done sa_25 -> sa_35
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="10" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="568">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2029,12 +2029,6 @@
   </si>
   <si>
     <t>Normal Admin Phone</t>
-  </si>
-  <si>
-    <t>Client Email</t>
-  </si>
-  <si>
-    <t>Auditor Email</t>
   </si>
   <si>
     <t>Member I.D Alphabet</t>
@@ -3359,7 +3353,7 @@
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3881,15 +3875,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" style="59" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="59" bestFit="1" customWidth="1"/>
@@ -3907,7 +3901,7 @@
         <v>548</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>527</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3968,7 +3962,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>559</v>
+        <v>424</v>
       </c>
       <c r="B10" s="57" t="s">
         <v>528</v>
@@ -3976,16 +3970,32 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>560</v>
-      </c>
-      <c r="B11" s="57" t="s">
-        <v>528</v>
+        <v>460</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="60" t="s">
+        <v>423</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="s">
+        <v>467</v>
+      </c>
+      <c r="B13" s="59" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B12" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5761,7 +5771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -6477,23 +6487,23 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B34" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B35" s="43" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B36" t="s">
         <v>526</v>
@@ -6501,18 +6511,18 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B37" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B38" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor code in SuperAdminTest class
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="567">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2050,6 +2050,9 @@
   </si>
   <si>
     <t>Admin Phone</t>
+  </si>
+  <si>
+    <t>auvenirad@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2396,6 +2399,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2403,9 +2409,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3872,7 +3875,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3894,8 +3897,8 @@
       <c r="A2" s="60" t="s">
         <v>550</v>
       </c>
-      <c r="B2" s="59" t="s">
-        <v>469</v>
+      <c r="B2" s="47" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3926,7 +3929,7 @@
       <c r="A6" s="60" t="s">
         <v>422</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="47" t="s">
         <v>469</v>
       </c>
     </row>
@@ -3990,6 +3993,8 @@
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
     <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4790,22 +4795,22 @@
       <c r="Q1" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="68" t="s">
+      <c r="R1" s="65" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="68"/>
-      <c r="T1" s="67" t="s">
+      <c r="S1" s="65"/>
+      <c r="T1" s="68" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="65"/>
-      <c r="V1" s="68" t="s">
+      <c r="U1" s="66"/>
+      <c r="V1" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="65" t="s">
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="66" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="69" t="s">
@@ -4857,8 +4862,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="67"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4914,6 +4919,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4924,17 +4940,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Vienpham update Smoke test @19-20-21
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="9" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="13" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="567">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2050,6 +2050,9 @@
   </si>
   <si>
     <t>Admin Phone</t>
+  </si>
+  <si>
+    <t>auvenirad@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -3346,7 +3349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -3628,7 +3631,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3871,8 +3874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3894,8 +3897,8 @@
       <c r="A2" s="60" t="s">
         <v>550</v>
       </c>
-      <c r="B2" s="59" t="s">
-        <v>469</v>
+      <c r="B2" s="47" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3926,7 +3929,7 @@
       <c r="A6" s="60" t="s">
         <v>422</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="47" t="s">
         <v>469</v>
       </c>
     </row>
@@ -3990,6 +3993,8 @@
   <hyperlinks>
     <hyperlink ref="B10" r:id="rId1"/>
     <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create new test verifyNotificationAuditorInviteClient, add new function getObjectIdOfEmailUser(), removeEngagementByInvitedClientEmail(), removeBusinessByInvitedClientEmail()
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="9" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="10" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -24,9 +24,11 @@
     <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId15"/>
     <sheet name="TodoTestPage" sheetId="16" r:id="rId16"/>
     <sheet name="SuperAdminTest" sheetId="17" r:id="rId17"/>
+    <sheet name="NotificationEmailTest" sheetId="18" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="17" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="578">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2054,6 +2056,39 @@
   <si>
     <t>auvenirad@gmail.com</t>
   </si>
+  <si>
+    <t>Auditor Password</t>
+  </si>
+  <si>
+    <t>New Client</t>
+  </si>
+  <si>
+    <t>client01.auvenir.inactive@gmail.com</t>
+  </si>
+  <si>
+    <t>New Client Email Password</t>
+  </si>
+  <si>
+    <t>New Client Password</t>
+  </si>
+  <si>
+    <t>New Client Full Name</t>
+  </si>
+  <si>
+    <t>New Client Test</t>
+  </si>
+  <si>
+    <t>Invited Client</t>
+  </si>
+  <si>
+    <t>Invited Client Email Password</t>
+  </si>
+  <si>
+    <t>Invited Client Password</t>
+  </si>
+  <si>
+    <t>engagement 01</t>
+  </si>
 </sst>
 </file>
 
@@ -2265,7 +2300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2399,9 +2434,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2409,6 +2441,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2423,6 +2458,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3874,7 +3910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -3995,6 +4031,124 @@
     <hyperlink ref="B12" r:id="rId2"/>
     <hyperlink ref="B2" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>423</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>567</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>471</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>568</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>570</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>571</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>572</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>574</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>575</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>576</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="60" t="s">
+        <v>484</v>
+      </c>
+      <c r="B12" s="73" t="s">
+        <v>577</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4795,22 +4949,22 @@
       <c r="Q1" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="65" t="s">
+      <c r="R1" s="68" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="65"/>
-      <c r="T1" s="68" t="s">
+      <c r="S1" s="68"/>
+      <c r="T1" s="67" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="66"/>
-      <c r="V1" s="65" t="s">
+      <c r="U1" s="65"/>
+      <c r="V1" s="68" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="66" t="s">
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="65" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="69" t="s">
@@ -4862,8 +5016,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="67"/>
-      <c r="AB2" s="67"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="66"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -4919,17 +5073,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4940,6 +5083,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update test verifyNotificationAuditorInviteTheClient(), read template email from excel file, create some function verify content of email
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="10" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="8520" firstSheet="10" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="599">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2075,9 +2075,6 @@
     <t>New Client Full Name</t>
   </si>
   <si>
-    <t>New Client Test</t>
-  </si>
-  <si>
     <t>Invited Client</t>
   </si>
   <si>
@@ -2088,6 +2085,74 @@
   </si>
   <si>
     <t>engagement 01</t>
+  </si>
+  <si>
+    <t>Auditor Full Name</t>
+  </si>
+  <si>
+    <t>Client Auvenir</t>
+  </si>
+  <si>
+    <t>Subject Email Auditor Invite Client</t>
+  </si>
+  <si>
+    <t>Invitation from %s to complete your engagement on the Auvenir Platform</t>
+  </si>
+  <si>
+    <t>Greeting Content</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Announcement Content</t>
+  </si>
+  <si>
+    <t>%s has invited you to complete your engagement. Please click below to get started!</t>
+  </si>
+  <si>
+    <t>Introducing Content</t>
+  </si>
+  <si>
+    <t>Auvenir is on a mission to make financial audits smarter and more efficient. Our technology helps auditors and clients collaborate better for faster, easier engagements.</t>
+  </si>
+  <si>
+    <t>Introducing Benefit Content</t>
+  </si>
+  <si>
+    <t>Here are some of the benefits.</t>
+  </si>
+  <si>
+    <t>First Benefit Content</t>
+  </si>
+  <si>
+    <t>- Highly secure, cloud based platform to upload your documents</t>
+  </si>
+  <si>
+    <t>Second Benefit Content</t>
+  </si>
+  <si>
+    <t>- Customized, detailed notifications and task management system keeps everyone on schedule and on budget</t>
+  </si>
+  <si>
+    <t>Third Benefit Content</t>
+  </si>
+  <si>
+    <t>- Bank and accounting system integrations</t>
+  </si>
+  <si>
+    <t>FeedBack Content</t>
+  </si>
+  <si>
+    <t>We welcome your feedback, ideas and suggestions to make the audit experience better. Send us an email at feedback@auvenir.com.</t>
+  </si>
+  <si>
+    <t>Goodbye Content</t>
+  </si>
+  <si>
+    <t>Best Regards,
+-Andi,
+Auvenir Customer Success Team</t>
   </si>
 </sst>
 </file>
@@ -2300,7 +2365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2431,6 +2496,15 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2458,7 +2532,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3210,11 +3283,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="72"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="75"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4038,10 +4111,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4053,7 +4126,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="64" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4061,15 +4134,15 @@
       <c r="A2" s="60" t="s">
         <v>423</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>503</v>
+      <c r="B2" s="7" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="32" t="s">
         <v>421</v>
       </c>
     </row>
@@ -4077,79 +4150,163 @@
       <c r="A4" s="60" t="s">
         <v>471</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="32" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>568</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>569</v>
+        <v>577</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>421</v>
+        <v>569</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
-        <v>571</v>
-      </c>
-      <c r="B7" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="B7" s="32" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>572</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>573</v>
+        <v>571</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
-        <v>574</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>488</v>
+        <v>572</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>575</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>421</v>
+        <v>573</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>576</v>
-      </c>
-      <c r="B11" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="B11" s="32" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
+        <v>575</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="s">
         <v>484</v>
       </c>
-      <c r="B12" s="73" t="s">
-        <v>577</v>
+      <c r="B13" s="65" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="60" t="s">
+        <v>579</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="60" t="s">
+        <v>581</v>
+      </c>
+      <c r="B15" s="65" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="60" t="s">
+        <v>583</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" s="60" t="s">
+        <v>585</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="60" t="s">
+        <v>587</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="60" t="s">
+        <v>589</v>
+      </c>
+      <c r="B19" s="66" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="60" t="s">
+        <v>591</v>
+      </c>
+      <c r="B20" s="66" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="60" t="s">
+        <v>593</v>
+      </c>
+      <c r="B21" s="66" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="60" t="s">
+        <v>595</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="60" t="s">
+        <v>597</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>598</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4901,94 +5058,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="67" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="67" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="67" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="67" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="67" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="67" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="67" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="67" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="64" t="s">
+      <c r="J1" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="64" t="s">
+      <c r="K1" s="67" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="64" t="s">
+      <c r="L1" s="67" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="67" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="64" t="s">
+      <c r="N1" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="64" t="s">
+      <c r="O1" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="64" t="s">
+      <c r="P1" s="67" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="64" t="s">
+      <c r="Q1" s="67" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="68" t="s">
+      <c r="R1" s="71" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="68"/>
-      <c r="T1" s="67" t="s">
+      <c r="S1" s="71"/>
+      <c r="T1" s="70" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="65"/>
-      <c r="V1" s="68" t="s">
+      <c r="U1" s="68"/>
+      <c r="V1" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="65" t="s">
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="68" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="69" t="s">
+      <c r="AB1" s="72" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -5016,8 +5173,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="66"/>
-      <c r="AB2" s="66"/>
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="69"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">

</xml_diff>

<commit_message>
Update test case verifyNotificationAuditorInviteClient (), Refactor test case in SuperAdminTest, Refactor Data Provider
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15570" windowHeight="8520" firstSheet="10" activeTab="17"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -25,9 +25,13 @@
     <sheet name="TodoTestPage" sheetId="16" r:id="rId16"/>
     <sheet name="SuperAdminTest" sheetId="17" r:id="rId17"/>
     <sheet name="NotificationEmailTest" sheetId="18" r:id="rId18"/>
+    <sheet name="ClientSignUpTest" sheetId="19" r:id="rId19"/>
+    <sheet name="ClientUITest" sheetId="20" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="18" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="19" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="17" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="672">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2154,6 +2158,225 @@
 -Andi,
 Auvenir Customer Success Team</t>
   </si>
+  <si>
+    <t>Image Logo</t>
+  </si>
+  <si>
+    <t>images/logo.png</t>
+  </si>
+  <si>
+    <t>Greeting Title</t>
+  </si>
+  <si>
+    <t>Announcement Title</t>
+  </si>
+  <si>
+    <t>has invited you to complete your engagement. Please click below to get started!</t>
+  </si>
+  <si>
+    <t>Auvenir Introducing Title</t>
+  </si>
+  <si>
+    <t>Introducing Benefit Title</t>
+  </si>
+  <si>
+    <t>First Benefit Title</t>
+  </si>
+  <si>
+    <t>Second Benefit Title</t>
+  </si>
+  <si>
+    <t>Third Benefit Title</t>
+  </si>
+  <si>
+    <t>Feedback Title</t>
+  </si>
+  <si>
+    <t>Goodbye Title</t>
+  </si>
+  <si>
+    <t>Titancorpvn</t>
+  </si>
+  <si>
+    <t>Parent Stakeholders</t>
+  </si>
+  <si>
+    <t>0123456789</t>
+  </si>
+  <si>
+    <t>cookies</t>
+  </si>
+  <si>
+    <t>Cookie Notice Partial Link</t>
+  </si>
+  <si>
+    <t>Cookie Notice</t>
+  </si>
+  <si>
+    <t>Cookie Notice Text</t>
+  </si>
+  <si>
+    <t>privacy</t>
+  </si>
+  <si>
+    <t>Privacy Statement Partial Link</t>
+  </si>
+  <si>
+    <t>Privacy Statement</t>
+  </si>
+  <si>
+    <t>Privacy Statement Text</t>
+  </si>
+  <si>
+    <t>terms</t>
+  </si>
+  <si>
+    <t>Terms Of Service Partial Link</t>
+  </si>
+  <si>
+    <t>Terms of Service</t>
+  </si>
+  <si>
+    <t>Terms Of Service Text</t>
+  </si>
+  <si>
+    <t>© 2017 Auvenir Inc. All rights reserved.</t>
+  </si>
+  <si>
+    <t>Company Info</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>DueDate Column</t>
+  </si>
+  <si>
+    <t>Last Activity</t>
+  </si>
+  <si>
+    <t>Activity Column</t>
+  </si>
+  <si>
+    <t>Client Column</t>
+  </si>
+  <si>
+    <t>Completed Docs</t>
+  </si>
+  <si>
+    <t>Completed Docs Column</t>
+  </si>
+  <si>
+    <t>Audit Assignee</t>
+  </si>
+  <si>
+    <t>Audit Assignee Column</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Status Column</t>
+  </si>
+  <si>
+    <t>Audit Firm</t>
+  </si>
+  <si>
+    <t>Audit Firm Column</t>
+  </si>
+  <si>
+    <t>Engagement Column</t>
+  </si>
+  <si>
+    <t>Search...</t>
+  </si>
+  <si>
+    <t>Engagement Search</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Type Of Engagement Other</t>
+  </si>
+  <si>
+    <t>Notice to reader / Compilation</t>
+  </si>
+  <si>
+    <t>Type Of Engagement Notice To Reader Compilation</t>
+  </si>
+  <si>
+    <t>Type Of Engagement Review</t>
+  </si>
+  <si>
+    <t>Financial Audit</t>
+  </si>
+  <si>
+    <t>Type Of Engagement Financial Audit</t>
+  </si>
+  <si>
+    <t>Type of Engagement</t>
+  </si>
+  <si>
+    <t>Filter Type Of Engagement</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Filter All</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>Engagement Filters</t>
+  </si>
+  <si>
+    <t>All Engagements</t>
+  </si>
+  <si>
+    <t>Preview Header</t>
+  </si>
+  <si>
+    <t>Sign Out</t>
+  </si>
+  <si>
+    <t>Dashboard Sign Out</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Dashboard Settings</t>
+  </si>
+  <si>
+    <t>Dashboard  Username</t>
+  </si>
+  <si>
+    <t>Dashboard Username</t>
+  </si>
+  <si>
+    <t>Contacts</t>
+  </si>
+  <si>
+    <t>Header Contacts</t>
+  </si>
+  <si>
+    <t>Engagements</t>
+  </si>
+  <si>
+    <t>Header Engagements</t>
+  </si>
+  <si>
+    <t>images/logos/auvenir/logo_auvenir.svg</t>
+  </si>
+  <si>
+    <t>Logo Header White Partial Link</t>
+  </si>
+  <si>
+    <t>auvenirauditor01@gmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -2365,7 +2588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2505,6 +2728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3283,11 +3507,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="74"/>
-      <c r="E1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="76"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3444,12 +3668,108 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="153.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>599</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>601</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>602</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>604</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>605</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>606</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>607</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>608</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>609</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>610</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>598</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3984,7 +4304,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4087,7 +4407,7 @@
         <v>423</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>527</v>
+        <v>671</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4113,7 +4433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4308,6 +4628,53 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="67" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>612</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>611</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="auditor01.auvenir@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4410,6 +4777,273 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>670</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>668</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>666</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>664</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>662</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>660</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>658</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>656</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>654</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>652</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="60" t="s">
+        <v>650</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="s">
+        <v>648</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="60" t="s">
+        <v>647</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="60" t="s">
+        <v>645</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="60" t="s">
+        <v>643</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="60" t="s">
+        <v>641</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="60" t="s">
+        <v>640</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="60" t="s">
+        <v>638</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="60" t="s">
+        <v>636</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="60" t="s">
+        <v>634</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="60" t="s">
+        <v>632</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="60" t="s">
+        <v>631</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="60" t="s">
+        <v>629</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="60" t="s">
+        <v>627</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="60" t="s">
+        <v>625</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="60" t="s">
+        <v>623</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="60" t="s">
+        <v>621</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="60" t="s">
+        <v>619</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="60" t="s">
+        <v>617</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="60" t="s">
+        <v>615</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>614</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4670,10 +5304,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4905,7 +5539,9 @@
       <c r="C6" s="47" t="s">
         <v>421</v>
       </c>
-      <c r="D6" s="47"/>
+      <c r="D6" s="47" t="s">
+        <v>421</v>
+      </c>
       <c r="E6" s="55"/>
       <c r="F6" s="52" t="s">
         <v>500</v>
@@ -4941,43 +5577,43 @@
       <c r="K7" s="55"/>
       <c r="L7" s="55"/>
     </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="55"/>
+      <c r="C8" s="47" t="s">
+        <v>506</v>
+      </c>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
+        <v>502</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+    </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="55"/>
-      <c r="C10" s="47" t="s">
-        <v>506</v>
-      </c>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
-        <v>502</v>
-      </c>
-      <c r="B11" s="47" t="s">
-        <v>438</v>
-      </c>
-      <c r="C11" s="47" t="s">
-        <v>438</v>
-      </c>
-      <c r="D11" s="47" t="s">
-        <v>438</v>
-      </c>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
+      <c r="A10" s="60" t="s">
         <v>530</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59" t="s">
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59" t="s">
         <v>531</v>
       </c>
     </row>
@@ -4985,13 +5621,13 @@
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
     <hyperlink ref="H6" r:id="rId2"/>
-    <hyperlink ref="C10" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
     <hyperlink ref="C6" r:id="rId5"/>
     <hyperlink ref="C5" r:id="rId6"/>
-    <hyperlink ref="B11" r:id="rId7"/>
-    <hyperlink ref="C11" r:id="rId8"/>
-    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="B9" r:id="rId7"/>
+    <hyperlink ref="C9" r:id="rId8"/>
+    <hyperlink ref="D9" r:id="rId9"/>
     <hyperlink ref="C3" r:id="rId10"/>
     <hyperlink ref="G2" r:id="rId11"/>
     <hyperlink ref="F2" r:id="rId12"/>
@@ -5004,9 +5640,10 @@
     <hyperlink ref="L2" r:id="rId19" display="Changeit@123"/>
     <hyperlink ref="B2" r:id="rId20"/>
     <hyperlink ref="J2" r:id="rId21" display="Changeit@123"/>
+    <hyperlink ref="D6" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -5058,94 +5695,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="68" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="68" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="68" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="68" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="68" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="68" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="68" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="67" t="s">
+      <c r="J1" s="68" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="67" t="s">
+      <c r="K1" s="68" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="68" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="68" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="68" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="67" t="s">
+      <c r="O1" s="68" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="68" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="71" t="s">
+      <c r="R1" s="72" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="71"/>
-      <c r="T1" s="70" t="s">
+      <c r="S1" s="72"/>
+      <c r="T1" s="71" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="68"/>
-      <c r="V1" s="71" t="s">
+      <c r="U1" s="69"/>
+      <c r="V1" s="72" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71"/>
-      <c r="AA1" s="68" t="s">
+      <c r="W1" s="72"/>
+      <c r="X1" s="72"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="69" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="72" t="s">
+      <c r="AB1" s="73" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -5173,8 +5810,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="69"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">

</xml_diff>

<commit_message>
Update file data for Group Permission
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="14" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -27,11 +27,13 @@
     <sheet name="NotificationEmailTest" sheetId="18" r:id="rId18"/>
     <sheet name="ClientSignUpTest" sheetId="19" r:id="rId19"/>
     <sheet name="ClientUITest" sheetId="20" r:id="rId20"/>
+    <sheet name="GroupPermissionTest" sheetId="21" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="18" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="19" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="20" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="17" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="697">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2376,6 +2378,81 @@
   </si>
   <si>
     <t>auvenirauditor01@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin Auditor</t>
+  </si>
+  <si>
+    <t>auditor01.adm@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin Auditor Password</t>
+  </si>
+  <si>
+    <t>Lead Auditor</t>
+  </si>
+  <si>
+    <t>auditor01.lead@gmail.com</t>
+  </si>
+  <si>
+    <t>Lead Auditor Password</t>
+  </si>
+  <si>
+    <t>auditor01@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin Client</t>
+  </si>
+  <si>
+    <t>client01.adm@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin Client Password</t>
+  </si>
+  <si>
+    <t>Lead Client</t>
+  </si>
+  <si>
+    <t>client01.lead@gmail.com</t>
+  </si>
+  <si>
+    <t>Lead Client Password</t>
+  </si>
+  <si>
+    <t>client01@gmail.com</t>
+  </si>
+  <si>
+    <t>Engagement 1 Name</t>
+  </si>
+  <si>
+    <t>Engagement GP01</t>
+  </si>
+  <si>
+    <t>Engagement 2 Name</t>
+  </si>
+  <si>
+    <t>Engagement GP02</t>
+  </si>
+  <si>
+    <t>To Do 1 name</t>
+  </si>
+  <si>
+    <t>To Do 2 name</t>
+  </si>
+  <si>
+    <t>ToDo 02</t>
+  </si>
+  <si>
+    <t>To Do 3 name</t>
+  </si>
+  <si>
+    <t>ToDo 03</t>
+  </si>
+  <si>
+    <t>To Do 4 name</t>
+  </si>
+  <si>
+    <t>ToDo 04</t>
   </si>
 </sst>
 </file>
@@ -2732,6 +2809,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2739,9 +2819,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5047,6 +5124,177 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="59" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>672</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>674</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>675</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>677</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>423</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>567</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>679</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>681</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>682</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>684</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="60" t="s">
+        <v>424</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="s">
+        <v>460</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="60" t="s">
+        <v>686</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="60" t="s">
+        <v>688</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="60" t="s">
+        <v>690</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="60" t="s">
+        <v>691</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="60" t="s">
+        <v>693</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="60" t="s">
+        <v>695</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>696</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
@@ -5306,7 +5554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -5743,22 +5991,22 @@
       <c r="Q1" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="69" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="72"/>
-      <c r="T1" s="71" t="s">
+      <c r="S1" s="69"/>
+      <c r="T1" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="69"/>
-      <c r="V1" s="72" t="s">
+      <c r="U1" s="70"/>
+      <c r="V1" s="69" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="69" t="s">
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
+      <c r="Y1" s="69"/>
+      <c r="Z1" s="69"/>
+      <c r="AA1" s="70" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="73" t="s">
@@ -5810,8 +6058,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="70"/>
-      <c r="AB2" s="70"/>
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -5867,6 +6115,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -5877,17 +6136,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
done group permission tc #1
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725" firstSheet="18" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -27,11 +27,13 @@
     <sheet name="NotificationEmailTest" sheetId="18" r:id="rId18"/>
     <sheet name="ClientSignUpTest" sheetId="19" r:id="rId19"/>
     <sheet name="ClientUITest" sheetId="20" r:id="rId20"/>
+    <sheet name="GroupPermissionTest" sheetId="21" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="18" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="19" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="20" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="17" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="699">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2376,6 +2378,87 @@
   </si>
   <si>
     <t>auvenirauditor01@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin Auditor</t>
+  </si>
+  <si>
+    <t>auditor01.adm@gmail.com</t>
+  </si>
+  <si>
+    <t>Lead Auditor</t>
+  </si>
+  <si>
+    <t>auditor01.lead@gmail.com</t>
+  </si>
+  <si>
+    <t>auditor01@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin Client</t>
+  </si>
+  <si>
+    <t>client01.adm@gmail.com</t>
+  </si>
+  <si>
+    <t>Lead Client</t>
+  </si>
+  <si>
+    <t>client01.lead@gmail.com</t>
+  </si>
+  <si>
+    <t>client01@gmail.com</t>
+  </si>
+  <si>
+    <t>Engagement 1 Name</t>
+  </si>
+  <si>
+    <t>Engagement GP01</t>
+  </si>
+  <si>
+    <t>Engagement 2 Name</t>
+  </si>
+  <si>
+    <t>Engagement GP02</t>
+  </si>
+  <si>
+    <t>To Do 1 name</t>
+  </si>
+  <si>
+    <t>To Do 2 name</t>
+  </si>
+  <si>
+    <t>ToDo 02</t>
+  </si>
+  <si>
+    <t>To Do 3 name</t>
+  </si>
+  <si>
+    <t>ToDo 03</t>
+  </si>
+  <si>
+    <t>To Do 4 name</t>
+  </si>
+  <si>
+    <t>ToDo 04</t>
+  </si>
+  <si>
+    <t>Can Create An Engagement</t>
+  </si>
+  <si>
+    <t>Admin Auditor Auvenir Password</t>
+  </si>
+  <si>
+    <t>Lead Auditor Auvenir Password</t>
+  </si>
+  <si>
+    <t>Admin Client Auvenir Password</t>
+  </si>
+  <si>
+    <t>Lead Client Auvenir Password</t>
+  </si>
+  <si>
+    <t>CreateEngagement</t>
   </si>
 </sst>
 </file>
@@ -2732,6 +2815,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2739,9 +2825,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5047,6 +5130,232 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="59" customWidth="1"/>
+    <col min="3" max="4" width="25.28515625" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>693</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>672</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>673</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>694</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>674</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>675</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>695</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>423</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>467</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>677</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>678</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>696</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>679</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>680</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>697</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="60" t="s">
+        <v>424</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="s">
+        <v>460</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="60" t="s">
+        <v>682</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="60" t="s">
+        <v>684</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="60" t="s">
+        <v>686</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="60" t="s">
+        <v>687</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="60" t="s">
+        <v>689</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>690</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="60" t="s">
+        <v>691</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>692</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
@@ -5306,7 +5615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -5743,22 +6052,22 @@
       <c r="Q1" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="69" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="72"/>
-      <c r="T1" s="71" t="s">
+      <c r="S1" s="69"/>
+      <c r="T1" s="72" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="69"/>
-      <c r="V1" s="72" t="s">
+      <c r="U1" s="70"/>
+      <c r="V1" s="69" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="69" t="s">
+      <c r="W1" s="69"/>
+      <c r="X1" s="69"/>
+      <c r="Y1" s="69"/>
+      <c r="Z1" s="69"/>
+      <c r="AA1" s="70" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="73" t="s">
@@ -5810,8 +6119,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="70"/>
-      <c r="AB2" s="70"/>
+      <c r="AA2" s="71"/>
+      <c r="AB2" s="71"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -5867,6 +6176,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -5877,17 +6197,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Create LeadAuditorTest, LeadAuditorService, LeadAuditorPage
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="14" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="17" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="712">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2454,6 +2454,51 @@
   <si>
     <t>ToDo 04</t>
   </si>
+  <si>
+    <t>File Request 1</t>
+  </si>
+  <si>
+    <t>File Request 1 Client</t>
+  </si>
+  <si>
+    <t>File Request 2</t>
+  </si>
+  <si>
+    <t>File Request 2 Client</t>
+  </si>
+  <si>
+    <t>File Request 3</t>
+  </si>
+  <si>
+    <t>File Request 3 Client</t>
+  </si>
+  <si>
+    <t>File Request 4</t>
+  </si>
+  <si>
+    <t>File 01.txt</t>
+  </si>
+  <si>
+    <t>File 01 - Client.txt</t>
+  </si>
+  <si>
+    <t>File 02.txt</t>
+  </si>
+  <si>
+    <t>File 03.txt</t>
+  </si>
+  <si>
+    <t>File 04.txt</t>
+  </si>
+  <si>
+    <t>File 02 - Client.txt</t>
+  </si>
+  <si>
+    <t>File 03 - Client.txt</t>
+  </si>
+  <si>
+    <t>Total Request File In Auditor Lead</t>
+  </si>
 </sst>
 </file>
 
@@ -2665,7 +2710,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2809,9 +2854,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2819,6 +2861,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2833,6 +2878,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5126,15 +5172,15 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" style="59" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="59" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="59"/>
   </cols>
@@ -5287,6 +5333,70 @@
       </c>
       <c r="B19" s="7" t="s">
         <v>696</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="60" t="s">
+        <v>697</v>
+      </c>
+      <c r="B20" s="77" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="60" t="s">
+        <v>698</v>
+      </c>
+      <c r="B21" s="77" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="60" t="s">
+        <v>699</v>
+      </c>
+      <c r="B22" s="77" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="60" t="s">
+        <v>700</v>
+      </c>
+      <c r="B23" s="77" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="60" t="s">
+        <v>701</v>
+      </c>
+      <c r="B24" s="77" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="60" t="s">
+        <v>702</v>
+      </c>
+      <c r="B25" s="77" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="60" t="s">
+        <v>703</v>
+      </c>
+      <c r="B26" s="77" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="52" t="s">
+        <v>711</v>
+      </c>
+      <c r="B27" s="59">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -5991,22 +6101,22 @@
       <c r="Q1" s="68" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="69" t="s">
+      <c r="R1" s="72" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="69"/>
-      <c r="T1" s="72" t="s">
+      <c r="S1" s="72"/>
+      <c r="T1" s="71" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="70"/>
-      <c r="V1" s="69" t="s">
+      <c r="U1" s="69"/>
+      <c r="V1" s="72" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="69"/>
-      <c r="X1" s="69"/>
-      <c r="Y1" s="69"/>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="70" t="s">
+      <c r="W1" s="72"/>
+      <c r="X1" s="72"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="69" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="73" t="s">
@@ -6058,8 +6168,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="71"/>
+      <c r="AA2" s="70"/>
+      <c r="AB2" s="70"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -6115,17 +6225,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -6136,6 +6235,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update test data for iniiliaze data
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="523">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -953,543 +953,18 @@
     <t>expires</t>
   </si>
   <si>
-    <t>{"name" : "tramcompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "huongtram@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "huong","firstName" : "tram","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:40:13.453Z</t>
-  </si>
-  <si>
-    <t>AUwNlTknX9uX-eocvmew0EszS</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:03:49.194Z</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:20.126Z</t>
-  </si>
-  <si>
-    <t>5923faefa4f66bc75c90c260</t>
-  </si>
-  <si>
-    <t>tram</t>
-  </si>
-  <si>
-    <t>huong</t>
-  </si>
-  <si>
-    <t>huongtram@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "tiencompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "toctien@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "toc","firstName" : "tien","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:49:13.453Z</t>
-  </si>
-  <si>
-    <t>AUwNlTknX9uX-eocvmew9EszS</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:03:48.194Z</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:29.126Z</t>
-  </si>
-  <si>
-    <t>5923faefa4f66bc75c90c259</t>
-  </si>
-  <si>
-    <t>tien</t>
-  </si>
-  <si>
-    <t>toc</t>
-  </si>
-  <si>
-    <t>toctien@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "nhicompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "dongnhi@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "dong","firstName" : "nhi","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:48:13.453Z</t>
-  </si>
-  <si>
-    <t>AUwNlTknX9uX-eocvmew8EszS</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:03:47.194Z</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:28.126Z</t>
-  </si>
-  <si>
-    <t>5923faefa4f66bc75c90c258</t>
-  </si>
-  <si>
-    <t>nhi</t>
-  </si>
-  <si>
-    <t>dong</t>
-  </si>
-  <si>
-    <t>dongnhi@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "mycompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "khoimy@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "khoi","firstName" : "my","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:47:13.453Z</t>
-  </si>
-  <si>
-    <t>AUwNlTknX9uX-eocvmew7EszS</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:03:46.194Z</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:27.126Z</t>
-  </si>
-  <si>
-    <t>5923faefa4f66bc75c90c257</t>
-  </si>
-  <si>
-    <t>my</t>
-  </si>
-  <si>
-    <t>khoi</t>
-  </si>
-  <si>
-    <t>khoimy@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "phuongcompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "bichphuong@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "bich","firstName" : "phuong","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:46:13.453Z</t>
-  </si>
-  <si>
-    <t>AUwNlTknX9uX-eocvmew6EszS</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:03:45.194Z</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:26.126Z</t>
-  </si>
-  <si>
-    <t>5923faefa4f66bc75c90c256</t>
-  </si>
-  <si>
-    <t>phuong</t>
-  </si>
-  <si>
-    <t>bich</t>
-  </si>
-  <si>
-    <t>bichphuong@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "lecompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "miule@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "miu","firstName" : "le","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:45:13.453Z</t>
-  </si>
-  <si>
-    <t>AUwNlTknX9uX-eocvmew5EszS</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:03:44.194Z</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:25.126Z</t>
-  </si>
-  <si>
-    <t>5923faefa4f66bc75c90c255</t>
-  </si>
-  <si>
-    <t>le</t>
-  </si>
-  <si>
-    <t>miu</t>
-  </si>
-  <si>
-    <t>miule@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "chicompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "thuychi@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "thuy","firstName" : "chi","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:44:13.453Z</t>
-  </si>
-  <si>
-    <t>AUwNlTknX9uX-eocvmew4EszS</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:03:43.194Z</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:24.126Z</t>
-  </si>
-  <si>
-    <t>5923faefa4f66bc75c90c254</t>
-  </si>
-  <si>
-    <t>chi</t>
-  </si>
-  <si>
-    <t>thuy</t>
-  </si>
-  <si>
-    <t>thuychi@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "quyencompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "lequyen@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "le","firstName" : "quyen","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:43:13.453Z</t>
-  </si>
-  <si>
-    <t>AUwNlTknX9uX-eocvmew3EszS</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:03:42.194Z</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:23.126Z</t>
-  </si>
-  <si>
-    <t>5923faefa4f66bc75c90c253</t>
-  </si>
-  <si>
-    <t>quyen</t>
-  </si>
-  <si>
-    <t>lequyen@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "linhcompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "uyenlinh@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "uyen","firstName" : "linh","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:42:13.453Z</t>
-  </si>
-  <si>
-    <t>AUwNlTknX9uX-eocvmew2EszS</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:03:41.194Z</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:22.126Z</t>
-  </si>
-  <si>
-    <t>5923faefa4f66bc75c90c252</t>
-  </si>
-  <si>
-    <t>linh</t>
-  </si>
-  <si>
-    <t>uyen</t>
-  </si>
-  <si>
-    <t>uyenlinh@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "hacompany","parentStakeholders" : "","overseasOps" : false,"publiclyListed" : false,"previousLegalName" : "","legalNameChanged" : false,"fiscalYearEnd" : null,"accountingFramework" : "","logo" : "","timezone" : "","website" : "","industry" : "","__v" : 1}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "haho@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "ho","firstName" : "ha","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:13.453Z</t>
-  </si>
-  <si>
-    <t>AUwNlTknX9uX-eocvmew1EszS</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:00:40.194Z</t>
-  </si>
-  <si>
-    <t>2017-05-23T09:41:21.126Z</t>
-  </si>
-  <si>
-    <t>5923faefa4f66bc75c90c251</t>
-  </si>
-  <si>
-    <t>ho</t>
-  </si>
-  <si>
-    <t>ha</t>
-  </si>
-  <si>
-    <t>haho@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "auditor","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "huyauditor@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "auditor","firstName" : "huy","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T07:31:54.456Z</t>
-  </si>
-  <si>
-    <t>DwaPhuT7HzBo-dc5D0v7QjP3G</t>
-  </si>
-  <si>
-    <t>2017-05-19T09:29:14.720Z</t>
-  </si>
-  <si>
-    <t>2017-05-22T08:37:36.797Z</t>
-  </si>
-  <si>
-    <t>58f707a6004d69fc2aeb8e50</t>
-  </si>
-  <si>
-    <t>auditor</t>
-  </si>
-  <si>
     <t>huy</t>
   </si>
   <si>
-    <t>AUDITOR</t>
-  </si>
-  <si>
-    <t>huyauditor@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "toan","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "toantrieu@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "trieu","firstName" : "toan","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T07:37:54.456Z</t>
-  </si>
-  <si>
-    <t>DwaPhuT7HzBo-dc4D0v7QjP3G</t>
-  </si>
-  <si>
-    <t>2017-05-19T08:29:14.720Z</t>
-  </si>
-  <si>
-    <t>2017-05-22T08:35:36.797Z</t>
-  </si>
-  <si>
-    <t>58f707a6004d69fc2aeb8e49</t>
-  </si>
-  <si>
-    <t>trieu</t>
-  </si>
-  <si>
-    <t>toan</t>
-  </si>
-  <si>
-    <t>toantrieu@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "minh","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "minhnguyen@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "nguyen","firstName" : "minh","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T04:45:43.514Z</t>
-  </si>
-  <si>
-    <t>DwaPhuT7HzBo-dc4D9v7QjP3G</t>
-  </si>
-  <si>
-    <t>2017-05-19T08:28:14.720Z</t>
-  </si>
-  <si>
-    <t>2017-05-22T08:34:36.797Z</t>
-  </si>
-  <si>
-    <t>58f707a6004d69fc2aeb8e48</t>
-  </si>
-  <si>
     <t>nguyen</t>
   </si>
   <si>
-    <t>minh</t>
-  </si>
-  <si>
-    <t>minhnguyen@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "vien","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "vienpham@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "pham","firstName" : "vien","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-22T10:14:12.447Z</t>
-  </si>
-  <si>
-    <t>DwaPhuT7HzBo-dc4D7v7QjP3G</t>
-  </si>
-  <si>
-    <t>2017-05-19T08:27:14.720Z</t>
-  </si>
-  <si>
-    <t>2017-05-22T08:33:36.797Z</t>
-  </si>
-  <si>
-    <t>58f707a6004d69fc2aeb8e47</t>
-  </si>
-  <si>
-    <t>pham</t>
-  </si>
-  <si>
-    <t>vien</t>
-  </si>
-  <si>
-    <t>vienpham@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "duong","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "duongnguyen@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "nguyen","firstName" : "duong","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T07:37:51.456Z</t>
-  </si>
-  <si>
-    <t>DwaPhuT7HzBo-dc4D6v7QjP3G</t>
-  </si>
-  <si>
-    <t>2017-05-19T08:26:14.720Z</t>
-  </si>
-  <si>
-    <t>2017-05-22T08:32:36.797Z</t>
-  </si>
-  <si>
-    <t>58f707a6004d69fc2aeb8e46</t>
-  </si>
-  <si>
-    <t>duong</t>
-  </si>
-  <si>
-    <t>duongnguyen@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "tan","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "tannguyen@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "nguyen","firstName" : "tan","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T04:46:49.514Z</t>
-  </si>
-  <si>
-    <t>DwaPhuT7HzBo-dc4D5v7QjP3G</t>
-  </si>
-  <si>
-    <t>2017-05-19T08:25:14.720Z</t>
-  </si>
-  <si>
-    <t>2017-05-22T08:31:36.797Z</t>
-  </si>
-  <si>
-    <t>58f707a6004d69fc2aeb8e45</t>
-  </si>
-  <si>
-    <t>tan</t>
-  </si>
-  <si>
-    <t>tannguyen@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "thuan","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "thuanduong@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "duong","firstName" : "thuan","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-22T10:15:11.447Z</t>
-  </si>
-  <si>
-    <t>DwaPhuT7HzBo-dc4D4v7QjP3G</t>
-  </si>
-  <si>
-    <t>2017-05-19T08:24:14.720Z</t>
-  </si>
-  <si>
     <t>2017-05-22T08:39:36.797Z</t>
   </si>
   <si>
-    <t>58f707a6004d69fc2aeb8e44</t>
-  </si>
-  <si>
-    <t>thuan</t>
-  </si>
-  <si>
-    <t>thuanduong@gmail.com</t>
-  </si>
-  <si>
-    <t>{"name" : "trung","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
-  </si>
-  <si>
-    <t>{"status" : "ACTIVE","email" : "trungngo@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "ngo","firstName" : "trung","__v" : 0}</t>
-  </si>
-  <si>
-    <t>2017-05-23T07:38:56.456Z</t>
-  </si>
-  <si>
-    <t>DwaPhuT7HzBo-dc4D3v7QjP3G</t>
-  </si>
-  <si>
-    <t>2017-05-19T08:23:14.720Z</t>
-  </si>
-  <si>
-    <t>2017-05-22T08:38:36.797Z</t>
-  </si>
-  <si>
-    <t>58f707a6004d69fc2aeb8e43</t>
-  </si>
-  <si>
-    <t>ngo</t>
-  </si>
-  <si>
-    <t>trung</t>
-  </si>
-  <si>
-    <t>trungngo@gmail.com</t>
-  </si>
-  <si>
     <t>{"name" : "doai","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
   </si>
   <si>
-    <t>{"status" : "ACTIVE","email" : "doaitran@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "tran","firstName" : "doai","__v" : 0}</t>
-  </si>
-  <si>
     <t>2017-05-23T04:45:49.514Z</t>
   </si>
   <si>
@@ -1511,15 +986,9 @@
     <t>doai</t>
   </si>
   <si>
-    <t>doaitran@gmail.com</t>
-  </si>
-  <si>
     <t>{"name" : "huy","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
   </si>
   <si>
-    <t>{"status" : "ACTIVE","email" : "huyhuynh@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "huynh","firstName" : "huy","__v" : 0}</t>
-  </si>
-  <si>
     <t>2017-05-22T10:14:11.447Z</t>
   </si>
   <si>
@@ -1541,9 +1010,6 @@
     <t>{"name" : "cuong","logoDisplayAgreed" : false,"affiliatedFirmName" : "","affiliated" : false,"phone" : "","size" : "","address" : {"country" : "","postalCode" : "","stateProvince" : "","city" : "","streetAddress" : "","unit" : ""},"logo" : "","__v" : 0}</t>
   </si>
   <si>
-    <t>{"status" : "ACTIVE","email" : "cuongnguyen@gmail.com","type" : "ADMIN","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "","lastName" : "nguyen","firstName" : "cuong","__v" : 0}</t>
-  </si>
-  <si>
     <t>2017-05-23T07:37:56.456Z</t>
   </si>
   <si>
@@ -1563,9 +1029,6 @@
   </si>
   <si>
     <t>ADMIN</t>
-  </si>
-  <si>
-    <t>cuongnguyen@gmail.com</t>
   </si>
   <si>
     <t>Firm Json</t>
@@ -2436,6 +1899,36 @@
   </si>
   <si>
     <t>general client</t>
+  </si>
+  <si>
+    <t>saf.adm.auvenir@gmail.com</t>
+  </si>
+  <si>
+    <t>chr.adm.auvenir@gmail.com</t>
+  </si>
+  <si>
+    <t>ff.adm.auvenir@gmail.com</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "chr.adm.auvenir@gmail.com","type" : "ADMIN","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "","lastName" : "nguyen","firstName" : "cuong","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "saf.adm.auvenir@gmail.com","type" : "ADMIN","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "huynh","firstName" : "huy","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "ff.adm.auvenir@gmail.com","type" : "ADMIN","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "tran","firstName" : "doai","__v" : 0}</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>User3</t>
+  </si>
+  <si>
+    <t>adm.auvenir@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2795,6 +2288,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2802,9 +2298,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3478,10 +2971,10 @@
         <v>45</v>
       </c>
       <c r="D1" s="61" t="s">
-        <v>499</v>
+        <v>320</v>
       </c>
       <c r="E1" s="61" t="s">
-        <v>500</v>
+        <v>321</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>47</v>
@@ -3492,7 +2985,7 @@
         <v>38</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>438</v>
+        <v>259</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>32</v>
@@ -3512,7 +3005,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>458</v>
+        <v>279</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3584,7 +3077,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>429</v>
+        <v>250</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>33</v>
@@ -3604,7 +3097,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -3615,26 +3108,26 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>430</v>
+        <v>251</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>399</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>431</v>
+        <v>252</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="51" t="s">
-        <v>436</v>
+        <v>257</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>437</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -3676,45 +3169,45 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="50" t="s">
-        <v>422</v>
+        <v>243</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>423</v>
+        <v>244</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>424</v>
+        <v>245</v>
       </c>
       <c r="E1" s="50" t="s">
         <v>25</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>439</v>
+        <v>260</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>441</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>425</v>
+        <v>246</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>435</v>
+        <v>256</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>433</v>
+        <v>254</v>
       </c>
       <c r="D2" s="47" t="s">
-        <v>434</v>
+        <v>255</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="F2" s="53" t="s">
-        <v>440</v>
+        <v>261</v>
       </c>
       <c r="G2" s="53" t="s">
-        <v>442</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -3754,82 +3247,82 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
-        <v>599</v>
+        <v>420</v>
       </c>
       <c r="B2" s="59" t="s">
-        <v>600</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>601</v>
+        <v>422</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>582</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
-        <v>602</v>
+        <v>423</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>603</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>604</v>
+        <v>425</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>586</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
-        <v>605</v>
+        <v>426</v>
       </c>
       <c r="B6" s="59" t="s">
-        <v>588</v>
+        <v>409</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
-        <v>606</v>
+        <v>427</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>590</v>
+        <v>411</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>607</v>
+        <v>428</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>592</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
-        <v>608</v>
+        <v>429</v>
       </c>
       <c r="B9" s="59" t="s">
-        <v>594</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>609</v>
+        <v>430</v>
       </c>
       <c r="B10" s="59" t="s">
-        <v>596</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>610</v>
+        <v>431</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>598</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -3841,8 +3334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3876,206 +3369,206 @@
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="50" t="s">
-        <v>422</v>
+        <v>243</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>423</v>
+        <v>244</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>424</v>
+        <v>245</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>483</v>
+        <v>304</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>472</v>
+        <v>293</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>468</v>
+        <v>289</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>467</v>
+        <v>288</v>
       </c>
       <c r="I1" s="52" t="s">
-        <v>460</v>
+        <v>281</v>
       </c>
       <c r="J1" s="56" t="s">
-        <v>470</v>
+        <v>291</v>
       </c>
       <c r="K1" s="56" t="s">
-        <v>471</v>
+        <v>292</v>
       </c>
       <c r="L1" s="56" t="s">
-        <v>459</v>
+        <v>280</v>
       </c>
       <c r="M1" s="52" t="s">
-        <v>474</v>
+        <v>295</v>
       </c>
       <c r="N1" s="52" t="s">
-        <v>473</v>
+        <v>294</v>
       </c>
       <c r="O1" s="52" t="s">
-        <v>462</v>
+        <v>283</v>
       </c>
       <c r="P1" s="52" t="s">
-        <v>484</v>
+        <v>305</v>
       </c>
       <c r="Q1" s="52" t="s">
-        <v>486</v>
+        <v>307</v>
       </c>
       <c r="R1" s="52" t="s">
-        <v>487</v>
+        <v>308</v>
       </c>
       <c r="S1" s="52" t="s">
-        <v>465</v>
+        <v>286</v>
       </c>
       <c r="T1" s="52" t="s">
-        <v>475</v>
+        <v>296</v>
       </c>
       <c r="U1" s="52" t="s">
-        <v>476</v>
+        <v>297</v>
       </c>
       <c r="V1" s="52" t="s">
-        <v>477</v>
+        <v>298</v>
       </c>
       <c r="W1" s="52" t="s">
-        <v>478</v>
+        <v>299</v>
       </c>
       <c r="X1" s="52" t="s">
+        <v>314</v>
+      </c>
+      <c r="Y1" s="52" t="s">
         <v>493</v>
-      </c>
-      <c r="Y1" s="52" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>425</v>
+        <v>246</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>469</v>
+        <v>522</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>503</v>
+        <v>324</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>488</v>
+        <v>309</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="57" t="s">
-        <v>464</v>
+        <v>285</v>
       </c>
       <c r="G2" s="57" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="I2" s="47" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="J2" s="57" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="K2" s="57" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="L2" s="57" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="M2" s="57" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="N2" s="58" t="s">
-        <v>490</v>
+        <v>311</v>
       </c>
       <c r="O2" s="55" t="s">
-        <v>463</v>
+        <v>284</v>
       </c>
       <c r="P2" s="55" t="s">
-        <v>461</v>
+        <v>282</v>
       </c>
       <c r="Q2" t="s">
-        <v>466</v>
+        <v>287</v>
       </c>
       <c r="R2" s="55" t="s">
-        <v>485</v>
+        <v>306</v>
       </c>
       <c r="S2" t="s">
-        <v>491</v>
+        <v>312</v>
       </c>
       <c r="T2" t="s">
-        <v>479</v>
+        <v>300</v>
       </c>
       <c r="U2" t="s">
-        <v>480</v>
+        <v>301</v>
       </c>
       <c r="V2" t="s">
-        <v>481</v>
+        <v>302</v>
       </c>
       <c r="W2" t="s">
-        <v>489</v>
+        <v>310</v>
       </c>
       <c r="X2" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y2" t="s">
         <v>494</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>426</v>
+        <v>247</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>427</v>
+        <v>248</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>496</v>
+        <v>317</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>428</v>
+        <v>249</v>
       </c>
       <c r="E3" s="7"/>
       <c r="P3" s="55" t="s">
-        <v>461</v>
+        <v>282</v>
       </c>
       <c r="Q3" s="55" t="s">
-        <v>466</v>
+        <v>287</v>
       </c>
       <c r="R3" s="55" t="s">
-        <v>485</v>
+        <v>306</v>
       </c>
       <c r="S3" s="55" t="s">
-        <v>492</v>
+        <v>313</v>
       </c>
       <c r="T3" s="55" t="s">
-        <v>479</v>
+        <v>300</v>
       </c>
       <c r="U3" s="55" t="s">
-        <v>480</v>
+        <v>301</v>
       </c>
       <c r="V3" s="55" t="s">
-        <v>481</v>
+        <v>302</v>
       </c>
       <c r="W3" s="55" t="s">
-        <v>482</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
-        <v>432</v>
+        <v>253</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>435</v>
+        <v>256</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>433</v>
+        <v>254</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>434</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -4143,47 +3636,47 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="56" t="s">
-        <v>515</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
-        <v>484</v>
+        <v>305</v>
       </c>
       <c r="B2" s="55" t="s">
-        <v>461</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>514</v>
+        <v>335</v>
       </c>
       <c r="B3" s="55" t="s">
-        <v>513</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>512</v>
+        <v>333</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>511</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>510</v>
+        <v>331</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>509</v>
+        <v>330</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>508</v>
+        <v>329</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>507</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -4224,58 +3717,58 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="56" t="s">
-        <v>423</v>
+        <v>244</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>467</v>
+        <v>288</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>422</v>
+        <v>243</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>468</v>
+        <v>289</v>
       </c>
       <c r="F1" s="56" t="s">
-        <v>424</v>
+        <v>245</v>
       </c>
       <c r="G1" s="56" t="s">
-        <v>459</v>
+        <v>280</v>
       </c>
       <c r="H1" s="56" t="s">
-        <v>460</v>
+        <v>281</v>
       </c>
       <c r="I1" s="60" t="s">
-        <v>478</v>
+        <v>299</v>
       </c>
       <c r="J1" s="60" t="s">
-        <v>516</v>
+        <v>337</v>
       </c>
       <c r="K1" s="60" t="s">
-        <v>544</v>
+        <v>365</v>
       </c>
       <c r="L1" s="60" t="s">
-        <v>537</v>
+        <v>358</v>
       </c>
       <c r="M1" s="60" t="s">
-        <v>484</v>
+        <v>305</v>
       </c>
       <c r="N1" s="60" t="s">
-        <v>517</v>
+        <v>338</v>
       </c>
       <c r="O1" s="60" t="s">
-        <v>518</v>
+        <v>339</v>
       </c>
       <c r="P1" s="60" t="s">
-        <v>546</v>
+        <v>367</v>
       </c>
       <c r="Q1" s="60" t="s">
-        <v>519</v>
+        <v>340</v>
       </c>
       <c r="R1" s="60" t="s">
-        <v>520</v>
+        <v>341</v>
       </c>
       <c r="S1" s="60" t="s">
-        <v>521</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4283,82 +3776,82 @@
         <v>49</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>527</v>
+        <v>348</v>
       </c>
       <c r="C2" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="D2" t="s">
-        <v>469</v>
+        <v>290</v>
       </c>
       <c r="E2" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="F2" s="62" t="s">
-        <v>538</v>
+        <v>359</v>
       </c>
       <c r="G2" s="62" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="H2" s="62" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="I2" t="s">
-        <v>539</v>
+        <v>360</v>
       </c>
       <c r="J2" t="s">
-        <v>522</v>
+        <v>343</v>
       </c>
       <c r="K2" s="63" t="s">
-        <v>545</v>
+        <v>366</v>
       </c>
       <c r="L2" t="s">
-        <v>540</v>
+        <v>361</v>
       </c>
       <c r="M2" t="s">
-        <v>523</v>
+        <v>344</v>
       </c>
       <c r="N2" t="s">
-        <v>541</v>
+        <v>362</v>
       </c>
       <c r="O2" t="s">
-        <v>542</v>
+        <v>363</v>
       </c>
       <c r="P2" s="59" t="s">
-        <v>547</v>
+        <v>368</v>
       </c>
       <c r="Q2" s="62" t="s">
-        <v>532</v>
+        <v>353</v>
       </c>
       <c r="R2" s="62" t="s">
-        <v>533</v>
+        <v>354</v>
       </c>
       <c r="S2" s="62" t="s">
-        <v>543</v>
+        <v>364</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>524</v>
+        <v>345</v>
       </c>
       <c r="B3" s="43"/>
       <c r="J3" s="43" t="s">
-        <v>534</v>
+        <v>355</v>
       </c>
       <c r="K3" s="43"/>
       <c r="L3" s="43" t="s">
-        <v>534</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>525</v>
+        <v>346</v>
       </c>
       <c r="J4" t="s">
-        <v>526</v>
+        <v>347</v>
       </c>
       <c r="L4" t="s">
-        <v>526</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -4394,98 +3887,98 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
-        <v>550</v>
+        <v>371</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>566</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>548</v>
+        <v>369</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
-        <v>549</v>
+        <v>370</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>550</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>551</v>
+        <v>372</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>552</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
-        <v>422</v>
+        <v>243</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>469</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
-        <v>563</v>
+        <v>384</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>564</v>
+        <v>385</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>553</v>
+        <v>374</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
-        <v>565</v>
+        <v>386</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>552</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>424</v>
+        <v>245</v>
       </c>
       <c r="B10" s="57" t="s">
-        <v>528</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>460</v>
+        <v>281</v>
       </c>
       <c r="B11" s="59" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
-        <v>423</v>
+        <v>244</v>
       </c>
       <c r="B12" s="57" t="s">
-        <v>671</v>
+        <v>492</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>467</v>
+        <v>288</v>
       </c>
       <c r="B13" s="59" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -4522,31 +4015,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
-        <v>423</v>
+        <v>244</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>496</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>567</v>
+        <v>388</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
-        <v>471</v>
+        <v>292</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>577</v>
+        <v>398</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>1</v>
@@ -4554,146 +4047,146 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
-        <v>568</v>
+        <v>389</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>569</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
-        <v>570</v>
+        <v>391</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>571</v>
+        <v>392</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
-        <v>572</v>
+        <v>393</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>578</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>573</v>
+        <v>394</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>488</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>574</v>
+        <v>395</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
-        <v>575</v>
+        <v>396</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>484</v>
+        <v>305</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>576</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
-        <v>579</v>
+        <v>400</v>
       </c>
       <c r="B14" s="65" t="s">
-        <v>580</v>
+        <v>401</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="s">
-        <v>581</v>
+        <v>402</v>
       </c>
       <c r="B15" s="65" t="s">
-        <v>582</v>
+        <v>403</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
-        <v>583</v>
+        <v>404</v>
       </c>
       <c r="B16" s="65" t="s">
-        <v>584</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
-        <v>585</v>
+        <v>406</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>586</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
-        <v>587</v>
+        <v>408</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>588</v>
+        <v>409</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>589</v>
+        <v>410</v>
       </c>
       <c r="B19" s="66" t="s">
-        <v>590</v>
+        <v>411</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
-        <v>591</v>
+        <v>412</v>
       </c>
       <c r="B20" s="66" t="s">
-        <v>592</v>
+        <v>413</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
-        <v>593</v>
+        <v>414</v>
       </c>
       <c r="B21" s="66" t="s">
-        <v>594</v>
+        <v>415</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="s">
-        <v>595</v>
+        <v>416</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>596</v>
+        <v>417</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="60" t="s">
-        <v>597</v>
+        <v>418</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>598</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -4728,15 +4221,15 @@
         <v>126</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>613</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>612</v>
+        <v>433</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>611</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -4873,242 +4366,242 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
-        <v>670</v>
+        <v>491</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>669</v>
+        <v>490</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>668</v>
+        <v>489</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>667</v>
+        <v>488</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
-        <v>666</v>
+        <v>487</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>665</v>
+        <v>486</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>664</v>
+        <v>485</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>663</v>
+        <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
-        <v>662</v>
+        <v>483</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>661</v>
+        <v>482</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
-        <v>660</v>
+        <v>481</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>659</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>658</v>
+        <v>479</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>657</v>
+        <v>478</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
-        <v>656</v>
+        <v>477</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>655</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>654</v>
+        <v>475</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>653</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>652</v>
+        <v>473</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>651</v>
+        <v>472</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
-        <v>650</v>
+        <v>471</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>649</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>648</v>
+        <v>469</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>513</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
-        <v>647</v>
+        <v>468</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>646</v>
+        <v>467</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="s">
-        <v>645</v>
+        <v>466</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>644</v>
+        <v>465</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
-        <v>643</v>
+        <v>464</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>642</v>
+        <v>463</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
-        <v>641</v>
+        <v>462</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>484</v>
+        <v>305</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
-        <v>640</v>
+        <v>461</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>639</v>
+        <v>460</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>638</v>
+        <v>459</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>637</v>
+        <v>458</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
-        <v>636</v>
+        <v>457</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>635</v>
+        <v>456</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
-        <v>634</v>
+        <v>455</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>633</v>
+        <v>454</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="s">
-        <v>632</v>
+        <v>453</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>478</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="60" t="s">
-        <v>631</v>
+        <v>452</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>630</v>
+        <v>451</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
-        <v>629</v>
+        <v>450</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>628</v>
+        <v>449</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
-        <v>627</v>
+        <v>448</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>626</v>
+        <v>447</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="s">
-        <v>625</v>
+        <v>446</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>624</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="60" t="s">
-        <v>623</v>
+        <v>444</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>622</v>
+        <v>443</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
-        <v>621</v>
+        <v>442</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>620</v>
+        <v>441</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="s">
-        <v>619</v>
+        <v>440</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>618</v>
+        <v>439</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="60" t="s">
-        <v>617</v>
+        <v>438</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>616</v>
+        <v>437</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="60" t="s">
-        <v>615</v>
+        <v>436</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>614</v>
+        <v>435</v>
       </c>
     </row>
   </sheetData>
@@ -5409,161 +4902,161 @@
     <row r="1" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="56" t="s">
-        <v>422</v>
+        <v>243</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>423</v>
+        <v>244</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>424</v>
+        <v>245</v>
       </c>
       <c r="E1" s="56" t="s">
-        <v>483</v>
+        <v>304</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>472</v>
+        <v>293</v>
       </c>
       <c r="G1" s="52" t="s">
-        <v>468</v>
+        <v>289</v>
       </c>
       <c r="H1" s="52" t="s">
-        <v>467</v>
+        <v>288</v>
       </c>
       <c r="I1" s="52" t="s">
-        <v>460</v>
+        <v>281</v>
       </c>
       <c r="J1" s="56" t="s">
-        <v>470</v>
+        <v>291</v>
       </c>
       <c r="K1" s="56" t="s">
-        <v>471</v>
+        <v>292</v>
       </c>
       <c r="L1" s="56" t="s">
-        <v>459</v>
+        <v>280</v>
       </c>
       <c r="M1" s="52" t="s">
-        <v>474</v>
+        <v>295</v>
       </c>
       <c r="N1" s="52" t="s">
-        <v>473</v>
+        <v>294</v>
       </c>
       <c r="O1" s="52" t="s">
-        <v>462</v>
+        <v>283</v>
       </c>
       <c r="P1" s="52" t="s">
-        <v>484</v>
+        <v>305</v>
       </c>
       <c r="Q1" s="52" t="s">
-        <v>486</v>
+        <v>307</v>
       </c>
       <c r="R1" s="52" t="s">
-        <v>487</v>
+        <v>308</v>
       </c>
       <c r="S1" s="52" t="s">
-        <v>465</v>
+        <v>286</v>
       </c>
       <c r="T1" s="52" t="s">
-        <v>475</v>
+        <v>296</v>
       </c>
       <c r="U1" s="52" t="s">
-        <v>476</v>
+        <v>297</v>
       </c>
       <c r="V1" s="52" t="s">
-        <v>477</v>
+        <v>298</v>
       </c>
       <c r="W1" s="52" t="s">
-        <v>478</v>
+        <v>299</v>
       </c>
       <c r="X1" s="52" t="s">
-        <v>493</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
-        <v>425</v>
+        <v>246</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>469</v>
+        <v>290</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>527</v>
+        <v>348</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>528</v>
+        <v>349</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="57" t="s">
-        <v>464</v>
+        <v>285</v>
       </c>
       <c r="G2" s="57" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="I2" s="47" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="J2" s="57" t="s">
-        <v>495</v>
+        <v>316</v>
       </c>
       <c r="K2" s="57" t="s">
-        <v>495</v>
+        <v>316</v>
       </c>
       <c r="L2" s="57" t="s">
-        <v>495</v>
+        <v>316</v>
       </c>
       <c r="M2" s="57" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="N2" s="58" t="s">
-        <v>490</v>
+        <v>311</v>
       </c>
       <c r="O2" s="55" t="s">
-        <v>463</v>
+        <v>284</v>
       </c>
       <c r="P2" s="55" t="s">
-        <v>529</v>
+        <v>350</v>
       </c>
       <c r="Q2" s="55" t="s">
-        <v>466</v>
+        <v>287</v>
       </c>
       <c r="R2" s="55" t="s">
-        <v>485</v>
+        <v>306</v>
       </c>
       <c r="S2" s="55" t="s">
-        <v>491</v>
+        <v>312</v>
       </c>
       <c r="T2" s="55" t="s">
-        <v>479</v>
+        <v>300</v>
       </c>
       <c r="U2" s="55" t="s">
-        <v>480</v>
+        <v>301</v>
       </c>
       <c r="V2" s="55" t="s">
-        <v>481</v>
+        <v>302</v>
       </c>
       <c r="W2" s="55" t="s">
-        <v>489</v>
+        <v>310</v>
       </c>
       <c r="X2" s="55" t="s">
-        <v>494</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>426</v>
+        <v>247</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>427</v>
+        <v>248</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>496</v>
+        <v>317</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>428</v>
+        <v>249</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="55"/>
@@ -5571,16 +5064,16 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
-        <v>432</v>
+        <v>253</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>435</v>
+        <v>256</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>433</v>
+        <v>254</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>434</v>
+        <v>255</v>
       </c>
       <c r="E4" s="55"/>
       <c r="F4" s="55"/>
@@ -5588,11 +5081,11 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>497</v>
+        <v>318</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="47" t="s">
-        <v>429</v>
+        <v>250</v>
       </c>
       <c r="D5" s="47"/>
       <c r="E5" s="55"/>
@@ -5601,24 +5094,24 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>498</v>
+        <v>319</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="C6" s="47" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
       <c r="E6" s="55"/>
       <c r="F6" s="52" t="s">
-        <v>500</v>
+        <v>321</v>
       </c>
       <c r="G6" s="47"/>
       <c r="H6" s="47" t="s">
-        <v>504</v>
+        <v>325</v>
       </c>
       <c r="I6" s="55"/>
       <c r="J6" s="55"/>
@@ -5627,16 +5120,16 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>499</v>
+        <v>320</v>
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="47" t="s">
-        <v>505</v>
+        <v>326</v>
       </c>
       <c r="D7" s="55"/>
       <c r="E7" s="55"/>
       <c r="F7" s="52" t="s">
-        <v>501</v>
+        <v>322</v>
       </c>
       <c r="G7" s="55"/>
       <c r="H7" s="55" t="s">
@@ -5653,7 +5146,7 @@
       </c>
       <c r="B8" s="55"/>
       <c r="C8" s="47" t="s">
-        <v>506</v>
+        <v>327</v>
       </c>
       <c r="D8" s="55"/>
       <c r="E8" s="55"/>
@@ -5662,16 +5155,16 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
-        <v>502</v>
+        <v>323</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>438</v>
+        <v>259</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>438</v>
+        <v>259</v>
       </c>
       <c r="D9" s="47" t="s">
-        <v>438</v>
+        <v>259</v>
       </c>
       <c r="E9" s="55"/>
       <c r="F9" s="55"/>
@@ -5679,25 +5172,25 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>530</v>
+        <v>351</v>
       </c>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
       <c r="D10" s="59" t="s">
-        <v>531</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
-        <v>500</v>
+        <v>321</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>504</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
-        <v>501</v>
+        <v>322</v>
       </c>
       <c r="C12" s="59" t="s">
         <v>40</v>
@@ -5830,22 +5323,22 @@
       <c r="Q1" s="69" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="73" t="s">
+      <c r="R1" s="70" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="73"/>
-      <c r="T1" s="72" t="s">
+      <c r="S1" s="70"/>
+      <c r="T1" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="70"/>
-      <c r="V1" s="73" t="s">
+      <c r="U1" s="71"/>
+      <c r="V1" s="70" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="70" t="s">
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="70"/>
+      <c r="AA1" s="71" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="74" t="s">
@@ -5897,8 +5390,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="71"/>
+      <c r="AA2" s="72"/>
+      <c r="AB2" s="72"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -5954,6 +5447,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -5964,17 +5468,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5983,821 +5476,237 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="59"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>420</v>
-      </c>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>419</v>
+        <v>241</v>
       </c>
       <c r="C1" t="s">
-        <v>418</v>
+        <v>240</v>
       </c>
       <c r="D1" t="s">
-        <v>417</v>
-      </c>
-      <c r="E1" s="48" t="s">
-        <v>416</v>
+        <v>239</v>
+      </c>
+      <c r="E1" t="s">
+        <v>238</v>
       </c>
       <c r="F1" s="48" t="s">
-        <v>415</v>
+        <v>237</v>
       </c>
       <c r="G1" s="48" t="s">
-        <v>414</v>
+        <v>236</v>
       </c>
       <c r="H1" s="48" t="s">
-        <v>413</v>
+        <v>235</v>
       </c>
       <c r="I1" s="48" t="s">
-        <v>412</v>
-      </c>
-      <c r="J1" t="s">
-        <v>411</v>
+        <v>234</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>233</v>
       </c>
       <c r="K1" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
-        <v>409</v>
-      </c>
-      <c r="B2" t="s">
-        <v>408</v>
+        <v>232</v>
+      </c>
+      <c r="L1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>519</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>514</v>
       </c>
       <c r="C2" t="s">
-        <v>407</v>
+        <v>230</v>
       </c>
       <c r="D2" t="s">
-        <v>332</v>
+        <v>229</v>
       </c>
       <c r="E2" t="s">
-        <v>406</v>
+        <v>206</v>
       </c>
       <c r="F2" t="s">
-        <v>405</v>
+        <v>228</v>
       </c>
       <c r="G2" t="s">
-        <v>404</v>
+        <v>227</v>
       </c>
       <c r="H2" t="s">
-        <v>403</v>
+        <v>226</v>
       </c>
       <c r="I2" t="s">
-        <v>402</v>
+        <v>225</v>
       </c>
       <c r="J2" t="s">
-        <v>401</v>
+        <v>224</v>
       </c>
       <c r="K2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
-        <v>399</v>
-      </c>
-      <c r="B3" t="s">
-        <v>313</v>
-      </c>
-      <c r="C3" t="s">
-        <v>312</v>
+        <v>516</v>
+      </c>
+      <c r="L2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>520</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>513</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>230</v>
       </c>
       <c r="D3" t="s">
-        <v>398</v>
+        <v>205</v>
       </c>
       <c r="E3" t="s">
-        <v>397</v>
+        <v>221</v>
       </c>
       <c r="F3" t="s">
-        <v>368</v>
+        <v>220</v>
       </c>
       <c r="G3" t="s">
-        <v>396</v>
+        <v>207</v>
       </c>
       <c r="H3" t="s">
-        <v>395</v>
+        <v>219</v>
       </c>
       <c r="I3" t="s">
-        <v>394</v>
+        <v>218</v>
       </c>
       <c r="J3" t="s">
-        <v>393</v>
+        <v>217</v>
       </c>
       <c r="K3" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
-        <v>391</v>
-      </c>
-      <c r="B4" t="s">
-        <v>313</v>
-      </c>
-      <c r="C4" t="s">
-        <v>390</v>
+        <v>517</v>
+      </c>
+      <c r="L3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
+        <v>521</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>515</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>230</v>
       </c>
       <c r="D4" t="s">
-        <v>389</v>
+        <v>215</v>
       </c>
       <c r="E4" t="s">
-        <v>388</v>
+        <v>214</v>
       </c>
       <c r="F4" t="s">
-        <v>387</v>
+        <v>213</v>
       </c>
       <c r="G4" t="s">
-        <v>386</v>
+        <v>212</v>
       </c>
       <c r="H4" t="s">
-        <v>385</v>
+        <v>211</v>
       </c>
       <c r="I4" t="s">
-        <v>384</v>
+        <v>210</v>
       </c>
       <c r="J4" t="s">
-        <v>383</v>
+        <v>209</v>
       </c>
       <c r="K4" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
-        <v>381</v>
-      </c>
-      <c r="B5" t="s">
-        <v>313</v>
-      </c>
-      <c r="C5" t="s">
-        <v>380</v>
-      </c>
-      <c r="D5" t="s">
-        <v>379</v>
-      </c>
-      <c r="E5" t="s">
-        <v>378</v>
-      </c>
-      <c r="F5" t="s">
-        <v>377</v>
-      </c>
-      <c r="G5" t="s">
-        <v>376</v>
-      </c>
-      <c r="H5" t="s">
-        <v>375</v>
-      </c>
-      <c r="I5" t="s">
-        <v>374</v>
-      </c>
-      <c r="J5" t="s">
-        <v>373</v>
-      </c>
-      <c r="K5" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="B6" t="s">
-        <v>313</v>
-      </c>
-      <c r="C6" t="s">
-        <v>370</v>
-      </c>
-      <c r="D6" t="s">
-        <v>352</v>
-      </c>
-      <c r="E6" t="s">
-        <v>369</v>
-      </c>
-      <c r="F6" t="s">
-        <v>368</v>
-      </c>
-      <c r="G6" t="s">
-        <v>367</v>
-      </c>
-      <c r="H6" t="s">
-        <v>366</v>
-      </c>
-      <c r="I6" t="s">
-        <v>365</v>
-      </c>
-      <c r="J6" t="s">
-        <v>364</v>
-      </c>
-      <c r="K6" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
-        <v>362</v>
-      </c>
-      <c r="B7" t="s">
-        <v>313</v>
-      </c>
-      <c r="C7" t="s">
-        <v>361</v>
-      </c>
-      <c r="D7" t="s">
-        <v>332</v>
-      </c>
-      <c r="E7" t="s">
-        <v>360</v>
-      </c>
-      <c r="F7" t="s">
-        <v>359</v>
-      </c>
-      <c r="G7" t="s">
-        <v>358</v>
-      </c>
-      <c r="H7" t="s">
-        <v>357</v>
-      </c>
-      <c r="I7" t="s">
-        <v>356</v>
-      </c>
-      <c r="J7" t="s">
-        <v>355</v>
-      </c>
-      <c r="K7" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="47" t="s">
-        <v>353</v>
-      </c>
-      <c r="B8" t="s">
-        <v>313</v>
-      </c>
-      <c r="C8" t="s">
-        <v>352</v>
-      </c>
-      <c r="D8" t="s">
-        <v>332</v>
-      </c>
-      <c r="E8" t="s">
-        <v>351</v>
-      </c>
-      <c r="F8" t="s">
-        <v>350</v>
-      </c>
-      <c r="G8" t="s">
-        <v>349</v>
-      </c>
-      <c r="H8" t="s">
-        <v>348</v>
-      </c>
-      <c r="I8" t="s">
-        <v>347</v>
-      </c>
-      <c r="J8" t="s">
-        <v>346</v>
-      </c>
-      <c r="K8" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
-        <v>344</v>
-      </c>
-      <c r="B9" t="s">
-        <v>313</v>
-      </c>
-      <c r="C9" t="s">
-        <v>343</v>
-      </c>
-      <c r="D9" t="s">
-        <v>342</v>
-      </c>
-      <c r="E9" t="s">
-        <v>341</v>
-      </c>
-      <c r="F9" t="s">
-        <v>340</v>
-      </c>
-      <c r="G9" t="s">
-        <v>339</v>
-      </c>
-      <c r="H9" t="s">
-        <v>338</v>
-      </c>
-      <c r="I9" t="s">
-        <v>337</v>
-      </c>
-      <c r="J9" t="s">
-        <v>336</v>
-      </c>
-      <c r="K9" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
-        <v>334</v>
-      </c>
-      <c r="B10" t="s">
-        <v>313</v>
-      </c>
-      <c r="C10" t="s">
-        <v>333</v>
-      </c>
-      <c r="D10" t="s">
-        <v>332</v>
-      </c>
-      <c r="E10" t="s">
-        <v>331</v>
-      </c>
-      <c r="F10" t="s">
-        <v>330</v>
-      </c>
-      <c r="G10" t="s">
-        <v>329</v>
-      </c>
-      <c r="H10" t="s">
-        <v>328</v>
-      </c>
-      <c r="I10" t="s">
-        <v>327</v>
-      </c>
-      <c r="J10" t="s">
-        <v>326</v>
-      </c>
-      <c r="K10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
-        <v>324</v>
-      </c>
-      <c r="B11" t="s">
-        <v>313</v>
-      </c>
-      <c r="C11" t="s">
-        <v>323</v>
-      </c>
-      <c r="D11" t="s">
-        <v>322</v>
-      </c>
-      <c r="E11" t="s">
-        <v>321</v>
-      </c>
-      <c r="F11" t="s">
-        <v>320</v>
-      </c>
-      <c r="G11" t="s">
-        <v>319</v>
-      </c>
-      <c r="H11" t="s">
-        <v>318</v>
-      </c>
-      <c r="I11" t="s">
-        <v>317</v>
-      </c>
-      <c r="J11" t="s">
-        <v>316</v>
-      </c>
-      <c r="K11" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="47" t="s">
-        <v>314</v>
-      </c>
-      <c r="B12" t="s">
-        <v>313</v>
-      </c>
-      <c r="C12" t="s">
-        <v>312</v>
-      </c>
-      <c r="D12" t="s">
-        <v>311</v>
-      </c>
-      <c r="E12" t="s">
-        <v>310</v>
-      </c>
-      <c r="F12" t="s">
-        <v>309</v>
-      </c>
-      <c r="G12" t="s">
-        <v>308</v>
-      </c>
-      <c r="H12" t="s">
-        <v>307</v>
-      </c>
-      <c r="I12" t="s">
-        <v>306</v>
-      </c>
-      <c r="J12" t="s">
-        <v>305</v>
-      </c>
-      <c r="K12" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
-        <v>303</v>
-      </c>
-      <c r="B13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" t="s">
-        <v>302</v>
-      </c>
-      <c r="D13" t="s">
-        <v>301</v>
-      </c>
-      <c r="E13" t="s">
-        <v>300</v>
-      </c>
-      <c r="F13" t="s">
-        <v>299</v>
-      </c>
-      <c r="G13" t="s">
-        <v>298</v>
-      </c>
-      <c r="H13" t="s">
-        <v>297</v>
-      </c>
-      <c r="I13" t="s">
-        <v>296</v>
-      </c>
-      <c r="J13" t="s">
-        <v>295</v>
-      </c>
-      <c r="K13" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="47" t="s">
-        <v>293</v>
-      </c>
-      <c r="B14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" t="s">
-        <v>292</v>
-      </c>
-      <c r="D14" t="s">
-        <v>291</v>
-      </c>
-      <c r="E14" t="s">
-        <v>290</v>
-      </c>
-      <c r="F14" t="s">
-        <v>289</v>
-      </c>
-      <c r="G14" t="s">
-        <v>288</v>
-      </c>
-      <c r="H14" t="s">
-        <v>287</v>
-      </c>
-      <c r="I14" t="s">
-        <v>286</v>
-      </c>
-      <c r="J14" t="s">
-        <v>285</v>
-      </c>
-      <c r="K14" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="47" t="s">
-        <v>283</v>
-      </c>
-      <c r="B15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" t="s">
-        <v>262</v>
-      </c>
-      <c r="D15" t="s">
-        <v>282</v>
-      </c>
-      <c r="E15" t="s">
-        <v>281</v>
-      </c>
-      <c r="F15" t="s">
-        <v>280</v>
-      </c>
-      <c r="G15" t="s">
-        <v>279</v>
-      </c>
-      <c r="H15" t="s">
-        <v>278</v>
-      </c>
-      <c r="I15" t="s">
-        <v>277</v>
-      </c>
-      <c r="J15" t="s">
-        <v>276</v>
-      </c>
-      <c r="K15" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
-        <v>274</v>
-      </c>
-      <c r="B16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" t="s">
-        <v>273</v>
-      </c>
-      <c r="D16" t="s">
-        <v>272</v>
-      </c>
-      <c r="E16" t="s">
-        <v>271</v>
-      </c>
-      <c r="F16" t="s">
-        <v>270</v>
-      </c>
-      <c r="G16" t="s">
-        <v>269</v>
-      </c>
-      <c r="H16" t="s">
-        <v>268</v>
-      </c>
-      <c r="I16" t="s">
-        <v>267</v>
-      </c>
-      <c r="J16" t="s">
-        <v>266</v>
-      </c>
-      <c r="K16" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
-        <v>264</v>
-      </c>
-      <c r="B17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" t="s">
-        <v>263</v>
-      </c>
-      <c r="D17" t="s">
-        <v>262</v>
-      </c>
-      <c r="E17" t="s">
-        <v>261</v>
-      </c>
-      <c r="F17" t="s">
-        <v>260</v>
-      </c>
-      <c r="G17" t="s">
-        <v>259</v>
-      </c>
-      <c r="H17" t="s">
-        <v>258</v>
-      </c>
-      <c r="I17" t="s">
-        <v>257</v>
-      </c>
-      <c r="J17" t="s">
-        <v>256</v>
-      </c>
-      <c r="K17" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="47" t="s">
-        <v>254</v>
-      </c>
-      <c r="B18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" t="s">
-        <v>253</v>
-      </c>
-      <c r="D18" t="s">
-        <v>252</v>
-      </c>
-      <c r="E18" t="s">
-        <v>251</v>
-      </c>
-      <c r="F18" t="s">
-        <v>250</v>
-      </c>
-      <c r="G18" t="s">
-        <v>249</v>
-      </c>
-      <c r="H18" t="s">
-        <v>248</v>
-      </c>
-      <c r="I18" t="s">
-        <v>247</v>
-      </c>
-      <c r="J18" t="s">
-        <v>246</v>
-      </c>
-      <c r="K18" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="47" t="s">
-        <v>244</v>
-      </c>
-      <c r="B19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" t="s">
-        <v>243</v>
-      </c>
-      <c r="D19" t="s">
-        <v>242</v>
-      </c>
-      <c r="E19" t="s">
-        <v>241</v>
-      </c>
-      <c r="F19" t="s">
-        <v>240</v>
-      </c>
-      <c r="G19" t="s">
-        <v>239</v>
-      </c>
-      <c r="H19" t="s">
-        <v>238</v>
-      </c>
-      <c r="I19" t="s">
-        <v>237</v>
-      </c>
-      <c r="J19" t="s">
-        <v>236</v>
-      </c>
-      <c r="K19" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="47" t="s">
-        <v>234</v>
-      </c>
-      <c r="B20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" t="s">
-        <v>233</v>
-      </c>
-      <c r="D20" t="s">
-        <v>232</v>
-      </c>
-      <c r="E20" t="s">
-        <v>231</v>
-      </c>
-      <c r="F20" t="s">
-        <v>230</v>
-      </c>
-      <c r="G20" t="s">
-        <v>229</v>
-      </c>
-      <c r="H20" t="s">
-        <v>228</v>
-      </c>
-      <c r="I20" t="s">
-        <v>227</v>
-      </c>
-      <c r="J20" t="s">
-        <v>226</v>
-      </c>
-      <c r="K20" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
-        <v>224</v>
-      </c>
-      <c r="B21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" t="s">
-        <v>223</v>
-      </c>
-      <c r="D21" t="s">
-        <v>222</v>
-      </c>
-      <c r="E21" t="s">
-        <v>221</v>
-      </c>
-      <c r="F21" t="s">
-        <v>220</v>
-      </c>
-      <c r="G21" t="s">
-        <v>219</v>
-      </c>
-      <c r="H21" t="s">
-        <v>218</v>
-      </c>
-      <c r="I21" t="s">
-        <v>217</v>
-      </c>
-      <c r="J21" t="s">
-        <v>216</v>
-      </c>
-      <c r="K21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="47" t="s">
-        <v>214</v>
-      </c>
-      <c r="B22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" t="s">
-        <v>213</v>
-      </c>
-      <c r="D22" t="s">
-        <v>212</v>
-      </c>
-      <c r="E22" t="s">
-        <v>211</v>
-      </c>
-      <c r="F22" t="s">
-        <v>210</v>
-      </c>
-      <c r="G22" t="s">
-        <v>209</v>
-      </c>
-      <c r="H22" t="s">
+        <v>518</v>
+      </c>
+      <c r="L4" t="s">
         <v>208</v>
       </c>
-      <c r="I22" t="s">
-        <v>207</v>
-      </c>
-      <c r="J22" t="s">
-        <v>206</v>
-      </c>
-      <c r="K22" t="s">
-        <v>205</v>
-      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="47"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="47"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="47"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="47"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="47"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="47"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="47"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="47"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="47"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="47"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="47"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="47"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="47"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="47"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="47"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="47"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="47"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="47"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
-    <hyperlink ref="A14" r:id="rId13"/>
-    <hyperlink ref="A15" r:id="rId14"/>
-    <hyperlink ref="A16" r:id="rId15"/>
-    <hyperlink ref="A17" r:id="rId16"/>
-    <hyperlink ref="A18" r:id="rId17"/>
-    <hyperlink ref="A19" r:id="rId18"/>
-    <hyperlink ref="A20" r:id="rId19"/>
-    <hyperlink ref="A21" r:id="rId20"/>
-    <hyperlink ref="A22" r:id="rId21"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -6805,7 +5714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -7208,10 +6117,10 @@
     </row>
     <row r="14" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>535</v>
+        <v>356</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>536</v>
+        <v>357</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
@@ -7439,7 +6348,7 @@
         <v>36</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>429</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -7447,172 +6356,172 @@
         <v>37</v>
       </c>
       <c r="B24" s="49" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="54" t="s">
-        <v>674</v>
+        <v>495</v>
       </c>
       <c r="B25" s="68" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="54" t="s">
-        <v>675</v>
+        <v>496</v>
       </c>
       <c r="B26" s="68" t="s">
-        <v>676</v>
+        <v>497</v>
       </c>
     </row>
     <row r="27" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="54" t="s">
-        <v>677</v>
+        <v>498</v>
       </c>
       <c r="B27" s="68" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="54" t="s">
-        <v>678</v>
+        <v>499</v>
       </c>
       <c r="B28" s="68" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
-        <v>679</v>
+        <v>500</v>
       </c>
       <c r="B29" s="68" t="s">
-        <v>680</v>
+        <v>501</v>
       </c>
     </row>
     <row r="30" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="54" t="s">
-        <v>681</v>
+        <v>502</v>
       </c>
       <c r="B30" s="68" t="s">
-        <v>434</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
-        <v>682</v>
+        <v>503</v>
       </c>
       <c r="B31" s="68" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="32" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="54" t="s">
-        <v>683</v>
+        <v>504</v>
       </c>
       <c r="B32" s="68" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="54" t="s">
-        <v>684</v>
+        <v>505</v>
       </c>
       <c r="B33" s="68" t="s">
-        <v>685</v>
+        <v>506</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="54" t="s">
-        <v>686</v>
+        <v>507</v>
       </c>
       <c r="B34" s="68" t="s">
-        <v>687</v>
+        <v>508</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="54" t="s">
-        <v>688</v>
+        <v>509</v>
       </c>
       <c r="B35" s="68" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="54" t="s">
-        <v>689</v>
+        <v>510</v>
       </c>
       <c r="B36" s="68" t="s">
-        <v>421</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="54" t="s">
-        <v>690</v>
+        <v>511</v>
       </c>
       <c r="B37" s="68" t="s">
-        <v>691</v>
+        <v>512</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="54" t="s">
-        <v>443</v>
+        <v>264</v>
       </c>
       <c r="C38" s="43" t="s">
-        <v>444</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="54" t="s">
-        <v>445</v>
+        <v>266</v>
       </c>
       <c r="C39" s="43" t="s">
-        <v>446</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="54" t="s">
-        <v>447</v>
+        <v>268</v>
       </c>
       <c r="C40" t="s">
-        <v>448</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="54" t="s">
-        <v>449</v>
+        <v>270</v>
       </c>
       <c r="C41" t="s">
-        <v>450</v>
+        <v>271</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="54" t="s">
-        <v>451</v>
+        <v>272</v>
       </c>
       <c r="C42" t="s">
-        <v>452</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="54" t="s">
-        <v>453</v>
+        <v>274</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>454</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="54" t="s">
-        <v>455</v>
+        <v>276</v>
       </c>
       <c r="C44" t="s">
-        <v>456</v>
+        <v>277</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="54" t="s">
-        <v>457</v>
+        <v>278</v>
       </c>
       <c r="C45" s="43" t="s">
         <v>69</v>
@@ -7620,47 +6529,47 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="47" t="s">
-        <v>433</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>554</v>
+        <v>375</v>
       </c>
       <c r="B47" t="s">
-        <v>558</v>
+        <v>379</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>555</v>
+        <v>376</v>
       </c>
       <c r="B48" s="43" t="s">
-        <v>559</v>
+        <v>380</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>556</v>
+        <v>377</v>
       </c>
       <c r="B49" t="s">
-        <v>526</v>
+        <v>347</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>557</v>
+        <v>378</v>
       </c>
       <c r="B50" t="s">
-        <v>560</v>
+        <v>381</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>561</v>
+        <v>382</v>
       </c>
       <c r="B51" t="s">
-        <v>562</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add company name excel
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="565">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2054,6 +2054,9 @@
   </si>
   <si>
     <t>File 04.txt</t>
+  </si>
+  <si>
+    <t>Auvenir</t>
   </si>
 </sst>
 </file>
@@ -2416,8 +2419,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2426,9 +2434,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2443,8 +2448,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3196,11 +3199,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="76"/>
-      <c r="E1" s="77"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="79"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4745,10 +4748,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4925,116 +4928,126 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
-        <v>543</v>
+        <v>333</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>330</v>
+        <v>564</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>545</v>
+        <v>330</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
-        <v>550</v>
-      </c>
-      <c r="B20" s="78" t="s">
-        <v>551</v>
+        <v>548</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>549</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
-        <v>552</v>
-      </c>
-      <c r="B21" s="78" t="s">
-        <v>553</v>
+        <v>550</v>
+      </c>
+      <c r="B21" s="69" t="s">
+        <v>551</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="s">
-        <v>554</v>
-      </c>
-      <c r="B22" s="78" t="s">
-        <v>555</v>
+        <v>552</v>
+      </c>
+      <c r="B22" s="69" t="s">
+        <v>553</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="60" t="s">
-        <v>556</v>
-      </c>
-      <c r="B23" s="78" t="s">
-        <v>557</v>
+        <v>554</v>
+      </c>
+      <c r="B23" s="69" t="s">
+        <v>555</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
-        <v>558</v>
-      </c>
-      <c r="B24" s="78" t="s">
-        <v>559</v>
+        <v>556</v>
+      </c>
+      <c r="B24" s="69" t="s">
+        <v>557</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
-        <v>560</v>
-      </c>
-      <c r="B25" s="78" t="s">
-        <v>561</v>
+        <v>558</v>
+      </c>
+      <c r="B25" s="69" t="s">
+        <v>559</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="s">
-        <v>562</v>
-      </c>
-      <c r="B26" s="78" t="s">
-        <v>563</v>
+        <v>560</v>
+      </c>
+      <c r="B26" s="69" t="s">
+        <v>561</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="79"/>
+      <c r="A27" s="60" t="s">
+        <v>562</v>
+      </c>
+      <c r="B27" s="69" t="s">
+        <v>563</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="70"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5707,94 +5720,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="71" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="69" t="s">
+      <c r="G1" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="71" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="71" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="71" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="K1" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="69" t="s">
+      <c r="L1" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="69" t="s">
+      <c r="M1" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="69" t="s">
+      <c r="N1" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="69" t="s">
+      <c r="O1" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="69" t="s">
+      <c r="P1" s="71" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="69" t="s">
+      <c r="Q1" s="71" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="73" t="s">
+      <c r="R1" s="72" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="73"/>
-      <c r="T1" s="72" t="s">
+      <c r="S1" s="72"/>
+      <c r="T1" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="70"/>
-      <c r="V1" s="73" t="s">
+      <c r="U1" s="73"/>
+      <c r="V1" s="72" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="70" t="s">
+      <c r="W1" s="72"/>
+      <c r="X1" s="72"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="73" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="74" t="s">
+      <c r="AB1" s="76" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -5822,8 +5835,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="71"/>
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="74"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -5879,6 +5892,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -5889,17 +5913,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update test Excel file
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="567">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -5310,8 +5310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5444,7 +5444,7 @@
         <v>316</v>
       </c>
       <c r="K2" s="57" t="s">
-        <v>316</v>
+        <v>242</v>
       </c>
       <c r="L2" s="57" t="s">
         <v>316</v>
@@ -5656,7 +5656,7 @@
     <hyperlink ref="I2" r:id="rId15"/>
     <hyperlink ref="C2" r:id="rId16"/>
     <hyperlink ref="D2" r:id="rId17"/>
-    <hyperlink ref="K2" r:id="rId18" display="Changeit@123"/>
+    <hyperlink ref="K2" r:id="rId18"/>
     <hyperlink ref="L2" r:id="rId19" display="Changeit@123"/>
     <hyperlink ref="B2" r:id="rId20"/>
     <hyperlink ref="J2" r:id="rId21" display="Changeit@123"/>
@@ -5920,7 +5920,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6059,6 +6059,12 @@
       <c r="L3" t="s">
         <v>216</v>
       </c>
+      <c r="M3" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="N3" s="59" t="s">
+        <v>566</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
@@ -6096,6 +6102,12 @@
       </c>
       <c r="L4" t="s">
         <v>208</v>
+      </c>
+      <c r="M4" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="N4" s="59" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Change class: initData to beforeTest
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -2430,9 +2430,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2440,6 +2437,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3476,8 +3476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5764,22 +5764,22 @@
       <c r="Q1" s="71" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="75" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="72"/>
-      <c r="T1" s="75" t="s">
+      <c r="S1" s="75"/>
+      <c r="T1" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="73"/>
-      <c r="V1" s="72" t="s">
+      <c r="U1" s="72"/>
+      <c r="V1" s="75" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="73" t="s">
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="72" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="76" t="s">
@@ -5831,8 +5831,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="74"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -5888,17 +5888,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -5909,6 +5898,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5919,7 +5919,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update Class GroupPermissionInitialTest, add new test for create (Lead Auditor, Admin Client, Auditor Member)
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="571">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2056,7 +2056,25 @@
     <t>File 04.txt</t>
   </si>
   <si>
-    <t>Auvenir</t>
+    <t>Admin Auditor Email Password</t>
+  </si>
+  <si>
+    <t>Admin Auditor Full Name</t>
+  </si>
+  <si>
+    <t>Lead Auditor Email Password</t>
+  </si>
+  <si>
+    <t>Admin Client Email Password</t>
+  </si>
+  <si>
+    <t>Lead Client Email Password</t>
+  </si>
+  <si>
+    <t>Auvenir Thuan</t>
+  </si>
+  <si>
+    <t>Firm Auvenir</t>
   </si>
 </sst>
 </file>
@@ -2123,7 +2141,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2145,12 +2163,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2275,7 +2287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2420,12 +2432,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2434,6 +2442,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3199,11 +3210,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="78"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4748,10 +4759,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4778,7 +4789,7 @@
       <c r="A2" s="60" t="s">
         <v>525</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>526</v>
       </c>
       <c r="C2" s="28" t="s">
@@ -4800,39 +4811,37 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
-        <v>528</v>
+        <v>564</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>529</v>
+        <v>242</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
-        <v>530</v>
+        <v>565</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>242</v>
+        <v>525</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
-        <v>244</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>531</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>170</v>
-      </c>
+        <v>528</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="C6" s="7"/>
       <c r="D6" s="7"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
-        <v>288</v>
+        <v>530</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>242</v>
@@ -4842,41 +4851,39 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>532</v>
+        <v>566</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>533</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>168</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
-        <v>534</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="C9" s="7"/>
+        <v>244</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>531</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>170</v>
+      </c>
       <c r="D9" s="7"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>535</v>
+        <v>288</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>168</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>537</v>
+        <v>292</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>242</v>
@@ -4886,10 +4893,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
-        <v>245</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>538</v>
+        <v>532</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>533</v>
       </c>
       <c r="C12" s="28" t="s">
         <v>168</v>
@@ -4898,7 +4905,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>281</v>
+        <v>534</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>242</v>
@@ -4908,150 +4915,237 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
-        <v>539</v>
+        <v>567</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>540</v>
+        <v>242</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>542</v>
-      </c>
-      <c r="C15" s="7"/>
+        <v>536</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
-        <v>333</v>
+        <v>537</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>564</v>
+        <v>242</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
-        <v>543</v>
+        <v>568</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>330</v>
+        <v>242</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
-        <v>544</v>
+        <v>245</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>545</v>
-      </c>
-      <c r="C18" s="7"/>
+        <v>538</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>546</v>
+        <v>281</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>547</v>
+        <v>242</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
-        <v>548</v>
+        <v>280</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>549</v>
+        <v>242</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
-        <v>550</v>
-      </c>
-      <c r="B21" s="69" t="s">
-        <v>551</v>
+        <v>539</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>540</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="s">
-        <v>552</v>
-      </c>
-      <c r="B22" s="69" t="s">
-        <v>553</v>
+        <v>541</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>542</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="60" t="s">
-        <v>554</v>
-      </c>
-      <c r="B23" s="69" t="s">
-        <v>555</v>
+        <v>333</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>569</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
-        <v>556</v>
-      </c>
-      <c r="B24" s="69" t="s">
-        <v>557</v>
+        <v>543</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>330</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
-        <v>558</v>
-      </c>
-      <c r="B25" s="69" t="s">
-        <v>559</v>
+        <v>544</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>545</v>
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="s">
-        <v>560</v>
-      </c>
-      <c r="B26" s="69" t="s">
-        <v>561</v>
+        <v>546</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>547</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="60" t="s">
-        <v>562</v>
-      </c>
-      <c r="B27" s="69" t="s">
-        <v>563</v>
+        <v>548</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>549</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="70"/>
+      <c r="A28" s="60" t="s">
+        <v>550</v>
+      </c>
+      <c r="B28" s="69" t="s">
+        <v>551</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="60" t="s">
+        <v>552</v>
+      </c>
+      <c r="B29" s="69" t="s">
+        <v>553</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="60" t="s">
+        <v>554</v>
+      </c>
+      <c r="B30" s="69" t="s">
+        <v>555</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="60" t="s">
+        <v>556</v>
+      </c>
+      <c r="B31" s="69" t="s">
+        <v>557</v>
+      </c>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="60" t="s">
+        <v>558</v>
+      </c>
+      <c r="B32" s="69" t="s">
+        <v>559</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="60" t="s">
+        <v>560</v>
+      </c>
+      <c r="B33" s="69" t="s">
+        <v>561</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="60" t="s">
+        <v>562</v>
+      </c>
+      <c r="B34" s="69" t="s">
+        <v>563</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B12" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -5720,94 +5814,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="70" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="70" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="70" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="70" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="70" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="70" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="70" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="70" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="71" t="s">
+      <c r="J1" s="70" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="70" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="71" t="s">
+      <c r="L1" s="70" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="70" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="71" t="s">
+      <c r="N1" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="71" t="s">
+      <c r="O1" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="71" t="s">
+      <c r="P1" s="70" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="71" t="s">
+      <c r="Q1" s="70" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="74" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="72"/>
-      <c r="T1" s="75" t="s">
+      <c r="S1" s="74"/>
+      <c r="T1" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="73"/>
-      <c r="V1" s="72" t="s">
+      <c r="U1" s="71"/>
+      <c r="V1" s="74" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="73" t="s">
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="74"/>
+      <c r="AA1" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="76" t="s">
+      <c r="AB1" s="75" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -5835,8 +5929,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="74"/>
+      <c r="AA2" s="72"/>
+      <c r="AB2" s="72"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -5892,17 +5986,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -5913,6 +5996,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update more initial user
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="14" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="594">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2085,6 +2085,66 @@
   <si>
     <t>Firm Auvenir</t>
   </si>
+  <si>
+    <t>SUPER ADMIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doai </t>
+  </si>
+  <si>
+    <t>Tran</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e43</t>
+  </si>
+  <si>
+    <t>User4</t>
+  </si>
+  <si>
+    <t>chr.auvenirad@gmail.com</t>
+  </si>
+  <si>
+    <t>chr.auvenirclient01@gmail.com</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>client1</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e44</t>
+  </si>
+  <si>
+    <t>User5</t>
+  </si>
+  <si>
+    <t>chr.auvenirauditor01@gmail.com</t>
+  </si>
+  <si>
+    <t>User6</t>
+  </si>
+  <si>
+    <t>AUDITOR</t>
+  </si>
+  <si>
+    <t>auditor</t>
+  </si>
+  <si>
+    <t>auditor1</t>
+  </si>
+  <si>
+    <t>58f707a6004d69fc2aeb8e45</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "chr.auvenirauditor01@gmail.com","type" : "AUDITOR","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "tran","firstName" : "doai","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "chr.auvenirclient01@gmail.com","type" : "CLIENT","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "tran","firstName" : "doai","__v" : 0}</t>
+  </si>
+  <si>
+    <t>{"status" : "ACTIVE","email" : "chr.auvenirad@gmail.com","type" : "SUPER ADMIN","notifications" : {"todoCompleted" : {"email" : false},"fileUpload" : {"email" : false},"newRequest" : {"email" : false},"newComment" : {"email" : false},"newTodo" : {"email" : false},"documentUploaded" : {"email" : false},"joinEngagement" : {"email" : false},"engagementInvite" : {"email" : false}},"referral" : "","agreements" : [],"integrations" : [],"verified" : false,"phone" : "","jobTitle" : "auditor","lastName" : "tran","firstName" : "doai","__v" : 0}</t>
+  </si>
 </sst>
 </file>
 
@@ -2296,7 +2356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2441,11 +2501,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2454,6 +2512,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3219,11 +3280,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="79"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3845,7 +3906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
@@ -4023,7 +4084,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4053,7 +4114,7 @@
       <c r="A3" s="60" t="s">
         <v>369</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="47" t="s">
         <v>242</v>
       </c>
     </row>
@@ -4143,6 +4204,7 @@
     <hyperlink ref="B12" r:id="rId2"/>
     <hyperlink ref="B2" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4770,7 +4832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
@@ -5417,8 +5479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5524,7 +5586,7 @@
         <v>246</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>290</v>
+        <v>522</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>348</v>
@@ -5823,94 +5885,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="71" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="70" t="s">
+      <c r="H1" s="71" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="71" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="71" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="70" t="s">
+      <c r="K1" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="70" t="s">
+      <c r="L1" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="70" t="s">
+      <c r="M1" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="70" t="s">
+      <c r="N1" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="70" t="s">
+      <c r="O1" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="70" t="s">
+      <c r="P1" s="71" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="70" t="s">
+      <c r="Q1" s="71" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="71" t="s">
+      <c r="R1" s="75" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="71"/>
+      <c r="S1" s="75"/>
       <c r="T1" s="74" t="s">
         <v>196</v>
       </c>
       <c r="U1" s="72"/>
-      <c r="V1" s="71" t="s">
+      <c r="V1" s="75" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
       <c r="AA1" s="72" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="75" t="s">
+      <c r="AB1" s="76" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -5995,17 +6057,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -6016,6 +6067,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6024,17 +6086,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="59"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
@@ -6042,9 +6104,10 @@
     <col min="8" max="8" width="23.7109375" customWidth="1"/>
     <col min="9" max="9" width="29.5703125" customWidth="1"/>
     <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>241</v>
       </c>
@@ -6085,7 +6148,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>519</v>
       </c>
@@ -6129,7 +6192,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>520</v>
       </c>
@@ -6173,7 +6236,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>521</v>
       </c>
@@ -6217,40 +6280,177 @@
         <v>566</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="47"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="47"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="47"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
+        <v>578</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>579</v>
+      </c>
+      <c r="C5" t="s">
+        <v>574</v>
+      </c>
+      <c r="D5" t="s">
+        <v>575</v>
+      </c>
+      <c r="E5" t="s">
+        <v>576</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>577</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="I5" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="J5" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="K5" s="59" t="s">
+        <v>593</v>
+      </c>
+      <c r="L5" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="M5" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="N5" s="59" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
+        <v>584</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>580</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>581</v>
+      </c>
+      <c r="E6" t="s">
+        <v>582</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>583</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="I6" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="J6" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="K6" s="59" t="s">
+        <v>592</v>
+      </c>
+      <c r="L6" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="M6" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="N6" s="59" t="s">
+        <v>566</v>
+      </c>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="59"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
+        <v>586</v>
+      </c>
+      <c r="B7" s="70" t="s">
+        <v>585</v>
+      </c>
+      <c r="C7" t="s">
+        <v>587</v>
+      </c>
+      <c r="D7" t="s">
+        <v>588</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>589</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>590</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="J7" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="K7" s="59" t="s">
+        <v>591</v>
+      </c>
+      <c r="L7" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="M7" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="N7" s="59" t="s">
+        <v>566</v>
+      </c>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="47"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="47"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="47"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="47"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="47"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="47"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="47"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="47"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="47"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
@@ -6276,9 +6476,12 @@
     <hyperlink ref="B3" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -6286,7 +6489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
data provider for group permission
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="14" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="18" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="581">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2080,10 +2080,31 @@
     <t>Lead Client Email Password</t>
   </si>
   <si>
-    <t>Auvenir Thuan</t>
-  </si>
-  <si>
     <t>Firm Auvenir</t>
+  </si>
+  <si>
+    <t>Category 1</t>
+  </si>
+  <si>
+    <t>Lead Auditor Comment  1</t>
+  </si>
+  <si>
+    <t>General Auditor Comment  4</t>
+  </si>
+  <si>
+    <t>Auvenir Company</t>
+  </si>
+  <si>
+    <t>To Do 5 name</t>
+  </si>
+  <si>
+    <t>To Do 6 name</t>
+  </si>
+  <si>
+    <t>ToDo 06</t>
+  </si>
+  <si>
+    <t>ToDo 05</t>
   </si>
 </sst>
 </file>
@@ -2296,7 +2317,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2441,6 +2462,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3219,11 +3242,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="78"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="80"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3490,8 +3513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4768,16 +4791,17 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5703125" style="59" customWidth="1"/>
-    <col min="2" max="3" width="25.28515625" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="59" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" style="59" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="59"/>
   </cols>
@@ -4822,7 +4846,7 @@
       <c r="A4" s="60" t="s">
         <v>567</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="16" t="s">
         <v>242</v>
       </c>
       <c r="C4" s="7"/>
@@ -5021,7 +5045,7 @@
         <v>333</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -5068,83 +5092,135 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
-        <v>550</v>
-      </c>
-      <c r="B28" s="69" t="s">
-        <v>551</v>
+        <v>577</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>580</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="s">
-        <v>552</v>
-      </c>
-      <c r="B29" s="69" t="s">
-        <v>553</v>
+        <v>578</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>579</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="60" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B30" s="69" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="60" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B31" s="69" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B32" s="69" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="60" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B33" s="69" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="60" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B34" s="69" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>573</v>
+        <v>560</v>
+      </c>
+      <c r="B35" s="69" t="s">
+        <v>561</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="60" t="s">
+        <v>562</v>
+      </c>
+      <c r="B36" s="69" t="s">
+        <v>563</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="52" t="s">
+        <v>329</v>
+      </c>
+      <c r="B38" s="70" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="52" t="s">
+        <v>574</v>
+      </c>
+      <c r="B39" s="70" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="59" t="s">
+        <v>308</v>
+      </c>
+      <c r="B40" s="59" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="71" t="s">
+        <v>575</v>
+      </c>
+      <c r="B41" s="58" t="s">
+        <v>575</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5152,9 +5228,10 @@
     <hyperlink ref="B6" r:id="rId2"/>
     <hyperlink ref="B9" r:id="rId3"/>
     <hyperlink ref="B12" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -5823,94 +5900,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="72" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="72" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="70" t="s">
+      <c r="H1" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="72" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="70" t="s">
+      <c r="K1" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="70" t="s">
+      <c r="L1" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="70" t="s">
+      <c r="M1" s="72" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="70" t="s">
+      <c r="N1" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="70" t="s">
+      <c r="O1" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="70" t="s">
+      <c r="P1" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="70" t="s">
+      <c r="Q1" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="71" t="s">
+      <c r="R1" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="71"/>
-      <c r="T1" s="74" t="s">
+      <c r="S1" s="73"/>
+      <c r="T1" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="72"/>
-      <c r="V1" s="71" t="s">
+      <c r="U1" s="74"/>
+      <c r="V1" s="73" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
-      <c r="Z1" s="71"/>
-      <c r="AA1" s="72" t="s">
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="74" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="75" t="s">
+      <c r="AB1" s="77" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -5938,8 +6015,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">

</xml_diff>

<commit_message>
Vienpham add dataprovider @47,48, 53, 54
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="604">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2166,6 +2166,15 @@
   <si>
     <t>General Auditor Comment  4</t>
   </si>
+  <si>
+    <t>Lead Comment  1</t>
+  </si>
+  <si>
+    <t>General Client Comment  2</t>
+  </si>
+  <si>
+    <t>LeadClient 1</t>
+  </si>
 </sst>
 </file>
 
@@ -2377,7 +2386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2523,6 +2532,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3301,11 +3311,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="80"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4851,10 +4861,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5289,6 +5299,22 @@
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="60" t="s">
+        <v>601</v>
+      </c>
+      <c r="B42" s="71" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="60" t="s">
+        <v>602</v>
+      </c>
+      <c r="B43" s="59" t="s">
+        <v>602</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5968,94 +5994,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="72" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="72" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="72" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="72" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="71" t="s">
+      <c r="J1" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="72" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="71" t="s">
+      <c r="L1" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="72" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="71" t="s">
+      <c r="N1" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="71" t="s">
+      <c r="O1" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="71" t="s">
+      <c r="P1" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="71" t="s">
+      <c r="Q1" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="72"/>
-      <c r="T1" s="75" t="s">
+      <c r="S1" s="73"/>
+      <c r="T1" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="73"/>
-      <c r="V1" s="72" t="s">
+      <c r="U1" s="74"/>
+      <c r="V1" s="73" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="73" t="s">
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
+      <c r="AA1" s="74" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="76" t="s">
+      <c r="AB1" s="77" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -6083,8 +6109,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="74"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">

</xml_diff>

<commit_message>
Vienpham update TEstData permision test
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -2173,7 +2173,7 @@
     <t>General Client Comment  2</t>
   </si>
   <si>
-    <t>LeadClient 1</t>
+    <t>Lead Client 1</t>
   </si>
 </sst>
 </file>
@@ -2536,9 +2536,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2546,6 +2543,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4863,8 +4863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6042,22 +6042,22 @@
       <c r="Q1" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="73" t="s">
+      <c r="R1" s="76" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="73"/>
-      <c r="T1" s="76" t="s">
+      <c r="S1" s="76"/>
+      <c r="T1" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="74"/>
-      <c r="V1" s="73" t="s">
+      <c r="U1" s="73"/>
+      <c r="V1" s="76" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="74" t="s">
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="73" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="77" t="s">
@@ -6109,8 +6109,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="75"/>
-      <c r="AB2" s="75"/>
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="74"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -6166,17 +6166,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -6187,6 +6176,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
refactor dataprovider: sheetname, column, add more in excel
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="619">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2175,12 +2175,57 @@
   <si>
     <t>Lead Client 1</t>
   </si>
+  <si>
+    <t>Lead Auditor Full Name</t>
+  </si>
+  <si>
+    <t>Admin Client Full Name</t>
+  </si>
+  <si>
+    <t>Role Client</t>
+  </si>
+  <si>
+    <t>Client Phone Number</t>
+  </si>
+  <si>
+    <t>Parent Stack Holder</t>
+  </si>
+  <si>
+    <t>Auvenir Auditor</t>
+  </si>
+  <si>
+    <t>Lead Client Full Name</t>
+  </si>
+  <si>
+    <t>Your engagement invitation has been sent.</t>
+  </si>
+  <si>
+    <t>Your team member has been removed.</t>
+  </si>
+  <si>
+    <t>Success Message Invitation</t>
+  </si>
+  <si>
+    <t>Success Message Remove Team Member</t>
+  </si>
+  <si>
+    <t>Client Full Name</t>
+  </si>
+  <si>
+    <t>Auvenir Client</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>Lead Text</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2236,6 +2281,12 @@
       <b/>
       <sz val="9"/>
       <color rgb="FF000080"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11.3"/>
+      <color rgb="FFA581FF"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -2386,7 +2437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2532,7 +2583,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2559,6 +2609,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3311,11 +3369,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="80"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="79"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -3583,7 +3641,7 @@
   <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3862,7 +3920,7 @@
     <hyperlink ref="C2" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -3871,7 +3929,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4597,7 +4655,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4861,10 +4919,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4962,31 +5020,31 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
-        <v>244</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>531</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="D9" s="7"/>
+    <row r="9" spans="1:4" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="83" t="s">
+        <v>604</v>
+      </c>
+      <c r="B9" s="82" t="s">
+        <v>528</v>
+      </c>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
-        <v>288</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="C10" s="7"/>
+        <v>244</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>531</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>170</v>
+      </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>242</v>
@@ -4996,51 +5054,49 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
-        <v>532</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>533</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>168</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" s="7"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
-        <v>534</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+    <row r="13" spans="1:4" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="83" t="s">
+        <v>398</v>
+      </c>
+      <c r="B13" s="82" t="s">
+        <v>609</v>
+      </c>
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
-        <v>570</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="C14" s="7"/>
+        <v>532</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>533</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>536</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>168</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
-        <v>537</v>
+        <v>570</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>242</v>
@@ -5048,22 +5104,22 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
-        <v>571</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+    <row r="17" spans="1:4" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="83" t="s">
+        <v>605</v>
+      </c>
+      <c r="B17" s="82" t="s">
+        <v>532</v>
+      </c>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
-        <v>245</v>
+        <v>535</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C18" s="28" t="s">
         <v>168</v>
@@ -5072,7 +5128,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>281</v>
+        <v>537</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>242</v>
@@ -5082,7 +5138,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
-        <v>280</v>
+        <v>571</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>242</v>
@@ -5090,238 +5146,544 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="60" t="s">
-        <v>539</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>540</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
+    <row r="21" spans="1:4" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="83" t="s">
+        <v>610</v>
+      </c>
+      <c r="B21" s="82" t="s">
+        <v>535</v>
+      </c>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="s">
-        <v>541</v>
+        <v>245</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>542</v>
-      </c>
-      <c r="C22" s="7"/>
+        <v>538</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>168</v>
+      </c>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="60" t="s">
-        <v>333</v>
+        <v>281</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>593</v>
+        <v>242</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
-        <v>543</v>
+        <v>280</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>330</v>
+        <v>242</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="60" t="s">
-        <v>544</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>545</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+    <row r="25" spans="1:4" s="81" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="83" t="s">
+        <v>615</v>
+      </c>
+      <c r="B25" s="82" t="s">
+        <v>616</v>
+      </c>
+      <c r="C25" s="82"/>
+      <c r="D25" s="82"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="60" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
-        <v>594</v>
+        <v>333</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="s">
-        <v>596</v>
+        <v>543</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>597</v>
+        <v>330</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="60" t="s">
-        <v>550</v>
-      </c>
-      <c r="B30" s="69" t="s">
-        <v>551</v>
+        <v>544</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>545</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="60" t="s">
-        <v>552</v>
-      </c>
-      <c r="B31" s="69" t="s">
-        <v>553</v>
+        <v>546</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>547</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
-        <v>554</v>
-      </c>
-      <c r="B32" s="69" t="s">
-        <v>555</v>
+        <v>548</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>549</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="60" t="s">
-        <v>556</v>
-      </c>
-      <c r="B33" s="69" t="s">
-        <v>557</v>
+        <v>594</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>595</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="60" t="s">
-        <v>558</v>
-      </c>
-      <c r="B34" s="69" t="s">
-        <v>559</v>
+        <v>596</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>597</v>
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="60" t="s">
-        <v>560</v>
+        <v>550</v>
       </c>
       <c r="B35" s="69" t="s">
-        <v>561</v>
+        <v>551</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="60" t="s">
-        <v>562</v>
+        <v>552</v>
       </c>
       <c r="B36" s="69" t="s">
-        <v>563</v>
+        <v>553</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>572</v>
+        <v>554</v>
+      </c>
+      <c r="B37" s="69" t="s">
+        <v>555</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="60" t="s">
-        <v>329</v>
+        <v>556</v>
       </c>
       <c r="B38" s="69" t="s">
-        <v>598</v>
+        <v>557</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="60" t="s">
-        <v>599</v>
+        <v>558</v>
       </c>
       <c r="B39" s="69" t="s">
-        <v>599</v>
+        <v>559</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="60" t="s">
-        <v>308</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>306</v>
+        <v>560</v>
+      </c>
+      <c r="B40" s="69" t="s">
+        <v>561</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="60" t="s">
-        <v>600</v>
+        <v>562</v>
       </c>
       <c r="B41" s="69" t="s">
-        <v>600</v>
+        <v>563</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
-        <v>601</v>
-      </c>
-      <c r="B42" s="71" t="s">
-        <v>603</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="60" t="s">
+        <v>329</v>
+      </c>
+      <c r="B43" s="69" t="s">
+        <v>598</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="60" t="s">
+        <v>599</v>
+      </c>
+      <c r="B44" s="69" t="s">
+        <v>599</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="60" t="s">
+        <v>308</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="60" t="s">
+        <v>600</v>
+      </c>
+      <c r="B46" s="69" t="s">
+        <v>600</v>
+      </c>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="60" t="s">
+        <v>601</v>
+      </c>
+      <c r="B47" s="69" t="s">
+        <v>603</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="60" t="s">
         <v>602</v>
       </c>
-      <c r="B43" s="59" t="s">
+      <c r="B48" s="7" t="s">
         <v>602</v>
       </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="80" t="s">
+        <v>243</v>
+      </c>
+      <c r="B49" s="82" t="s">
+        <v>522</v>
+      </c>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="B50" s="82" t="s">
+        <v>242</v>
+      </c>
+      <c r="C50" s="82"/>
+      <c r="D50" s="82"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="82" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="82"/>
+      <c r="D51" s="82"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="82">
+        <v>4167877865</v>
+      </c>
+      <c r="C52" s="82"/>
+      <c r="D52" s="82"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="82" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="82"/>
+      <c r="D53" s="82"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="82" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" s="82"/>
+      <c r="D54" s="82"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="83" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="82" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="82"/>
+      <c r="D55" s="82"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="83" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="C56" s="82"/>
+      <c r="D56" s="82"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="83" t="s">
+        <v>11</v>
+      </c>
+      <c r="B57" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="82"/>
+      <c r="D57" s="82"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="83" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="82">
+        <v>12</v>
+      </c>
+      <c r="C58" s="82"/>
+      <c r="D58" s="82"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="83" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="C59" s="82"/>
+      <c r="D59" s="82"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="83" t="s">
+        <v>15</v>
+      </c>
+      <c r="B60" s="82" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="82"/>
+      <c r="D60" s="82"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="83" t="s">
+        <v>356</v>
+      </c>
+      <c r="B61" s="82" t="s">
+        <v>357</v>
+      </c>
+      <c r="C61" s="82"/>
+      <c r="D61" s="82"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="82" t="s">
+        <v>70</v>
+      </c>
+      <c r="C62" s="82"/>
+      <c r="D62" s="82"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="B63" s="82">
+        <v>165782</v>
+      </c>
+      <c r="C63" s="82"/>
+      <c r="D63" s="82"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="84">
+        <v>43012</v>
+      </c>
+      <c r="C64" s="82"/>
+      <c r="D64" s="82"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="83" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" s="82">
+        <v>1234567890</v>
+      </c>
+      <c r="C65" s="82"/>
+      <c r="D65" s="82"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="82" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="82"/>
+      <c r="D66" s="82"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" s="82" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" s="82"/>
+      <c r="D67" s="82"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="83" t="s">
+        <v>606</v>
+      </c>
+      <c r="B68" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="C68" s="82"/>
+      <c r="D68" s="82"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="83" t="s">
+        <v>607</v>
+      </c>
+      <c r="B69" s="85">
+        <v>1234567899</v>
+      </c>
+      <c r="C69" s="82"/>
+      <c r="D69" s="82"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="83" t="s">
+        <v>608</v>
+      </c>
+      <c r="B70" s="85" t="s">
+        <v>432</v>
+      </c>
+      <c r="C70" s="82"/>
+      <c r="D70" s="82"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="83" t="s">
+        <v>613</v>
+      </c>
+      <c r="B71" s="85" t="s">
+        <v>611</v>
+      </c>
+      <c r="C71" s="82"/>
+      <c r="D71" s="82"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="83" t="s">
+        <v>614</v>
+      </c>
+      <c r="B72" s="85" t="s">
+        <v>612</v>
+      </c>
+      <c r="C72" s="82"/>
+      <c r="D72" s="82"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="83" t="s">
+        <v>618</v>
+      </c>
+      <c r="B73" s="85" t="s">
+        <v>617</v>
+      </c>
+      <c r="C73" s="82"/>
+      <c r="D73" s="82"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B12" r:id="rId4"/>
+    <hyperlink ref="B10" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId4"/>
     <hyperlink ref="B4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5994,94 +6356,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="71" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="71" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="71" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="71" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="71" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="71" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="71" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="72" t="s">
+      <c r="J1" s="71" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="71" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="71" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="72" t="s">
+      <c r="M1" s="71" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="72" t="s">
+      <c r="N1" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="72" t="s">
+      <c r="O1" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="72" t="s">
+      <c r="P1" s="71" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="72" t="s">
+      <c r="Q1" s="71" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="76" t="s">
+      <c r="R1" s="75" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="76"/>
-      <c r="T1" s="75" t="s">
+      <c r="S1" s="75"/>
+      <c r="T1" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="73"/>
-      <c r="V1" s="76" t="s">
+      <c r="U1" s="72"/>
+      <c r="V1" s="75" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="76"/>
-      <c r="AA1" s="73" t="s">
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="72" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="77" t="s">
+      <c r="AB1" s="76" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="71"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -6109,8 +6471,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="74"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -6599,7 +6961,7 @@
   <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="A20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7474,6 +7836,6 @@
     <hyperlink ref="B24" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add prefix for some cases
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -2225,7 +2225,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2281,12 +2281,6 @@
       <b/>
       <sz val="9"/>
       <color rgb="FF000080"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11.3"/>
-      <color rgb="FFA581FF"/>
       <name val="Courier New"/>
       <family val="3"/>
     </font>
@@ -2437,7 +2431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2583,8 +2577,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2593,9 +2595,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2609,14 +2608,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3369,11 +3360,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="78"/>
-      <c r="E1" s="79"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="84"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>
@@ -4921,8 +4912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5020,15 +5011,15 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" s="81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="83" t="s">
+    <row r="9" spans="1:4" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="74" t="s">
         <v>604</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="73" t="s">
         <v>528</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
@@ -5062,15 +5053,15 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" s="81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="83" t="s">
+    <row r="13" spans="1:4" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="74" t="s">
         <v>398</v>
       </c>
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="73" t="s">
         <v>609</v>
       </c>
-      <c r="C13" s="82"/>
-      <c r="D13" s="82"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
@@ -5104,15 +5095,15 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" s="81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="83" t="s">
+    <row r="17" spans="1:4" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="74" t="s">
         <v>605</v>
       </c>
-      <c r="B17" s="82" t="s">
+      <c r="B17" s="73" t="s">
         <v>532</v>
       </c>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
@@ -5146,15 +5137,15 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" s="81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="83" t="s">
+    <row r="21" spans="1:4" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="74" t="s">
         <v>610</v>
       </c>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="73" t="s">
         <v>535</v>
       </c>
-      <c r="C21" s="82"/>
-      <c r="D21" s="82"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="s">
@@ -5188,15 +5179,15 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" s="81" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="83" t="s">
+    <row r="25" spans="1:4" s="72" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="74" t="s">
         <v>615</v>
       </c>
-      <c r="B25" s="82" t="s">
+      <c r="B25" s="73" t="s">
         <v>616</v>
       </c>
-      <c r="C25" s="82"/>
-      <c r="D25" s="82"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="s">
@@ -5429,254 +5420,254 @@
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="80" t="s">
+      <c r="A49" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="B49" s="82" t="s">
+      <c r="B49" s="73" t="s">
         <v>522</v>
       </c>
-      <c r="C49" s="82"/>
-      <c r="D49" s="82"/>
+      <c r="C49" s="73"/>
+      <c r="D49" s="73"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="80" t="s">
+      <c r="A50" s="71" t="s">
         <v>289</v>
       </c>
-      <c r="B50" s="82" t="s">
+      <c r="B50" s="73" t="s">
         <v>242</v>
       </c>
-      <c r="C50" s="82"/>
-      <c r="D50" s="82"/>
+      <c r="C50" s="73"/>
+      <c r="D50" s="73"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="83" t="s">
+      <c r="A51" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="82" t="s">
+      <c r="B51" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="C51" s="82"/>
-      <c r="D51" s="82"/>
+      <c r="C51" s="73"/>
+      <c r="D51" s="73"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="83" t="s">
+      <c r="A52" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="82">
+      <c r="B52" s="73">
         <v>4167877865</v>
       </c>
-      <c r="C52" s="82"/>
-      <c r="D52" s="82"/>
+      <c r="C52" s="73"/>
+      <c r="D52" s="73"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="83" t="s">
+      <c r="A53" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="82" t="s">
+      <c r="B53" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="C53" s="82"/>
-      <c r="D53" s="82"/>
+      <c r="C53" s="73"/>
+      <c r="D53" s="73"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="83" t="s">
+      <c r="A54" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B54" s="82" t="s">
+      <c r="B54" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="C54" s="82"/>
-      <c r="D54" s="82"/>
+      <c r="C54" s="73"/>
+      <c r="D54" s="73"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="83" t="s">
+      <c r="A55" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B55" s="82" t="s">
+      <c r="B55" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="82"/>
-      <c r="D55" s="82"/>
+      <c r="C55" s="73"/>
+      <c r="D55" s="73"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="83" t="s">
+      <c r="A56" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="82" t="s">
+      <c r="B56" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="C56" s="82"/>
-      <c r="D56" s="82"/>
+      <c r="C56" s="73"/>
+      <c r="D56" s="73"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="83" t="s">
+      <c r="A57" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="B57" s="82" t="s">
+      <c r="B57" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="82"/>
-      <c r="D57" s="82"/>
+      <c r="C57" s="73"/>
+      <c r="D57" s="73"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="83" t="s">
+      <c r="A58" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="82">
+      <c r="B58" s="73">
         <v>12</v>
       </c>
-      <c r="C58" s="82"/>
-      <c r="D58" s="82"/>
+      <c r="C58" s="73"/>
+      <c r="D58" s="73"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="83" t="s">
+      <c r="A59" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="82" t="s">
+      <c r="B59" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="C59" s="82"/>
-      <c r="D59" s="82"/>
+      <c r="C59" s="73"/>
+      <c r="D59" s="73"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="83" t="s">
+      <c r="A60" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="82" t="s">
+      <c r="B60" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C60" s="82"/>
-      <c r="D60" s="82"/>
+      <c r="C60" s="73"/>
+      <c r="D60" s="73"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="83" t="s">
+      <c r="A61" s="74" t="s">
         <v>356</v>
       </c>
-      <c r="B61" s="82" t="s">
+      <c r="B61" s="73" t="s">
         <v>357</v>
       </c>
-      <c r="C61" s="82"/>
-      <c r="D61" s="82"/>
+      <c r="C61" s="73"/>
+      <c r="D61" s="73"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="83" t="s">
+      <c r="A62" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="B62" s="82" t="s">
+      <c r="B62" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="C62" s="82"/>
-      <c r="D62" s="82"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="73"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="83" t="s">
+      <c r="A63" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="B63" s="82">
+      <c r="B63" s="73">
         <v>165782</v>
       </c>
-      <c r="C63" s="82"/>
-      <c r="D63" s="82"/>
+      <c r="C63" s="73"/>
+      <c r="D63" s="73"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="83" t="s">
+      <c r="A64" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="84">
+      <c r="B64" s="75">
         <v>43012</v>
       </c>
-      <c r="C64" s="82"/>
-      <c r="D64" s="82"/>
+      <c r="C64" s="73"/>
+      <c r="D64" s="73"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="83" t="s">
+      <c r="A65" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="B65" s="82">
+      <c r="B65" s="73">
         <v>1234567890</v>
       </c>
-      <c r="C65" s="82"/>
-      <c r="D65" s="82"/>
+      <c r="C65" s="73"/>
+      <c r="D65" s="73"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="83" t="s">
+      <c r="A66" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B66" s="82" t="s">
+      <c r="B66" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="82"/>
-      <c r="D66" s="82"/>
+      <c r="C66" s="73"/>
+      <c r="D66" s="73"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="83" t="s">
+      <c r="A67" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="B67" s="82" t="s">
+      <c r="B67" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="C67" s="82"/>
-      <c r="D67" s="82"/>
+      <c r="C67" s="73"/>
+      <c r="D67" s="73"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="83" t="s">
+      <c r="A68" s="74" t="s">
         <v>606</v>
       </c>
-      <c r="B68" s="82" t="s">
+      <c r="B68" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C68" s="82"/>
-      <c r="D68" s="82"/>
+      <c r="C68" s="73"/>
+      <c r="D68" s="73"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="83" t="s">
+      <c r="A69" s="74" t="s">
         <v>607</v>
       </c>
-      <c r="B69" s="85">
+      <c r="B69" s="73">
         <v>1234567899</v>
       </c>
-      <c r="C69" s="82"/>
-      <c r="D69" s="82"/>
+      <c r="C69" s="73"/>
+      <c r="D69" s="73"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="83" t="s">
+      <c r="A70" s="74" t="s">
         <v>608</v>
       </c>
-      <c r="B70" s="85" t="s">
+      <c r="B70" s="73" t="s">
         <v>432</v>
       </c>
-      <c r="C70" s="82"/>
-      <c r="D70" s="82"/>
+      <c r="C70" s="73"/>
+      <c r="D70" s="73"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="83" t="s">
+      <c r="A71" s="74" t="s">
         <v>613</v>
       </c>
-      <c r="B71" s="85" t="s">
+      <c r="B71" s="73" t="s">
         <v>611</v>
       </c>
-      <c r="C71" s="82"/>
-      <c r="D71" s="82"/>
+      <c r="C71" s="73"/>
+      <c r="D71" s="73"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="83" t="s">
+      <c r="A72" s="74" t="s">
         <v>614</v>
       </c>
-      <c r="B72" s="85" t="s">
+      <c r="B72" s="73" t="s">
         <v>612</v>
       </c>
-      <c r="C72" s="82"/>
-      <c r="D72" s="82"/>
+      <c r="C72" s="73"/>
+      <c r="D72" s="73"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="83" t="s">
+      <c r="A73" s="74" t="s">
         <v>618</v>
       </c>
-      <c r="B73" s="85" t="s">
+      <c r="B73" s="73" t="s">
         <v>617</v>
       </c>
-      <c r="C73" s="82"/>
-      <c r="D73" s="82"/>
+      <c r="C73" s="73"/>
+      <c r="D73" s="73"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6356,94 +6347,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="76" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="76" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="76" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="76" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="76" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="71" t="s">
+      <c r="H1" s="76" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="76" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="71" t="s">
+      <c r="J1" s="76" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="71" t="s">
+      <c r="K1" s="76" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="71" t="s">
+      <c r="L1" s="76" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="76" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="71" t="s">
+      <c r="N1" s="76" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="71" t="s">
+      <c r="O1" s="76" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="71" t="s">
+      <c r="P1" s="76" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="71" t="s">
+      <c r="Q1" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="75" t="s">
+      <c r="R1" s="77" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="75"/>
-      <c r="T1" s="74" t="s">
+      <c r="S1" s="77"/>
+      <c r="T1" s="80" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="72"/>
-      <c r="V1" s="75" t="s">
+      <c r="U1" s="78"/>
+      <c r="V1" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="72" t="s">
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="78" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="76" t="s">
+      <c r="AB1" s="81" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -6471,8 +6462,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -6528,6 +6519,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -6538,17 +6540,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Create GroupPermissionTodoTest, fix issue wait element not displayed
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="583">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2105,6 +2105,12 @@
   </si>
   <si>
     <t>ToDo 05</t>
+  </si>
+  <si>
+    <t>General Auditor Comment 4</t>
+  </si>
+  <si>
+    <t>Lead Auditor Comment 1</t>
   </si>
 </sst>
 </file>
@@ -2467,9 +2473,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2477,6 +2480,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4793,8 +4799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4960,7 +4966,7 @@
       <c r="A15" s="60" t="s">
         <v>535</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="16" t="s">
         <v>536</v>
       </c>
       <c r="C15" s="28" t="s">
@@ -5203,7 +5209,7 @@
         <v>574</v>
       </c>
       <c r="B39" s="70" t="s">
-        <v>574</v>
+        <v>582</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -5219,7 +5225,7 @@
         <v>575</v>
       </c>
       <c r="B41" s="58" t="s">
-        <v>575</v>
+        <v>581</v>
       </c>
     </row>
   </sheetData>
@@ -5229,9 +5235,10 @@
     <hyperlink ref="B9" r:id="rId3"/>
     <hyperlink ref="B12" r:id="rId4"/>
     <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="B15" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -5948,22 +5955,22 @@
       <c r="Q1" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="73" t="s">
+      <c r="R1" s="76" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="73"/>
-      <c r="T1" s="76" t="s">
+      <c r="S1" s="76"/>
+      <c r="T1" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="74"/>
-      <c r="V1" s="73" t="s">
+      <c r="U1" s="73"/>
+      <c r="V1" s="76" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
-      <c r="AA1" s="74" t="s">
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="73" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="77" t="s">
@@ -6015,8 +6022,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="75"/>
-      <c r="AB2" s="75"/>
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="74"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -6072,17 +6079,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -6093,6 +6089,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update 2 test for admin and super admin on Group permission
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="15" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="601">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -3282,7 +3282,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4853,7 +4853,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
@@ -5560,232 +5560,239 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24" customWidth="1"/>
-    <col min="15" max="15" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.42578125" customWidth="1"/>
-    <col min="19" max="19" width="28" customWidth="1"/>
-    <col min="20" max="20" width="17.42578125" customWidth="1"/>
-    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="59" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24" customWidth="1"/>
+    <col min="16" max="16" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.42578125" customWidth="1"/>
+    <col min="20" max="20" width="28" customWidth="1"/>
+    <col min="21" max="21" width="17.42578125" customWidth="1"/>
+    <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="60" t="s">
+        <v>371</v>
+      </c>
+      <c r="C1" s="56" t="s">
         <v>243</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="D1" s="56" t="s">
         <v>244</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="E1" s="56" t="s">
         <v>245</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="F1" s="56" t="s">
         <v>304</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="G1" s="52" t="s">
         <v>293</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="H1" s="52" t="s">
         <v>289</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="I1" s="52" t="s">
         <v>288</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="J1" s="52" t="s">
         <v>281</v>
       </c>
-      <c r="J1" s="56" t="s">
+      <c r="K1" s="56" t="s">
         <v>291</v>
       </c>
-      <c r="K1" s="56" t="s">
+      <c r="L1" s="56" t="s">
         <v>292</v>
       </c>
-      <c r="L1" s="56" t="s">
+      <c r="M1" s="56" t="s">
         <v>280</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="N1" s="52" t="s">
         <v>295</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="O1" s="52" t="s">
         <v>294</v>
       </c>
-      <c r="O1" s="52" t="s">
+      <c r="P1" s="52" t="s">
         <v>283</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="Q1" s="52" t="s">
         <v>305</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="R1" s="52" t="s">
         <v>307</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="S1" s="52" t="s">
         <v>308</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="T1" s="52" t="s">
         <v>286</v>
       </c>
-      <c r="T1" s="52" t="s">
+      <c r="U1" s="52" t="s">
         <v>296</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="V1" s="52" t="s">
         <v>297</v>
       </c>
-      <c r="V1" s="52" t="s">
+      <c r="W1" s="52" t="s">
         <v>298</v>
       </c>
-      <c r="W1" s="52" t="s">
+      <c r="X1" s="52" t="s">
         <v>299</v>
       </c>
-      <c r="X1" s="52" t="s">
+      <c r="Y1" s="52" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="55" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="55" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="47" t="s">
+        <v>387</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>522</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="E2" s="16" t="s">
         <v>349</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="G2" s="57" t="s">
         <v>285</v>
-      </c>
-      <c r="G2" s="57" t="s">
-        <v>242</v>
       </c>
       <c r="H2" s="57" t="s">
         <v>242</v>
       </c>
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="57" t="s">
         <v>242</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="K2" s="57" t="s">
         <v>316</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="L2" s="57" t="s">
         <v>242</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="M2" s="57" t="s">
         <v>316</v>
       </c>
-      <c r="M2" s="57" t="s">
+      <c r="N2" s="57" t="s">
         <v>242</v>
       </c>
-      <c r="N2" s="58" t="s">
+      <c r="O2" s="58" t="s">
         <v>311</v>
       </c>
-      <c r="O2" s="55" t="s">
+      <c r="P2" s="55" t="s">
         <v>284</v>
       </c>
-      <c r="P2" s="55" t="s">
+      <c r="Q2" s="55" t="s">
         <v>350</v>
       </c>
-      <c r="Q2" s="55" t="s">
+      <c r="R2" s="55" t="s">
         <v>287</v>
       </c>
-      <c r="R2" s="55" t="s">
+      <c r="S2" s="55" t="s">
         <v>306</v>
       </c>
-      <c r="S2" s="55" t="s">
+      <c r="T2" s="55" t="s">
         <v>312</v>
       </c>
-      <c r="T2" s="55" t="s">
+      <c r="U2" s="55" t="s">
         <v>300</v>
       </c>
-      <c r="U2" s="55" t="s">
+      <c r="V2" s="55" t="s">
         <v>301</v>
       </c>
-      <c r="V2" s="55" t="s">
+      <c r="W2" s="55" t="s">
         <v>302</v>
       </c>
-      <c r="W2" s="55" t="s">
+      <c r="X2" s="55" t="s">
         <v>310</v>
       </c>
-      <c r="X2" s="55" t="s">
+      <c r="Y2" s="55" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>247</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="C3" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="16" t="s">
         <v>249</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="55"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="55"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H3" s="55"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="56" t="s">
         <v>253</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="C4" s="47" t="s">
         <v>256</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="D4" s="47" t="s">
         <v>254</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="E4" s="47" t="s">
         <v>255</v>
       </c>
-      <c r="E4" s="55"/>
       <c r="F4" s="55"/>
       <c r="G4" s="55"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H4" s="55"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
         <v>318</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47" t="s">
         <v>250</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="55"/>
+      <c r="E5" s="47"/>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H5" s="55"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
         <v>319</v>
       </c>
@@ -5798,125 +5805,130 @@
       <c r="D6" s="47" t="s">
         <v>242</v>
       </c>
-      <c r="E6" s="55"/>
-      <c r="F6" s="52" t="s">
+      <c r="E6" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="F6" s="55"/>
+      <c r="G6" s="52" t="s">
         <v>321</v>
       </c>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47" t="s">
+      <c r="H6" s="47"/>
+      <c r="I6" s="47" t="s">
         <v>325</v>
       </c>
-      <c r="I6" s="55"/>
       <c r="J6" s="55"/>
       <c r="K6" s="55"/>
       <c r="L6" s="55"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M6" s="55"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
         <v>320</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="55"/>
+      <c r="D7" s="47" t="s">
         <v>326</v>
       </c>
-      <c r="D7" s="55"/>
       <c r="E7" s="55"/>
-      <c r="F7" s="52" t="s">
+      <c r="F7" s="55"/>
+      <c r="G7" s="52" t="s">
         <v>322</v>
       </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55" t="s">
+      <c r="H7" s="55"/>
+      <c r="I7" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="55"/>
       <c r="J7" s="55"/>
       <c r="K7" s="55"/>
       <c r="L7" s="55"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="M7" s="55"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="55"/>
+      <c r="D8" s="47" t="s">
         <v>327</v>
       </c>
-      <c r="D8" s="55"/>
       <c r="E8" s="55"/>
       <c r="F8" s="55"/>
       <c r="G8" s="55"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H8" s="55"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="56" t="s">
         <v>323</v>
       </c>
-      <c r="B9" s="47" t="s">
-        <v>259</v>
-      </c>
       <c r="C9" s="47" t="s">
         <v>259</v>
       </c>
       <c r="D9" s="47" t="s">
         <v>259</v>
       </c>
-      <c r="E9" s="55"/>
+      <c r="E9" s="47" t="s">
+        <v>259</v>
+      </c>
       <c r="F9" s="55"/>
       <c r="G9" s="55"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H9" s="55"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
         <v>351</v>
       </c>
-      <c r="B10" s="59"/>
       <c r="C10" s="59"/>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="59"/>
+      <c r="E10" s="59" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="52" t="s">
         <v>321</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="D11" s="47" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
         <v>322</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="D12" s="59" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1"/>
-    <hyperlink ref="H6" r:id="rId2"/>
-    <hyperlink ref="C8" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C5" r:id="rId6"/>
-    <hyperlink ref="B9" r:id="rId7"/>
-    <hyperlink ref="C9" r:id="rId8"/>
-    <hyperlink ref="D9" r:id="rId9"/>
-    <hyperlink ref="C3" r:id="rId10"/>
-    <hyperlink ref="G2" r:id="rId11"/>
-    <hyperlink ref="F2" r:id="rId12"/>
-    <hyperlink ref="M2" r:id="rId13"/>
-    <hyperlink ref="H2" r:id="rId14"/>
-    <hyperlink ref="I2" r:id="rId15"/>
-    <hyperlink ref="C2" r:id="rId16"/>
-    <hyperlink ref="D2" r:id="rId17"/>
-    <hyperlink ref="K2" r:id="rId18"/>
-    <hyperlink ref="L2" r:id="rId19" display="Changeit@123"/>
-    <hyperlink ref="B2" r:id="rId20"/>
-    <hyperlink ref="J2" r:id="rId21" display="Changeit@123"/>
-    <hyperlink ref="D6" r:id="rId22"/>
-    <hyperlink ref="C11" r:id="rId23"/>
+    <hyperlink ref="D7" r:id="rId1"/>
+    <hyperlink ref="I6" r:id="rId2"/>
+    <hyperlink ref="D8" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D5" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="E9" r:id="rId9"/>
+    <hyperlink ref="D3" r:id="rId10"/>
+    <hyperlink ref="H2" r:id="rId11"/>
+    <hyperlink ref="G2" r:id="rId12"/>
+    <hyperlink ref="N2" r:id="rId13"/>
+    <hyperlink ref="I2" r:id="rId14"/>
+    <hyperlink ref="J2" r:id="rId15"/>
+    <hyperlink ref="D2" r:id="rId16"/>
+    <hyperlink ref="E2" r:id="rId17"/>
+    <hyperlink ref="L2" r:id="rId18"/>
+    <hyperlink ref="M2" r:id="rId19" display="Changeit@123"/>
+    <hyperlink ref="C2" r:id="rId20"/>
+    <hyperlink ref="K2" r:id="rId21" display="Changeit@123"/>
+    <hyperlink ref="E6" r:id="rId22"/>
+    <hyperlink ref="D11" r:id="rId23"/>
+    <hyperlink ref="B6" r:id="rId24"/>
+    <hyperlink ref="B2" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update testdata for group permission
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="15" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="17" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -15,28 +15,28 @@
     <sheet name="accounts" sheetId="8" r:id="rId6"/>
     <sheet name="authSessions" sheetId="9" r:id="rId7"/>
     <sheet name="usersRegression" sheetId="10" r:id="rId8"/>
-    <sheet name="AuditorSignUpTest" sheetId="1" r:id="rId9"/>
-    <sheet name="ForgotPassword" sheetId="2" r:id="rId10"/>
-    <sheet name="Login" sheetId="3" r:id="rId11"/>
-    <sheet name="ClientTestData" sheetId="12" r:id="rId12"/>
-    <sheet name="EmailTemplateData" sheetId="13" r:id="rId13"/>
-    <sheet name="SmokeTest" sheetId="14" r:id="rId14"/>
-    <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId15"/>
-    <sheet name="TodoTestPage" sheetId="16" r:id="rId16"/>
-    <sheet name="SuperAdminTest" sheetId="17" r:id="rId17"/>
-    <sheet name="NotificationEmailTest" sheetId="18" r:id="rId18"/>
-    <sheet name="ClientSignUpTest" sheetId="19" r:id="rId19"/>
-    <sheet name="ClientUITest" sheetId="20" r:id="rId20"/>
+    <sheet name="ForgotPassword" sheetId="2" r:id="rId9"/>
+    <sheet name="Login" sheetId="3" r:id="rId10"/>
+    <sheet name="ClientTestData" sheetId="12" r:id="rId11"/>
+    <sheet name="EmailTemplateData" sheetId="13" r:id="rId12"/>
+    <sheet name="SmokeTest" sheetId="14" r:id="rId13"/>
+    <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId14"/>
+    <sheet name="TodoTestPage" sheetId="16" r:id="rId15"/>
+    <sheet name="SuperAdminTest" sheetId="17" r:id="rId16"/>
+    <sheet name="NotificationEmailTest" sheetId="18" r:id="rId17"/>
+    <sheet name="ClientSignUpTest" sheetId="19" r:id="rId18"/>
+    <sheet name="ClientUITest" sheetId="20" r:id="rId19"/>
+    <sheet name="AuditorSignUpTest" sheetId="1" r:id="rId20"/>
     <sheet name="GroupPermissionTest" sheetId="23" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="17" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="18" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="19" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="20" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="17" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="12" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="15" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="601">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2080,9 +2080,6 @@
     <t>Lead Client Email Password</t>
   </si>
   <si>
-    <t>Firm Auvenir</t>
-  </si>
-  <si>
     <t>SUPER ADMIN</t>
   </si>
   <si>
@@ -2165,6 +2162,9 @@
   </si>
   <si>
     <t>General Auditor Comment  4</t>
+  </si>
+  <si>
+    <t>Auditor Sign upData</t>
   </si>
 </sst>
 </file>
@@ -2377,7 +2377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2526,9 +2526,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2536,6 +2533,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2550,6 +2550,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3182,103 +3183,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="46.85546875" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="61" t="s">
-        <v>320</v>
-      </c>
-      <c r="E1" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>259</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2" display="12345678x@X"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4" display="auvenir.automation.s3@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId5"/>
-    <hyperlink ref="E2" r:id="rId6"/>
-    <hyperlink ref="F2" r:id="rId7"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3385,7 +3289,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -3460,7 +3364,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -3568,7 +3472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y10"/>
   <sheetViews>
@@ -3856,12 +3760,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3923,7 +3827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
@@ -4100,7 +4004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -4231,7 +4135,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -4434,7 +4338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4477,6 +4381,273 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>491</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>489</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>487</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>485</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>483</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>481</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>479</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>477</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>475</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>473</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="60" t="s">
+        <v>471</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="s">
+        <v>469</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="60" t="s">
+        <v>468</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="60" t="s">
+        <v>466</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="60" t="s">
+        <v>464</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="60" t="s">
+        <v>462</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="60" t="s">
+        <v>461</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="60" t="s">
+        <v>459</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="60" t="s">
+        <v>457</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="60" t="s">
+        <v>455</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="60" t="s">
+        <v>453</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="60" t="s">
+        <v>450</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="60" t="s">
+        <v>446</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="60" t="s">
+        <v>444</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="60" t="s">
+        <v>442</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="60" t="s">
+        <v>440</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="60" t="s">
+        <v>438</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="60" t="s">
+        <v>436</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>435</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4584,277 +4755,894 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A2" sqref="A2:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.85546875" style="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="59"/>
+    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="60" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
-        <v>491</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
-        <v>489</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
-        <v>487</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
-        <v>485</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
-        <v>483</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
-        <v>481</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
-        <v>479</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
-        <v>477</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
-        <v>475</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
-        <v>473</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
-        <v>471</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
-        <v>469</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
-        <v>468</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
-        <v>466</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
-        <v>464</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
-        <v>462</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
-        <v>461</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
-        <v>459</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="60" t="s">
-        <v>457</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="60" t="s">
-        <v>455</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="60" t="s">
-        <v>453</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
-        <v>452</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="60" t="s">
-        <v>450</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="60" t="s">
-        <v>446</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
-        <v>444</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="60" t="s">
-        <v>442</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="60" t="s">
-        <v>440</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="60" t="s">
-        <v>438</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="60" t="s">
-        <v>436</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>435</v>
+      <c r="C1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+    </row>
+    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="54" t="s">
+        <v>495</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="54" t="s">
+        <v>496</v>
+      </c>
+      <c r="B26" s="68" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="54" t="s">
+        <v>498</v>
+      </c>
+      <c r="B27" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="54" t="s">
+        <v>499</v>
+      </c>
+      <c r="B28" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="54" t="s">
+        <v>500</v>
+      </c>
+      <c r="B29" s="68" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="54" t="s">
+        <v>502</v>
+      </c>
+      <c r="B30" s="68" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="54" t="s">
+        <v>503</v>
+      </c>
+      <c r="B31" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="54" t="s">
+        <v>504</v>
+      </c>
+      <c r="B32" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
+        <v>505</v>
+      </c>
+      <c r="B33" s="68" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="54" t="s">
+        <v>507</v>
+      </c>
+      <c r="B34" s="68" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="54" t="s">
+        <v>509</v>
+      </c>
+      <c r="B35" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="54" t="s">
+        <v>510</v>
+      </c>
+      <c r="B36" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="54" t="s">
+        <v>511</v>
+      </c>
+      <c r="B37" s="68" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="54" t="s">
+        <v>264</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="54" t="s">
+        <v>266</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="54" t="s">
+        <v>268</v>
+      </c>
+      <c r="C40" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="54" t="s">
+        <v>270</v>
+      </c>
+      <c r="C41" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="54" t="s">
+        <v>272</v>
+      </c>
+      <c r="C42" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="54" t="s">
+        <v>274</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="54" t="s">
+        <v>276</v>
+      </c>
+      <c r="C44" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="54" t="s">
+        <v>278</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="47" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B47" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B48" s="43" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B49" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B50" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B51" t="s">
+        <v>383</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId2"/>
+    <hyperlink ref="B21" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="F10" r:id="rId7"/>
+    <hyperlink ref="G12" r:id="rId8"/>
+    <hyperlink ref="E16" r:id="rId9"/>
+    <hyperlink ref="E19" r:id="rId10"/>
+    <hyperlink ref="E9" r:id="rId11" display="ww@.test.com"/>
+    <hyperlink ref="F9" r:id="rId12"/>
+    <hyperlink ref="B23" r:id="rId13"/>
+    <hyperlink ref="B24" r:id="rId14"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5105,7 +5893,7 @@
         <v>333</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -5152,20 +5940,20 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
+        <v>593</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>594</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>595</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="s">
+        <v>595</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>596</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>597</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -5242,17 +6030,17 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>572</v>
+        <v>329</v>
+      </c>
+      <c r="B37" s="69" t="s">
+        <v>597</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="60" t="s">
-        <v>329</v>
+        <v>598</v>
       </c>
       <c r="B38" s="69" t="s">
         <v>598</v>
@@ -5262,33 +6050,180 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="60" t="s">
-        <v>599</v>
-      </c>
-      <c r="B39" s="69" t="s">
-        <v>599</v>
+        <v>308</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>306</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="60" t="s">
-        <v>308</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>306</v>
+        <v>599</v>
+      </c>
+      <c r="B40" s="69" t="s">
+        <v>599</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="60" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="80" t="s">
         <v>600</v>
       </c>
-      <c r="B41" s="69" t="s">
-        <v>600</v>
-      </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5297,9 +6232,11 @@
     <hyperlink ref="B9" r:id="rId3"/>
     <hyperlink ref="B12" r:id="rId4"/>
     <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="B44" r:id="rId6"/>
+    <hyperlink ref="B50" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -6016,22 +6953,22 @@
       <c r="Q1" s="71" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="72" t="s">
+      <c r="R1" s="75" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="72"/>
-      <c r="T1" s="75" t="s">
+      <c r="S1" s="75"/>
+      <c r="T1" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="73"/>
-      <c r="V1" s="72" t="s">
+      <c r="U1" s="72"/>
+      <c r="V1" s="75" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="73" t="s">
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="72" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="76" t="s">
@@ -6083,8 +7020,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="74"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -6140,17 +7077,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -6161,6 +7087,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6365,22 +7302,22 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
+        <v>576</v>
+      </c>
+      <c r="B5" s="47" t="s">
         <v>577</v>
       </c>
-      <c r="B5" s="47" t="s">
-        <v>578</v>
-      </c>
       <c r="C5" t="s">
+        <v>572</v>
+      </c>
+      <c r="D5" t="s">
         <v>573</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>574</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="59" t="s">
         <v>575</v>
-      </c>
-      <c r="F5" s="59" t="s">
-        <v>576</v>
       </c>
       <c r="G5" s="59" t="s">
         <v>212</v>
@@ -6395,7 +7332,7 @@
         <v>209</v>
       </c>
       <c r="K5" s="59" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L5" s="59" t="s">
         <v>208</v>
@@ -6409,22 +7346,22 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C6" t="s">
         <v>87</v>
       </c>
       <c r="D6" t="s">
+        <v>579</v>
+      </c>
+      <c r="E6" t="s">
         <v>580</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="59" t="s">
         <v>581</v>
-      </c>
-      <c r="F6" s="59" t="s">
-        <v>582</v>
       </c>
       <c r="G6" s="59" t="s">
         <v>212</v>
@@ -6439,7 +7376,7 @@
         <v>209</v>
       </c>
       <c r="K6" s="59" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L6" s="59" t="s">
         <v>208</v>
@@ -6464,22 +7401,22 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
+        <v>584</v>
+      </c>
+      <c r="B7" s="70" t="s">
+        <v>583</v>
+      </c>
+      <c r="C7" t="s">
         <v>585</v>
       </c>
-      <c r="B7" s="70" t="s">
-        <v>584</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>586</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="59" t="s">
         <v>587</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="F7" s="59" t="s">
         <v>588</v>
-      </c>
-      <c r="F7" s="59" t="s">
-        <v>589</v>
       </c>
       <c r="G7" s="59" t="s">
         <v>212</v>
@@ -6494,7 +7431,7 @@
         <v>209</v>
       </c>
       <c r="K7" s="59" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L7" s="59" t="s">
         <v>208</v>
@@ -6570,884 +7507,97 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="46.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-    </row>
-    <row r="14" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-    </row>
-    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="49" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="49" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="54" t="s">
-        <v>495</v>
-      </c>
-      <c r="B25" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="54" t="s">
-        <v>496</v>
-      </c>
-      <c r="B26" s="68" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54" t="s">
-        <v>498</v>
-      </c>
-      <c r="B27" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54" t="s">
-        <v>499</v>
-      </c>
-      <c r="B28" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="54" t="s">
-        <v>500</v>
-      </c>
-      <c r="B29" s="68" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
-        <v>502</v>
-      </c>
-      <c r="B30" s="68" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
-        <v>503</v>
-      </c>
-      <c r="B31" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54" t="s">
-        <v>504</v>
-      </c>
-      <c r="B32" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54" t="s">
-        <v>505</v>
-      </c>
-      <c r="B33" s="68" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="s">
-        <v>507</v>
-      </c>
-      <c r="B34" s="68" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54" t="s">
-        <v>509</v>
-      </c>
-      <c r="B35" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="54" t="s">
-        <v>510</v>
-      </c>
-      <c r="B36" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="54" t="s">
-        <v>511</v>
-      </c>
-      <c r="B37" s="68" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="54" t="s">
-        <v>264</v>
-      </c>
-      <c r="C38" s="43" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
-        <v>266</v>
-      </c>
-      <c r="C39" s="43" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
-        <v>268</v>
-      </c>
-      <c r="C40" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="54" t="s">
-        <v>270</v>
-      </c>
-      <c r="C41" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="54" t="s">
-        <v>272</v>
-      </c>
-      <c r="C42" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="54" t="s">
-        <v>274</v>
-      </c>
-      <c r="C43" s="43" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="54" t="s">
-        <v>276</v>
-      </c>
-      <c r="C44" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="54" t="s">
-        <v>278</v>
-      </c>
-      <c r="C45" s="43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="47" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="B47" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="B48" s="43" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="B49" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="B50" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="B51" t="s">
-        <v>383</v>
-      </c>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>321</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B9" r:id="rId2"/>
-    <hyperlink ref="B21" r:id="rId3"/>
-    <hyperlink ref="F3" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E8" r:id="rId6"/>
-    <hyperlink ref="F10" r:id="rId7"/>
-    <hyperlink ref="G12" r:id="rId8"/>
-    <hyperlink ref="E16" r:id="rId9"/>
-    <hyperlink ref="E19" r:id="rId10"/>
-    <hyperlink ref="E9" r:id="rId11" display="ww@.test.com"/>
-    <hyperlink ref="F9" r:id="rId12"/>
-    <hyperlink ref="B23" r:id="rId13"/>
-    <hyperlink ref="B24" r:id="rId14"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2" display="12345678x@X"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4" display="auvenir.automation.s3@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId5"/>
+    <hyperlink ref="E2" r:id="rId6"/>
+    <hyperlink ref="F2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update smoketest: super admin, admin; marketing test
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="17" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="17" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -14,29 +14,29 @@
     <sheet name="LoginData" sheetId="11" r:id="rId5"/>
     <sheet name="accounts" sheetId="8" r:id="rId6"/>
     <sheet name="authSessions" sheetId="9" r:id="rId7"/>
-    <sheet name="usersRegression" sheetId="10" r:id="rId8"/>
-    <sheet name="AuditorSignUpTest" sheetId="1" r:id="rId9"/>
-    <sheet name="ForgotPassword" sheetId="2" r:id="rId10"/>
-    <sheet name="Login" sheetId="3" r:id="rId11"/>
+    <sheet name="ForgotPassword" sheetId="2" r:id="rId8"/>
+    <sheet name="Login" sheetId="3" r:id="rId9"/>
+    <sheet name="usersRegression" sheetId="10" r:id="rId10"/>
+    <sheet name="EmailTemplateData" sheetId="13" r:id="rId11"/>
     <sheet name="ClientTestData" sheetId="12" r:id="rId12"/>
-    <sheet name="EmailTemplateData" sheetId="13" r:id="rId13"/>
-    <sheet name="SmokeTest" sheetId="14" r:id="rId14"/>
-    <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId15"/>
-    <sheet name="TodoTestPage" sheetId="16" r:id="rId16"/>
-    <sheet name="SuperAdminTest" sheetId="17" r:id="rId17"/>
-    <sheet name="NotificationEmailTest" sheetId="18" r:id="rId18"/>
-    <sheet name="ClientSignUpTest" sheetId="19" r:id="rId19"/>
-    <sheet name="ClientUITest" sheetId="20" r:id="rId20"/>
+    <sheet name="AuditorTodoListTest" sheetId="15" r:id="rId13"/>
+    <sheet name="ClientUITest" sheetId="20" r:id="rId14"/>
+    <sheet name="TodoTestPage" sheetId="16" r:id="rId15"/>
+    <sheet name="SuperAdminTest" sheetId="17" r:id="rId16"/>
+    <sheet name="NotificationEmailTest" sheetId="18" r:id="rId17"/>
+    <sheet name="ClientSignUpTest" sheetId="19" r:id="rId18"/>
+    <sheet name="AuditorSignUpTest" sheetId="1" r:id="rId19"/>
+    <sheet name="SmokeTest" sheetId="14" r:id="rId20"/>
     <sheet name="GroupPermissionTest" sheetId="24" r:id="rId21"/>
   </sheets>
   <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="14" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="18" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="19" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="20" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="12" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="17" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="20" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="19" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="15" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="624">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2232,6 +2232,9 @@
   <si>
     <t>Super Admin Auvenir Password</t>
   </si>
+  <si>
+    <t>Super Admin Auvernir Password</t>
+  </si>
 </sst>
 </file>
 
@@ -2443,7 +2446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2590,11 +2593,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2603,6 +2604,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2617,7 +2621,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3250,206 +3254,510 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="34" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="46.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.140625" style="59"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="61" t="s">
-        <v>320</v>
-      </c>
-      <c r="E1" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>259</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="H1" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="K1" t="s">
+        <v>232</v>
+      </c>
+      <c r="L1" t="s">
+        <v>231</v>
+      </c>
+      <c r="M1" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="48" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>519</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>514</v>
+      </c>
+      <c r="C2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H2" t="s">
+        <v>226</v>
+      </c>
+      <c r="I2" t="s">
+        <v>225</v>
+      </c>
+      <c r="J2" t="s">
+        <v>224</v>
+      </c>
+      <c r="K2" t="s">
+        <v>516</v>
+      </c>
+      <c r="L2" t="s">
+        <v>223</v>
+      </c>
+      <c r="M2" t="s">
+        <v>565</v>
+      </c>
+      <c r="N2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>520</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>513</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" t="s">
+        <v>219</v>
+      </c>
+      <c r="I3" t="s">
+        <v>218</v>
+      </c>
+      <c r="J3" t="s">
+        <v>217</v>
+      </c>
+      <c r="K3" t="s">
+        <v>517</v>
+      </c>
+      <c r="L3" t="s">
+        <v>216</v>
+      </c>
+      <c r="M3" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="N3" s="59" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
+        <v>521</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>515</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G4" t="s">
+        <v>212</v>
+      </c>
+      <c r="H4" t="s">
+        <v>211</v>
+      </c>
+      <c r="I4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J4" t="s">
+        <v>209</v>
+      </c>
+      <c r="K4" t="s">
+        <v>518</v>
+      </c>
+      <c r="L4" t="s">
+        <v>208</v>
+      </c>
+      <c r="M4" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="N4" s="59" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
+        <v>577</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>578</v>
+      </c>
+      <c r="C5" t="s">
+        <v>573</v>
+      </c>
+      <c r="D5" t="s">
+        <v>574</v>
+      </c>
+      <c r="E5" t="s">
+        <v>575</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>576</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="I5" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="J5" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="K5" s="59" t="s">
+        <v>592</v>
+      </c>
+      <c r="L5" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="M5" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="N5" s="59" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
+        <v>583</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>579</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" t="s">
+        <v>580</v>
+      </c>
+      <c r="E6" t="s">
+        <v>581</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>582</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="I6" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="J6" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="K6" s="59" t="s">
+        <v>591</v>
+      </c>
+      <c r="L6" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="M6" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="N6" s="59" t="s">
+        <v>566</v>
+      </c>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="59"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
+        <v>585</v>
+      </c>
+      <c r="B7" s="70" t="s">
+        <v>584</v>
+      </c>
+      <c r="C7" t="s">
+        <v>586</v>
+      </c>
+      <c r="D7" t="s">
+        <v>587</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>588</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>589</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="J7" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="K7" s="59" t="s">
+        <v>590</v>
+      </c>
+      <c r="L7" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="M7" s="59" t="s">
+        <v>565</v>
+      </c>
+      <c r="N7" s="59" t="s">
+        <v>566</v>
+      </c>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="47"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="47"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="47"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="47"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B12" s="47"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B13" s="47"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="47"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="47"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="47"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="47"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="47"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="47"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="47"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="47"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="47"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2" display="12345678x@X"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4" display="auvenir.automation.s3@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId5"/>
-    <hyperlink ref="E2" r:id="rId6"/>
-    <hyperlink ref="F2" r:id="rId7"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="33.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="44.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="43.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="153.7109375" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="59" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="79"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>250</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>242</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="B5" s="49" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
-        <v>257</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>258</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>420</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>422</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>423</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>425</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>426</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>427</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>428</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>429</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>430</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>431</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:E1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="B5" r:id="rId5"/>
-    <hyperlink ref="B6" r:id="rId6"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -3530,402 +3838,6 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="153.7109375" style="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="59" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="59" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" style="59" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="59"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="60" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
-        <v>420</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
-        <v>422</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
-        <v>423</v>
-      </c>
-      <c r="B4" s="59" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
-        <v>425</v>
-      </c>
-      <c r="B5" s="59" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
-        <v>426</v>
-      </c>
-      <c r="B6" s="59" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
-        <v>427</v>
-      </c>
-      <c r="B7" s="59" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
-        <v>428</v>
-      </c>
-      <c r="B8" s="59" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
-        <v>429</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
-        <v>430</v>
-      </c>
-      <c r="B10" s="59" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
-        <v>431</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>419</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" style="55" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.7109375" style="55" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.7109375" style="55" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24" customWidth="1"/>
-    <col min="15" max="15" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.42578125" style="55" customWidth="1"/>
-    <col min="19" max="19" width="28" customWidth="1"/>
-    <col min="20" max="20" width="17.42578125" customWidth="1"/>
-    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="50" t="s">
-        <v>243</v>
-      </c>
-      <c r="C1" s="50" t="s">
-        <v>244</v>
-      </c>
-      <c r="D1" s="50" t="s">
-        <v>245</v>
-      </c>
-      <c r="E1" s="50" t="s">
-        <v>304</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>293</v>
-      </c>
-      <c r="G1" s="52" t="s">
-        <v>289</v>
-      </c>
-      <c r="H1" s="52" t="s">
-        <v>288</v>
-      </c>
-      <c r="I1" s="52" t="s">
-        <v>281</v>
-      </c>
-      <c r="J1" s="56" t="s">
-        <v>291</v>
-      </c>
-      <c r="K1" s="56" t="s">
-        <v>292</v>
-      </c>
-      <c r="L1" s="56" t="s">
-        <v>280</v>
-      </c>
-      <c r="M1" s="52" t="s">
-        <v>295</v>
-      </c>
-      <c r="N1" s="52" t="s">
-        <v>294</v>
-      </c>
-      <c r="O1" s="52" t="s">
-        <v>283</v>
-      </c>
-      <c r="P1" s="52" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q1" s="52" t="s">
-        <v>307</v>
-      </c>
-      <c r="R1" s="52" t="s">
-        <v>308</v>
-      </c>
-      <c r="S1" s="52" t="s">
-        <v>286</v>
-      </c>
-      <c r="T1" s="52" t="s">
-        <v>296</v>
-      </c>
-      <c r="U1" s="52" t="s">
-        <v>297</v>
-      </c>
-      <c r="V1" s="52" t="s">
-        <v>298</v>
-      </c>
-      <c r="W1" s="52" t="s">
-        <v>299</v>
-      </c>
-      <c r="X1" s="52" t="s">
-        <v>314</v>
-      </c>
-      <c r="Y1" s="52" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
-        <v>246</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>522</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>324</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>309</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>285</v>
-      </c>
-      <c r="G2" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="H2" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="I2" s="47" t="s">
-        <v>242</v>
-      </c>
-      <c r="J2" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="K2" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="L2" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="M2" s="57" t="s">
-        <v>242</v>
-      </c>
-      <c r="N2" s="58" t="s">
-        <v>311</v>
-      </c>
-      <c r="O2" s="55" t="s">
-        <v>284</v>
-      </c>
-      <c r="P2" s="55" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>287</v>
-      </c>
-      <c r="R2" s="55" t="s">
-        <v>306</v>
-      </c>
-      <c r="S2" t="s">
-        <v>312</v>
-      </c>
-      <c r="T2" t="s">
-        <v>300</v>
-      </c>
-      <c r="U2" t="s">
-        <v>301</v>
-      </c>
-      <c r="V2" t="s">
-        <v>302</v>
-      </c>
-      <c r="W2" t="s">
-        <v>310</v>
-      </c>
-      <c r="X2" t="s">
-        <v>315</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>317</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>249</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="P3" s="55" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q3" s="55" t="s">
-        <v>287</v>
-      </c>
-      <c r="R3" s="55" t="s">
-        <v>306</v>
-      </c>
-      <c r="S3" s="55" t="s">
-        <v>313</v>
-      </c>
-      <c r="T3" s="55" t="s">
-        <v>300</v>
-      </c>
-      <c r="U3" s="55" t="s">
-        <v>301</v>
-      </c>
-      <c r="V3" s="55" t="s">
-        <v>302</v>
-      </c>
-      <c r="W3" s="55" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
-        <v>253</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>256</v>
-      </c>
-      <c r="C4" s="47" t="s">
-        <v>254</v>
-      </c>
-      <c r="D4" s="47" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="C7" s="47"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="16"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C10" s="47"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
-    <hyperlink ref="G2" r:id="rId3"/>
-    <hyperlink ref="F2" r:id="rId4"/>
-    <hyperlink ref="H2" r:id="rId5"/>
-    <hyperlink ref="B2" r:id="rId6"/>
-    <hyperlink ref="J2" r:id="rId7"/>
-    <hyperlink ref="I2" r:id="rId8"/>
-    <hyperlink ref="D2" r:id="rId9"/>
-    <hyperlink ref="K2" r:id="rId10"/>
-    <hyperlink ref="L2" r:id="rId11"/>
-    <hyperlink ref="C2" r:id="rId12"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3991,7 +3903,274 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.85546875" style="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>491</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
+        <v>489</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>487</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>485</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="60" t="s">
+        <v>483</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="60" t="s">
+        <v>481</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="60" t="s">
+        <v>479</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="60" t="s">
+        <v>477</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="60" t="s">
+        <v>475</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="60" t="s">
+        <v>473</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="60" t="s">
+        <v>471</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="s">
+        <v>469</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="60" t="s">
+        <v>468</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="60" t="s">
+        <v>466</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="60" t="s">
+        <v>464</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="60" t="s">
+        <v>462</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="60" t="s">
+        <v>461</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="60" t="s">
+        <v>459</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="60" t="s">
+        <v>457</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="60" t="s">
+        <v>455</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="60" t="s">
+        <v>453</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="60" t="s">
+        <v>452</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="60" t="s">
+        <v>450</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="60" t="s">
+        <v>448</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="60" t="s">
+        <v>446</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="60" t="s">
+        <v>444</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="60" t="s">
+        <v>442</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="60" t="s">
+        <v>440</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="60" t="s">
+        <v>438</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="60" t="s">
+        <v>436</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>435</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S4"/>
   <sheetViews>
@@ -4168,7 +4347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -4299,7 +4478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -4502,7 +4681,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -4545,6 +4724,890 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="20"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+    </row>
+    <row r="14" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+    </row>
+    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="54" t="s">
+        <v>495</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="54" t="s">
+        <v>496</v>
+      </c>
+      <c r="B26" s="68" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="54" t="s">
+        <v>498</v>
+      </c>
+      <c r="B27" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="54" t="s">
+        <v>499</v>
+      </c>
+      <c r="B28" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="54" t="s">
+        <v>500</v>
+      </c>
+      <c r="B29" s="68" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="54" t="s">
+        <v>502</v>
+      </c>
+      <c r="B30" s="68" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="54" t="s">
+        <v>503</v>
+      </c>
+      <c r="B31" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="54" t="s">
+        <v>504</v>
+      </c>
+      <c r="B32" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="54" t="s">
+        <v>505</v>
+      </c>
+      <c r="B33" s="68" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="54" t="s">
+        <v>507</v>
+      </c>
+      <c r="B34" s="68" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="54" t="s">
+        <v>509</v>
+      </c>
+      <c r="B35" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="54" t="s">
+        <v>510</v>
+      </c>
+      <c r="B36" s="68" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="54" t="s">
+        <v>511</v>
+      </c>
+      <c r="B37" s="68" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="54" t="s">
+        <v>264</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="54" t="s">
+        <v>266</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="54" t="s">
+        <v>268</v>
+      </c>
+      <c r="C40" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="54" t="s">
+        <v>270</v>
+      </c>
+      <c r="C41" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="54" t="s">
+        <v>272</v>
+      </c>
+      <c r="C42" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="54" t="s">
+        <v>274</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="54" t="s">
+        <v>276</v>
+      </c>
+      <c r="C44" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="54" t="s">
+        <v>278</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="47" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B47" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B48" s="43" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B49" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B50" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B51" t="s">
+        <v>383</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId2"/>
+    <hyperlink ref="B21" r:id="rId3"/>
+    <hyperlink ref="F3" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E8" r:id="rId6"/>
+    <hyperlink ref="F10" r:id="rId7"/>
+    <hyperlink ref="G12" r:id="rId8"/>
+    <hyperlink ref="E16" r:id="rId9"/>
+    <hyperlink ref="E19" r:id="rId10"/>
+    <hyperlink ref="E9" r:id="rId11" display="ww@.test.com"/>
+    <hyperlink ref="F9" r:id="rId12"/>
+    <hyperlink ref="B23" r:id="rId13"/>
+    <hyperlink ref="B24" r:id="rId14"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -4652,268 +5715,309 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.85546875" style="59" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="59"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.140625" style="55" customWidth="1"/>
+    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24" customWidth="1"/>
+    <col min="17" max="17" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.42578125" style="55" customWidth="1"/>
+    <col min="21" max="21" width="28" customWidth="1"/>
+    <col min="22" max="22" width="17.42578125" customWidth="1"/>
+    <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="60" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
-        <v>491</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
-        <v>489</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
-        <v>487</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
-        <v>485</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
-        <v>483</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
-        <v>481</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
-        <v>479</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
-        <v>477</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
-        <v>475</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
-        <v>473</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
-        <v>471</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
-        <v>469</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
-        <v>468</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
-        <v>466</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
-        <v>464</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
-        <v>462</v>
-      </c>
-      <c r="B17" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>623</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>304</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>293</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>289</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>288</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>281</v>
+      </c>
+      <c r="L1" s="56" t="s">
+        <v>291</v>
+      </c>
+      <c r="M1" s="56" t="s">
+        <v>292</v>
+      </c>
+      <c r="N1" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>295</v>
+      </c>
+      <c r="P1" s="52" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q1" s="52" t="s">
+        <v>283</v>
+      </c>
+      <c r="R1" s="52" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
-        <v>461</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
-        <v>459</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="60" t="s">
-        <v>457</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="60" t="s">
-        <v>455</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="60" t="s">
-        <v>453</v>
-      </c>
-      <c r="B22" s="7" t="s">
+      <c r="S1" s="52" t="s">
+        <v>307</v>
+      </c>
+      <c r="T1" s="52" t="s">
+        <v>308</v>
+      </c>
+      <c r="U1" s="52" t="s">
+        <v>286</v>
+      </c>
+      <c r="V1" s="52" t="s">
+        <v>296</v>
+      </c>
+      <c r="W1" s="52" t="s">
+        <v>297</v>
+      </c>
+      <c r="X1" s="52" t="s">
+        <v>298</v>
+      </c>
+      <c r="Y1" s="52" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
-        <v>452</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="60" t="s">
-        <v>450</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="60" t="s">
-        <v>448</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="60" t="s">
-        <v>446</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
-        <v>444</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="60" t="s">
-        <v>442</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="60" t="s">
-        <v>440</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="60" t="s">
-        <v>438</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="60" t="s">
-        <v>436</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>435</v>
-      </c>
+      <c r="Z1" s="52" t="s">
+        <v>314</v>
+      </c>
+      <c r="AA1" s="52" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="82" t="s">
+        <v>522</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>285</v>
+      </c>
+      <c r="I2" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="K2" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="L2" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="M2" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="N2" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="O2" s="57" t="s">
+        <v>242</v>
+      </c>
+      <c r="P2" s="58" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q2" s="55" t="s">
+        <v>284</v>
+      </c>
+      <c r="R2" s="55" t="s">
+        <v>282</v>
+      </c>
+      <c r="S2" t="s">
+        <v>287</v>
+      </c>
+      <c r="T2" s="55" t="s">
+        <v>306</v>
+      </c>
+      <c r="U2" t="s">
+        <v>312</v>
+      </c>
+      <c r="V2" t="s">
+        <v>300</v>
+      </c>
+      <c r="W2" t="s">
+        <v>301</v>
+      </c>
+      <c r="X2" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>310</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>315</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>247</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="82" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="R3" s="55" t="s">
+        <v>282</v>
+      </c>
+      <c r="S3" s="55" t="s">
+        <v>287</v>
+      </c>
+      <c r="T3" s="55" t="s">
+        <v>306</v>
+      </c>
+      <c r="U3" s="55" t="s">
+        <v>313</v>
+      </c>
+      <c r="V3" s="55" t="s">
+        <v>300</v>
+      </c>
+      <c r="W3" s="55" t="s">
+        <v>301</v>
+      </c>
+      <c r="X3" s="55" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y3" s="55" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="50" t="s">
+        <v>253</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>254</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="56"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="52"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A7" s="52"/>
+      <c r="E7" s="47"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="E10" s="47"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="O2" r:id="rId2"/>
+    <hyperlink ref="I2" r:id="rId3"/>
+    <hyperlink ref="H2" r:id="rId4"/>
+    <hyperlink ref="J2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId6"/>
+    <hyperlink ref="L2" r:id="rId7"/>
+    <hyperlink ref="K2" r:id="rId8"/>
+    <hyperlink ref="F2" r:id="rId9"/>
+    <hyperlink ref="M2" r:id="rId10"/>
+    <hyperlink ref="N2" r:id="rId11"/>
+    <hyperlink ref="E2" r:id="rId12"/>
+    <hyperlink ref="B2" r:id="rId13"/>
+    <hyperlink ref="C2" r:id="rId14"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -4921,8 +6025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5682,7 +6786,7 @@
       <c r="A74" s="52" t="s">
         <v>371</v>
       </c>
-      <c r="B74" s="81" t="s">
+      <c r="B74" s="72" t="s">
         <v>387</v>
       </c>
     </row>
@@ -6385,94 +7489,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="73" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="73" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="73" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="72" t="s">
+      <c r="J1" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="72" t="s">
+      <c r="L1" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="72" t="s">
+      <c r="M1" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="72" t="s">
+      <c r="N1" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="72" t="s">
+      <c r="O1" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="72" t="s">
+      <c r="P1" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="72" t="s">
+      <c r="Q1" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="73" t="s">
+      <c r="R1" s="77" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="73"/>
+      <c r="S1" s="77"/>
       <c r="T1" s="76" t="s">
         <v>196</v>
       </c>
       <c r="U1" s="74"/>
-      <c r="V1" s="73" t="s">
+      <c r="V1" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="73"/>
-      <c r="X1" s="73"/>
-      <c r="Y1" s="73"/>
-      <c r="Z1" s="73"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
       <c r="AA1" s="74" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="77" t="s">
+      <c r="AB1" s="78" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="72"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -6557,17 +7661,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -6578,6 +7671,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6586,1285 +7690,205 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y22"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="59"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.5703125" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="34" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="46.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F1" s="48" t="s">
-        <v>237</v>
-      </c>
-      <c r="G1" s="48" t="s">
-        <v>236</v>
-      </c>
-      <c r="H1" s="48" t="s">
-        <v>235</v>
-      </c>
-      <c r="I1" s="48" t="s">
-        <v>234</v>
-      </c>
-      <c r="J1" s="48" t="s">
-        <v>233</v>
-      </c>
-      <c r="K1" t="s">
-        <v>232</v>
-      </c>
-      <c r="L1" t="s">
-        <v>231</v>
-      </c>
-      <c r="M1" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="48" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
-        <v>519</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>514</v>
-      </c>
-      <c r="C2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D2" t="s">
-        <v>229</v>
-      </c>
-      <c r="E2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F2" t="s">
-        <v>228</v>
-      </c>
-      <c r="G2" t="s">
-        <v>227</v>
-      </c>
-      <c r="H2" t="s">
-        <v>226</v>
-      </c>
-      <c r="I2" t="s">
-        <v>225</v>
-      </c>
-      <c r="J2" t="s">
-        <v>224</v>
-      </c>
-      <c r="K2" t="s">
-        <v>516</v>
-      </c>
-      <c r="L2" t="s">
-        <v>223</v>
-      </c>
-      <c r="M2" t="s">
-        <v>565</v>
-      </c>
-      <c r="N2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
-        <v>520</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>513</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" t="s">
-        <v>205</v>
-      </c>
-      <c r="E3" t="s">
-        <v>221</v>
-      </c>
-      <c r="F3" t="s">
-        <v>220</v>
-      </c>
-      <c r="G3" t="s">
-        <v>207</v>
-      </c>
-      <c r="H3" t="s">
-        <v>219</v>
-      </c>
-      <c r="I3" t="s">
-        <v>218</v>
-      </c>
-      <c r="J3" t="s">
-        <v>217</v>
-      </c>
-      <c r="K3" t="s">
-        <v>517</v>
-      </c>
-      <c r="L3" t="s">
-        <v>216</v>
-      </c>
-      <c r="M3" s="59" t="s">
-        <v>565</v>
-      </c>
-      <c r="N3" s="59" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
-        <v>521</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>515</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>230</v>
-      </c>
-      <c r="D4" t="s">
-        <v>215</v>
-      </c>
-      <c r="E4" t="s">
-        <v>214</v>
-      </c>
-      <c r="F4" t="s">
-        <v>213</v>
-      </c>
-      <c r="G4" t="s">
-        <v>212</v>
-      </c>
-      <c r="H4" t="s">
-        <v>211</v>
-      </c>
-      <c r="I4" t="s">
-        <v>210</v>
-      </c>
-      <c r="J4" t="s">
-        <v>209</v>
-      </c>
-      <c r="K4" t="s">
-        <v>518</v>
-      </c>
-      <c r="L4" t="s">
-        <v>208</v>
-      </c>
-      <c r="M4" s="59" t="s">
-        <v>565</v>
-      </c>
-      <c r="N4" s="59" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
-        <v>577</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>578</v>
-      </c>
-      <c r="C5" t="s">
-        <v>573</v>
-      </c>
-      <c r="D5" t="s">
-        <v>574</v>
-      </c>
-      <c r="E5" t="s">
-        <v>575</v>
-      </c>
-      <c r="F5" s="59" t="s">
-        <v>576</v>
-      </c>
-      <c r="G5" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="H5" s="59" t="s">
-        <v>211</v>
-      </c>
-      <c r="I5" s="59" t="s">
-        <v>210</v>
-      </c>
-      <c r="J5" s="59" t="s">
-        <v>209</v>
-      </c>
-      <c r="K5" s="59" t="s">
-        <v>592</v>
-      </c>
-      <c r="L5" s="59" t="s">
-        <v>208</v>
-      </c>
-      <c r="M5" s="59" t="s">
-        <v>565</v>
-      </c>
-      <c r="N5" s="59" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
-        <v>583</v>
-      </c>
-      <c r="B6" s="47" t="s">
-        <v>579</v>
-      </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" t="s">
-        <v>580</v>
-      </c>
-      <c r="E6" t="s">
-        <v>581</v>
-      </c>
-      <c r="F6" s="59" t="s">
-        <v>582</v>
-      </c>
-      <c r="G6" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="H6" s="59" t="s">
-        <v>211</v>
-      </c>
-      <c r="I6" s="59" t="s">
-        <v>210</v>
-      </c>
-      <c r="J6" s="59" t="s">
-        <v>209</v>
-      </c>
-      <c r="K6" s="59" t="s">
-        <v>591</v>
-      </c>
-      <c r="L6" s="59" t="s">
-        <v>208</v>
-      </c>
-      <c r="M6" s="59" t="s">
-        <v>565</v>
-      </c>
-      <c r="N6" s="59" t="s">
-        <v>566</v>
-      </c>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="59"/>
-      <c r="V6" s="59"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="59"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
-        <v>585</v>
-      </c>
-      <c r="B7" s="70" t="s">
-        <v>584</v>
-      </c>
-      <c r="C7" t="s">
-        <v>586</v>
-      </c>
-      <c r="D7" t="s">
-        <v>587</v>
-      </c>
-      <c r="E7" s="59" t="s">
-        <v>588</v>
-      </c>
-      <c r="F7" s="59" t="s">
-        <v>589</v>
-      </c>
-      <c r="G7" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="H7" s="59" t="s">
-        <v>211</v>
-      </c>
-      <c r="I7" s="59" t="s">
-        <v>210</v>
-      </c>
-      <c r="J7" s="59" t="s">
-        <v>209</v>
-      </c>
-      <c r="K7" s="59" t="s">
-        <v>590</v>
-      </c>
-      <c r="L7" s="59" t="s">
-        <v>208</v>
-      </c>
-      <c r="M7" s="59" t="s">
-        <v>565</v>
-      </c>
-      <c r="N7" s="59" t="s">
-        <v>566</v>
-      </c>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B8" s="47"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B9" s="47"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B10" s="47"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B12" s="47"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="47"/>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B14" s="47"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="47"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B16" s="47"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="47"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="47"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="47"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="47"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="47"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>320</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>321</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2" display="12345678x@X"/>
     <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId4" display="auvenir.automation.s3@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId5"/>
+    <hyperlink ref="E2" r:id="rId6"/>
+    <hyperlink ref="F2" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="43.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-    </row>
-    <row r="14" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-    </row>
-    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+    <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="80"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="49" t="s">
+      <c r="B2" s="49" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="C2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="49" t="s">
+      <c r="B3" s="49" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="54" t="s">
-        <v>495</v>
-      </c>
-      <c r="B25" s="68" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" s="49" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B5" s="49" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="54" t="s">
-        <v>496</v>
-      </c>
-      <c r="B26" s="68" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="54" t="s">
-        <v>498</v>
-      </c>
-      <c r="B27" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54" t="s">
-        <v>499</v>
-      </c>
-      <c r="B28" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="54" t="s">
-        <v>500</v>
-      </c>
-      <c r="B29" s="68" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
-        <v>502</v>
-      </c>
-      <c r="B30" s="68" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
-        <v>503</v>
-      </c>
-      <c r="B31" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="54" t="s">
-        <v>504</v>
-      </c>
-      <c r="B32" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="54" t="s">
-        <v>505</v>
-      </c>
-      <c r="B33" s="68" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="54" t="s">
-        <v>507</v>
-      </c>
-      <c r="B34" s="68" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="54" t="s">
-        <v>509</v>
-      </c>
-      <c r="B35" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="54" t="s">
-        <v>510</v>
-      </c>
-      <c r="B36" s="68" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="54" t="s">
-        <v>511</v>
-      </c>
-      <c r="B37" s="68" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="54" t="s">
-        <v>264</v>
-      </c>
-      <c r="C38" s="43" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
-        <v>266</v>
-      </c>
-      <c r="C39" s="43" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
-        <v>268</v>
-      </c>
-      <c r="C40" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="54" t="s">
-        <v>270</v>
-      </c>
-      <c r="C41" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="54" t="s">
-        <v>272</v>
-      </c>
-      <c r="C42" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="54" t="s">
-        <v>274</v>
-      </c>
-      <c r="C43" s="43" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="54" t="s">
-        <v>276</v>
-      </c>
-      <c r="C44" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="54" t="s">
-        <v>278</v>
-      </c>
-      <c r="C45" s="43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="47" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="B47" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="B48" s="43" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="B49" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="B50" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="B51" t="s">
-        <v>383</v>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="B9" r:id="rId2"/>
-    <hyperlink ref="B21" r:id="rId3"/>
-    <hyperlink ref="F3" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E8" r:id="rId6"/>
-    <hyperlink ref="F10" r:id="rId7"/>
-    <hyperlink ref="G12" r:id="rId8"/>
-    <hyperlink ref="E16" r:id="rId9"/>
-    <hyperlink ref="E19" r:id="rId10"/>
-    <hyperlink ref="E9" r:id="rId11" display="ww@.test.com"/>
-    <hyperlink ref="F9" r:id="rId12"/>
-    <hyperlink ref="B23" r:id="rId13"/>
-    <hyperlink ref="B24" r:id="rId14"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix Client Invitation flow
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="18" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="19" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -2600,6 +2600,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2607,9 +2610,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6028,7 +6028,7 @@
   <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+      <selection activeCell="E72" sqref="E71:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6656,8 +6656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7358,7 +7358,7 @@
         <v>613</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>59</v>
+        <v>535</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -8168,22 +8168,22 @@
       <c r="Q1" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="78" t="s">
+      <c r="R1" s="75" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="78"/>
-      <c r="T1" s="77" t="s">
+      <c r="S1" s="75"/>
+      <c r="T1" s="78" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="75"/>
-      <c r="V1" s="78" t="s">
+      <c r="U1" s="76"/>
+      <c r="V1" s="75" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="75" t="s">
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="76" t="s">
         <v>194</v>
       </c>
       <c r="AB1" s="79" t="s">
@@ -8235,8 +8235,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="76"/>
-      <c r="AB2" s="76"/>
+      <c r="AA2" s="77"/>
+      <c r="AB2" s="77"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -8292,6 +8292,17 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -8302,17 +8313,6 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update excel data file, Refactor TodoRequest
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="18" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="18" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="651">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2237,6 +2237,87 @@
   <si>
     <t>Super Admin Auvernir Password</t>
   </si>
+  <si>
+    <t>Request Name 1</t>
+  </si>
+  <si>
+    <t>Request Name 2</t>
+  </si>
+  <si>
+    <t>Request Name 3</t>
+  </si>
+  <si>
+    <t>Request Name 4</t>
+  </si>
+  <si>
+    <t>Request Name 5</t>
+  </si>
+  <si>
+    <t>Request Name 6</t>
+  </si>
+  <si>
+    <t>File Request Name 1</t>
+  </si>
+  <si>
+    <t>File Request Name 2</t>
+  </si>
+  <si>
+    <t>File Request Name 3</t>
+  </si>
+  <si>
+    <t>File Request Name 4</t>
+  </si>
+  <si>
+    <t>File Request Name 5</t>
+  </si>
+  <si>
+    <t>File Request Name 6</t>
+  </si>
+  <si>
+    <t>Request 1</t>
+  </si>
+  <si>
+    <t>Request 2</t>
+  </si>
+  <si>
+    <t>Request 3</t>
+  </si>
+  <si>
+    <t>Request 4</t>
+  </si>
+  <si>
+    <t>Request 5</t>
+  </si>
+  <si>
+    <t>Request 6</t>
+  </si>
+  <si>
+    <t>TXT_helloAuvenir.png</t>
+  </si>
+  <si>
+    <t>TXT_Auvenir.jpg</t>
+  </si>
+  <si>
+    <t>TXT_Auvenir.pdf</t>
+  </si>
+  <si>
+    <t>TXT_Auvenir.xlsx</t>
+  </si>
+  <si>
+    <t>TXT_helloAuvenir.txt</t>
+  </si>
+  <si>
+    <t>To Do 7 name</t>
+  </si>
+  <si>
+    <t>ToDo 07</t>
+  </si>
+  <si>
+    <t>ToDo 08</t>
+  </si>
+  <si>
+    <t>To Do 8 name</t>
+  </si>
 </sst>
 </file>
 
@@ -2448,7 +2529,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2597,6 +2678,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6027,7 +6109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
@@ -6654,10 +6736,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7025,408 +7107,534 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="60" t="s">
-        <v>550</v>
-      </c>
-      <c r="B35" s="69" t="s">
-        <v>551</v>
+        <v>647</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>648</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="60" t="s">
-        <v>552</v>
-      </c>
-      <c r="B36" s="69" t="s">
-        <v>553</v>
+        <v>650</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>649</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B37" s="69" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="60" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B38" s="69" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="60" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B39" s="69" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="60" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B40" s="69" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="60" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B41" s="69" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>572</v>
+        <v>560</v>
+      </c>
+      <c r="B42" s="69" t="s">
+        <v>561</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="60" t="s">
-        <v>329</v>
+        <v>562</v>
       </c>
       <c r="B43" s="69" t="s">
-        <v>598</v>
+        <v>563</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="60" t="s">
-        <v>599</v>
-      </c>
-      <c r="B44" s="69" t="s">
-        <v>607</v>
+        <v>6</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>572</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="60" t="s">
-        <v>308</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>306</v>
+        <v>329</v>
+      </c>
+      <c r="B45" s="69" t="s">
+        <v>598</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="60" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B46" s="69" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="60" t="s">
-        <v>609</v>
+        <v>307</v>
       </c>
       <c r="B47" s="69" t="s">
-        <v>610</v>
+        <v>287</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="60" t="s">
-        <v>611</v>
+        <v>308</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>612</v>
+        <v>306</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="60" t="s">
-        <v>243</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>522</v>
+        <v>600</v>
+      </c>
+      <c r="B49" s="69" t="s">
+        <v>608</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="60" t="s">
-        <v>289</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>242</v>
+        <v>609</v>
+      </c>
+      <c r="B50" s="69" t="s">
+        <v>610</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="60" t="s">
-        <v>3</v>
+        <v>611</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>29</v>
+        <v>612</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="7">
-        <v>4167877865</v>
+        <v>243</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>522</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="60" t="s">
-        <v>5</v>
+        <v>289</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>82</v>
+        <v>242</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="60" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="B55" s="7">
+        <v>4167877865</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="60" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="60" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="7">
-        <v>12</v>
+        <v>8</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="60" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="60" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="60" t="s">
-        <v>356</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>357</v>
+        <v>13</v>
+      </c>
+      <c r="B61" s="7">
+        <v>12</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="60" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="60" t="s">
-        <v>18</v>
-      </c>
-      <c r="B63" s="7">
-        <v>165782</v>
+        <v>15</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="71">
-        <v>43012</v>
+        <v>356</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>357</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="B65" s="7">
-        <v>1234567890</v>
+        <v>17</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="B66" s="7">
+        <v>165782</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="B67" s="71">
+        <v>43012</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="60" t="s">
-        <v>613</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>59</v>
+        <v>20</v>
+      </c>
+      <c r="B68" s="7">
+        <v>1234567890</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="60" t="s">
-        <v>614</v>
-      </c>
-      <c r="B69" s="7">
-        <v>1234567899</v>
+        <v>21</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="60" t="s">
-        <v>615</v>
+        <v>23</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>432</v>
+        <v>24</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="60" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>617</v>
+        <v>59</v>
       </c>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="60" t="s">
-        <v>618</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>619</v>
+        <v>614</v>
+      </c>
+      <c r="B72" s="7">
+        <v>1234567899</v>
       </c>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="60" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>621</v>
+        <v>432</v>
       </c>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="52" t="s">
+      <c r="A74" s="60" t="s">
+        <v>616</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="60" t="s">
+        <v>618</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="60" t="s">
+        <v>620</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="52" t="s">
         <v>371</v>
       </c>
-      <c r="B74" s="72" t="s">
+      <c r="B77" s="72" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="52" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="52" t="s">
         <v>622</v>
       </c>
-      <c r="B75" s="7" t="s">
+      <c r="B78" s="7" t="s">
         <v>242</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="52" t="s">
+        <v>624</v>
+      </c>
+      <c r="B79" s="74" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="52" t="s">
+        <v>625</v>
+      </c>
+      <c r="B80" s="59" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="52" t="s">
+        <v>626</v>
+      </c>
+      <c r="B81" s="59" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="52" t="s">
+        <v>627</v>
+      </c>
+      <c r="B82" s="59" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="52" t="s">
+        <v>628</v>
+      </c>
+      <c r="B83" s="59" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="52" t="s">
+        <v>629</v>
+      </c>
+      <c r="B84" s="59" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="52" t="s">
+        <v>630</v>
+      </c>
+      <c r="B85" s="59" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="52" t="s">
+        <v>631</v>
+      </c>
+      <c r="B86" s="59" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="52" t="s">
+        <v>632</v>
+      </c>
+      <c r="B87" s="59" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="52" t="s">
+        <v>633</v>
+      </c>
+      <c r="B88" s="59" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="52" t="s">
+        <v>634</v>
+      </c>
+      <c r="B89" s="59" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="52" t="s">
+        <v>635</v>
+      </c>
+      <c r="B90" s="59" t="s">
+        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -7436,7 +7644,7 @@
     <hyperlink ref="B10" r:id="rId3"/>
     <hyperlink ref="B14" r:id="rId4"/>
     <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="B74" r:id="rId6"/>
+    <hyperlink ref="B77" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -8120,94 +8328,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="75" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="75" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="75" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="75" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="75" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="74" t="s">
+      <c r="H1" s="75" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="74" t="s">
+      <c r="I1" s="75" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="74" t="s">
+      <c r="J1" s="75" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="K1" s="75" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="74" t="s">
+      <c r="L1" s="75" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="74" t="s">
+      <c r="M1" s="75" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="74" t="s">
+      <c r="N1" s="75" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="74" t="s">
+      <c r="O1" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="74" t="s">
+      <c r="P1" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="74" t="s">
+      <c r="Q1" s="75" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="78" t="s">
+      <c r="R1" s="79" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="78"/>
-      <c r="T1" s="77" t="s">
+      <c r="S1" s="79"/>
+      <c r="T1" s="78" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="75"/>
-      <c r="V1" s="78" t="s">
+      <c r="U1" s="76"/>
+      <c r="V1" s="79" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="75" t="s">
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="76" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="79" t="s">
+      <c r="AB1" s="80" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="75"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -8235,8 +8443,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="76"/>
-      <c r="AB2" s="76"/>
+      <c r="AA2" s="77"/>
+      <c r="AB2" s="77"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -8440,11 +8648,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="83"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Update testData for smoketest and group Permission
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="19" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="17" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="4" r:id="rId1"/>
@@ -27,17 +27,15 @@
     <sheet name="ClientSignUpTest" sheetId="19" r:id="rId18"/>
     <sheet name="AuditorSignUpTest" sheetId="1" r:id="rId19"/>
     <sheet name="SmokeTest" sheetId="14" r:id="rId20"/>
-    <sheet name="SmokeTest-R" sheetId="25" r:id="rId21"/>
-    <sheet name="GroupPermissionTest" sheetId="24" r:id="rId22"/>
+    <sheet name="GroupPermissionTest" sheetId="24" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="12" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="17" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="13" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="21" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="20" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="16" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="19" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="20" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="15" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -47,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="624">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -2596,12 +2594,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2610,6 +2604,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2624,6 +2621,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5719,8 +5717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA10"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5844,7 +5842,7 @@
       <c r="C2" s="16" t="s">
         <v>242</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="82" t="s">
         <v>522</v>
       </c>
       <c r="E2" s="49" t="s">
@@ -5923,7 +5921,7 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="73" t="s">
+      <c r="D3" s="82" t="s">
         <v>248</v>
       </c>
       <c r="E3" s="16" t="s">
@@ -6025,639 +6023,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B75"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E72" sqref="E71:E72"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.5703125" style="59" customWidth="1"/>
-    <col min="2" max="2" width="58" style="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="59"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="60" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
-        <v>525</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
-        <v>527</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
-        <v>567</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
-        <v>568</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
-        <v>528</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
-        <v>530</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="60" t="s">
-        <v>569</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
-        <v>601</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
-        <v>244</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
-        <v>288</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="60" t="s">
-        <v>292</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="60" t="s">
-        <v>398</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="60" t="s">
-        <v>532</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="60" t="s">
-        <v>534</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
-        <v>570</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="60" t="s">
-        <v>603</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
-        <v>535</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
-        <v>537</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="60" t="s">
-        <v>571</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="60" t="s">
-        <v>604</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="60" t="s">
-        <v>245</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
-        <v>281</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="60" t="s">
-        <v>280</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="60" t="s">
-        <v>605</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="60" t="s">
-        <v>539</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="60" t="s">
-        <v>541</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="60" t="s">
-        <v>333</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="60" t="s">
-        <v>543</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="60" t="s">
-        <v>544</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="60" t="s">
-        <v>546</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="60" t="s">
-        <v>548</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="60" t="s">
-        <v>594</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="60" t="s">
-        <v>596</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="60" t="s">
-        <v>550</v>
-      </c>
-      <c r="B35" s="69" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="60" t="s">
-        <v>552</v>
-      </c>
-      <c r="B36" s="69" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="60" t="s">
-        <v>554</v>
-      </c>
-      <c r="B37" s="69" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="60" t="s">
-        <v>556</v>
-      </c>
-      <c r="B38" s="69" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="60" t="s">
-        <v>558</v>
-      </c>
-      <c r="B39" s="69" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="60" t="s">
-        <v>560</v>
-      </c>
-      <c r="B40" s="69" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="60" t="s">
-        <v>562</v>
-      </c>
-      <c r="B41" s="69" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="60" t="s">
-        <v>329</v>
-      </c>
-      <c r="B43" s="69" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="60" t="s">
-        <v>599</v>
-      </c>
-      <c r="B44" s="69" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="60" t="s">
-        <v>308</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="60" t="s">
-        <v>600</v>
-      </c>
-      <c r="B46" s="69" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="60" t="s">
-        <v>609</v>
-      </c>
-      <c r="B47" s="69" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="60" t="s">
-        <v>611</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="60" t="s">
-        <v>243</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="60" t="s">
-        <v>289</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="7">
-        <v>4167877865</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="60" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="B58" s="7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="60" t="s">
-        <v>356</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="60" t="s">
-        <v>18</v>
-      </c>
-      <c r="B63" s="7">
-        <v>165782</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="60" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" s="71">
-        <v>43012</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="B65" s="7">
-        <v>1234567890</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="60" t="s">
-        <v>613</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="60" t="s">
-        <v>614</v>
-      </c>
-      <c r="B69" s="7">
-        <v>1234567899</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="60" t="s">
-        <v>615</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="60" t="s">
-        <v>616</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="60" t="s">
-        <v>618</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="60" t="s">
-        <v>620</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="52" t="s">
-        <v>371</v>
-      </c>
-      <c r="B74" s="72" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="52" t="s">
-        <v>622</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B6" r:id="rId2"/>
-    <hyperlink ref="B10" r:id="rId3"/>
-    <hyperlink ref="B14" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="B74" r:id="rId6"/>
-    <hyperlink ref="B18" r:id="rId7"/>
-    <hyperlink ref="B12" r:id="rId8"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7358,7 +6727,7 @@
         <v>613</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>535</v>
+        <v>59</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -8120,94 +7489,94 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="73" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="73" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="73" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="74" t="s">
+      <c r="H1" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="I1" s="74" t="s">
+      <c r="I1" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="J1" s="74" t="s">
+      <c r="J1" s="73" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="K1" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="74" t="s">
+      <c r="L1" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="74" t="s">
+      <c r="M1" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="N1" s="74" t="s">
+      <c r="N1" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="74" t="s">
+      <c r="O1" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="74" t="s">
+      <c r="P1" s="73" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="74" t="s">
+      <c r="Q1" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="75" t="s">
+      <c r="R1" s="77" t="s">
         <v>197</v>
       </c>
-      <c r="S1" s="75"/>
-      <c r="T1" s="78" t="s">
+      <c r="S1" s="77"/>
+      <c r="T1" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="U1" s="76"/>
-      <c r="V1" s="75" t="s">
+      <c r="U1" s="74"/>
+      <c r="V1" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="76" t="s">
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="74" t="s">
         <v>194</v>
       </c>
-      <c r="AB1" s="79" t="s">
+      <c r="AB1" s="78" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="38"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
       <c r="R2" s="38" t="s">
         <v>138</v>
       </c>
@@ -8235,8 +7604,8 @@
       <c r="Z2" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="77"/>
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="75"/>
     </row>
     <row r="3" spans="1:28" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
@@ -8292,17 +7661,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -8313,6 +7671,17 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8440,11 +7809,11 @@
       <c r="B1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="81"/>
-      <c r="E1" s="82"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="81"/>
       <c r="F1" s="10" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
update gekodriver for ff
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1137" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="624">
   <si>
     <t>First and Last Name</t>
   </si>
@@ -5720,7 +5720,7 @@
   <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6025,602 +6025,766 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.5703125" style="59" customWidth="1"/>
-    <col min="2" max="2" width="58" style="59" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="59"/>
+    <col min="2" max="2" width="29.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="59" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="59" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="59"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="60" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="60" t="s">
+        <v>523</v>
+      </c>
+      <c r="D1" s="60" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="60" t="s">
         <v>525</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
         <v>527</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="60" t="s">
         <v>567</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
         <v>568</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>528</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
         <v>530</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
         <v>569</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
         <v>601</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="60" t="s">
         <v>244</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="60" t="s">
         <v>288</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="60" t="s">
         <v>292</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
         <v>398</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
         <v>532</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="60" t="s">
         <v>534</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
         <v>570</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="60" t="s">
         <v>603</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
         <v>535</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
         <v>537</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="60" t="s">
         <v>571</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
         <v>604</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="s">
         <v>245</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="60" t="s">
         <v>281</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
         <v>280</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
         <v>605</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="60" t="s">
         <v>539</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="60" t="s">
         <v>541</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="60" t="s">
         <v>333</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="s">
         <v>543</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="60" t="s">
         <v>544</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="60" t="s">
         <v>546</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="60" t="s">
         <v>548</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="60" t="s">
         <v>594</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="60" t="s">
         <v>596</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="60" t="s">
         <v>550</v>
       </c>
       <c r="B35" s="69" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="60" t="s">
         <v>552</v>
       </c>
       <c r="B36" s="69" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="60" t="s">
         <v>554</v>
       </c>
       <c r="B37" s="69" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="60" t="s">
         <v>556</v>
       </c>
       <c r="B38" s="69" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="60" t="s">
         <v>558</v>
       </c>
       <c r="B39" s="69" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="60" t="s">
         <v>560</v>
       </c>
       <c r="B40" s="69" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="60" t="s">
         <v>562</v>
       </c>
       <c r="B41" s="69" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
         <v>6</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="60" t="s">
         <v>329</v>
       </c>
       <c r="B43" s="69" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="60" t="s">
         <v>599</v>
       </c>
       <c r="B44" s="69" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="60" t="s">
         <v>308</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="60" t="s">
         <v>600</v>
       </c>
       <c r="B46" s="69" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="60" t="s">
         <v>609</v>
       </c>
       <c r="B47" s="69" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="60" t="s">
         <v>611</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="60" t="s">
         <v>243</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="60" t="s">
         <v>289</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="60" t="s">
         <v>3</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="7"/>
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="60" t="s">
         <v>4</v>
       </c>
       <c r="B52" s="7">
         <v>4167877865</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="60" t="s">
         <v>5</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="60" t="s">
         <v>6</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="60" t="s">
         <v>8</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="60" t="s">
         <v>10</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="60" t="s">
         <v>11</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="60" t="s">
         <v>13</v>
       </c>
       <c r="B58" s="7">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="60" t="s">
         <v>14</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="60" t="s">
         <v>15</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="60" t="s">
         <v>356</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="60" t="s">
         <v>17</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="60" t="s">
         <v>18</v>
       </c>
       <c r="B63" s="7">
         <v>165782</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="60" t="s">
         <v>19</v>
       </c>
       <c r="B64" s="71">
         <v>43012</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="60" t="s">
         <v>20</v>
       </c>
       <c r="B65" s="7">
         <v>1234567890</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="60" t="s">
         <v>21</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="60" t="s">
         <v>23</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="60" t="s">
         <v>613</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="60" t="s">
         <v>614</v>
       </c>
       <c r="B69" s="7">
         <v>1234567899</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="60" t="s">
         <v>615</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="60" t="s">
         <v>616</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="60" t="s">
         <v>618</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="60" t="s">
         <v>620</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="52" t="s">
         <v>371</v>
       </c>
@@ -6628,7 +6792,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="52" t="s">
         <v>622</v>
       </c>

</xml_diff>